<commit_message>
updated samples according to rggen/rggen#8
</commit_message>
<xml_diff>
--- a/block_0.xlsx
+++ b/block_0.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCBEBE58-F66D-4713-AE0A-F97865A3A2E9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{388FB45C-BB72-4435-B5C9-E6420A1D8F11}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="block_0" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="108">
   <si>
     <t>block name</t>
     <phoneticPr fontId="1"/>
@@ -330,19 +330,11 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>4:4</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>rwc</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
     <t>register_0.bit_field_2</t>
-  </si>
-  <si>
-    <t>bit_field_2</t>
-    <phoneticPr fontId="1"/>
   </si>
   <si>
     <t>rwe</t>
@@ -422,6 +414,46 @@
   </si>
   <si>
     <t>register_6.bit_field_4</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>0:2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>2:2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>bit_field_2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>bit_field_3</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>4:2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>6:2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>rws</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>register_3.bit_field_2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>bit_field_8</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>bit_field_9</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -1028,7 +1060,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:J40"/>
+  <dimension ref="B1:J42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1163,7 +1195,7 @@
       <c r="E8" s="28"/>
       <c r="F8" s="3"/>
       <c r="G8" s="3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="H8" s="3" t="s">
         <v>14</v>
@@ -1276,13 +1308,13 @@
       <c r="D14" s="21"/>
       <c r="E14" s="22"/>
       <c r="F14" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="G14" s="3" t="s">
         <v>22</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="I14" s="4"/>
       <c r="J14" s="5"/>
@@ -1299,7 +1331,7 @@
         <v>20</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="I15" s="4"/>
       <c r="J15" s="5"/>
@@ -1364,7 +1396,7 @@
       </c>
       <c r="I18" s="4"/>
       <c r="J18" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="19" spans="2:10">
@@ -1399,7 +1431,7 @@
         <v>12</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>13</v>
+        <v>98</v>
       </c>
       <c r="H20" s="3" t="s">
         <v>75</v>
@@ -1418,10 +1450,10 @@
         <v>76</v>
       </c>
       <c r="G21" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="H21" s="3" t="s">
         <v>77</v>
-      </c>
-      <c r="H21" s="3" t="s">
-        <v>78</v>
       </c>
       <c r="I21" s="4">
         <v>0</v>
@@ -1436,13 +1468,13 @@
       <c r="D22" s="21"/>
       <c r="E22" s="22"/>
       <c r="F22" s="3" t="s">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>88</v>
+        <v>102</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>81</v>
+        <v>104</v>
       </c>
       <c r="I22" s="4">
         <v>0</v>
@@ -1455,19 +1487,19 @@
       <c r="D23" s="21"/>
       <c r="E23" s="22"/>
       <c r="F23" s="3" t="s">
-        <v>19</v>
+        <v>101</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>89</v>
+        <v>103</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>81</v>
+        <v>104</v>
       </c>
       <c r="I23" s="4">
         <v>0</v>
       </c>
       <c r="J23" s="5" t="s">
-        <v>79</v>
+        <v>105</v>
       </c>
     </row>
     <row r="24" spans="2:10">
@@ -1479,17 +1511,15 @@
         <v>21</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="I24" s="4">
         <v>0</v>
       </c>
-      <c r="J24" s="5" t="s">
-        <v>91</v>
-      </c>
+      <c r="J24" s="5"/>
     </row>
     <row r="25" spans="2:10">
       <c r="B25" s="20"/>
@@ -1500,15 +1530,17 @@
         <v>35</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="I25" s="4">
         <v>0</v>
       </c>
-      <c r="J25" s="5"/>
+      <c r="J25" s="5" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="26" spans="2:10">
       <c r="B26" s="20"/>
@@ -1519,101 +1551,101 @@
         <v>61</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="H26" s="3" t="s">
-        <v>28</v>
+        <v>79</v>
       </c>
       <c r="I26" s="4">
         <v>0</v>
       </c>
       <c r="J26" s="5" t="s">
-        <v>27</v>
+        <v>89</v>
       </c>
     </row>
     <row r="27" spans="2:10">
-      <c r="B27" s="23"/>
-      <c r="C27" s="24"/>
-      <c r="D27" s="24"/>
-      <c r="E27" s="25"/>
+      <c r="B27" s="20"/>
+      <c r="C27" s="21"/>
+      <c r="D27" s="21"/>
+      <c r="E27" s="22"/>
       <c r="F27" s="3" t="s">
         <v>62</v>
       </c>
       <c r="G27" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="H27" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="I27" s="4">
+        <v>0</v>
+      </c>
+      <c r="J27" s="5"/>
+    </row>
+    <row r="28" spans="2:10">
+      <c r="B28" s="20"/>
+      <c r="C28" s="21"/>
+      <c r="D28" s="21"/>
+      <c r="E28" s="22"/>
+      <c r="F28" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="H28" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I28" s="4">
+        <v>0</v>
+      </c>
+      <c r="J28" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="2:10">
+      <c r="B29" s="23"/>
+      <c r="C29" s="24"/>
+      <c r="D29" s="24"/>
+      <c r="E29" s="25"/>
+      <c r="F29" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="G29" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="H29" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I29" s="4">
+        <v>0</v>
+      </c>
+      <c r="J29" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="30" spans="2:10">
+      <c r="B30" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="C30" s="27" t="s">
         <v>94</v>
       </c>
-      <c r="H27" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="I27" s="4">
-        <v>0</v>
-      </c>
-      <c r="J27" s="5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="28" spans="2:10">
-      <c r="B28" s="26" t="s">
-        <v>58</v>
-      </c>
-      <c r="C28" s="27" t="s">
-        <v>96</v>
-      </c>
-      <c r="D28" s="27"/>
-      <c r="E28" s="28"/>
-      <c r="F28" s="3" t="s">
+      <c r="D30" s="27"/>
+      <c r="E30" s="28"/>
+      <c r="F30" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G28" s="3" t="s">
+      <c r="G30" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="H28" s="3" t="s">
+      <c r="H30" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="I28" s="4">
-        <v>0</v>
-      </c>
-      <c r="J28" s="5"/>
-    </row>
-    <row r="29" spans="2:10">
-      <c r="B29" s="20"/>
-      <c r="C29" s="21"/>
-      <c r="D29" s="21"/>
-      <c r="E29" s="22"/>
-      <c r="F29" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="G29" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="H29" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="I29" s="4">
-        <v>0</v>
-      </c>
-      <c r="J29" s="5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="30" spans="2:10">
-      <c r="B30" s="20"/>
-      <c r="C30" s="21"/>
-      <c r="D30" s="21"/>
-      <c r="E30" s="22"/>
-      <c r="F30" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G30" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="H30" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="I30" s="4"/>
-      <c r="J30" s="5" t="s">
-        <v>95</v>
-      </c>
+      <c r="I30" s="4">
+        <v>0</v>
+      </c>
+      <c r="J30" s="5"/>
     </row>
     <row r="31" spans="2:10">
       <c r="B31" s="20"/>
@@ -1621,18 +1653,20 @@
       <c r="D31" s="21"/>
       <c r="E31" s="22"/>
       <c r="F31" s="3" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>33</v>
+        <v>16</v>
       </c>
       <c r="H31" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I31" s="4">
         <v>0</v>
       </c>
-      <c r="J31" s="5"/>
+      <c r="J31" s="5" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="32" spans="2:10">
       <c r="B32" s="20"/>
@@ -1640,19 +1674,17 @@
       <c r="D32" s="21"/>
       <c r="E32" s="22"/>
       <c r="F32" s="3" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="H32" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="I32" s="4">
-        <v>0</v>
-      </c>
+        <v>51</v>
+      </c>
+      <c r="I32" s="4"/>
       <c r="J32" s="5" t="s">
-        <v>25</v>
+        <v>93</v>
       </c>
     </row>
     <row r="33" spans="2:10">
@@ -1661,18 +1693,18 @@
       <c r="D33" s="21"/>
       <c r="E33" s="22"/>
       <c r="F33" s="3" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>59</v>
+        <v>33</v>
       </c>
       <c r="H33" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="I33" s="4"/>
-      <c r="J33" s="5" t="s">
-        <v>99</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="I33" s="4">
+        <v>0</v>
+      </c>
+      <c r="J33" s="5"/>
     </row>
     <row r="34" spans="2:10">
       <c r="B34" s="20"/>
@@ -1680,57 +1712,53 @@
       <c r="D34" s="21"/>
       <c r="E34" s="22"/>
       <c r="F34" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G34" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H34" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="I34" s="4">
+        <v>0</v>
+      </c>
+      <c r="J34" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="35" spans="2:10">
+      <c r="B35" s="20"/>
+      <c r="C35" s="21"/>
+      <c r="D35" s="21"/>
+      <c r="E35" s="22"/>
+      <c r="F35" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="G35" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="H35" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="I35" s="4"/>
+      <c r="J35" s="5" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="36" spans="2:10">
+      <c r="B36" s="20"/>
+      <c r="C36" s="21"/>
+      <c r="D36" s="21"/>
+      <c r="E36" s="22"/>
+      <c r="F36" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="G34" s="3" t="s">
+      <c r="G36" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="H34" s="3" t="s">
+      <c r="H36" s="3" t="s">
         <v>34</v>
-      </c>
-      <c r="I34" s="4">
-        <v>0</v>
-      </c>
-      <c r="J34" s="5"/>
-    </row>
-    <row r="35" spans="2:10">
-      <c r="B35" s="23"/>
-      <c r="C35" s="24"/>
-      <c r="D35" s="24"/>
-      <c r="E35" s="25"/>
-      <c r="F35" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="G35" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="H35" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="I35" s="4">
-        <v>0</v>
-      </c>
-      <c r="J35" s="5"/>
-    </row>
-    <row r="36" spans="2:10">
-      <c r="B36" s="26" t="s">
-        <v>56</v>
-      </c>
-      <c r="C36" s="27" t="s">
-        <v>54</v>
-      </c>
-      <c r="D36" s="27" t="s">
-        <v>39</v>
-      </c>
-      <c r="E36" s="28"/>
-      <c r="F36" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G36" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="H36" s="3" t="s">
-        <v>14</v>
       </c>
       <c r="I36" s="4">
         <v>0</v>
@@ -1743,32 +1771,30 @@
       <c r="D37" s="24"/>
       <c r="E37" s="25"/>
       <c r="F37" s="3" t="s">
-        <v>15</v>
+        <v>62</v>
       </c>
       <c r="G37" s="3" t="s">
-        <v>41</v>
+        <v>64</v>
       </c>
       <c r="H37" s="3" t="s">
-        <v>14</v>
+        <v>36</v>
       </c>
       <c r="I37" s="4">
         <v>0</v>
       </c>
       <c r="J37" s="5"/>
     </row>
-    <row r="38" spans="2:10" ht="93.75">
+    <row r="38" spans="2:10">
       <c r="B38" s="26" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C38" s="27" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D38" s="27" t="s">
-        <v>43</v>
-      </c>
-      <c r="E38" s="29" t="s">
-        <v>98</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="E38" s="28"/>
       <c r="F38" s="3" t="s">
         <v>12</v>
       </c>
@@ -1802,24 +1828,70 @@
       </c>
       <c r="J39" s="5"/>
     </row>
-    <row r="40" spans="2:10" ht="19.5" thickBot="1">
-      <c r="B40" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="C40" s="7" t="s">
+    <row r="40" spans="2:10" ht="93.75">
+      <c r="B40" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="C40" s="27" t="s">
+        <v>55</v>
+      </c>
+      <c r="D40" s="27" t="s">
+        <v>43</v>
+      </c>
+      <c r="E40" s="29" t="s">
+        <v>96</v>
+      </c>
+      <c r="F40" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G40" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="H40" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I40" s="4">
+        <v>0</v>
+      </c>
+      <c r="J40" s="5"/>
+    </row>
+    <row r="41" spans="2:10">
+      <c r="B41" s="23"/>
+      <c r="C41" s="24"/>
+      <c r="D41" s="24"/>
+      <c r="E41" s="25"/>
+      <c r="F41" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G41" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="H41" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I41" s="4">
+        <v>0</v>
+      </c>
+      <c r="J41" s="5"/>
+    </row>
+    <row r="42" spans="2:10" ht="19.5" thickBot="1">
+      <c r="B42" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="C42" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="D40" s="7" t="s">
+      <c r="D42" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="E40" s="8" t="s">
+      <c r="E42" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="F40" s="8"/>
-      <c r="G40" s="8"/>
-      <c r="H40" s="8"/>
-      <c r="I40" s="7"/>
-      <c r="J40" s="9"/>
+      <c r="F42" s="8"/>
+      <c r="G42" s="8"/>
+      <c r="H42" s="8"/>
+      <c r="I42" s="7"/>
+      <c r="J42" s="9"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>

</xml_diff>

<commit_message>
updated samples accordng to rggen/rggen#9
</commit_message>
<xml_diff>
--- a/block_0.xlsx
+++ b/block_0.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{388FB45C-BB72-4435-B5C9-E6420A1D8F11}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E778559-0067-4211-8838-062CD6A98616}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="122">
   <si>
     <t>block name</t>
     <phoneticPr fontId="1"/>
@@ -243,10 +243,6 @@
   </si>
   <si>
     <t>0x40</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>register_7</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -454,6 +450,66 @@
   </si>
   <si>
     <t>bit_field_9</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>register_10</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>register_7</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>0x18</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>bit_field_0</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>0:4</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>w0crs</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>bit_field_1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>bit_field_2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>bit_field_3</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>8:4</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>16:4</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>24:4</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>w1crs</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>w0src</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>w1src</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -1060,7 +1116,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:J42"/>
+  <dimension ref="B1:J46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1195,7 +1251,7 @@
       <c r="E8" s="28"/>
       <c r="F8" s="3"/>
       <c r="G8" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H8" s="3" t="s">
         <v>14</v>
@@ -1232,13 +1288,13 @@
       <c r="D10" s="21"/>
       <c r="E10" s="22"/>
       <c r="F10" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="G10" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="G10" s="3" t="s">
+      <c r="H10" s="3" t="s">
         <v>66</v>
-      </c>
-      <c r="H10" s="3" t="s">
-        <v>67</v>
       </c>
       <c r="I10" s="4"/>
       <c r="J10" s="5"/>
@@ -1249,16 +1305,16 @@
       <c r="D11" s="21"/>
       <c r="E11" s="22"/>
       <c r="F11" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="G11" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="G11" s="3" t="s">
+      <c r="H11" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="H11" s="3" t="s">
+      <c r="I11" s="4" t="s">
         <v>70</v>
-      </c>
-      <c r="I11" s="4" t="s">
-        <v>71</v>
       </c>
       <c r="J11" s="5"/>
     </row>
@@ -1268,13 +1324,13 @@
       <c r="D12" s="24"/>
       <c r="E12" s="25"/>
       <c r="F12" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="G12" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="G12" s="3" t="s">
+      <c r="H12" s="3" t="s">
         <v>73</v>
-      </c>
-      <c r="H12" s="3" t="s">
-        <v>74</v>
       </c>
       <c r="I12" s="4"/>
       <c r="J12" s="5"/>
@@ -1308,13 +1364,13 @@
       <c r="D14" s="21"/>
       <c r="E14" s="22"/>
       <c r="F14" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G14" s="3" t="s">
         <v>22</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I14" s="4"/>
       <c r="J14" s="5"/>
@@ -1331,7 +1387,7 @@
         <v>20</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I15" s="4"/>
       <c r="J15" s="5"/>
@@ -1396,7 +1452,7 @@
       </c>
       <c r="I18" s="4"/>
       <c r="J18" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="19" spans="2:10">
@@ -1431,10 +1487,10 @@
         <v>12</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I20" s="4">
         <v>0</v>
@@ -1447,19 +1503,19 @@
       <c r="D21" s="21"/>
       <c r="E21" s="22"/>
       <c r="F21" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="H21" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="G21" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="H21" s="3" t="s">
-        <v>77</v>
-      </c>
       <c r="I21" s="4">
         <v>0</v>
       </c>
       <c r="J21" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="22" spans="2:10">
@@ -1468,13 +1524,13 @@
       <c r="D22" s="21"/>
       <c r="E22" s="22"/>
       <c r="F22" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="I22" s="4">
         <v>0</v>
@@ -1487,19 +1543,19 @@
       <c r="D23" s="21"/>
       <c r="E23" s="22"/>
       <c r="F23" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G23" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="H23" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="H23" s="3" t="s">
+      <c r="I23" s="4">
+        <v>0</v>
+      </c>
+      <c r="J23" s="5" t="s">
         <v>104</v>
-      </c>
-      <c r="I23" s="4">
-        <v>0</v>
-      </c>
-      <c r="J23" s="5" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="24" spans="2:10">
@@ -1511,10 +1567,10 @@
         <v>21</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I24" s="4">
         <v>0</v>
@@ -1530,16 +1586,16 @@
         <v>35</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I25" s="4">
         <v>0</v>
       </c>
       <c r="J25" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="26" spans="2:10">
@@ -1548,19 +1604,19 @@
       <c r="D26" s="21"/>
       <c r="E26" s="22"/>
       <c r="F26" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G26" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="H26" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="I26" s="4">
+        <v>0</v>
+      </c>
+      <c r="J26" s="5" t="s">
         <v>88</v>
-      </c>
-      <c r="H26" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="I26" s="4">
-        <v>0</v>
-      </c>
-      <c r="J26" s="5" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="27" spans="2:10">
@@ -1569,13 +1625,13 @@
       <c r="D27" s="21"/>
       <c r="E27" s="22"/>
       <c r="F27" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H27" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I27" s="4">
         <v>0</v>
@@ -1588,10 +1644,10 @@
       <c r="D28" s="21"/>
       <c r="E28" s="22"/>
       <c r="F28" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H28" s="3" t="s">
         <v>28</v>
@@ -1609,10 +1665,10 @@
       <c r="D29" s="24"/>
       <c r="E29" s="25"/>
       <c r="F29" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H29" s="3" t="s">
         <v>28</v>
@@ -1626,10 +1682,10 @@
     </row>
     <row r="30" spans="2:10">
       <c r="B30" s="26" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C30" s="27" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D30" s="27"/>
       <c r="E30" s="28"/>
@@ -1684,7 +1740,7 @@
       </c>
       <c r="I32" s="4"/>
       <c r="J32" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="33" spans="2:10">
@@ -1736,14 +1792,14 @@
         <v>35</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H35" s="3" t="s">
         <v>51</v>
       </c>
       <c r="I35" s="4"/>
       <c r="J35" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="36" spans="2:10">
@@ -1752,10 +1808,10 @@
       <c r="D36" s="21"/>
       <c r="E36" s="22"/>
       <c r="F36" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H36" s="3" t="s">
         <v>34</v>
@@ -1771,10 +1827,10 @@
       <c r="D37" s="24"/>
       <c r="E37" s="25"/>
       <c r="F37" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G37" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H37" s="3" t="s">
         <v>36</v>
@@ -1785,113 +1841,193 @@
       <c r="J37" s="5"/>
     </row>
     <row r="38" spans="2:10">
-      <c r="B38" s="26" t="s">
+      <c r="B38" s="20" t="s">
+        <v>108</v>
+      </c>
+      <c r="C38" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="D38" s="21"/>
+      <c r="E38" s="22"/>
+      <c r="F38" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="G38" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="H38" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="I38" s="4">
+        <v>0</v>
+      </c>
+      <c r="J38" s="5"/>
+    </row>
+    <row r="39" spans="2:10">
+      <c r="B39" s="20"/>
+      <c r="C39" s="21"/>
+      <c r="D39" s="21"/>
+      <c r="E39" s="22"/>
+      <c r="F39" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="G39" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="H39" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="I39" s="4">
+        <v>0</v>
+      </c>
+      <c r="J39" s="5"/>
+    </row>
+    <row r="40" spans="2:10">
+      <c r="B40" s="20"/>
+      <c r="C40" s="21"/>
+      <c r="D40" s="21"/>
+      <c r="E40" s="22"/>
+      <c r="F40" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="G40" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="H40" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="I40" s="4">
+        <v>0</v>
+      </c>
+      <c r="J40" s="5"/>
+    </row>
+    <row r="41" spans="2:10">
+      <c r="B41" s="20"/>
+      <c r="C41" s="21"/>
+      <c r="D41" s="21"/>
+      <c r="E41" s="22"/>
+      <c r="F41" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="G41" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="H41" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="I41" s="4">
+        <v>0</v>
+      </c>
+      <c r="J41" s="5"/>
+    </row>
+    <row r="42" spans="2:10">
+      <c r="B42" s="26" t="s">
         <v>56</v>
       </c>
-      <c r="C38" s="27" t="s">
+      <c r="C42" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="D38" s="27" t="s">
+      <c r="D42" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="E38" s="28"/>
-      <c r="F38" s="3" t="s">
+      <c r="E42" s="28"/>
+      <c r="F42" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G38" s="3" t="s">
+      <c r="G42" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="H38" s="3" t="s">
+      <c r="H42" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="I38" s="4">
-        <v>0</v>
-      </c>
-      <c r="J38" s="5"/>
-    </row>
-    <row r="39" spans="2:10">
-      <c r="B39" s="23"/>
-      <c r="C39" s="24"/>
-      <c r="D39" s="24"/>
-      <c r="E39" s="25"/>
-      <c r="F39" s="3" t="s">
+      <c r="I42" s="4">
+        <v>0</v>
+      </c>
+      <c r="J42" s="5"/>
+    </row>
+    <row r="43" spans="2:10">
+      <c r="B43" s="23"/>
+      <c r="C43" s="24"/>
+      <c r="D43" s="24"/>
+      <c r="E43" s="25"/>
+      <c r="F43" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="G39" s="3" t="s">
+      <c r="G43" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="H39" s="3" t="s">
+      <c r="H43" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="I39" s="4">
-        <v>0</v>
-      </c>
-      <c r="J39" s="5"/>
-    </row>
-    <row r="40" spans="2:10" ht="93.75">
-      <c r="B40" s="26" t="s">
-        <v>57</v>
-      </c>
-      <c r="C40" s="27" t="s">
+      <c r="I43" s="4">
+        <v>0</v>
+      </c>
+      <c r="J43" s="5"/>
+    </row>
+    <row r="44" spans="2:10" ht="93.75">
+      <c r="B44" s="26" t="s">
+        <v>94</v>
+      </c>
+      <c r="C44" s="27" t="s">
         <v>55</v>
       </c>
-      <c r="D40" s="27" t="s">
+      <c r="D44" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="E40" s="29" t="s">
-        <v>96</v>
-      </c>
-      <c r="F40" s="3" t="s">
+      <c r="E44" s="29" t="s">
+        <v>95</v>
+      </c>
+      <c r="F44" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G40" s="3" t="s">
+      <c r="G44" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="H40" s="3" t="s">
+      <c r="H44" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="I40" s="4">
-        <v>0</v>
-      </c>
-      <c r="J40" s="5"/>
-    </row>
-    <row r="41" spans="2:10">
-      <c r="B41" s="23"/>
-      <c r="C41" s="24"/>
-      <c r="D41" s="24"/>
-      <c r="E41" s="25"/>
-      <c r="F41" s="3" t="s">
+      <c r="I44" s="4">
+        <v>0</v>
+      </c>
+      <c r="J44" s="5"/>
+    </row>
+    <row r="45" spans="2:10">
+      <c r="B45" s="23"/>
+      <c r="C45" s="24"/>
+      <c r="D45" s="24"/>
+      <c r="E45" s="25"/>
+      <c r="F45" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="G41" s="3" t="s">
+      <c r="G45" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="H41" s="3" t="s">
+      <c r="H45" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="I41" s="4">
-        <v>0</v>
-      </c>
-      <c r="J41" s="5"/>
-    </row>
-    <row r="42" spans="2:10" ht="19.5" thickBot="1">
-      <c r="B42" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="C42" s="7" t="s">
+      <c r="I45" s="4">
+        <v>0</v>
+      </c>
+      <c r="J45" s="5"/>
+    </row>
+    <row r="46" spans="2:10" ht="19.5" thickBot="1">
+      <c r="B46" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="C46" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="D42" s="7" t="s">
+      <c r="D46" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="E42" s="8" t="s">
+      <c r="E46" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="F42" s="8"/>
-      <c r="G42" s="8"/>
-      <c r="H42" s="8"/>
-      <c r="I42" s="7"/>
-      <c r="J42" s="9"/>
+      <c r="F46" s="8"/>
+      <c r="G46" s="8"/>
+      <c r="H46" s="8"/>
+      <c r="I46" s="7"/>
+      <c r="J46" s="9"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>

</xml_diff>

<commit_message>
added new samples for indirect register type
</commit_message>
<xml_diff>
--- a/block_0.xlsx
+++ b/block_0.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E778559-0067-4211-8838-062CD6A98616}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4538A425-AFAA-4977-8066-90742520B4CA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="block_0" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="130">
   <si>
     <t>block name</t>
     <phoneticPr fontId="1"/>
@@ -398,118 +398,150 @@
   </si>
   <si>
     <t>register_9</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>register_6.bit_field_4</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>0:2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>2:2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>bit_field_2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>bit_field_3</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>4:2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>6:2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>rws</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>register_3.bit_field_2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>bit_field_8</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>bit_field_9</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>register_7</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>0x18</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>bit_field_0</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>0:4</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>w0crs</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>bit_field_1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>bit_field_2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>bit_field_3</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>8:4</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>16:4</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>24:4</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>w1crs</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>w0src</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>w1src</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>register_12</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>register_10</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>0x40</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>bit_field_0</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>0:1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>rw</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>register_11</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
     <t>indirect:
 register_0.bit_field_0
 register_0.bit_field_1
-register_0.bit_field_2:0
-register_1:1</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>register_6.bit_field_4</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>0:2</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>2:2</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>bit_field_2</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>bit_field_3</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>4:2</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>6:2</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>rws</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>register_3.bit_field_2</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>bit_field_8</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>bit_field_9</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>register_10</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>register_7</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>0x18</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>bit_field_0</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>0:4</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>w0crs</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>bit_field_1</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>bit_field_2</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>bit_field_3</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>8:4</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>16:4</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>24:4</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>w1crs</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>w0src</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>w1src</t>
+register_0.bit_field_2:0</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>indirect:
+register_0.bit_field_2:1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>0x44</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -541,7 +573,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="19">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -799,11 +831,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
@@ -834,6 +881,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1116,7 +1167,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:J46"/>
+  <dimension ref="B1:J48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1487,7 +1538,7 @@
         <v>12</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H20" s="3" t="s">
         <v>74</v>
@@ -1506,7 +1557,7 @@
         <v>75</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H21" s="3" t="s">
         <v>76</v>
@@ -1524,13 +1575,13 @@
       <c r="D22" s="21"/>
       <c r="E22" s="22"/>
       <c r="F22" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I22" s="4">
         <v>0</v>
@@ -1543,19 +1594,19 @@
       <c r="D23" s="21"/>
       <c r="E23" s="22"/>
       <c r="F23" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G23" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="H23" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="H23" s="3" t="s">
+      <c r="I23" s="4">
+        <v>0</v>
+      </c>
+      <c r="J23" s="5" t="s">
         <v>103</v>
-      </c>
-      <c r="I23" s="4">
-        <v>0</v>
-      </c>
-      <c r="J23" s="5" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="24" spans="2:10">
@@ -1644,7 +1695,7 @@
       <c r="D28" s="21"/>
       <c r="E28" s="22"/>
       <c r="F28" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G28" s="3" t="s">
         <v>90</v>
@@ -1665,7 +1716,7 @@
       <c r="D29" s="24"/>
       <c r="E29" s="25"/>
       <c r="F29" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G29" s="3" t="s">
         <v>91</v>
@@ -1799,7 +1850,7 @@
       </c>
       <c r="I35" s="4"/>
       <c r="J35" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="36" spans="2:10">
@@ -1842,21 +1893,21 @@
     </row>
     <row r="38" spans="2:10">
       <c r="B38" s="20" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C38" s="21" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D38" s="21"/>
       <c r="E38" s="22"/>
       <c r="F38" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="G38" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="H38" s="3" t="s">
         <v>110</v>
-      </c>
-      <c r="G38" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="H38" s="3" t="s">
-        <v>112</v>
       </c>
       <c r="I38" s="4">
         <v>0</v>
@@ -1869,13 +1920,13 @@
       <c r="D39" s="21"/>
       <c r="E39" s="22"/>
       <c r="F39" s="3" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="G39" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H39" s="3" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="I39" s="4">
         <v>0</v>
@@ -1888,13 +1939,13 @@
       <c r="D40" s="21"/>
       <c r="E40" s="22"/>
       <c r="F40" s="3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="G40" s="3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="H40" s="3" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="I40" s="4">
         <v>0</v>
@@ -1907,13 +1958,13 @@
       <c r="D41" s="21"/>
       <c r="E41" s="22"/>
       <c r="F41" s="3" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="G41" s="3" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="H41" s="3" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="I41" s="4">
         <v>0</v>
@@ -1964,7 +2015,7 @@
       </c>
       <c r="J43" s="5"/>
     </row>
-    <row r="44" spans="2:10" ht="93.75">
+    <row r="44" spans="2:10" ht="75">
       <c r="B44" s="26" t="s">
         <v>94</v>
       </c>
@@ -1975,7 +2026,7 @@
         <v>43</v>
       </c>
       <c r="E44" s="29" t="s">
-        <v>95</v>
+        <v>127</v>
       </c>
       <c r="F44" s="3" t="s">
         <v>12</v>
@@ -2010,24 +2061,74 @@
       </c>
       <c r="J45" s="5"/>
     </row>
-    <row r="46" spans="2:10" ht="19.5" thickBot="1">
-      <c r="B46" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="C46" s="7" t="s">
+    <row r="46" spans="2:10" ht="37.5">
+      <c r="B46" s="30" t="s">
+        <v>121</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="D46" s="4"/>
+      <c r="E46" s="31" t="s">
+        <v>128</v>
+      </c>
+      <c r="F46" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="G46" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="H46" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="I46" s="4">
+        <v>0</v>
+      </c>
+      <c r="J46" s="5"/>
+    </row>
+    <row r="47" spans="2:10" ht="37.5">
+      <c r="B47" s="30" t="s">
+        <v>126</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="D47" s="4"/>
+      <c r="E47" s="31" t="s">
+        <v>128</v>
+      </c>
+      <c r="F47" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="G47" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="H47" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="I47" s="4">
+        <v>0</v>
+      </c>
+      <c r="J47" s="5"/>
+    </row>
+    <row r="48" spans="2:10" ht="19.5" thickBot="1">
+      <c r="B48" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="C48" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="D46" s="7" t="s">
+      <c r="D48" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="E46" s="8" t="s">
+      <c r="E48" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="F46" s="8"/>
-      <c r="G46" s="8"/>
-      <c r="H46" s="8"/>
-      <c r="I46" s="7"/>
-      <c r="J46" s="9"/>
+      <c r="F48" s="8"/>
+      <c r="G48" s="8"/>
+      <c r="H48" s="8"/>
+      <c r="I48" s="7"/>
+      <c r="J48" s="9"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>

</xml_diff>

<commit_message>
updated samples due to rggen/rggen#14
</commit_message>
<xml_diff>
--- a/block_0.xlsx
+++ b/block_0.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22130"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4538A425-AFAA-4977-8066-90742520B4CA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B3D9636-7600-4E7C-AD69-3D8102644F6F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="137">
   <si>
     <t>block name</t>
     <phoneticPr fontId="1"/>
@@ -542,6 +542,34 @@
   </si>
   <si>
     <t>0x44</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>0:4:4:16</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>8:4:4:16</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>bit_field_1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>4:4:4:16</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>rw</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>default: 0</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>0, 1, 2, 3</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -1167,7 +1195,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:J48"/>
+  <dimension ref="B1:J49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1986,7 +2014,7 @@
         <v>12</v>
       </c>
       <c r="G42" s="3" t="s">
-        <v>40</v>
+        <v>130</v>
       </c>
       <c r="H42" s="3" t="s">
         <v>14</v>
@@ -1997,61 +2025,61 @@
       <c r="J42" s="5"/>
     </row>
     <row r="43" spans="2:10">
-      <c r="B43" s="23"/>
-      <c r="C43" s="24"/>
-      <c r="D43" s="24"/>
-      <c r="E43" s="25"/>
+      <c r="B43" s="20"/>
+      <c r="C43" s="21"/>
+      <c r="D43" s="21"/>
+      <c r="E43" s="22"/>
       <c r="F43" s="3" t="s">
-        <v>15</v>
+        <v>132</v>
       </c>
       <c r="G43" s="3" t="s">
-        <v>41</v>
+        <v>133</v>
       </c>
       <c r="H43" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="I43" s="4">
-        <v>0</v>
+        <v>134</v>
+      </c>
+      <c r="I43" s="4" t="s">
+        <v>135</v>
       </c>
       <c r="J43" s="5"/>
     </row>
-    <row r="44" spans="2:10" ht="75">
-      <c r="B44" s="26" t="s">
-        <v>94</v>
-      </c>
-      <c r="C44" s="27" t="s">
-        <v>55</v>
-      </c>
-      <c r="D44" s="27" t="s">
-        <v>43</v>
-      </c>
-      <c r="E44" s="29" t="s">
-        <v>127</v>
-      </c>
+    <row r="44" spans="2:10">
+      <c r="B44" s="23"/>
+      <c r="C44" s="24"/>
+      <c r="D44" s="24"/>
+      <c r="E44" s="25"/>
       <c r="F44" s="3" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="G44" s="3" t="s">
-        <v>40</v>
+        <v>131</v>
       </c>
       <c r="H44" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="I44" s="4">
-        <v>0</v>
+      <c r="I44" s="4" t="s">
+        <v>136</v>
       </c>
       <c r="J44" s="5"/>
     </row>
-    <row r="45" spans="2:10">
-      <c r="B45" s="23"/>
-      <c r="C45" s="24"/>
-      <c r="D45" s="24"/>
-      <c r="E45" s="25"/>
+    <row r="45" spans="2:10" ht="75">
+      <c r="B45" s="26" t="s">
+        <v>94</v>
+      </c>
+      <c r="C45" s="27" t="s">
+        <v>55</v>
+      </c>
+      <c r="D45" s="27" t="s">
+        <v>43</v>
+      </c>
+      <c r="E45" s="29" t="s">
+        <v>127</v>
+      </c>
       <c r="F45" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="G45" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H45" s="3" t="s">
         <v>14</v>
@@ -2061,25 +2089,19 @@
       </c>
       <c r="J45" s="5"/>
     </row>
-    <row r="46" spans="2:10" ht="37.5">
-      <c r="B46" s="30" t="s">
-        <v>121</v>
-      </c>
-      <c r="C46" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="D46" s="4"/>
-      <c r="E46" s="31" t="s">
-        <v>128</v>
-      </c>
+    <row r="46" spans="2:10">
+      <c r="B46" s="23"/>
+      <c r="C46" s="24"/>
+      <c r="D46" s="24"/>
+      <c r="E46" s="25"/>
       <c r="F46" s="3" t="s">
-        <v>123</v>
+        <v>15</v>
       </c>
       <c r="G46" s="3" t="s">
-        <v>124</v>
+        <v>41</v>
       </c>
       <c r="H46" s="3" t="s">
-        <v>125</v>
+        <v>14</v>
       </c>
       <c r="I46" s="4">
         <v>0</v>
@@ -2088,10 +2110,10 @@
     </row>
     <row r="47" spans="2:10" ht="37.5">
       <c r="B47" s="30" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="D47" s="4"/>
       <c r="E47" s="31" t="s">
@@ -2111,24 +2133,49 @@
       </c>
       <c r="J47" s="5"/>
     </row>
-    <row r="48" spans="2:10" ht="19.5" thickBot="1">
-      <c r="B48" s="6" t="s">
+    <row r="48" spans="2:10" ht="37.5">
+      <c r="B48" s="30" t="s">
+        <v>126</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="D48" s="4"/>
+      <c r="E48" s="31" t="s">
+        <v>128</v>
+      </c>
+      <c r="F48" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="G48" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="H48" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="I48" s="4">
+        <v>0</v>
+      </c>
+      <c r="J48" s="5"/>
+    </row>
+    <row r="49" spans="2:10" ht="19.5" thickBot="1">
+      <c r="B49" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="C48" s="7" t="s">
+      <c r="C49" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="D48" s="7" t="s">
+      <c r="D49" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="E48" s="8" t="s">
+      <c r="E49" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="F48" s="8"/>
-      <c r="G48" s="8"/>
-      <c r="H48" s="8"/>
-      <c r="I48" s="7"/>
-      <c r="J48" s="9"/>
+      <c r="F49" s="8"/>
+      <c r="G49" s="8"/>
+      <c r="H49" s="8"/>
+      <c r="I49" s="7"/>
+      <c r="J49" s="9"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>

</xml_diff>

<commit_message>
use omittable offset address (refs #rggen/rggen-default-register-map#7)
</commit_message>
<xml_diff>
--- a/block_0.xlsx
+++ b/block_0.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22130"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B3D9636-7600-4E7C-AD69-3D8102644F6F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BADA353F-7578-4337-997E-6C33B6EA3AA3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="135">
   <si>
     <t>block name</t>
     <phoneticPr fontId="1"/>
@@ -66,10 +66,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>0x00</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>bit_field_0</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -211,10 +207,6 @@
   </si>
   <si>
     <t>register_1</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>0x04</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -1262,19 +1254,17 @@
       <c r="B5" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="18" t="s">
-        <v>11</v>
-      </c>
+      <c r="C5" s="18"/>
       <c r="D5" s="18"/>
       <c r="E5" s="19"/>
       <c r="F5" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="15" t="s">
+      <c r="H5" s="15" t="s">
         <v>13</v>
-      </c>
-      <c r="H5" s="15" t="s">
-        <v>14</v>
       </c>
       <c r="I5" s="14">
         <v>0</v>
@@ -1287,13 +1277,13 @@
       <c r="D6" s="21"/>
       <c r="E6" s="22"/>
       <c r="F6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="G6" s="3" t="s">
-        <v>16</v>
-      </c>
       <c r="H6" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I6" s="4">
         <v>0</v>
@@ -1306,13 +1296,13 @@
       <c r="D7" s="24"/>
       <c r="E7" s="25"/>
       <c r="F7" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G7" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="G7" s="3" t="s">
-        <v>18</v>
-      </c>
       <c r="H7" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I7" s="4">
         <v>0</v>
@@ -1321,19 +1311,17 @@
     </row>
     <row r="8" spans="2:10">
       <c r="B8" s="26" t="s">
-        <v>47</v>
-      </c>
-      <c r="C8" s="27" t="s">
-        <v>48</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="C8" s="27"/>
       <c r="D8" s="27"/>
       <c r="E8" s="28"/>
       <c r="F8" s="3"/>
       <c r="G8" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I8" s="4">
         <v>0</v>
@@ -1342,21 +1330,21 @@
     </row>
     <row r="9" spans="2:10">
       <c r="B9" s="26" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C9" s="27" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D9" s="27"/>
       <c r="E9" s="28"/>
       <c r="F9" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="H9" s="3" t="s">
         <v>49</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>51</v>
       </c>
       <c r="I9" s="4"/>
       <c r="J9" s="5"/>
@@ -1367,13 +1355,13 @@
       <c r="D10" s="21"/>
       <c r="E10" s="22"/>
       <c r="F10" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="H10" s="3" t="s">
         <v>64</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="H10" s="3" t="s">
-        <v>66</v>
       </c>
       <c r="I10" s="4"/>
       <c r="J10" s="5"/>
@@ -1384,16 +1372,16 @@
       <c r="D11" s="21"/>
       <c r="E11" s="22"/>
       <c r="F11" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="H11" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="G11" s="3" t="s">
+      <c r="I11" s="4" t="s">
         <v>68</v>
-      </c>
-      <c r="H11" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="I11" s="4" t="s">
-        <v>70</v>
       </c>
       <c r="J11" s="5"/>
     </row>
@@ -1403,34 +1391,34 @@
       <c r="D12" s="24"/>
       <c r="E12" s="25"/>
       <c r="F12" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="H12" s="3" t="s">
         <v>71</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="H12" s="3" t="s">
-        <v>73</v>
       </c>
       <c r="I12" s="4"/>
       <c r="J12" s="5"/>
     </row>
     <row r="13" spans="2:10">
       <c r="B13" s="26" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C13" s="27" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D13" s="27"/>
       <c r="E13" s="28"/>
       <c r="F13" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="I13" s="4">
         <v>0</v>
@@ -1443,13 +1431,13 @@
       <c r="D14" s="21"/>
       <c r="E14" s="22"/>
       <c r="F14" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="I14" s="4"/>
       <c r="J14" s="5"/>
@@ -1460,34 +1448,34 @@
       <c r="D15" s="21"/>
       <c r="E15" s="22"/>
       <c r="F15" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="I15" s="4"/>
       <c r="J15" s="5"/>
     </row>
     <row r="16" spans="2:10">
       <c r="B16" s="26" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C16" s="27" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D16" s="27"/>
       <c r="E16" s="28"/>
       <c r="F16" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G16" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G16" s="3" t="s">
-        <v>13</v>
-      </c>
       <c r="H16" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I16" s="4">
         <v>0</v>
@@ -1500,19 +1488,19 @@
       <c r="D17" s="21"/>
       <c r="E17" s="22"/>
       <c r="F17" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G17" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H17" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="H17" s="3" t="s">
-        <v>23</v>
-      </c>
       <c r="I17" s="4">
         <v>0</v>
       </c>
       <c r="J17" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="18" spans="2:10">
@@ -1521,17 +1509,17 @@
       <c r="D18" s="21"/>
       <c r="E18" s="22"/>
       <c r="F18" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="I18" s="4"/>
       <c r="J18" s="5" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="19" spans="2:10">
@@ -1540,13 +1528,13 @@
       <c r="D19" s="24"/>
       <c r="E19" s="25"/>
       <c r="F19" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G19" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="G19" s="3" t="s">
-        <v>20</v>
-      </c>
       <c r="H19" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I19" s="4">
         <v>0</v>
@@ -1555,21 +1543,21 @@
     </row>
     <row r="20" spans="2:10">
       <c r="B20" s="26" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C20" s="27" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D20" s="27"/>
       <c r="E20" s="28"/>
       <c r="F20" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="I20" s="4">
         <v>0</v>
@@ -1582,19 +1570,19 @@
       <c r="D21" s="21"/>
       <c r="E21" s="22"/>
       <c r="F21" s="3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="I21" s="4">
         <v>0</v>
       </c>
       <c r="J21" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="22" spans="2:10">
@@ -1603,13 +1591,13 @@
       <c r="D22" s="21"/>
       <c r="E22" s="22"/>
       <c r="F22" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="G22" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="G22" s="3" t="s">
+      <c r="H22" s="3" t="s">
         <v>100</v>
-      </c>
-      <c r="H22" s="3" t="s">
-        <v>102</v>
       </c>
       <c r="I22" s="4">
         <v>0</v>
@@ -1622,19 +1610,19 @@
       <c r="D23" s="21"/>
       <c r="E23" s="22"/>
       <c r="F23" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="G23" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="G23" s="3" t="s">
+      <c r="H23" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="I23" s="4">
+        <v>0</v>
+      </c>
+      <c r="J23" s="5" t="s">
         <v>101</v>
-      </c>
-      <c r="H23" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="I23" s="4">
-        <v>0</v>
-      </c>
-      <c r="J23" s="5" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="24" spans="2:10">
@@ -1643,13 +1631,13 @@
       <c r="D24" s="21"/>
       <c r="E24" s="22"/>
       <c r="F24" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="I24" s="4">
         <v>0</v>
@@ -1662,19 +1650,19 @@
       <c r="D25" s="21"/>
       <c r="E25" s="22"/>
       <c r="F25" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="I25" s="4">
         <v>0</v>
       </c>
       <c r="J25" s="5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="26" spans="2:10">
@@ -1683,19 +1671,19 @@
       <c r="D26" s="21"/>
       <c r="E26" s="22"/>
       <c r="F26" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="H26" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="I26" s="4">
         <v>0</v>
       </c>
       <c r="J26" s="5" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="27" spans="2:10">
@@ -1704,13 +1692,13 @@
       <c r="D27" s="21"/>
       <c r="E27" s="22"/>
       <c r="F27" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="H27" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="I27" s="4">
         <v>0</v>
@@ -1723,19 +1711,19 @@
       <c r="D28" s="21"/>
       <c r="E28" s="22"/>
       <c r="F28" s="3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="H28" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I28" s="4">
         <v>0</v>
       </c>
       <c r="J28" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="29" spans="2:10">
@@ -1744,38 +1732,38 @@
       <c r="D29" s="24"/>
       <c r="E29" s="25"/>
       <c r="F29" s="3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="H29" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I29" s="4">
         <v>0</v>
       </c>
       <c r="J29" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="30" spans="2:10">
       <c r="B30" s="26" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C30" s="27" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D30" s="27"/>
       <c r="E30" s="28"/>
       <c r="F30" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G30" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G30" s="3" t="s">
-        <v>13</v>
-      </c>
       <c r="H30" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I30" s="4">
         <v>0</v>
@@ -1788,19 +1776,19 @@
       <c r="D31" s="21"/>
       <c r="E31" s="22"/>
       <c r="F31" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G31" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="G31" s="3" t="s">
-        <v>16</v>
-      </c>
       <c r="H31" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I31" s="4">
         <v>0</v>
       </c>
       <c r="J31" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="32" spans="2:10">
@@ -1809,17 +1797,17 @@
       <c r="D32" s="21"/>
       <c r="E32" s="22"/>
       <c r="F32" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H32" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="I32" s="4"/>
       <c r="J32" s="5" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="33" spans="2:10">
@@ -1828,13 +1816,13 @@
       <c r="D33" s="21"/>
       <c r="E33" s="22"/>
       <c r="F33" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H33" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I33" s="4">
         <v>0</v>
@@ -1847,19 +1835,19 @@
       <c r="D34" s="21"/>
       <c r="E34" s="22"/>
       <c r="F34" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H34" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I34" s="4">
         <v>0</v>
       </c>
       <c r="J34" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="35" spans="2:10">
@@ -1868,17 +1856,17 @@
       <c r="D35" s="21"/>
       <c r="E35" s="22"/>
       <c r="F35" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H35" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="I35" s="4"/>
       <c r="J35" s="5" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="36" spans="2:10">
@@ -1887,13 +1875,13 @@
       <c r="D36" s="21"/>
       <c r="E36" s="22"/>
       <c r="F36" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="G36" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="G36" s="3" t="s">
-        <v>62</v>
-      </c>
       <c r="H36" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I36" s="4">
         <v>0</v>
@@ -1906,13 +1894,13 @@
       <c r="D37" s="24"/>
       <c r="E37" s="25"/>
       <c r="F37" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="G37" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="G37" s="3" t="s">
-        <v>63</v>
-      </c>
       <c r="H37" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I37" s="4">
         <v>0</v>
@@ -1921,21 +1909,21 @@
     </row>
     <row r="38" spans="2:10">
       <c r="B38" s="20" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C38" s="21" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D38" s="21"/>
       <c r="E38" s="22"/>
       <c r="F38" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="G38" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="H38" s="3" t="s">
         <v>108</v>
-      </c>
-      <c r="G38" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="H38" s="3" t="s">
-        <v>110</v>
       </c>
       <c r="I38" s="4">
         <v>0</v>
@@ -1948,13 +1936,13 @@
       <c r="D39" s="21"/>
       <c r="E39" s="22"/>
       <c r="F39" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="G39" s="3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="H39" s="3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="I39" s="4">
         <v>0</v>
@@ -1967,13 +1955,13 @@
       <c r="D40" s="21"/>
       <c r="E40" s="22"/>
       <c r="F40" s="3" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="G40" s="3" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="H40" s="3" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="I40" s="4">
         <v>0</v>
@@ -1986,13 +1974,13 @@
       <c r="D41" s="21"/>
       <c r="E41" s="22"/>
       <c r="F41" s="3" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="G41" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H41" s="3" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="I41" s="4">
         <v>0</v>
@@ -2001,23 +1989,23 @@
     </row>
     <row r="42" spans="2:10">
       <c r="B42" s="26" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C42" s="27" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D42" s="27" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E42" s="28"/>
       <c r="F42" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G42" s="3" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="H42" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I42" s="4">
         <v>0</v>
@@ -2030,16 +2018,16 @@
       <c r="D43" s="21"/>
       <c r="E43" s="22"/>
       <c r="F43" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="G43" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="H43" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="G43" s="3" t="s">
+      <c r="I43" s="4" t="s">
         <v>133</v>
-      </c>
-      <c r="H43" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="I43" s="4" t="s">
-        <v>135</v>
       </c>
       <c r="J43" s="5"/>
     </row>
@@ -2049,40 +2037,40 @@
       <c r="D44" s="24"/>
       <c r="E44" s="25"/>
       <c r="F44" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G44" s="3" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="H44" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I44" s="4" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="J44" s="5"/>
     </row>
     <row r="45" spans="2:10" ht="75">
       <c r="B45" s="26" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C45" s="27" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D45" s="27" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E45" s="29" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F45" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G45" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H45" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I45" s="4">
         <v>0</v>
@@ -2095,13 +2083,13 @@
       <c r="D46" s="24"/>
       <c r="E46" s="25"/>
       <c r="F46" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G46" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H46" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I46" s="4">
         <v>0</v>
@@ -2110,23 +2098,23 @@
     </row>
     <row r="47" spans="2:10" ht="37.5">
       <c r="B47" s="30" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D47" s="4"/>
       <c r="E47" s="31" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="F47" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="G47" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="H47" s="3" t="s">
         <v>123</v>
-      </c>
-      <c r="G47" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="H47" s="3" t="s">
-        <v>125</v>
       </c>
       <c r="I47" s="4">
         <v>0</v>
@@ -2135,23 +2123,23 @@
     </row>
     <row r="48" spans="2:10" ht="37.5">
       <c r="B48" s="30" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D48" s="4"/>
       <c r="E48" s="31" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="F48" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="G48" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="H48" s="3" t="s">
         <v>123</v>
-      </c>
-      <c r="G48" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="H48" s="3" t="s">
-        <v>125</v>
       </c>
       <c r="I48" s="4">
         <v>0</v>
@@ -2160,16 +2148,16 @@
     </row>
     <row r="49" spans="2:10" ht="19.5" thickBot="1">
       <c r="B49" s="6" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C49" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D49" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="D49" s="7" t="s">
+      <c r="E49" s="8" t="s">
         <v>45</v>
-      </c>
-      <c r="E49" s="8" t="s">
-        <v>46</v>
       </c>
       <c r="F49" s="8"/>
       <c r="G49" s="8"/>

</xml_diff>

<commit_message>
updated samples according to rggen/rggen#15
</commit_message>
<xml_diff>
--- a/block_0.xlsx
+++ b/block_0.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22130"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BADA353F-7578-4337-997E-6C33B6EA3AA3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E300817D-30C5-44AE-B3AF-7928CCFFD6BF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="141">
   <si>
     <t>block name</t>
     <phoneticPr fontId="1"/>
@@ -90,10 +90,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>8:1</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>bit_field_3</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -250,10 +246,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>register_3.bit_field_1</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>bit_field_6</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -330,10 +322,6 @@
   </si>
   <si>
     <t>rwl</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>bit_field_1</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -562,6 +550,42 @@
   </si>
   <si>
     <t>0, 1, 2, 3</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>bit_field_2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>8:1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>rw</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>9:2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>w1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>bit_field_1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>4:4</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>wo1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>register_3.bit_field_3</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -1187,7 +1211,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:J49"/>
+  <dimension ref="B1:J51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1291,37 +1315,37 @@
       <c r="J6" s="5"/>
     </row>
     <row r="7" spans="2:10">
-      <c r="B7" s="23"/>
-      <c r="C7" s="24"/>
-      <c r="D7" s="24"/>
-      <c r="E7" s="25"/>
+      <c r="B7" s="20"/>
+      <c r="C7" s="21"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="22"/>
       <c r="F7" s="3" t="s">
-        <v>16</v>
+        <v>132</v>
       </c>
       <c r="G7" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="I7" s="4">
+        <v>0</v>
+      </c>
+      <c r="J7" s="5"/>
+    </row>
+    <row r="8" spans="2:10">
+      <c r="B8" s="23"/>
+      <c r="C8" s="24"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="25"/>
+      <c r="F8" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H7" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="I7" s="4">
-        <v>0</v>
-      </c>
-      <c r="J7" s="5"/>
-    </row>
-    <row r="8" spans="2:10">
-      <c r="B8" s="26" t="s">
-        <v>46</v>
-      </c>
-      <c r="C8" s="27"/>
-      <c r="D8" s="27"/>
-      <c r="E8" s="28"/>
-      <c r="F8" s="3"/>
       <c r="G8" s="3" t="s">
-        <v>81</v>
+        <v>135</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>13</v>
+        <v>136</v>
       </c>
       <c r="I8" s="4">
         <v>0</v>
@@ -1330,38 +1354,40 @@
     </row>
     <row r="9" spans="2:10">
       <c r="B9" s="26" t="s">
-        <v>50</v>
-      </c>
-      <c r="C9" s="27" t="s">
-        <v>25</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="C9" s="27"/>
       <c r="D9" s="27"/>
       <c r="E9" s="28"/>
-      <c r="F9" s="3" t="s">
+      <c r="F9" s="3"/>
+      <c r="G9" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I9" s="4">
+        <v>0</v>
+      </c>
+      <c r="J9" s="5"/>
+    </row>
+    <row r="10" spans="2:10">
+      <c r="B10" s="26" t="s">
+        <v>49</v>
+      </c>
+      <c r="C10" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" s="27"/>
+      <c r="E10" s="28"/>
+      <c r="F10" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="G10" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="G9" s="3" t="s">
+      <c r="H10" s="3" t="s">
         <v>48</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="I9" s="4"/>
-      <c r="J9" s="5"/>
-    </row>
-    <row r="10" spans="2:10">
-      <c r="B10" s="20"/>
-      <c r="C10" s="21"/>
-      <c r="D10" s="21"/>
-      <c r="E10" s="22"/>
-      <c r="F10" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="H10" s="3" t="s">
-        <v>64</v>
       </c>
       <c r="I10" s="4"/>
       <c r="J10" s="5"/>
@@ -1372,74 +1398,74 @@
       <c r="D11" s="21"/>
       <c r="E11" s="22"/>
       <c r="F11" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="I11" s="4"/>
+      <c r="J11" s="5"/>
+    </row>
+    <row r="12" spans="2:10">
+      <c r="B12" s="20"/>
+      <c r="C12" s="21"/>
+      <c r="D12" s="21"/>
+      <c r="E12" s="22"/>
+      <c r="F12" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="H12" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="G11" s="3" t="s">
+      <c r="I12" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="H11" s="3" t="s">
+      <c r="J12" s="5"/>
+    </row>
+    <row r="13" spans="2:10">
+      <c r="B13" s="23"/>
+      <c r="C13" s="24"/>
+      <c r="D13" s="24"/>
+      <c r="E13" s="25"/>
+      <c r="F13" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="I11" s="4" t="s">
+      <c r="G13" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="J11" s="5"/>
-    </row>
-    <row r="12" spans="2:10">
-      <c r="B12" s="23"/>
-      <c r="C12" s="24"/>
-      <c r="D12" s="24"/>
-      <c r="E12" s="25"/>
-      <c r="F12" s="3" t="s">
+      <c r="H13" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="G12" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="H12" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="I12" s="4"/>
-      <c r="J12" s="5"/>
-    </row>
-    <row r="13" spans="2:10">
-      <c r="B13" s="26" t="s">
-        <v>28</v>
-      </c>
-      <c r="C13" s="27" t="s">
-        <v>25</v>
-      </c>
-      <c r="D13" s="27"/>
-      <c r="E13" s="28"/>
-      <c r="F13" s="3" t="s">
+      <c r="I13" s="4"/>
+      <c r="J13" s="5"/>
+    </row>
+    <row r="14" spans="2:10">
+      <c r="B14" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="D14" s="27"/>
+      <c r="E14" s="28"/>
+      <c r="F14" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="G14" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="G13" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="H13" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="I13" s="4">
-        <v>0</v>
-      </c>
-      <c r="J13" s="5"/>
-    </row>
-    <row r="14" spans="2:10">
-      <c r="B14" s="20"/>
-      <c r="C14" s="21"/>
-      <c r="D14" s="21"/>
-      <c r="E14" s="22"/>
-      <c r="F14" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="G14" s="3" t="s">
-        <v>21</v>
-      </c>
       <c r="H14" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="I14" s="4"/>
+        <v>50</v>
+      </c>
+      <c r="I14" s="4">
+        <v>0</v>
+      </c>
       <c r="J14" s="5"/>
     </row>
     <row r="15" spans="2:10">
@@ -1448,38 +1474,34 @@
       <c r="D15" s="21"/>
       <c r="E15" s="22"/>
       <c r="F15" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="I15" s="4">
+        <v>0</v>
+      </c>
+      <c r="J15" s="5"/>
+    </row>
+    <row r="16" spans="2:10">
+      <c r="B16" s="20"/>
+      <c r="C16" s="21"/>
+      <c r="D16" s="21"/>
+      <c r="E16" s="22"/>
+      <c r="F16" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="G15" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="H15" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="I15" s="4"/>
-      <c r="J15" s="5"/>
-    </row>
-    <row r="16" spans="2:10">
-      <c r="B16" s="26" t="s">
-        <v>36</v>
-      </c>
-      <c r="C16" s="27" t="s">
-        <v>29</v>
-      </c>
-      <c r="D16" s="27"/>
-      <c r="E16" s="28"/>
-      <c r="F16" s="3" t="s">
-        <v>11</v>
-      </c>
       <c r="G16" s="3" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="I16" s="4">
-        <v>0</v>
-      </c>
+        <v>76</v>
+      </c>
+      <c r="I16" s="4"/>
       <c r="J16" s="5"/>
     </row>
     <row r="17" spans="2:10">
@@ -1488,116 +1510,116 @@
       <c r="D17" s="21"/>
       <c r="E17" s="22"/>
       <c r="F17" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="I17" s="4"/>
+      <c r="J17" s="5"/>
+    </row>
+    <row r="18" spans="2:10">
+      <c r="B18" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="D18" s="27"/>
+      <c r="E18" s="28"/>
+      <c r="F18" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I18" s="4">
+        <v>0</v>
+      </c>
+      <c r="J18" s="5"/>
+    </row>
+    <row r="19" spans="2:10">
+      <c r="B19" s="20"/>
+      <c r="C19" s="21"/>
+      <c r="D19" s="21"/>
+      <c r="E19" s="22"/>
+      <c r="F19" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G17" s="3" t="s">
+      <c r="G19" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H19" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="H17" s="3" t="s">
+      <c r="I19" s="4">
+        <v>0</v>
+      </c>
+      <c r="J19" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="2:10">
+      <c r="B20" s="20"/>
+      <c r="C20" s="21"/>
+      <c r="D20" s="21"/>
+      <c r="E20" s="22"/>
+      <c r="F20" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="I20" s="4"/>
+      <c r="J20" s="5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="21" spans="2:10">
+      <c r="B21" s="23"/>
+      <c r="C21" s="24"/>
+      <c r="D21" s="24"/>
+      <c r="E21" s="25"/>
+      <c r="F21" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H21" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="I17" s="4">
-        <v>0</v>
-      </c>
-      <c r="J17" s="5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="18" spans="2:10">
-      <c r="B18" s="20"/>
-      <c r="C18" s="21"/>
-      <c r="D18" s="21"/>
-      <c r="E18" s="22"/>
-      <c r="F18" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G18" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="H18" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="I18" s="4"/>
-      <c r="J18" s="5" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="19" spans="2:10">
-      <c r="B19" s="23"/>
-      <c r="C19" s="24"/>
-      <c r="D19" s="24"/>
-      <c r="E19" s="25"/>
-      <c r="F19" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="G19" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="H19" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="I19" s="4">
-        <v>0</v>
-      </c>
-      <c r="J19" s="5"/>
-    </row>
-    <row r="20" spans="2:10">
-      <c r="B20" s="26" t="s">
-        <v>41</v>
-      </c>
-      <c r="C20" s="27" t="s">
-        <v>37</v>
-      </c>
-      <c r="D20" s="27"/>
-      <c r="E20" s="28"/>
-      <c r="F20" s="3" t="s">
+      <c r="I21" s="4">
+        <v>0</v>
+      </c>
+      <c r="J21" s="5"/>
+    </row>
+    <row r="22" spans="2:10">
+      <c r="B22" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="C22" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="D22" s="27"/>
+      <c r="E22" s="28"/>
+      <c r="F22" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="G20" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="H20" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="I20" s="4">
-        <v>0</v>
-      </c>
-      <c r="J20" s="5"/>
-    </row>
-    <row r="21" spans="2:10">
-      <c r="B21" s="20"/>
-      <c r="C21" s="21"/>
-      <c r="D21" s="21"/>
-      <c r="E21" s="22"/>
-      <c r="F21" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="G21" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="H21" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="I21" s="4">
-        <v>0</v>
-      </c>
-      <c r="J21" s="5" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="22" spans="2:10">
-      <c r="B22" s="20"/>
-      <c r="C22" s="21"/>
-      <c r="D22" s="21"/>
-      <c r="E22" s="22"/>
-      <c r="F22" s="3" t="s">
-        <v>96</v>
-      </c>
       <c r="G22" s="3" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="I22" s="4">
         <v>0</v>
@@ -1610,19 +1632,19 @@
       <c r="D23" s="21"/>
       <c r="E23" s="22"/>
       <c r="F23" s="3" t="s">
-        <v>97</v>
+        <v>71</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>100</v>
+        <v>72</v>
       </c>
       <c r="I23" s="4">
         <v>0</v>
       </c>
       <c r="J23" s="5" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="24" spans="2:10">
@@ -1631,13 +1653,13 @@
       <c r="D24" s="21"/>
       <c r="E24" s="22"/>
       <c r="F24" s="3" t="s">
-        <v>20</v>
+        <v>93</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>83</v>
+        <v>95</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>76</v>
+        <v>97</v>
       </c>
       <c r="I24" s="4">
         <v>0</v>
@@ -1650,19 +1672,19 @@
       <c r="D25" s="21"/>
       <c r="E25" s="22"/>
       <c r="F25" s="3" t="s">
-        <v>34</v>
+        <v>94</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>84</v>
+        <v>96</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>76</v>
+        <v>97</v>
       </c>
       <c r="I25" s="4">
         <v>0</v>
       </c>
       <c r="J25" s="5" t="s">
-        <v>75</v>
+        <v>140</v>
       </c>
     </row>
     <row r="26" spans="2:10">
@@ -1671,20 +1693,18 @@
       <c r="D26" s="21"/>
       <c r="E26" s="22"/>
       <c r="F26" s="3" t="s">
-        <v>58</v>
+        <v>19</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="H26" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="I26" s="4">
         <v>0</v>
       </c>
-      <c r="J26" s="5" t="s">
-        <v>86</v>
-      </c>
+      <c r="J26" s="5"/>
     </row>
     <row r="27" spans="2:10">
       <c r="B27" s="20"/>
@@ -1692,18 +1712,20 @@
       <c r="D27" s="21"/>
       <c r="E27" s="22"/>
       <c r="F27" s="3" t="s">
-        <v>59</v>
+        <v>33</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="H27" s="3" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="I27" s="4">
         <v>0</v>
       </c>
-      <c r="J27" s="5"/>
+      <c r="J27" s="5" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="28" spans="2:10">
       <c r="B28" s="20"/>
@@ -1711,104 +1733,104 @@
       <c r="D28" s="21"/>
       <c r="E28" s="22"/>
       <c r="F28" s="3" t="s">
-        <v>102</v>
+        <v>56</v>
       </c>
       <c r="G28" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="H28" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="I28" s="4">
+        <v>0</v>
+      </c>
+      <c r="J28" s="5" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="29" spans="2:10">
+      <c r="B29" s="20"/>
+      <c r="C29" s="21"/>
+      <c r="D29" s="21"/>
+      <c r="E29" s="22"/>
+      <c r="F29" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="G29" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="H29" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="I29" s="4">
+        <v>0</v>
+      </c>
+      <c r="J29" s="5"/>
+    </row>
+    <row r="30" spans="2:10">
+      <c r="B30" s="20"/>
+      <c r="C30" s="21"/>
+      <c r="D30" s="21"/>
+      <c r="E30" s="22"/>
+      <c r="F30" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="G30" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="H30" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="I30" s="4">
+        <v>0</v>
+      </c>
+      <c r="J30" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="31" spans="2:10">
+      <c r="B31" s="23"/>
+      <c r="C31" s="24"/>
+      <c r="D31" s="24"/>
+      <c r="E31" s="25"/>
+      <c r="F31" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="G31" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="H31" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="I31" s="4">
+        <v>0</v>
+      </c>
+      <c r="J31" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="32" spans="2:10">
+      <c r="B32" s="26" t="s">
+        <v>54</v>
+      </c>
+      <c r="C32" s="27" t="s">
         <v>88</v>
       </c>
-      <c r="H28" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="I28" s="4">
-        <v>0</v>
-      </c>
-      <c r="J28" s="5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="29" spans="2:10">
-      <c r="B29" s="23"/>
-      <c r="C29" s="24"/>
-      <c r="D29" s="24"/>
-      <c r="E29" s="25"/>
-      <c r="F29" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="G29" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="H29" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="I29" s="4">
-        <v>0</v>
-      </c>
-      <c r="J29" s="5" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="30" spans="2:10">
-      <c r="B30" s="26" t="s">
-        <v>55</v>
-      </c>
-      <c r="C30" s="27" t="s">
-        <v>91</v>
-      </c>
-      <c r="D30" s="27"/>
-      <c r="E30" s="28"/>
-      <c r="F30" s="3" t="s">
+      <c r="D32" s="27"/>
+      <c r="E32" s="28"/>
+      <c r="F32" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="G30" s="3" t="s">
+      <c r="G32" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="H30" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="I30" s="4">
-        <v>0</v>
-      </c>
-      <c r="J30" s="5"/>
-    </row>
-    <row r="31" spans="2:10">
-      <c r="B31" s="20"/>
-      <c r="C31" s="21"/>
-      <c r="D31" s="21"/>
-      <c r="E31" s="22"/>
-      <c r="F31" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G31" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="H31" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="I31" s="4">
-        <v>0</v>
-      </c>
-      <c r="J31" s="5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="32" spans="2:10">
-      <c r="B32" s="20"/>
-      <c r="C32" s="21"/>
-      <c r="D32" s="21"/>
-      <c r="E32" s="22"/>
-      <c r="F32" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G32" s="3" t="s">
-        <v>21</v>
-      </c>
       <c r="H32" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="I32" s="4"/>
-      <c r="J32" s="5" t="s">
-        <v>90</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="I32" s="4">
+        <v>0</v>
+      </c>
+      <c r="J32" s="5"/>
     </row>
     <row r="33" spans="2:10">
       <c r="B33" s="20"/>
@@ -1816,18 +1838,20 @@
       <c r="D33" s="21"/>
       <c r="E33" s="22"/>
       <c r="F33" s="3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="H33" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="I33" s="4">
         <v>0</v>
       </c>
-      <c r="J33" s="5"/>
+      <c r="J33" s="5" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="34" spans="2:10">
       <c r="B34" s="20"/>
@@ -1835,19 +1859,17 @@
       <c r="D34" s="21"/>
       <c r="E34" s="22"/>
       <c r="F34" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G34" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="G34" s="3" t="s">
-        <v>19</v>
-      </c>
       <c r="H34" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="I34" s="4">
-        <v>0</v>
-      </c>
+        <v>48</v>
+      </c>
+      <c r="I34" s="4"/>
       <c r="J34" s="5" t="s">
-        <v>24</v>
+        <v>87</v>
       </c>
     </row>
     <row r="35" spans="2:10">
@@ -1856,18 +1878,18 @@
       <c r="D35" s="21"/>
       <c r="E35" s="22"/>
       <c r="F35" s="3" t="s">
-        <v>34</v>
+        <v>17</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>56</v>
+        <v>31</v>
       </c>
       <c r="H35" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="I35" s="4"/>
-      <c r="J35" s="5" t="s">
-        <v>93</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="I35" s="4">
+        <v>0</v>
+      </c>
+      <c r="J35" s="5"/>
     </row>
     <row r="36" spans="2:10">
       <c r="B36" s="20"/>
@@ -1875,55 +1897,53 @@
       <c r="D36" s="21"/>
       <c r="E36" s="22"/>
       <c r="F36" s="3" t="s">
-        <v>58</v>
+        <v>19</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>60</v>
+        <v>18</v>
       </c>
       <c r="H36" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="I36" s="4">
+        <v>0</v>
+      </c>
+      <c r="J36" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="37" spans="2:10">
+      <c r="B37" s="20"/>
+      <c r="C37" s="21"/>
+      <c r="D37" s="21"/>
+      <c r="E37" s="22"/>
+      <c r="F37" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="I36" s="4">
-        <v>0</v>
-      </c>
-      <c r="J36" s="5"/>
-    </row>
-    <row r="37" spans="2:10">
-      <c r="B37" s="23"/>
-      <c r="C37" s="24"/>
-      <c r="D37" s="24"/>
-      <c r="E37" s="25"/>
-      <c r="F37" s="3" t="s">
-        <v>59</v>
-      </c>
       <c r="G37" s="3" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="H37" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="I37" s="4">
-        <v>0</v>
-      </c>
-      <c r="J37" s="5"/>
+        <v>48</v>
+      </c>
+      <c r="I37" s="4"/>
+      <c r="J37" s="5" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="38" spans="2:10">
-      <c r="B38" s="20" t="s">
-        <v>104</v>
-      </c>
-      <c r="C38" s="21" t="s">
-        <v>105</v>
-      </c>
+      <c r="B38" s="20"/>
+      <c r="C38" s="21"/>
       <c r="D38" s="21"/>
       <c r="E38" s="22"/>
       <c r="F38" s="3" t="s">
-        <v>106</v>
+        <v>56</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>107</v>
+        <v>58</v>
       </c>
       <c r="H38" s="3" t="s">
-        <v>108</v>
+        <v>32</v>
       </c>
       <c r="I38" s="4">
         <v>0</v>
@@ -1931,18 +1951,18 @@
       <c r="J38" s="5"/>
     </row>
     <row r="39" spans="2:10">
-      <c r="B39" s="20"/>
-      <c r="C39" s="21"/>
-      <c r="D39" s="21"/>
-      <c r="E39" s="22"/>
+      <c r="B39" s="23"/>
+      <c r="C39" s="24"/>
+      <c r="D39" s="24"/>
+      <c r="E39" s="25"/>
       <c r="F39" s="3" t="s">
-        <v>109</v>
+        <v>57</v>
       </c>
       <c r="G39" s="3" t="s">
-        <v>112</v>
+        <v>59</v>
       </c>
       <c r="H39" s="3" t="s">
-        <v>115</v>
+        <v>34</v>
       </c>
       <c r="I39" s="4">
         <v>0</v>
@@ -1950,18 +1970,22 @@
       <c r="J39" s="5"/>
     </row>
     <row r="40" spans="2:10">
-      <c r="B40" s="20"/>
-      <c r="C40" s="21"/>
+      <c r="B40" s="20" t="s">
+        <v>101</v>
+      </c>
+      <c r="C40" s="21" t="s">
+        <v>102</v>
+      </c>
       <c r="D40" s="21"/>
       <c r="E40" s="22"/>
       <c r="F40" s="3" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="G40" s="3" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="H40" s="3" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
       <c r="I40" s="4">
         <v>0</v>
@@ -1974,13 +1998,13 @@
       <c r="D41" s="21"/>
       <c r="E41" s="22"/>
       <c r="F41" s="3" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="G41" s="3" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="H41" s="3" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="I41" s="4">
         <v>0</v>
@@ -1988,24 +2012,18 @@
       <c r="J41" s="5"/>
     </row>
     <row r="42" spans="2:10">
-      <c r="B42" s="26" t="s">
-        <v>54</v>
-      </c>
-      <c r="C42" s="27" t="s">
-        <v>52</v>
-      </c>
-      <c r="D42" s="27" t="s">
-        <v>38</v>
-      </c>
-      <c r="E42" s="28"/>
+      <c r="B42" s="20"/>
+      <c r="C42" s="21"/>
+      <c r="D42" s="21"/>
+      <c r="E42" s="22"/>
       <c r="F42" s="3" t="s">
-        <v>11</v>
+        <v>107</v>
       </c>
       <c r="G42" s="3" t="s">
-        <v>128</v>
+        <v>110</v>
       </c>
       <c r="H42" s="3" t="s">
-        <v>13</v>
+        <v>113</v>
       </c>
       <c r="I42" s="4">
         <v>0</v>
@@ -2018,62 +2036,60 @@
       <c r="D43" s="21"/>
       <c r="E43" s="22"/>
       <c r="F43" s="3" t="s">
-        <v>130</v>
+        <v>108</v>
       </c>
       <c r="G43" s="3" t="s">
-        <v>131</v>
+        <v>111</v>
       </c>
       <c r="H43" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="I43" s="4" t="s">
-        <v>133</v>
+        <v>114</v>
+      </c>
+      <c r="I43" s="4">
+        <v>0</v>
       </c>
       <c r="J43" s="5"/>
     </row>
     <row r="44" spans="2:10">
-      <c r="B44" s="23"/>
-      <c r="C44" s="24"/>
-      <c r="D44" s="24"/>
-      <c r="E44" s="25"/>
+      <c r="B44" s="26" t="s">
+        <v>53</v>
+      </c>
+      <c r="C44" s="27" t="s">
+        <v>51</v>
+      </c>
+      <c r="D44" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="E44" s="28"/>
       <c r="F44" s="3" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="G44" s="3" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="H44" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="I44" s="4" t="s">
-        <v>134</v>
+      <c r="I44" s="4">
+        <v>0</v>
       </c>
       <c r="J44" s="5"/>
     </row>
-    <row r="45" spans="2:10" ht="75">
-      <c r="B45" s="26" t="s">
-        <v>92</v>
-      </c>
-      <c r="C45" s="27" t="s">
-        <v>53</v>
-      </c>
-      <c r="D45" s="27" t="s">
-        <v>42</v>
-      </c>
-      <c r="E45" s="29" t="s">
-        <v>125</v>
-      </c>
+    <row r="45" spans="2:10">
+      <c r="B45" s="20"/>
+      <c r="C45" s="21"/>
+      <c r="D45" s="21"/>
+      <c r="E45" s="22"/>
       <c r="F45" s="3" t="s">
-        <v>11</v>
+        <v>127</v>
       </c>
       <c r="G45" s="3" t="s">
-        <v>39</v>
+        <v>128</v>
       </c>
       <c r="H45" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="I45" s="4">
-        <v>0</v>
+        <v>129</v>
+      </c>
+      <c r="I45" s="4" t="s">
+        <v>130</v>
       </c>
       <c r="J45" s="5"/>
     </row>
@@ -2083,87 +2099,133 @@
       <c r="D46" s="24"/>
       <c r="E46" s="25"/>
       <c r="F46" s="3" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="G46" s="3" t="s">
-        <v>40</v>
+        <v>126</v>
       </c>
       <c r="H46" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="I46" s="4">
-        <v>0</v>
+      <c r="I46" s="4" t="s">
+        <v>131</v>
       </c>
       <c r="J46" s="5"/>
     </row>
-    <row r="47" spans="2:10" ht="37.5">
-      <c r="B47" s="30" t="s">
+    <row r="47" spans="2:10" ht="75">
+      <c r="B47" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="C47" s="27" t="s">
+        <v>52</v>
+      </c>
+      <c r="D47" s="27" t="s">
+        <v>41</v>
+      </c>
+      <c r="E47" s="29" t="s">
+        <v>122</v>
+      </c>
+      <c r="F47" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G47" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H47" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I47" s="4">
+        <v>0</v>
+      </c>
+      <c r="J47" s="5"/>
+    </row>
+    <row r="48" spans="2:10">
+      <c r="B48" s="23"/>
+      <c r="C48" s="24"/>
+      <c r="D48" s="24"/>
+      <c r="E48" s="25"/>
+      <c r="F48" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G48" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="H48" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I48" s="4">
+        <v>0</v>
+      </c>
+      <c r="J48" s="5"/>
+    </row>
+    <row r="49" spans="2:10" ht="37.5">
+      <c r="B49" s="30" t="s">
+        <v>116</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="D49" s="4"/>
+      <c r="E49" s="31" t="s">
+        <v>123</v>
+      </c>
+      <c r="F49" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="G49" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="C47" s="4" t="s">
+      <c r="H49" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="D47" s="4"/>
-      <c r="E47" s="31" t="s">
-        <v>126</v>
-      </c>
-      <c r="F47" s="3" t="s">
+      <c r="I49" s="4">
+        <v>0</v>
+      </c>
+      <c r="J49" s="5"/>
+    </row>
+    <row r="50" spans="2:10" ht="37.5">
+      <c r="B50" s="30" t="s">
         <v>121</v>
       </c>
-      <c r="G47" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="H47" s="3" t="s">
+      <c r="C50" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="D50" s="4"/>
+      <c r="E50" s="31" t="s">
         <v>123</v>
       </c>
-      <c r="I47" s="4">
-        <v>0</v>
-      </c>
-      <c r="J47" s="5"/>
-    </row>
-    <row r="48" spans="2:10" ht="37.5">
-      <c r="B48" s="30" t="s">
-        <v>124</v>
-      </c>
-      <c r="C48" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="D48" s="4"/>
-      <c r="E48" s="31" t="s">
-        <v>126</v>
-      </c>
-      <c r="F48" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="G48" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="H48" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="I48" s="4">
-        <v>0</v>
-      </c>
-      <c r="J48" s="5"/>
-    </row>
-    <row r="49" spans="2:10" ht="19.5" thickBot="1">
-      <c r="B49" s="6" t="s">
+      <c r="F50" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="C49" s="7" t="s">
+      <c r="G50" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="H50" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="I50" s="4">
+        <v>0</v>
+      </c>
+      <c r="J50" s="5"/>
+    </row>
+    <row r="51" spans="2:10" ht="19.5" thickBot="1">
+      <c r="B51" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="C51" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D51" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="D49" s="7" t="s">
+      <c r="E51" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="E49" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="F49" s="8"/>
-      <c r="G49" s="8"/>
-      <c r="H49" s="8"/>
-      <c r="I49" s="7"/>
-      <c r="J49" s="9"/>
+      <c r="F51" s="8"/>
+      <c r="G51" s="8"/>
+      <c r="H51" s="8"/>
+      <c r="I51" s="7"/>
+      <c r="J51" s="9"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>

</xml_diff>

<commit_message>
added w0t and w1t bit field types (refs: rggen/rggen#42)
</commit_message>
<xml_diff>
--- a/block_0.xlsx
+++ b/block_0.xlsx
@@ -1,26 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23211"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E300817D-30C5-44AE-B3AF-7928CCFFD6BF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{DA7EB6AA-2B73-41EE-A500-8BA87648E7CD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="block_0" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191028" calcCompleted="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="119">
   <si>
     <t>block name</t>
     <phoneticPr fontId="1"/>
@@ -90,39 +98,194 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
+    <t>8:1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
     <t>bit_field_3</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
+    <t>9:2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>w1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>register_1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>0:1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>register_2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>0x08</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ro</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>8:4</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>16:8</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>rof</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>0xab</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>24:8</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>reserved</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>register_3</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>wo</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>wo1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>w0trg</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
     <t>16:4</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
+    <t>w1trg</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>register_4</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>0x0C</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>rc</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>register_0.bit_field_0</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>12:4</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>register_4.bit_field_1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>rs</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>register_5</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>0x10</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>0:2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>rwc</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>2:2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>register_3.bit_field_2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>4:2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>rws</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>6:2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>register_3.bit_field_3</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
     <t>bit_field_4</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>8:4</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>rc</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>rs</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>register_0.bit_field_0</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>0x08</t>
+    <t>8:2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>rwe</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>bit_field_5</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>10:2</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
     <t>register_0.bit_field_2</t>
+  </si>
+  <si>
+    <t>bit_field_6</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>12:2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>bit_field_7</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>16:2</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -130,11 +293,31 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>register_3</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>0x0C</t>
+    <t>bit_field_8</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>18:2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>register_0.bit_field_2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>bit_field_9</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>20:2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>register_6</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>0x14</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -142,31 +325,90 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
+    <t>register_6.bit_field_1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
     <t>w1c</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>12:4</t>
-    <phoneticPr fontId="1"/>
+    <t>20:4</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>register_6.bit_field_4</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>bit_field_6</t>
+  </si>
+  <si>
+    <t>24:4</t>
   </si>
   <si>
     <t>w0s</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>bit_field_5</t>
-    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>bit_field_7</t>
+  </si>
+  <si>
+    <t>28:4</t>
   </si>
   <si>
     <t>w1s</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>register_4</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>0x10</t>
+  </si>
+  <si>
+    <t>bit_field_8</t>
+  </si>
+  <si>
+    <t>32:4</t>
+  </si>
+  <si>
+    <t>w0t</t>
+  </si>
+  <si>
+    <t>bit_field_9</t>
+  </si>
+  <si>
+    <t>36:4</t>
+  </si>
+  <si>
+    <t>w1t</t>
+  </si>
+  <si>
+    <t>register_7</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>0x1C</t>
+  </si>
+  <si>
+    <t>w0crs</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>w1crs</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>w0src</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>24:4</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>w1src</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>register_8</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>0x20</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -174,338 +416,35 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>0:8:4:16</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>8:8:4:16</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>register_5</t>
+    <t>0:4:4:16</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>4:4:4:16</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>default: 0</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>8:4:4:16</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>0, 1, 2, 3</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>register_9</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>0x40</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
     <t>[2, 4]</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>0x80</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>[32]</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>external</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>register_1</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>bit_field_0</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>0:4</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>ro</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>register_2</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>wo</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>0x20</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>0x40</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>register_8</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>register_6</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>20:4</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>bit_field_6</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>bit_field_7</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>24:4</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>28:4</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>bit_field_1</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>8:4</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>ro</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>bit_field_2</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>16:8</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>rof</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>0xab</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>bit_field_3</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>24:8</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>reserved</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>rwc</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>bit_field_1</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>rwc</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>register_0.bit_field_2</t>
-  </si>
-  <si>
-    <t>rwe</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>rwl</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>w0trg</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>w1trg</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>0:1</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>register_4.bit_field_1</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>8:2</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>10:2</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>12:2</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>register_1</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>16:2</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>18:2</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>20:2</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>register_6.bit_field_1</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>0x14</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>register_9</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>register_6.bit_field_4</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>0:2</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>2:2</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>bit_field_2</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>bit_field_3</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>4:2</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>6:2</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>rws</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>register_3.bit_field_2</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>bit_field_8</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>bit_field_9</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>register_7</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>0x18</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>bit_field_0</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>0:4</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>w0crs</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>bit_field_1</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>bit_field_2</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>bit_field_3</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>8:4</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>16:4</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>24:4</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>w1crs</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>w0src</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>w1src</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>register_12</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>register_10</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>0x40</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>bit_field_0</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>0:1</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>rw</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>register_11</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -516,76 +455,44 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
+    <t>0:8:4:16</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>8:8:4:16</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>register_10</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
     <t>indirect:
 register_0.bit_field_2:1</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
+    <t>register_11</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
     <t>0x44</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>0:4:4:16</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>8:4:4:16</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>bit_field_1</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>4:4:4:16</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>rw</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>default: 0</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>0, 1, 2, 3</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>bit_field_2</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>8:1</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>rw</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>9:2</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>w1</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>bit_field_1</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>4:4</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>wo1</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>register_3.bit_field_3</t>
+    <t>register_12</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>0x80</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[32]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>external</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -1211,9 +1118,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:J51"/>
+  <dimension ref="B1:J53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="H42" sqref="H42"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
   <cols>
@@ -1320,13 +1229,13 @@
       <c r="D7" s="21"/>
       <c r="E7" s="22"/>
       <c r="F7" s="3" t="s">
-        <v>132</v>
+        <v>16</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>133</v>
+        <v>17</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>134</v>
+        <v>13</v>
       </c>
       <c r="I7" s="4">
         <v>0</v>
@@ -1339,13 +1248,13 @@
       <c r="D8" s="24"/>
       <c r="E8" s="25"/>
       <c r="F8" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>135</v>
+        <v>19</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>136</v>
+        <v>20</v>
       </c>
       <c r="I8" s="4">
         <v>0</v>
@@ -1354,14 +1263,14 @@
     </row>
     <row r="9" spans="2:10">
       <c r="B9" s="26" t="s">
-        <v>45</v>
+        <v>21</v>
       </c>
       <c r="C9" s="27"/>
       <c r="D9" s="27"/>
       <c r="E9" s="28"/>
       <c r="F9" s="3"/>
       <c r="G9" s="3" t="s">
-        <v>78</v>
+        <v>22</v>
       </c>
       <c r="H9" s="3" t="s">
         <v>13</v>
@@ -1373,7 +1282,7 @@
     </row>
     <row r="10" spans="2:10">
       <c r="B10" s="26" t="s">
-        <v>49</v>
+        <v>23</v>
       </c>
       <c r="C10" s="27" t="s">
         <v>24</v>
@@ -1381,13 +1290,13 @@
       <c r="D10" s="27"/>
       <c r="E10" s="28"/>
       <c r="F10" s="3" t="s">
-        <v>46</v>
+        <v>11</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>47</v>
+        <v>12</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>48</v>
+        <v>25</v>
       </c>
       <c r="I10" s="4"/>
       <c r="J10" s="5"/>
@@ -1398,13 +1307,13 @@
       <c r="D11" s="21"/>
       <c r="E11" s="22"/>
       <c r="F11" s="3" t="s">
-        <v>60</v>
+        <v>14</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>61</v>
+        <v>26</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>62</v>
+        <v>25</v>
       </c>
       <c r="I11" s="4"/>
       <c r="J11" s="5"/>
@@ -1415,16 +1324,16 @@
       <c r="D12" s="21"/>
       <c r="E12" s="22"/>
       <c r="F12" s="3" t="s">
-        <v>63</v>
+        <v>16</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>64</v>
+        <v>27</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>65</v>
+        <v>28</v>
       </c>
       <c r="I12" s="4" t="s">
-        <v>66</v>
+        <v>29</v>
       </c>
       <c r="J12" s="5"/>
     </row>
@@ -1434,20 +1343,20 @@
       <c r="D13" s="24"/>
       <c r="E13" s="25"/>
       <c r="F13" s="3" t="s">
-        <v>67</v>
+        <v>18</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>68</v>
+        <v>30</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>69</v>
+        <v>31</v>
       </c>
       <c r="I13" s="4"/>
       <c r="J13" s="5"/>
     </row>
     <row r="14" spans="2:10">
       <c r="B14" s="26" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="C14" s="27" t="s">
         <v>24</v>
@@ -1455,13 +1364,13 @@
       <c r="D14" s="27"/>
       <c r="E14" s="28"/>
       <c r="F14" s="3" t="s">
-        <v>46</v>
+        <v>11</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>47</v>
+        <v>12</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="I14" s="4">
         <v>0</v>
@@ -1474,13 +1383,13 @@
       <c r="D15" s="21"/>
       <c r="E15" s="22"/>
       <c r="F15" s="3" t="s">
-        <v>137</v>
+        <v>14</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>138</v>
+        <v>15</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>139</v>
+        <v>34</v>
       </c>
       <c r="I15" s="4">
         <v>0</v>
@@ -1496,10 +1405,10 @@
         <v>16</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>76</v>
+        <v>35</v>
       </c>
       <c r="I16" s="4"/>
       <c r="J16" s="5"/>
@@ -1510,23 +1419,23 @@
       <c r="D17" s="21"/>
       <c r="E17" s="22"/>
       <c r="F17" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>77</v>
+        <v>37</v>
       </c>
       <c r="I17" s="4"/>
       <c r="J17" s="5"/>
     </row>
     <row r="18" spans="2:10">
       <c r="B18" s="26" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C18" s="27" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="D18" s="27"/>
       <c r="E18" s="28"/>
@@ -1537,7 +1446,7 @@
         <v>12</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>21</v>
+        <v>40</v>
       </c>
       <c r="I18" s="4">
         <v>0</v>
@@ -1553,16 +1462,16 @@
         <v>14</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>21</v>
+        <v>40</v>
       </c>
       <c r="I19" s="4">
         <v>0</v>
       </c>
       <c r="J19" s="5" t="s">
-        <v>23</v>
+        <v>41</v>
       </c>
     </row>
     <row r="20" spans="2:10">
@@ -1574,14 +1483,14 @@
         <v>16</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>48</v>
+        <v>25</v>
       </c>
       <c r="I20" s="4"/>
       <c r="J20" s="5" t="s">
-        <v>79</v>
+        <v>43</v>
       </c>
     </row>
     <row r="21" spans="2:10">
@@ -1590,13 +1499,13 @@
       <c r="D21" s="24"/>
       <c r="E21" s="25"/>
       <c r="F21" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>22</v>
+        <v>44</v>
       </c>
       <c r="I21" s="4">
         <v>0</v>
@@ -1605,10 +1514,10 @@
     </row>
     <row r="22" spans="2:10">
       <c r="B22" s="26" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="C22" s="27" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="D22" s="27"/>
       <c r="E22" s="28"/>
@@ -1616,10 +1525,10 @@
         <v>11</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>91</v>
+        <v>47</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>70</v>
+        <v>48</v>
       </c>
       <c r="I22" s="4">
         <v>0</v>
@@ -1632,19 +1541,19 @@
       <c r="D23" s="21"/>
       <c r="E23" s="22"/>
       <c r="F23" s="3" t="s">
-        <v>71</v>
+        <v>14</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>92</v>
+        <v>49</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>72</v>
+        <v>48</v>
       </c>
       <c r="I23" s="4">
         <v>0</v>
       </c>
       <c r="J23" s="5" t="s">
-        <v>98</v>
+        <v>50</v>
       </c>
     </row>
     <row r="24" spans="2:10">
@@ -1653,13 +1562,13 @@
       <c r="D24" s="21"/>
       <c r="E24" s="22"/>
       <c r="F24" s="3" t="s">
-        <v>93</v>
+        <v>16</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>95</v>
+        <v>51</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>97</v>
+        <v>52</v>
       </c>
       <c r="I24" s="4">
         <v>0</v>
@@ -1672,19 +1581,19 @@
       <c r="D25" s="21"/>
       <c r="E25" s="22"/>
       <c r="F25" s="3" t="s">
-        <v>94</v>
+        <v>18</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>96</v>
+        <v>53</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>97</v>
+        <v>52</v>
       </c>
       <c r="I25" s="4">
         <v>0</v>
       </c>
       <c r="J25" s="5" t="s">
-        <v>140</v>
+        <v>54</v>
       </c>
     </row>
     <row r="26" spans="2:10">
@@ -1693,13 +1602,13 @@
       <c r="D26" s="21"/>
       <c r="E26" s="22"/>
       <c r="F26" s="3" t="s">
-        <v>19</v>
+        <v>55</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>80</v>
+        <v>56</v>
       </c>
       <c r="H26" s="3" t="s">
-        <v>74</v>
+        <v>57</v>
       </c>
       <c r="I26" s="4">
         <v>0</v>
@@ -1712,19 +1621,19 @@
       <c r="D27" s="21"/>
       <c r="E27" s="22"/>
       <c r="F27" s="3" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>81</v>
+        <v>59</v>
       </c>
       <c r="H27" s="3" t="s">
-        <v>74</v>
+        <v>57</v>
       </c>
       <c r="I27" s="4">
         <v>0</v>
       </c>
       <c r="J27" s="5" t="s">
-        <v>73</v>
+        <v>60</v>
       </c>
     </row>
     <row r="28" spans="2:10">
@@ -1733,19 +1642,19 @@
       <c r="D28" s="21"/>
       <c r="E28" s="22"/>
       <c r="F28" s="3" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>82</v>
+        <v>62</v>
       </c>
       <c r="H28" s="3" t="s">
-        <v>74</v>
+        <v>57</v>
       </c>
       <c r="I28" s="4">
         <v>0</v>
       </c>
       <c r="J28" s="5" t="s">
-        <v>83</v>
+        <v>21</v>
       </c>
     </row>
     <row r="29" spans="2:10">
@@ -1754,13 +1663,13 @@
       <c r="D29" s="21"/>
       <c r="E29" s="22"/>
       <c r="F29" s="3" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>84</v>
+        <v>64</v>
       </c>
       <c r="H29" s="3" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="I29" s="4">
         <v>0</v>
@@ -1773,19 +1682,19 @@
       <c r="D30" s="21"/>
       <c r="E30" s="22"/>
       <c r="F30" s="3" t="s">
-        <v>99</v>
+        <v>66</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>85</v>
+        <v>67</v>
       </c>
       <c r="H30" s="3" t="s">
-        <v>26</v>
+        <v>65</v>
       </c>
       <c r="I30" s="4">
         <v>0</v>
       </c>
       <c r="J30" s="5" t="s">
-        <v>25</v>
+        <v>68</v>
       </c>
     </row>
     <row r="31" spans="2:10">
@@ -1794,27 +1703,27 @@
       <c r="D31" s="24"/>
       <c r="E31" s="25"/>
       <c r="F31" s="3" t="s">
-        <v>100</v>
+        <v>69</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>86</v>
+        <v>70</v>
       </c>
       <c r="H31" s="3" t="s">
-        <v>26</v>
+        <v>65</v>
       </c>
       <c r="I31" s="4">
         <v>0</v>
       </c>
       <c r="J31" s="5" t="s">
-        <v>45</v>
+        <v>21</v>
       </c>
     </row>
     <row r="32" spans="2:10">
       <c r="B32" s="26" t="s">
-        <v>54</v>
+        <v>71</v>
       </c>
       <c r="C32" s="27" t="s">
-        <v>88</v>
+        <v>72</v>
       </c>
       <c r="D32" s="27"/>
       <c r="E32" s="28"/>
@@ -1825,7 +1734,7 @@
         <v>12</v>
       </c>
       <c r="H32" s="3" t="s">
-        <v>29</v>
+        <v>73</v>
       </c>
       <c r="I32" s="4">
         <v>0</v>
@@ -1844,13 +1753,13 @@
         <v>15</v>
       </c>
       <c r="H33" s="3" t="s">
-        <v>29</v>
+        <v>73</v>
       </c>
       <c r="I33" s="4">
         <v>0</v>
       </c>
       <c r="J33" s="5" t="s">
-        <v>23</v>
+        <v>41</v>
       </c>
     </row>
     <row r="34" spans="2:10">
@@ -1862,14 +1771,14 @@
         <v>16</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="H34" s="3" t="s">
-        <v>48</v>
+        <v>25</v>
       </c>
       <c r="I34" s="4"/>
       <c r="J34" s="5" t="s">
-        <v>87</v>
+        <v>74</v>
       </c>
     </row>
     <row r="35" spans="2:10">
@@ -1878,13 +1787,13 @@
       <c r="D35" s="21"/>
       <c r="E35" s="22"/>
       <c r="F35" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="H35" s="3" t="s">
-        <v>30</v>
+        <v>75</v>
       </c>
       <c r="I35" s="4">
         <v>0</v>
@@ -1897,19 +1806,19 @@
       <c r="D36" s="21"/>
       <c r="E36" s="22"/>
       <c r="F36" s="3" t="s">
-        <v>19</v>
+        <v>55</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="H36" s="3" t="s">
-        <v>30</v>
+        <v>75</v>
       </c>
       <c r="I36" s="4">
         <v>0</v>
       </c>
       <c r="J36" s="5" t="s">
-        <v>23</v>
+        <v>41</v>
       </c>
     </row>
     <row r="37" spans="2:10">
@@ -1918,32 +1827,32 @@
       <c r="D37" s="21"/>
       <c r="E37" s="22"/>
       <c r="F37" s="3" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
       <c r="G37" s="3" t="s">
-        <v>55</v>
+        <v>76</v>
       </c>
       <c r="H37" s="3" t="s">
-        <v>48</v>
+        <v>25</v>
       </c>
       <c r="I37" s="4"/>
       <c r="J37" s="5" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="38" spans="2:10">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="38" spans="2:10" ht="15.75">
       <c r="B38" s="20"/>
       <c r="C38" s="21"/>
       <c r="D38" s="21"/>
       <c r="E38" s="22"/>
       <c r="F38" s="3" t="s">
-        <v>56</v>
+        <v>78</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>58</v>
+        <v>79</v>
       </c>
       <c r="H38" s="3" t="s">
-        <v>32</v>
+        <v>80</v>
       </c>
       <c r="I38" s="4">
         <v>0</v>
@@ -1951,18 +1860,18 @@
       <c r="J38" s="5"/>
     </row>
     <row r="39" spans="2:10">
-      <c r="B39" s="23"/>
-      <c r="C39" s="24"/>
-      <c r="D39" s="24"/>
-      <c r="E39" s="25"/>
+      <c r="B39" s="20"/>
+      <c r="C39" s="21"/>
+      <c r="D39" s="21"/>
+      <c r="E39" s="22"/>
       <c r="F39" s="3" t="s">
-        <v>57</v>
+        <v>81</v>
       </c>
       <c r="G39" s="3" t="s">
-        <v>59</v>
+        <v>82</v>
       </c>
       <c r="H39" s="3" t="s">
-        <v>34</v>
+        <v>83</v>
       </c>
       <c r="I39" s="4">
         <v>0</v>
@@ -1970,22 +1879,18 @@
       <c r="J39" s="5"/>
     </row>
     <row r="40" spans="2:10">
-      <c r="B40" s="20" t="s">
-        <v>101</v>
-      </c>
-      <c r="C40" s="21" t="s">
-        <v>102</v>
-      </c>
+      <c r="B40" s="20"/>
+      <c r="C40" s="21"/>
       <c r="D40" s="21"/>
       <c r="E40" s="22"/>
       <c r="F40" s="3" t="s">
-        <v>103</v>
+        <v>84</v>
       </c>
       <c r="G40" s="3" t="s">
-        <v>104</v>
+        <v>85</v>
       </c>
       <c r="H40" s="3" t="s">
-        <v>105</v>
+        <v>86</v>
       </c>
       <c r="I40" s="4">
         <v>0</v>
@@ -1993,18 +1898,18 @@
       <c r="J40" s="5"/>
     </row>
     <row r="41" spans="2:10">
-      <c r="B41" s="20"/>
-      <c r="C41" s="21"/>
-      <c r="D41" s="21"/>
-      <c r="E41" s="22"/>
+      <c r="B41" s="23"/>
+      <c r="C41" s="24"/>
+      <c r="D41" s="24"/>
+      <c r="E41" s="25"/>
       <c r="F41" s="3" t="s">
-        <v>106</v>
+        <v>87</v>
       </c>
       <c r="G41" s="3" t="s">
-        <v>109</v>
+        <v>88</v>
       </c>
       <c r="H41" s="3" t="s">
-        <v>112</v>
+        <v>89</v>
       </c>
       <c r="I41" s="4">
         <v>0</v>
@@ -2012,18 +1917,22 @@
       <c r="J41" s="5"/>
     </row>
     <row r="42" spans="2:10">
-      <c r="B42" s="20"/>
-      <c r="C42" s="21"/>
+      <c r="B42" s="20" t="s">
+        <v>90</v>
+      </c>
+      <c r="C42" s="21" t="s">
+        <v>91</v>
+      </c>
       <c r="D42" s="21"/>
       <c r="E42" s="22"/>
       <c r="F42" s="3" t="s">
-        <v>107</v>
+        <v>11</v>
       </c>
       <c r="G42" s="3" t="s">
-        <v>110</v>
+        <v>12</v>
       </c>
       <c r="H42" s="3" t="s">
-        <v>113</v>
+        <v>92</v>
       </c>
       <c r="I42" s="4">
         <v>0</v>
@@ -2036,13 +1945,13 @@
       <c r="D43" s="21"/>
       <c r="E43" s="22"/>
       <c r="F43" s="3" t="s">
-        <v>108</v>
+        <v>14</v>
       </c>
       <c r="G43" s="3" t="s">
-        <v>111</v>
+        <v>26</v>
       </c>
       <c r="H43" s="3" t="s">
-        <v>114</v>
+        <v>93</v>
       </c>
       <c r="I43" s="4">
         <v>0</v>
@@ -2050,24 +1959,18 @@
       <c r="J43" s="5"/>
     </row>
     <row r="44" spans="2:10">
-      <c r="B44" s="26" t="s">
-        <v>53</v>
-      </c>
-      <c r="C44" s="27" t="s">
-        <v>51</v>
-      </c>
-      <c r="D44" s="27" t="s">
-        <v>37</v>
-      </c>
-      <c r="E44" s="28"/>
+      <c r="B44" s="20"/>
+      <c r="C44" s="21"/>
+      <c r="D44" s="21"/>
+      <c r="E44" s="22"/>
       <c r="F44" s="3" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="G44" s="3" t="s">
-        <v>125</v>
+        <v>36</v>
       </c>
       <c r="H44" s="3" t="s">
-        <v>13</v>
+        <v>94</v>
       </c>
       <c r="I44" s="4">
         <v>0</v>
@@ -2080,62 +1983,60 @@
       <c r="D45" s="21"/>
       <c r="E45" s="22"/>
       <c r="F45" s="3" t="s">
-        <v>127</v>
+        <v>18</v>
       </c>
       <c r="G45" s="3" t="s">
-        <v>128</v>
+        <v>95</v>
       </c>
       <c r="H45" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="I45" s="4" t="s">
-        <v>130</v>
+        <v>96</v>
+      </c>
+      <c r="I45" s="4">
+        <v>0</v>
       </c>
       <c r="J45" s="5"/>
     </row>
     <row r="46" spans="2:10">
-      <c r="B46" s="23"/>
-      <c r="C46" s="24"/>
-      <c r="D46" s="24"/>
-      <c r="E46" s="25"/>
+      <c r="B46" s="26" t="s">
+        <v>97</v>
+      </c>
+      <c r="C46" s="27" t="s">
+        <v>98</v>
+      </c>
+      <c r="D46" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="E46" s="28"/>
       <c r="F46" s="3" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="G46" s="3" t="s">
-        <v>126</v>
+        <v>100</v>
       </c>
       <c r="H46" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="I46" s="4" t="s">
-        <v>131</v>
+      <c r="I46" s="4">
+        <v>0</v>
       </c>
       <c r="J46" s="5"/>
     </row>
-    <row r="47" spans="2:10" ht="75">
-      <c r="B47" s="26" t="s">
-        <v>89</v>
-      </c>
-      <c r="C47" s="27" t="s">
-        <v>52</v>
-      </c>
-      <c r="D47" s="27" t="s">
-        <v>41</v>
-      </c>
-      <c r="E47" s="29" t="s">
-        <v>122</v>
-      </c>
+    <row r="47" spans="2:10">
+      <c r="B47" s="20"/>
+      <c r="C47" s="21"/>
+      <c r="D47" s="21"/>
+      <c r="E47" s="22"/>
       <c r="F47" s="3" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="G47" s="3" t="s">
-        <v>38</v>
+        <v>101</v>
       </c>
       <c r="H47" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="I47" s="4">
-        <v>0</v>
+      <c r="I47" s="4" t="s">
+        <v>102</v>
       </c>
       <c r="J47" s="5"/>
     </row>
@@ -2145,87 +2046,133 @@
       <c r="D48" s="24"/>
       <c r="E48" s="25"/>
       <c r="F48" s="3" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="G48" s="3" t="s">
-        <v>39</v>
+        <v>103</v>
       </c>
       <c r="H48" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="I48" s="4">
-        <v>0</v>
+      <c r="I48" s="4" t="s">
+        <v>104</v>
       </c>
       <c r="J48" s="5"/>
     </row>
-    <row r="49" spans="2:10" ht="37.5">
-      <c r="B49" s="30" t="s">
+    <row r="49" spans="2:10" ht="75">
+      <c r="B49" s="26" t="s">
+        <v>105</v>
+      </c>
+      <c r="C49" s="27" t="s">
+        <v>106</v>
+      </c>
+      <c r="D49" s="27" t="s">
+        <v>107</v>
+      </c>
+      <c r="E49" s="29" t="s">
+        <v>108</v>
+      </c>
+      <c r="F49" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G49" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="H49" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I49" s="4">
+        <v>0</v>
+      </c>
+      <c r="J49" s="5"/>
+    </row>
+    <row r="50" spans="2:10">
+      <c r="B50" s="23"/>
+      <c r="C50" s="24"/>
+      <c r="D50" s="24"/>
+      <c r="E50" s="25"/>
+      <c r="F50" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G50" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="H50" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I50" s="4">
+        <v>0</v>
+      </c>
+      <c r="J50" s="5"/>
+    </row>
+    <row r="51" spans="2:10" ht="37.5">
+      <c r="B51" s="30" t="s">
+        <v>111</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="D51" s="4"/>
+      <c r="E51" s="31" t="s">
+        <v>112</v>
+      </c>
+      <c r="F51" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G51" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H51" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I51" s="4">
+        <v>0</v>
+      </c>
+      <c r="J51" s="5"/>
+    </row>
+    <row r="52" spans="2:10" ht="37.5">
+      <c r="B52" s="30" t="s">
+        <v>113</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="D52" s="4"/>
+      <c r="E52" s="31" t="s">
+        <v>112</v>
+      </c>
+      <c r="F52" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G52" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H52" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I52" s="4">
+        <v>0</v>
+      </c>
+      <c r="J52" s="5"/>
+    </row>
+    <row r="53" spans="2:10" ht="19.5" thickBot="1">
+      <c r="B53" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="C53" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="C49" s="4" t="s">
+      <c r="D53" s="7" t="s">
         <v>117</v>
       </c>
-      <c r="D49" s="4"/>
-      <c r="E49" s="31" t="s">
-        <v>123</v>
-      </c>
-      <c r="F49" s="3" t="s">
+      <c r="E53" s="8" t="s">
         <v>118</v>
       </c>
-      <c r="G49" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="H49" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="I49" s="4">
-        <v>0</v>
-      </c>
-      <c r="J49" s="5"/>
-    </row>
-    <row r="50" spans="2:10" ht="37.5">
-      <c r="B50" s="30" t="s">
-        <v>121</v>
-      </c>
-      <c r="C50" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="D50" s="4"/>
-      <c r="E50" s="31" t="s">
-        <v>123</v>
-      </c>
-      <c r="F50" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="G50" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="H50" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="I50" s="4">
-        <v>0</v>
-      </c>
-      <c r="J50" s="5"/>
-    </row>
-    <row r="51" spans="2:10" ht="19.5" thickBot="1">
-      <c r="B51" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="C51" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="D51" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="E51" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="F51" s="8"/>
-      <c r="G51" s="8"/>
-      <c r="H51" s="8"/>
-      <c r="I51" s="7"/>
-      <c r="J51" s="9"/>
+      <c r="F53" s="8"/>
+      <c r="G53" s="8"/>
+      <c r="H53" s="8"/>
+      <c r="I53" s="7"/>
+      <c r="J53" s="9"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>

</xml_diff>

<commit_message>
updated samples accrding to rggen/rggen#44
</commit_message>
<xml_diff>
--- a/block_0.xlsx
+++ b/block_0.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23216"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DA7EB6AA-2B73-41EE-A500-8BA87648E7CD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{955F897A-F574-4096-946C-0CD784ED9154}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="139">
   <si>
     <t>block name</t>
     <phoneticPr fontId="1"/>
@@ -114,6 +114,24 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
+    <t>bit_field_4</t>
+  </si>
+  <si>
+    <t>11:2</t>
+  </si>
+  <si>
+    <t>wrc</t>
+  </si>
+  <si>
+    <t>bit_field_5</t>
+  </si>
+  <si>
+    <t>13:2</t>
+  </si>
+  <si>
+    <t>wrs</t>
+  </si>
+  <si>
     <t>register_1</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -405,11 +423,51 @@
   </si>
   <si>
     <t>register_8</t>
-    <phoneticPr fontId="1"/>
   </si>
   <si>
     <t>0x20</t>
-    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>wc</t>
+  </si>
+  <si>
+    <t>bit_field_1</t>
+  </si>
+  <si>
+    <t>8:4</t>
+  </si>
+  <si>
+    <t>ws</t>
+  </si>
+  <si>
+    <t>bit_field_2</t>
+  </si>
+  <si>
+    <t>16:4</t>
+  </si>
+  <si>
+    <t>woc</t>
+  </si>
+  <si>
+    <t>bit_field_3</t>
+  </si>
+  <si>
+    <t>wos</t>
+  </si>
+  <si>
+    <t>wcrs</t>
+  </si>
+  <si>
+    <t>40:4</t>
+  </si>
+  <si>
+    <t>wsrc</t>
+  </si>
+  <si>
+    <t>register_9</t>
+  </si>
+  <si>
+    <t>0x30</t>
   </si>
   <si>
     <t>[4]</t>
@@ -436,12 +494,10 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>register_9</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>0x40</t>
-    <phoneticPr fontId="1"/>
+    <t>register_10</t>
+  </si>
+  <si>
+    <t>0x50</t>
   </si>
   <si>
     <t>[2, 4]</t>
@@ -463,8 +519,7 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>register_10</t>
-    <phoneticPr fontId="1"/>
+    <t>register_11</t>
   </si>
   <si>
     <t>indirect:
@@ -472,16 +527,13 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>register_11</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>0x44</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>register_12</t>
-    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>0x54</t>
+  </si>
+  <si>
+    <t>register_13</t>
   </si>
   <si>
     <t>0x80</t>
@@ -524,7 +576,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="20">
+  <borders count="29">
     <border>
       <left/>
       <right/>
@@ -797,11 +849,136 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
@@ -838,6 +1015,19 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
@@ -1118,10 +1308,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:J53"/>
+  <dimension ref="B1:J61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="H42" sqref="H42"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="G54" sqref="G54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
@@ -1243,10 +1433,10 @@
       <c r="J7" s="5"/>
     </row>
     <row r="8" spans="2:10">
-      <c r="B8" s="23"/>
-      <c r="C8" s="24"/>
-      <c r="D8" s="24"/>
-      <c r="E8" s="25"/>
+      <c r="B8" s="20"/>
+      <c r="C8" s="21"/>
+      <c r="D8" s="21"/>
+      <c r="E8" s="22"/>
       <c r="F8" s="3" t="s">
         <v>18</v>
       </c>
@@ -1262,91 +1452,93 @@
       <c r="J8" s="5"/>
     </row>
     <row r="9" spans="2:10">
-      <c r="B9" s="26" t="s">
+      <c r="B9" s="20"/>
+      <c r="C9" s="21"/>
+      <c r="D9" s="21"/>
+      <c r="E9" s="22"/>
+      <c r="F9" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="27"/>
-      <c r="D9" s="27"/>
-      <c r="E9" s="28"/>
-      <c r="F9" s="3"/>
       <c r="G9" s="3" t="s">
         <v>22</v>
       </c>
       <c r="H9" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="I9" s="4">
+        <v>0</v>
+      </c>
+      <c r="J9" s="5"/>
+    </row>
+    <row r="10" spans="2:10">
+      <c r="B10" s="23"/>
+      <c r="C10" s="24"/>
+      <c r="D10" s="24"/>
+      <c r="E10" s="25"/>
+      <c r="F10" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="I10" s="4">
+        <v>0</v>
+      </c>
+      <c r="J10" s="5"/>
+    </row>
+    <row r="11" spans="2:10">
+      <c r="B11" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" s="27"/>
+      <c r="D11" s="27"/>
+      <c r="E11" s="28"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="H11" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="I9" s="4">
-        <v>0</v>
-      </c>
-      <c r="J9" s="5"/>
-    </row>
-    <row r="10" spans="2:10">
-      <c r="B10" s="26" t="s">
-        <v>23</v>
-      </c>
-      <c r="C10" s="27" t="s">
-        <v>24</v>
-      </c>
-      <c r="D10" s="27"/>
-      <c r="E10" s="28"/>
-      <c r="F10" s="3" t="s">
+      <c r="I11" s="4">
+        <v>0</v>
+      </c>
+      <c r="J11" s="5"/>
+    </row>
+    <row r="12" spans="2:10">
+      <c r="B12" s="26" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12" s="27"/>
+      <c r="E12" s="28"/>
+      <c r="F12" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="G10" s="3" t="s">
+      <c r="G12" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="H10" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="I10" s="4"/>
-      <c r="J10" s="5"/>
-    </row>
-    <row r="11" spans="2:10">
-      <c r="B11" s="20"/>
-      <c r="C11" s="21"/>
-      <c r="D11" s="21"/>
-      <c r="E11" s="22"/>
-      <c r="F11" s="3" t="s">
+      <c r="H12" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="I12" s="4"/>
+      <c r="J12" s="5"/>
+    </row>
+    <row r="13" spans="2:10">
+      <c r="B13" s="20"/>
+      <c r="C13" s="21"/>
+      <c r="D13" s="21"/>
+      <c r="E13" s="22"/>
+      <c r="F13" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G11" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="H11" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="I11" s="4"/>
-      <c r="J11" s="5"/>
-    </row>
-    <row r="12" spans="2:10">
-      <c r="B12" s="20"/>
-      <c r="C12" s="21"/>
-      <c r="D12" s="21"/>
-      <c r="E12" s="22"/>
-      <c r="F12" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="H12" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="I12" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="J12" s="5"/>
-    </row>
-    <row r="13" spans="2:10">
-      <c r="B13" s="23"/>
-      <c r="C13" s="24"/>
-      <c r="D13" s="24"/>
-      <c r="E13" s="25"/>
-      <c r="F13" s="3" t="s">
-        <v>18</v>
-      </c>
       <c r="G13" s="3" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H13" s="3" t="s">
         <v>31</v>
@@ -1355,62 +1547,62 @@
       <c r="J13" s="5"/>
     </row>
     <row r="14" spans="2:10">
-      <c r="B14" s="26" t="s">
-        <v>32</v>
-      </c>
-      <c r="C14" s="27" t="s">
-        <v>24</v>
-      </c>
-      <c r="D14" s="27"/>
-      <c r="E14" s="28"/>
+      <c r="B14" s="20"/>
+      <c r="C14" s="21"/>
+      <c r="D14" s="21"/>
+      <c r="E14" s="22"/>
       <c r="F14" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="I14" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="J14" s="5"/>
+    </row>
+    <row r="15" spans="2:10">
+      <c r="B15" s="23"/>
+      <c r="C15" s="24"/>
+      <c r="D15" s="24"/>
+      <c r="E15" s="25"/>
+      <c r="F15" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="I15" s="4"/>
+      <c r="J15" s="5"/>
+    </row>
+    <row r="16" spans="2:10">
+      <c r="B16" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="C16" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="D16" s="27"/>
+      <c r="E16" s="28"/>
+      <c r="F16" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="G14" s="3" t="s">
+      <c r="G16" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="H14" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="I14" s="4">
-        <v>0</v>
-      </c>
-      <c r="J14" s="5"/>
-    </row>
-    <row r="15" spans="2:10">
-      <c r="B15" s="20"/>
-      <c r="C15" s="21"/>
-      <c r="D15" s="21"/>
-      <c r="E15" s="22"/>
-      <c r="F15" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G15" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="H15" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="I15" s="4">
-        <v>0</v>
-      </c>
-      <c r="J15" s="5"/>
-    </row>
-    <row r="16" spans="2:10">
-      <c r="B16" s="20"/>
-      <c r="C16" s="21"/>
-      <c r="D16" s="21"/>
-      <c r="E16" s="22"/>
-      <c r="F16" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G16" s="3" t="s">
-        <v>26</v>
-      </c>
       <c r="H16" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="I16" s="4"/>
+        <v>39</v>
+      </c>
+      <c r="I16" s="4">
+        <v>0</v>
+      </c>
       <c r="J16" s="5"/>
     </row>
     <row r="17" spans="2:10">
@@ -1419,38 +1611,34 @@
       <c r="D17" s="21"/>
       <c r="E17" s="22"/>
       <c r="F17" s="3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>36</v>
+        <v>15</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="I17" s="4"/>
+        <v>40</v>
+      </c>
+      <c r="I17" s="4">
+        <v>0</v>
+      </c>
       <c r="J17" s="5"/>
     </row>
     <row r="18" spans="2:10">
-      <c r="B18" s="26" t="s">
-        <v>38</v>
-      </c>
-      <c r="C18" s="27" t="s">
-        <v>39</v>
-      </c>
-      <c r="D18" s="27"/>
-      <c r="E18" s="28"/>
+      <c r="B18" s="20"/>
+      <c r="C18" s="21"/>
+      <c r="D18" s="21"/>
+      <c r="E18" s="22"/>
       <c r="F18" s="3" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="I18" s="4">
-        <v>0</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="I18" s="4"/>
       <c r="J18" s="5"/>
     </row>
     <row r="19" spans="2:10">
@@ -1459,116 +1647,116 @@
       <c r="D19" s="21"/>
       <c r="E19" s="22"/>
       <c r="F19" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="I19" s="4"/>
+      <c r="J19" s="5"/>
+    </row>
+    <row r="20" spans="2:10">
+      <c r="B20" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="C20" s="27" t="s">
+        <v>45</v>
+      </c>
+      <c r="D20" s="27"/>
+      <c r="E20" s="28"/>
+      <c r="F20" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="I20" s="4">
+        <v>0</v>
+      </c>
+      <c r="J20" s="5"/>
+    </row>
+    <row r="21" spans="2:10">
+      <c r="B21" s="20"/>
+      <c r="C21" s="21"/>
+      <c r="D21" s="21"/>
+      <c r="E21" s="22"/>
+      <c r="F21" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G19" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="H19" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="I19" s="4">
-        <v>0</v>
-      </c>
-      <c r="J19" s="5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="20" spans="2:10">
-      <c r="B20" s="20"/>
-      <c r="C20" s="21"/>
-      <c r="D20" s="21"/>
-      <c r="E20" s="22"/>
-      <c r="F20" s="3" t="s">
+      <c r="G21" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="H21" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="I21" s="4">
+        <v>0</v>
+      </c>
+      <c r="J21" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="22" spans="2:10">
+      <c r="B22" s="20"/>
+      <c r="C22" s="21"/>
+      <c r="D22" s="21"/>
+      <c r="E22" s="22"/>
+      <c r="F22" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="G20" s="3" t="s">
+      <c r="G22" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="H22" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="I22" s="4"/>
+      <c r="J22" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="23" spans="2:10">
+      <c r="B23" s="23"/>
+      <c r="C23" s="24"/>
+      <c r="D23" s="24"/>
+      <c r="E23" s="25"/>
+      <c r="F23" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G23" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="H20" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="I20" s="4"/>
-      <c r="J20" s="5" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="21" spans="2:10">
-      <c r="B21" s="23"/>
-      <c r="C21" s="24"/>
-      <c r="D21" s="24"/>
-      <c r="E21" s="25"/>
-      <c r="F21" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="G21" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="H21" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="I21" s="4">
-        <v>0</v>
-      </c>
-      <c r="J21" s="5"/>
-    </row>
-    <row r="22" spans="2:10">
-      <c r="B22" s="26" t="s">
-        <v>45</v>
-      </c>
-      <c r="C22" s="27" t="s">
-        <v>46</v>
-      </c>
-      <c r="D22" s="27"/>
-      <c r="E22" s="28"/>
-      <c r="F22" s="3" t="s">
+      <c r="H23" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="I23" s="4">
+        <v>0</v>
+      </c>
+      <c r="J23" s="5"/>
+    </row>
+    <row r="24" spans="2:10">
+      <c r="B24" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="C24" s="27" t="s">
+        <v>52</v>
+      </c>
+      <c r="D24" s="27"/>
+      <c r="E24" s="28"/>
+      <c r="F24" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="G22" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="H22" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="I22" s="4">
-        <v>0</v>
-      </c>
-      <c r="J22" s="5"/>
-    </row>
-    <row r="23" spans="2:10">
-      <c r="B23" s="20"/>
-      <c r="C23" s="21"/>
-      <c r="D23" s="21"/>
-      <c r="E23" s="22"/>
-      <c r="F23" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G23" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="H23" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="I23" s="4">
-        <v>0</v>
-      </c>
-      <c r="J23" s="5" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="24" spans="2:10">
-      <c r="B24" s="20"/>
-      <c r="C24" s="21"/>
-      <c r="D24" s="21"/>
-      <c r="E24" s="22"/>
-      <c r="F24" s="3" t="s">
-        <v>16</v>
-      </c>
       <c r="G24" s="3" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="I24" s="4">
         <v>0</v>
@@ -1581,19 +1769,19 @@
       <c r="D25" s="21"/>
       <c r="E25" s="22"/>
       <c r="F25" s="3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="I25" s="4">
         <v>0</v>
       </c>
       <c r="J25" s="5" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="26" spans="2:10">
@@ -1602,13 +1790,13 @@
       <c r="D26" s="21"/>
       <c r="E26" s="22"/>
       <c r="F26" s="3" t="s">
-        <v>55</v>
+        <v>16</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="H26" s="3" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="I26" s="4">
         <v>0</v>
@@ -1621,13 +1809,13 @@
       <c r="D27" s="21"/>
       <c r="E27" s="22"/>
       <c r="F27" s="3" t="s">
-        <v>58</v>
+        <v>18</v>
       </c>
       <c r="G27" s="3" t="s">
         <v>59</v>
       </c>
       <c r="H27" s="3" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="I27" s="4">
         <v>0</v>
@@ -1648,14 +1836,12 @@
         <v>62</v>
       </c>
       <c r="H28" s="3" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="I28" s="4">
         <v>0</v>
       </c>
-      <c r="J28" s="5" t="s">
-        <v>21</v>
-      </c>
+      <c r="J28" s="5"/>
     </row>
     <row r="29" spans="2:10">
       <c r="B29" s="20"/>
@@ -1663,18 +1849,20 @@
       <c r="D29" s="21"/>
       <c r="E29" s="22"/>
       <c r="F29" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="G29" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="H29" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="G29" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="H29" s="3" t="s">
-        <v>65</v>
-      </c>
       <c r="I29" s="4">
         <v>0</v>
       </c>
-      <c r="J29" s="5"/>
+      <c r="J29" s="5" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="30" spans="2:10">
       <c r="B30" s="20"/>
@@ -1682,26 +1870,26 @@
       <c r="D30" s="21"/>
       <c r="E30" s="22"/>
       <c r="F30" s="3" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="H30" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I30" s="4">
         <v>0</v>
       </c>
       <c r="J30" s="5" t="s">
-        <v>68</v>
+        <v>27</v>
       </c>
     </row>
     <row r="31" spans="2:10">
-      <c r="B31" s="23"/>
-      <c r="C31" s="24"/>
-      <c r="D31" s="24"/>
-      <c r="E31" s="25"/>
+      <c r="B31" s="20"/>
+      <c r="C31" s="21"/>
+      <c r="D31" s="21"/>
+      <c r="E31" s="22"/>
       <c r="F31" s="3" t="s">
         <v>69</v>
       </c>
@@ -1709,77 +1897,77 @@
         <v>70</v>
       </c>
       <c r="H31" s="3" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="I31" s="4">
         <v>0</v>
       </c>
-      <c r="J31" s="5" t="s">
-        <v>21</v>
-      </c>
+      <c r="J31" s="5"/>
     </row>
     <row r="32" spans="2:10">
-      <c r="B32" s="26" t="s">
+      <c r="B32" s="20"/>
+      <c r="C32" s="21"/>
+      <c r="D32" s="21"/>
+      <c r="E32" s="22"/>
+      <c r="F32" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="G32" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="H32" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="C32" s="27" t="s">
-        <v>72</v>
-      </c>
-      <c r="D32" s="27"/>
-      <c r="E32" s="28"/>
-      <c r="F32" s="3" t="s">
+      <c r="I32" s="4">
+        <v>0</v>
+      </c>
+      <c r="J32" s="5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="33" spans="2:10">
+      <c r="B33" s="23"/>
+      <c r="C33" s="24"/>
+      <c r="D33" s="24"/>
+      <c r="E33" s="25"/>
+      <c r="F33" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="G33" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="H33" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="I33" s="4">
+        <v>0</v>
+      </c>
+      <c r="J33" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="34" spans="2:10">
+      <c r="B34" s="26" t="s">
+        <v>77</v>
+      </c>
+      <c r="C34" s="27" t="s">
+        <v>78</v>
+      </c>
+      <c r="D34" s="27"/>
+      <c r="E34" s="28"/>
+      <c r="F34" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="G32" s="3" t="s">
+      <c r="G34" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="H32" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="I32" s="4">
-        <v>0</v>
-      </c>
-      <c r="J32" s="5"/>
-    </row>
-    <row r="33" spans="2:10">
-      <c r="B33" s="20"/>
-      <c r="C33" s="21"/>
-      <c r="D33" s="21"/>
-      <c r="E33" s="22"/>
-      <c r="F33" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G33" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="H33" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="I33" s="4">
-        <v>0</v>
-      </c>
-      <c r="J33" s="5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="34" spans="2:10">
-      <c r="B34" s="20"/>
-      <c r="C34" s="21"/>
-      <c r="D34" s="21"/>
-      <c r="E34" s="22"/>
-      <c r="F34" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G34" s="3" t="s">
-        <v>26</v>
-      </c>
       <c r="H34" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="I34" s="4"/>
-      <c r="J34" s="5" t="s">
-        <v>74</v>
-      </c>
+        <v>79</v>
+      </c>
+      <c r="I34" s="4">
+        <v>0</v>
+      </c>
+      <c r="J34" s="5"/>
     </row>
     <row r="35" spans="2:10">
       <c r="B35" s="20"/>
@@ -1787,18 +1975,20 @@
       <c r="D35" s="21"/>
       <c r="E35" s="22"/>
       <c r="F35" s="3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>42</v>
+        <v>15</v>
       </c>
       <c r="H35" s="3" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="I35" s="4">
         <v>0</v>
       </c>
-      <c r="J35" s="5"/>
+      <c r="J35" s="5" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="36" spans="2:10">
       <c r="B36" s="20"/>
@@ -1806,19 +1996,17 @@
       <c r="D36" s="21"/>
       <c r="E36" s="22"/>
       <c r="F36" s="3" t="s">
-        <v>55</v>
+        <v>16</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="H36" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="I36" s="4">
-        <v>0</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="I36" s="4"/>
       <c r="J36" s="5" t="s">
-        <v>41</v>
+        <v>80</v>
       </c>
     </row>
     <row r="37" spans="2:10">
@@ -1827,37 +2015,39 @@
       <c r="D37" s="21"/>
       <c r="E37" s="22"/>
       <c r="F37" s="3" t="s">
-        <v>58</v>
+        <v>18</v>
       </c>
       <c r="G37" s="3" t="s">
-        <v>76</v>
+        <v>48</v>
       </c>
       <c r="H37" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="I37" s="4"/>
-      <c r="J37" s="5" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="38" spans="2:10" ht="15.75">
+        <v>81</v>
+      </c>
+      <c r="I37" s="4">
+        <v>0</v>
+      </c>
+      <c r="J37" s="5"/>
+    </row>
+    <row r="38" spans="2:10">
       <c r="B38" s="20"/>
       <c r="C38" s="21"/>
       <c r="D38" s="21"/>
       <c r="E38" s="22"/>
       <c r="F38" s="3" t="s">
-        <v>78</v>
+        <v>61</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>79</v>
+        <v>42</v>
       </c>
       <c r="H38" s="3" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="I38" s="4">
         <v>0</v>
       </c>
-      <c r="J38" s="5"/>
+      <c r="J38" s="5" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="39" spans="2:10">
       <c r="B39" s="20"/>
@@ -1865,20 +2055,20 @@
       <c r="D39" s="21"/>
       <c r="E39" s="22"/>
       <c r="F39" s="3" t="s">
-        <v>81</v>
+        <v>64</v>
       </c>
       <c r="G39" s="3" t="s">
         <v>82</v>
       </c>
       <c r="H39" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="I39" s="4"/>
+      <c r="J39" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="I39" s="4">
-        <v>0</v>
-      </c>
-      <c r="J39" s="5"/>
-    </row>
-    <row r="40" spans="2:10">
+    </row>
+    <row r="40" spans="2:10" ht="15.75">
       <c r="B40" s="20"/>
       <c r="C40" s="21"/>
       <c r="D40" s="21"/>
@@ -1898,10 +2088,10 @@
       <c r="J40" s="5"/>
     </row>
     <row r="41" spans="2:10">
-      <c r="B41" s="23"/>
-      <c r="C41" s="24"/>
-      <c r="D41" s="24"/>
-      <c r="E41" s="25"/>
+      <c r="B41" s="20"/>
+      <c r="C41" s="21"/>
+      <c r="D41" s="21"/>
+      <c r="E41" s="22"/>
       <c r="F41" s="3" t="s">
         <v>87</v>
       </c>
@@ -1917,19 +2107,15 @@
       <c r="J41" s="5"/>
     </row>
     <row r="42" spans="2:10">
-      <c r="B42" s="20" t="s">
-        <v>90</v>
-      </c>
-      <c r="C42" s="21" t="s">
-        <v>91</v>
-      </c>
+      <c r="B42" s="20"/>
+      <c r="C42" s="21"/>
       <c r="D42" s="21"/>
       <c r="E42" s="22"/>
       <c r="F42" s="3" t="s">
-        <v>11</v>
+        <v>90</v>
       </c>
       <c r="G42" s="3" t="s">
-        <v>12</v>
+        <v>91</v>
       </c>
       <c r="H42" s="3" t="s">
         <v>92</v>
@@ -1940,18 +2126,18 @@
       <c r="J42" s="5"/>
     </row>
     <row r="43" spans="2:10">
-      <c r="B43" s="20"/>
-      <c r="C43" s="21"/>
-      <c r="D43" s="21"/>
-      <c r="E43" s="22"/>
+      <c r="B43" s="23"/>
+      <c r="C43" s="24"/>
+      <c r="D43" s="24"/>
+      <c r="E43" s="25"/>
       <c r="F43" s="3" t="s">
-        <v>14</v>
+        <v>93</v>
       </c>
       <c r="G43" s="3" t="s">
-        <v>26</v>
+        <v>94</v>
       </c>
       <c r="H43" s="3" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="I43" s="4">
         <v>0</v>
@@ -1959,18 +2145,22 @@
       <c r="J43" s="5"/>
     </row>
     <row r="44" spans="2:10">
-      <c r="B44" s="20"/>
-      <c r="C44" s="21"/>
+      <c r="B44" s="20" t="s">
+        <v>96</v>
+      </c>
+      <c r="C44" s="21" t="s">
+        <v>97</v>
+      </c>
       <c r="D44" s="21"/>
       <c r="E44" s="22"/>
       <c r="F44" s="3" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="G44" s="3" t="s">
-        <v>36</v>
+        <v>12</v>
       </c>
       <c r="H44" s="3" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="I44" s="4">
         <v>0</v>
@@ -1983,196 +2173,352 @@
       <c r="D45" s="21"/>
       <c r="E45" s="22"/>
       <c r="F45" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G45" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="H45" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="I45" s="4">
+        <v>0</v>
+      </c>
+      <c r="J45" s="5"/>
+    </row>
+    <row r="46" spans="2:10">
+      <c r="B46" s="20"/>
+      <c r="C46" s="21"/>
+      <c r="D46" s="21"/>
+      <c r="E46" s="22"/>
+      <c r="F46" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G46" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="H46" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="I46" s="4">
+        <v>0</v>
+      </c>
+      <c r="J46" s="5"/>
+    </row>
+    <row r="47" spans="2:10">
+      <c r="B47" s="32"/>
+      <c r="C47" s="33"/>
+      <c r="D47" s="33"/>
+      <c r="E47" s="34"/>
+      <c r="F47" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="G45" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="H45" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="I45" s="4">
-        <v>0</v>
-      </c>
-      <c r="J45" s="5"/>
-    </row>
-    <row r="46" spans="2:10">
-      <c r="B46" s="26" t="s">
-        <v>97</v>
-      </c>
-      <c r="C46" s="27" t="s">
-        <v>98</v>
-      </c>
-      <c r="D46" s="27" t="s">
-        <v>99</v>
-      </c>
-      <c r="E46" s="28"/>
-      <c r="F46" s="3" t="s">
+      <c r="G47" s="35" t="s">
+        <v>101</v>
+      </c>
+      <c r="H47" s="35" t="s">
+        <v>102</v>
+      </c>
+      <c r="I47" s="36">
+        <v>0</v>
+      </c>
+      <c r="J47" s="37"/>
+    </row>
+    <row r="48" spans="2:10">
+      <c r="B48" s="38" t="s">
+        <v>103</v>
+      </c>
+      <c r="C48" s="39" t="s">
+        <v>104</v>
+      </c>
+      <c r="D48" s="39"/>
+      <c r="E48" s="40"/>
+      <c r="F48" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="G46" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="H46" s="3" t="s">
+      <c r="G48" s="41" t="s">
+        <v>12</v>
+      </c>
+      <c r="H48" s="41" t="s">
+        <v>105</v>
+      </c>
+      <c r="I48" s="42">
+        <v>0</v>
+      </c>
+      <c r="J48" s="43"/>
+    </row>
+    <row r="49" spans="2:10">
+      <c r="B49" s="20"/>
+      <c r="C49" s="21"/>
+      <c r="D49" s="21"/>
+      <c r="E49" s="22"/>
+      <c r="F49" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="G49" s="25" t="s">
+        <v>107</v>
+      </c>
+      <c r="H49" s="25" t="s">
+        <v>108</v>
+      </c>
+      <c r="I49" s="24">
+        <v>0</v>
+      </c>
+      <c r="J49" s="44"/>
+    </row>
+    <row r="50" spans="2:10">
+      <c r="B50" s="20"/>
+      <c r="C50" s="21"/>
+      <c r="D50" s="21"/>
+      <c r="E50" s="22"/>
+      <c r="F50" s="25" t="s">
+        <v>109</v>
+      </c>
+      <c r="G50" s="25" t="s">
+        <v>110</v>
+      </c>
+      <c r="H50" s="25" t="s">
+        <v>111</v>
+      </c>
+      <c r="I50" s="24">
+        <v>0</v>
+      </c>
+      <c r="J50" s="44"/>
+    </row>
+    <row r="51" spans="2:10">
+      <c r="B51" s="20"/>
+      <c r="C51" s="21"/>
+      <c r="D51" s="21"/>
+      <c r="E51" s="22"/>
+      <c r="F51" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="G51" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="H51" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="I51" s="4">
+        <v>0</v>
+      </c>
+      <c r="J51" s="5"/>
+    </row>
+    <row r="52" spans="2:10">
+      <c r="B52" s="20"/>
+      <c r="C52" s="21"/>
+      <c r="D52" s="21"/>
+      <c r="E52" s="22"/>
+      <c r="F52" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G52" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="H52" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="I52" s="4">
+        <v>0</v>
+      </c>
+      <c r="J52" s="5"/>
+    </row>
+    <row r="53" spans="2:10">
+      <c r="B53" s="20"/>
+      <c r="C53" s="21"/>
+      <c r="D53" s="21"/>
+      <c r="E53" s="22"/>
+      <c r="F53" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G53" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="H53" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="I53" s="4">
+        <v>0</v>
+      </c>
+      <c r="J53" s="5"/>
+    </row>
+    <row r="54" spans="2:10">
+      <c r="B54" s="26" t="s">
+        <v>117</v>
+      </c>
+      <c r="C54" s="27" t="s">
+        <v>118</v>
+      </c>
+      <c r="D54" s="27" t="s">
+        <v>119</v>
+      </c>
+      <c r="E54" s="28"/>
+      <c r="F54" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G54" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="H54" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="I46" s="4">
-        <v>0</v>
-      </c>
-      <c r="J46" s="5"/>
-    </row>
-    <row r="47" spans="2:10">
-      <c r="B47" s="20"/>
-      <c r="C47" s="21"/>
-      <c r="D47" s="21"/>
-      <c r="E47" s="22"/>
-      <c r="F47" s="3" t="s">
+      <c r="I54" s="4">
+        <v>0</v>
+      </c>
+      <c r="J54" s="5"/>
+    </row>
+    <row r="55" spans="2:10">
+      <c r="B55" s="20"/>
+      <c r="C55" s="21"/>
+      <c r="D55" s="21"/>
+      <c r="E55" s="22"/>
+      <c r="F55" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G47" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="H47" s="3" t="s">
+      <c r="G55" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="H55" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="I47" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="J47" s="5"/>
-    </row>
-    <row r="48" spans="2:10">
-      <c r="B48" s="23"/>
-      <c r="C48" s="24"/>
-      <c r="D48" s="24"/>
-      <c r="E48" s="25"/>
-      <c r="F48" s="3" t="s">
+      <c r="I55" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="J55" s="5"/>
+    </row>
+    <row r="56" spans="2:10">
+      <c r="B56" s="23"/>
+      <c r="C56" s="24"/>
+      <c r="D56" s="24"/>
+      <c r="E56" s="25"/>
+      <c r="F56" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="G48" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="H48" s="3" t="s">
+      <c r="G56" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="H56" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="I48" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="J48" s="5"/>
-    </row>
-    <row r="49" spans="2:10" ht="75">
-      <c r="B49" s="26" t="s">
-        <v>105</v>
-      </c>
-      <c r="C49" s="27" t="s">
-        <v>106</v>
-      </c>
-      <c r="D49" s="27" t="s">
-        <v>107</v>
-      </c>
-      <c r="E49" s="29" t="s">
-        <v>108</v>
-      </c>
-      <c r="F49" s="3" t="s">
+      <c r="I56" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="J56" s="5"/>
+    </row>
+    <row r="57" spans="2:10" ht="75">
+      <c r="B57" s="26" t="s">
+        <v>125</v>
+      </c>
+      <c r="C57" s="27" t="s">
+        <v>126</v>
+      </c>
+      <c r="D57" s="27" t="s">
+        <v>127</v>
+      </c>
+      <c r="E57" s="29" t="s">
+        <v>128</v>
+      </c>
+      <c r="F57" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="G49" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="H49" s="3" t="s">
+      <c r="G57" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="H57" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="I49" s="4">
-        <v>0</v>
-      </c>
-      <c r="J49" s="5"/>
-    </row>
-    <row r="50" spans="2:10">
-      <c r="B50" s="23"/>
-      <c r="C50" s="24"/>
-      <c r="D50" s="24"/>
-      <c r="E50" s="25"/>
-      <c r="F50" s="3" t="s">
+      <c r="I57" s="4">
+        <v>0</v>
+      </c>
+      <c r="J57" s="5"/>
+    </row>
+    <row r="58" spans="2:10">
+      <c r="B58" s="23"/>
+      <c r="C58" s="24"/>
+      <c r="D58" s="24"/>
+      <c r="E58" s="25"/>
+      <c r="F58" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G50" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="H50" s="3" t="s">
+      <c r="G58" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="H58" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="I50" s="4">
-        <v>0</v>
-      </c>
-      <c r="J50" s="5"/>
-    </row>
-    <row r="51" spans="2:10" ht="37.5">
-      <c r="B51" s="30" t="s">
-        <v>111</v>
-      </c>
-      <c r="C51" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="D51" s="4"/>
-      <c r="E51" s="31" t="s">
-        <v>112</v>
-      </c>
-      <c r="F51" s="3" t="s">
+      <c r="I58" s="4">
+        <v>0</v>
+      </c>
+      <c r="J58" s="5"/>
+    </row>
+    <row r="59" spans="2:10" ht="37.5">
+      <c r="B59" s="30" t="s">
+        <v>131</v>
+      </c>
+      <c r="C59" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="D59" s="4"/>
+      <c r="E59" s="31" t="s">
+        <v>132</v>
+      </c>
+      <c r="F59" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="G51" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="H51" s="3" t="s">
+      <c r="G59" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="H59" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="I51" s="4">
-        <v>0</v>
-      </c>
-      <c r="J51" s="5"/>
-    </row>
-    <row r="52" spans="2:10" ht="37.5">
-      <c r="B52" s="30" t="s">
-        <v>113</v>
-      </c>
-      <c r="C52" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="D52" s="4"/>
-      <c r="E52" s="31" t="s">
-        <v>112</v>
-      </c>
-      <c r="F52" s="3" t="s">
+      <c r="I59" s="4">
+        <v>0</v>
+      </c>
+      <c r="J59" s="5"/>
+    </row>
+    <row r="60" spans="2:10" ht="37.5">
+      <c r="B60" s="30" t="s">
+        <v>133</v>
+      </c>
+      <c r="C60" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="D60" s="4"/>
+      <c r="E60" s="31" t="s">
+        <v>132</v>
+      </c>
+      <c r="F60" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="G52" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="H52" s="3" t="s">
+      <c r="G60" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="H60" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="I52" s="4">
-        <v>0</v>
-      </c>
-      <c r="J52" s="5"/>
-    </row>
-    <row r="53" spans="2:10" ht="19.5" thickBot="1">
-      <c r="B53" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="C53" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="D53" s="7" t="s">
-        <v>117</v>
-      </c>
-      <c r="E53" s="8" t="s">
-        <v>118</v>
-      </c>
-      <c r="F53" s="8"/>
-      <c r="G53" s="8"/>
-      <c r="H53" s="8"/>
-      <c r="I53" s="7"/>
-      <c r="J53" s="9"/>
+      <c r="I60" s="4">
+        <v>0</v>
+      </c>
+      <c r="J60" s="5"/>
+    </row>
+    <row r="61" spans="2:10" ht="19.5" thickBot="1">
+      <c r="B61" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="C61" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="D61" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="E61" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="F61" s="8"/>
+      <c r="G61" s="8"/>
+      <c r="H61" s="8"/>
+      <c r="I61" s="7"/>
+      <c r="J61" s="9"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>

</xml_diff>

<commit_message>
update XLSX register map due to rggen/rggen#73
</commit_message>
<xml_diff>
--- a/block_0.xlsx
+++ b/block_0.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23815"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23822"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="9" documentId="8_{955F897A-F574-4096-946C-0CD784ED9154}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{48F0242F-3CAD-4F42-BE08-A0533DC53045}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B738F93D-E31D-4967-AA03-32B92FB6B062}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="138">
   <si>
     <t>block name</t>
     <phoneticPr fontId="1"/>
@@ -82,8 +82,7 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>0:4</t>
-    <phoneticPr fontId="1"/>
+    <t>4</t>
   </si>
   <si>
     <t>rw</t>
@@ -97,366 +96,334 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
+    <t>bit_field_2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>bit_field_3</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>w1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>bit_field_4</t>
+  </si>
+  <si>
+    <t>wrc</t>
+  </si>
+  <si>
+    <t>bit_field_5</t>
+  </si>
+  <si>
+    <t>wrs</t>
+  </si>
+  <si>
+    <t>register_1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>register_2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>0x08</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>4:0</t>
+  </si>
+  <si>
+    <t>ro</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>4:8</t>
+  </si>
+  <si>
+    <t>8:16</t>
+  </si>
+  <si>
+    <t>rof</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>0xab</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>8:24</t>
+  </si>
+  <si>
+    <t>reserved</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>register_3</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>wo</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
     <t>4:4</t>
-    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>wo1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>w0trg</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>4:16</t>
+  </si>
+  <si>
+    <t>w1trg</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>register_4</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>0x0C</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>rc</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>register_0.bit_field_0</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>4:12</t>
+  </si>
+  <si>
+    <t>register_4.bit_field_1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>rs</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>register_5</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>0x10</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>2:0</t>
+  </si>
+  <si>
+    <t>rwc</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>2:2</t>
+  </si>
+  <si>
+    <t>register_3.bit_field_2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>2:4</t>
+  </si>
+  <si>
+    <t>rws</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>2:6</t>
+  </si>
+  <si>
+    <t>register_3.bit_field_3</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>bit_field_4</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>2:8</t>
+  </si>
+  <si>
+    <t>rwe</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>bit_field_5</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>2:10</t>
+  </si>
+  <si>
+    <t>register_0.bit_field_2</t>
+  </si>
+  <si>
+    <t>bit_field_6</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>2:12</t>
+  </si>
+  <si>
+    <t>bit_field_7</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>2:16</t>
+  </si>
+  <si>
+    <t>rwl</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>bit_field_8</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>2:18</t>
+  </si>
+  <si>
+    <t>register_0.bit_field_2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>bit_field_9</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>2:20</t>
+  </si>
+  <si>
+    <t>register_6</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>0x14</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>w0c</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>4:4</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>register_6.bit_field_1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>w1c</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>4:20</t>
+  </si>
+  <si>
+    <t>register_6.bit_field_4</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>bit_field_6</t>
+  </si>
+  <si>
+    <t>4:24</t>
+  </si>
+  <si>
+    <t>w0s</t>
+  </si>
+  <si>
+    <t>bit_field_7</t>
+  </si>
+  <si>
+    <t>4:28</t>
+  </si>
+  <si>
+    <t>w1s</t>
+  </si>
+  <si>
+    <t>bit_field_8</t>
+  </si>
+  <si>
+    <t>4:32</t>
+  </si>
+  <si>
+    <t>w0t</t>
+  </si>
+  <si>
+    <t>bit_field_9</t>
+  </si>
+  <si>
+    <t>4:36</t>
+  </si>
+  <si>
+    <t>w1t</t>
+  </si>
+  <si>
+    <t>register_7</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>0x1C</t>
+  </si>
+  <si>
+    <t>w0crs</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>w1crs</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>w0src</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>w1src</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>register_8</t>
+  </si>
+  <si>
+    <t>0x20</t>
+  </si>
+  <si>
+    <t>wc</t>
+  </si>
+  <si>
+    <t>bit_field_1</t>
+  </si>
+  <si>
+    <t>ws</t>
   </si>
   <si>
     <t>bit_field_2</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>8:1</t>
-    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>woc</t>
   </si>
   <si>
     <t>bit_field_3</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>9:2</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>w1</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>bit_field_4</t>
-  </si>
-  <si>
-    <t>11:2</t>
-  </si>
-  <si>
-    <t>wrc</t>
-  </si>
-  <si>
-    <t>bit_field_5</t>
-  </si>
-  <si>
-    <t>13:2</t>
-  </si>
-  <si>
-    <t>wrs</t>
-  </si>
-  <si>
-    <t>register_1</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>0:1</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>register_2</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>0x08</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>ro</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>8:4</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>16:8</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>rof</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>0xab</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>24:8</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>reserved</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>register_3</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>wo</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>wo1</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>w0trg</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>16:4</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>w1trg</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>register_4</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>0x0C</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>rc</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>register_0.bit_field_0</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>12:4</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>register_4.bit_field_1</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>rs</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>register_5</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>0x10</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>0:2</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>rwc</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>2:2</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>register_3.bit_field_2</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>4:2</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>rws</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>6:2</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>register_3.bit_field_3</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>bit_field_4</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>8:2</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>rwe</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>bit_field_5</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>10:2</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>register_0.bit_field_2</t>
-  </si>
-  <si>
-    <t>bit_field_6</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>12:2</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>bit_field_7</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>16:2</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>rwl</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>bit_field_8</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>18:2</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>register_0.bit_field_2</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>bit_field_9</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>20:2</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>register_6</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>0x14</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>w0c</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>register_6.bit_field_1</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>w1c</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>20:4</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>register_6.bit_field_4</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>bit_field_6</t>
-  </si>
-  <si>
-    <t>24:4</t>
-  </si>
-  <si>
-    <t>w0s</t>
-  </si>
-  <si>
-    <t>bit_field_7</t>
-  </si>
-  <si>
-    <t>28:4</t>
-  </si>
-  <si>
-    <t>w1s</t>
-  </si>
-  <si>
-    <t>bit_field_8</t>
-  </si>
-  <si>
-    <t>32:4</t>
-  </si>
-  <si>
-    <t>w0t</t>
-  </si>
-  <si>
-    <t>bit_field_9</t>
-  </si>
-  <si>
-    <t>36:4</t>
-  </si>
-  <si>
-    <t>w1t</t>
-  </si>
-  <si>
-    <t>register_7</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>0x1C</t>
-  </si>
-  <si>
-    <t>w0crs</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>w1crs</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>w0src</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>24:4</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>w1src</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>register_8</t>
-  </si>
-  <si>
-    <t>0x20</t>
-  </si>
-  <si>
-    <t>wc</t>
-  </si>
-  <si>
-    <t>bit_field_1</t>
-  </si>
-  <si>
-    <t>8:4</t>
-  </si>
-  <si>
-    <t>ws</t>
-  </si>
-  <si>
-    <t>bit_field_2</t>
-  </si>
-  <si>
-    <t>16:4</t>
-  </si>
-  <si>
-    <t>woc</t>
-  </si>
-  <si>
-    <t>bit_field_3</t>
   </si>
   <si>
     <t>wos</t>
@@ -465,7 +432,7 @@
     <t>wcrs</t>
   </si>
   <si>
-    <t>40:4</t>
+    <t>4:40</t>
   </si>
   <si>
     <t>wsrc</t>
@@ -481,20 +448,17 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>0:4:4:16</t>
-    <phoneticPr fontId="1"/>
+    <t>4:0:4:16</t>
   </si>
   <si>
     <t>4:4:4:16</t>
-    <phoneticPr fontId="1"/>
   </si>
   <si>
     <t>default: 0</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>8:4:4:16</t>
-    <phoneticPr fontId="1"/>
+    <t>4:8:4:16</t>
   </si>
   <si>
     <t>0, 1, 2, 3</t>
@@ -518,12 +482,10 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>0:8:4:16</t>
-    <phoneticPr fontId="1"/>
+    <t>8:0:4:16</t>
   </si>
   <si>
     <t>8:8:4:16</t>
-    <phoneticPr fontId="1"/>
   </si>
   <si>
     <t>register_11</t>
@@ -532,6 +494,9 @@
     <t>indirect:
 register_0.bit_field_2:1</t>
     <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>1:0</t>
   </si>
   <si>
     <t>register_12</t>
@@ -1381,8 +1346,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:K61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4:K61"/>
+    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="G61" sqref="G61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
@@ -1480,7 +1445,7 @@
         <v>16</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="H6" s="3" t="s">
         <v>14</v>
@@ -1497,10 +1462,10 @@
       <c r="D7" s="9"/>
       <c r="E7" s="10"/>
       <c r="F7" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G7" s="3" t="s">
         <v>18</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>19</v>
       </c>
       <c r="H7" s="3" t="s">
         <v>14</v>
@@ -1517,13 +1482,13 @@
       <c r="D8" s="9"/>
       <c r="E8" s="10"/>
       <c r="F8" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G8" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="G8" s="3" t="s">
+      <c r="H8" s="3" t="s">
         <v>21</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>22</v>
       </c>
       <c r="I8" s="4">
         <v>0</v>
@@ -1537,13 +1502,13 @@
       <c r="D9" s="9"/>
       <c r="E9" s="10"/>
       <c r="F9" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H9" s="3" t="s">
         <v>23</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>25</v>
       </c>
       <c r="I9" s="4">
         <v>0</v>
@@ -1557,13 +1522,13 @@
       <c r="D10" s="11"/>
       <c r="E10" s="12"/>
       <c r="F10" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="I10" s="4">
         <v>0</v>
@@ -1573,14 +1538,14 @@
     </row>
     <row r="11" spans="2:11">
       <c r="B11" s="31" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C11" s="13"/>
       <c r="D11" s="13"/>
       <c r="E11" s="14"/>
       <c r="F11" s="3"/>
       <c r="G11" s="3" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="H11" s="3" t="s">
         <v>14</v>
@@ -1593,10 +1558,10 @@
     </row>
     <row r="12" spans="2:11">
       <c r="B12" s="31" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D12" s="13"/>
       <c r="E12" s="14"/>
@@ -1604,10 +1569,10 @@
         <v>12</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="I12" s="4"/>
       <c r="J12" s="42"/>
@@ -1622,10 +1587,10 @@
         <v>16</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="I13" s="4"/>
       <c r="J13" s="42"/>
@@ -1637,16 +1602,16 @@
       <c r="D14" s="9"/>
       <c r="E14" s="10"/>
       <c r="F14" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="I14" s="4" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="J14" s="42"/>
       <c r="K14" s="43"/>
@@ -1657,13 +1622,13 @@
       <c r="D15" s="11"/>
       <c r="E15" s="12"/>
       <c r="F15" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="I15" s="4"/>
       <c r="J15" s="42"/>
@@ -1671,10 +1636,10 @@
     </row>
     <row r="16" spans="2:11">
       <c r="B16" s="31" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C16" s="13" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D16" s="13"/>
       <c r="E16" s="14"/>
@@ -1682,10 +1647,10 @@
         <v>12</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="I16" s="4">
         <v>0</v>
@@ -1702,10 +1667,10 @@
         <v>16</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>17</v>
+        <v>39</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="I17" s="4">
         <v>0</v>
@@ -1719,13 +1684,13 @@
       <c r="D18" s="9"/>
       <c r="E18" s="10"/>
       <c r="F18" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="I18" s="4"/>
       <c r="J18" s="42"/>
@@ -1737,13 +1702,13 @@
       <c r="D19" s="9"/>
       <c r="E19" s="10"/>
       <c r="F19" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="I19" s="4"/>
       <c r="J19" s="42"/>
@@ -1751,10 +1716,10 @@
     </row>
     <row r="20" spans="2:11">
       <c r="B20" s="31" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C20" s="13" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D20" s="13"/>
       <c r="E20" s="14"/>
@@ -1762,10 +1727,10 @@
         <v>12</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="I20" s="4">
         <v>0</v>
@@ -1782,16 +1747,16 @@
         <v>16</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="I21" s="4">
         <v>0</v>
       </c>
       <c r="J21" s="42" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="K21" s="43"/>
     </row>
@@ -1801,17 +1766,17 @@
       <c r="D22" s="9"/>
       <c r="E22" s="10"/>
       <c r="F22" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="I22" s="4"/>
       <c r="J22" s="42" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="K22" s="43"/>
     </row>
@@ -1821,13 +1786,13 @@
       <c r="D23" s="11"/>
       <c r="E23" s="12"/>
       <c r="F23" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="I23" s="4">
         <v>0</v>
@@ -1837,10 +1802,10 @@
     </row>
     <row r="24" spans="2:11">
       <c r="B24" s="31" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C24" s="13" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D24" s="13"/>
       <c r="E24" s="14"/>
@@ -1848,10 +1813,10 @@
         <v>12</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="I24" s="4">
         <v>0</v>
@@ -1868,16 +1833,16 @@
         <v>16</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="H25" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="I25" s="4">
+        <v>0</v>
+      </c>
+      <c r="J25" s="42" t="s">
         <v>56</v>
-      </c>
-      <c r="I25" s="4">
-        <v>0</v>
-      </c>
-      <c r="J25" s="42" t="s">
-        <v>58</v>
       </c>
       <c r="K25" s="43"/>
     </row>
@@ -1887,13 +1852,13 @@
       <c r="D26" s="9"/>
       <c r="E26" s="10"/>
       <c r="F26" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="H26" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="I26" s="4">
         <v>0</v>
@@ -1907,19 +1872,19 @@
       <c r="D27" s="9"/>
       <c r="E27" s="10"/>
       <c r="F27" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="H27" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="I27" s="4">
+        <v>0</v>
+      </c>
+      <c r="J27" s="42" t="s">
         <v>60</v>
-      </c>
-      <c r="I27" s="4">
-        <v>0</v>
-      </c>
-      <c r="J27" s="42" t="s">
-        <v>62</v>
       </c>
       <c r="K27" s="43"/>
     </row>
@@ -1929,13 +1894,13 @@
       <c r="D28" s="9"/>
       <c r="E28" s="10"/>
       <c r="F28" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="H28" s="3" t="s">
         <v>63</v>
-      </c>
-      <c r="G28" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="H28" s="3" t="s">
-        <v>65</v>
       </c>
       <c r="I28" s="4">
         <v>0</v>
@@ -1949,19 +1914,19 @@
       <c r="D29" s="9"/>
       <c r="E29" s="10"/>
       <c r="F29" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="G29" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="H29" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="I29" s="4">
+        <v>0</v>
+      </c>
+      <c r="J29" s="42" t="s">
         <v>66</v>
-      </c>
-      <c r="G29" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="H29" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="I29" s="4">
-        <v>0</v>
-      </c>
-      <c r="J29" s="42" t="s">
-        <v>68</v>
       </c>
       <c r="K29" s="43"/>
     </row>
@@ -1971,19 +1936,19 @@
       <c r="D30" s="9"/>
       <c r="E30" s="10"/>
       <c r="F30" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H30" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I30" s="4">
         <v>0</v>
       </c>
       <c r="J30" s="42" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="K30" s="43"/>
     </row>
@@ -1993,13 +1958,13 @@
       <c r="D31" s="9"/>
       <c r="E31" s="10"/>
       <c r="F31" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="G31" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="H31" s="3" t="s">
         <v>71</v>
-      </c>
-      <c r="G31" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="H31" s="3" t="s">
-        <v>73</v>
       </c>
       <c r="I31" s="4">
         <v>0</v>
@@ -2013,19 +1978,19 @@
       <c r="D32" s="9"/>
       <c r="E32" s="10"/>
       <c r="F32" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="G32" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="H32" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="I32" s="4">
+        <v>0</v>
+      </c>
+      <c r="J32" s="42" t="s">
         <v>74</v>
-      </c>
-      <c r="G32" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="H32" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="I32" s="4">
-        <v>0</v>
-      </c>
-      <c r="J32" s="42" t="s">
-        <v>76</v>
       </c>
       <c r="K32" s="43"/>
     </row>
@@ -2035,28 +2000,28 @@
       <c r="D33" s="11"/>
       <c r="E33" s="12"/>
       <c r="F33" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H33" s="3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="I33" s="4">
         <v>0</v>
       </c>
       <c r="J33" s="42" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="K33" s="43"/>
     </row>
     <row r="34" spans="2:11">
       <c r="B34" s="31" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C34" s="13" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D34" s="13"/>
       <c r="E34" s="14"/>
@@ -2064,10 +2029,10 @@
         <v>12</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="H34" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="I34" s="4">
         <v>0</v>
@@ -2084,16 +2049,16 @@
         <v>16</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>17</v>
+        <v>80</v>
       </c>
       <c r="H35" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="I35" s="4">
         <v>0</v>
       </c>
       <c r="J35" s="42" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="K35" s="43"/>
     </row>
@@ -2103,17 +2068,17 @@
       <c r="D36" s="9"/>
       <c r="E36" s="10"/>
       <c r="F36" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="H36" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="I36" s="4"/>
       <c r="J36" s="42" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K36" s="43"/>
     </row>
@@ -2123,13 +2088,13 @@
       <c r="D37" s="9"/>
       <c r="E37" s="10"/>
       <c r="F37" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G37" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="H37" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I37" s="4">
         <v>0</v>
@@ -2143,19 +2108,19 @@
       <c r="D38" s="9"/>
       <c r="E38" s="10"/>
       <c r="F38" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="H38" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I38" s="4">
         <v>0</v>
       </c>
       <c r="J38" s="42" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="K38" s="43"/>
     </row>
@@ -2165,17 +2130,17 @@
       <c r="D39" s="9"/>
       <c r="E39" s="10"/>
       <c r="F39" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G39" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H39" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="I39" s="4"/>
       <c r="J39" s="42" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="K39" s="43"/>
     </row>
@@ -2185,13 +2150,13 @@
       <c r="D40" s="9"/>
       <c r="E40" s="10"/>
       <c r="F40" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="G40" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="G40" s="3" t="s">
+      <c r="H40" s="3" t="s">
         <v>87</v>
-      </c>
-      <c r="H40" s="3" t="s">
-        <v>88</v>
       </c>
       <c r="I40" s="4">
         <v>0</v>
@@ -2205,13 +2170,13 @@
       <c r="D41" s="9"/>
       <c r="E41" s="10"/>
       <c r="F41" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="G41" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="G41" s="3" t="s">
+      <c r="H41" s="3" t="s">
         <v>90</v>
-      </c>
-      <c r="H41" s="3" t="s">
-        <v>91</v>
       </c>
       <c r="I41" s="4">
         <v>0</v>
@@ -2225,13 +2190,13 @@
       <c r="D42" s="9"/>
       <c r="E42" s="10"/>
       <c r="F42" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="G42" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="G42" s="3" t="s">
+      <c r="H42" s="3" t="s">
         <v>93</v>
-      </c>
-      <c r="H42" s="3" t="s">
-        <v>94</v>
       </c>
       <c r="I42" s="4">
         <v>0</v>
@@ -2245,13 +2210,13 @@
       <c r="D43" s="11"/>
       <c r="E43" s="12"/>
       <c r="F43" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="G43" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="G43" s="3" t="s">
+      <c r="H43" s="3" t="s">
         <v>96</v>
-      </c>
-      <c r="H43" s="3" t="s">
-        <v>97</v>
       </c>
       <c r="I43" s="4">
         <v>0</v>
@@ -2261,10 +2226,10 @@
     </row>
     <row r="44" spans="2:11">
       <c r="B44" s="29" t="s">
+        <v>97</v>
+      </c>
+      <c r="C44" s="9" t="s">
         <v>98</v>
-      </c>
-      <c r="C44" s="9" t="s">
-        <v>99</v>
       </c>
       <c r="D44" s="9"/>
       <c r="E44" s="10"/>
@@ -2272,10 +2237,10 @@
         <v>12</v>
       </c>
       <c r="G44" s="3" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="H44" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="I44" s="4">
         <v>0</v>
@@ -2292,10 +2257,10 @@
         <v>16</v>
       </c>
       <c r="G45" s="3" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="H45" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="I45" s="4">
         <v>0</v>
@@ -2309,13 +2274,13 @@
       <c r="D46" s="9"/>
       <c r="E46" s="10"/>
       <c r="F46" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G46" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="H46" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I46" s="4">
         <v>0</v>
@@ -2329,13 +2294,13 @@
       <c r="D47" s="17"/>
       <c r="E47" s="18"/>
       <c r="F47" s="19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G47" s="19" t="s">
-        <v>103</v>
+        <v>86</v>
       </c>
       <c r="H47" s="19" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="I47" s="20">
         <v>0</v>
@@ -2345,10 +2310,10 @@
     </row>
     <row r="48" spans="2:11">
       <c r="B48" s="33" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C48" s="21" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D48" s="21"/>
       <c r="E48" s="22"/>
@@ -2356,10 +2321,10 @@
         <v>12</v>
       </c>
       <c r="G48" s="23" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="H48" s="23" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="I48" s="24">
         <v>0</v>
@@ -2373,13 +2338,13 @@
       <c r="D49" s="9"/>
       <c r="E49" s="10"/>
       <c r="F49" s="12" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="G49" s="12" t="s">
-        <v>109</v>
+        <v>31</v>
       </c>
       <c r="H49" s="12" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="I49" s="11">
         <v>0</v>
@@ -2393,13 +2358,13 @@
       <c r="D50" s="9"/>
       <c r="E50" s="10"/>
       <c r="F50" s="12" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="G50" s="12" t="s">
-        <v>112</v>
+        <v>42</v>
       </c>
       <c r="H50" s="12" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="I50" s="11">
         <v>0</v>
@@ -2413,13 +2378,13 @@
       <c r="D51" s="9"/>
       <c r="E51" s="10"/>
       <c r="F51" s="3" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="G51" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H51" s="3" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="I51" s="4">
         <v>0</v>
@@ -2433,13 +2398,13 @@
       <c r="D52" s="9"/>
       <c r="E52" s="10"/>
       <c r="F52" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G52" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H52" s="3" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="I52" s="4">
         <v>0</v>
@@ -2453,13 +2418,13 @@
       <c r="D53" s="9"/>
       <c r="E53" s="10"/>
       <c r="F53" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="G53" s="3" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="H53" s="3" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="I53" s="4">
         <v>0</v>
@@ -2469,20 +2434,20 @@
     </row>
     <row r="54" spans="2:11">
       <c r="B54" s="31" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="C54" s="13" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="D54" s="13" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="E54" s="14"/>
       <c r="F54" s="3" t="s">
         <v>12</v>
       </c>
       <c r="G54" s="3" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="H54" s="3" t="s">
         <v>14</v>
@@ -2502,13 +2467,13 @@
         <v>16</v>
       </c>
       <c r="G55" s="3" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="H55" s="3" t="s">
         <v>14</v>
       </c>
       <c r="I55" s="4" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="J55" s="42"/>
       <c r="K55" s="43"/>
@@ -2519,38 +2484,38 @@
       <c r="D56" s="11"/>
       <c r="E56" s="12"/>
       <c r="F56" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G56" s="3" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="H56" s="3" t="s">
         <v>14</v>
       </c>
       <c r="I56" s="4" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="J56" s="42"/>
       <c r="K56" s="43"/>
     </row>
     <row r="57" spans="2:11" ht="93.75">
       <c r="B57" s="31" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="C57" s="13" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="D57" s="13" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="E57" s="15" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="F57" s="3" t="s">
         <v>12</v>
       </c>
       <c r="G57" s="3" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="H57" s="3" t="s">
         <v>14</v>
@@ -2570,7 +2535,7 @@
         <v>16</v>
       </c>
       <c r="G58" s="3" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="H58" s="3" t="s">
         <v>14</v>
@@ -2583,20 +2548,20 @@
     </row>
     <row r="59" spans="2:11" ht="56.25">
       <c r="B59" s="34" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="D59" s="4"/>
       <c r="E59" s="16" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="F59" s="3" t="s">
         <v>12</v>
       </c>
       <c r="G59" s="3" t="s">
-        <v>30</v>
+        <v>131</v>
       </c>
       <c r="H59" s="3" t="s">
         <v>14</v>
@@ -2609,20 +2574,20 @@
     </row>
     <row r="60" spans="2:11" ht="56.25">
       <c r="B60" s="34" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="D60" s="4"/>
       <c r="E60" s="16" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="F60" s="3" t="s">
         <v>12</v>
       </c>
       <c r="G60" s="3" t="s">
-        <v>30</v>
+        <v>131</v>
       </c>
       <c r="H60" s="3" t="s">
         <v>14</v>
@@ -2635,16 +2600,16 @@
     </row>
     <row r="61" spans="2:11">
       <c r="B61" s="35" t="s">
+        <v>134</v>
+      </c>
+      <c r="C61" s="36" t="s">
+        <v>135</v>
+      </c>
+      <c r="D61" s="36" t="s">
+        <v>136</v>
+      </c>
+      <c r="E61" s="37" t="s">
         <v>137</v>
-      </c>
-      <c r="C61" s="36" t="s">
-        <v>138</v>
-      </c>
-      <c r="D61" s="36" t="s">
-        <v>139</v>
-      </c>
-      <c r="E61" s="37" t="s">
-        <v>140</v>
       </c>
       <c r="F61" s="37"/>
       <c r="G61" s="37"/>

</xml_diff>

<commit_message>
add 'reserved' register type (refs: rggen/rggen#72)
</commit_message>
<xml_diff>
--- a/block_0.xlsx
+++ b/block_0.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23822"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B738F93D-E31D-4967-AA03-32B92FB6B062}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A7ED93E1-3BBC-4C98-962C-360EDA37A395}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="141">
   <si>
     <t>block name</t>
     <phoneticPr fontId="1"/>
@@ -506,6 +506,15 @@
   </si>
   <si>
     <t>register_13</t>
+  </si>
+  <si>
+    <t>0x60</t>
+  </si>
+  <si>
+    <t>reserved</t>
+  </si>
+  <si>
+    <t>register_14</t>
   </si>
   <si>
     <t>0x80</t>
@@ -548,7 +557,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="33">
+  <borders count="35">
     <border>
       <left/>
       <right/>
@@ -1006,11 +1015,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
@@ -1064,6 +1099,8 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
@@ -1344,10 +1381,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:K61"/>
+  <dimension ref="B1:K62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="G61" sqref="G61"/>
+    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
+      <selection activeCell="K62" sqref="K62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
@@ -2599,24 +2636,42 @@
       <c r="K60" s="43"/>
     </row>
     <row r="61" spans="2:11">
-      <c r="B61" s="35" t="s">
+      <c r="B61" s="31" t="s">
         <v>134</v>
       </c>
-      <c r="C61" s="36" t="s">
+      <c r="C61" s="13" t="s">
         <v>135</v>
       </c>
-      <c r="D61" s="36" t="s">
+      <c r="D61" s="13"/>
+      <c r="E61" s="15" t="s">
         <v>136</v>
       </c>
-      <c r="E61" s="37" t="s">
+      <c r="F61" s="14"/>
+      <c r="G61" s="14"/>
+      <c r="H61" s="14"/>
+      <c r="I61" s="13"/>
+      <c r="J61" s="49"/>
+      <c r="K61" s="50"/>
+    </row>
+    <row r="62" spans="2:11">
+      <c r="B62" s="35" t="s">
         <v>137</v>
       </c>
-      <c r="F61" s="37"/>
-      <c r="G61" s="37"/>
-      <c r="H61" s="37"/>
-      <c r="I61" s="36"/>
-      <c r="J61" s="47"/>
-      <c r="K61" s="48"/>
+      <c r="C62" s="36" t="s">
+        <v>138</v>
+      </c>
+      <c r="D62" s="36" t="s">
+        <v>139</v>
+      </c>
+      <c r="E62" s="37" t="s">
+        <v>140</v>
+      </c>
+      <c r="F62" s="37"/>
+      <c r="G62" s="37"/>
+      <c r="H62" s="37"/>
+      <c r="I62" s="36"/>
+      <c r="J62" s="47"/>
+      <c r="K62" s="48"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>

</xml_diff>

<commit_message>
add samples due to adding bit field types with trigger signal
(refs: rggen/rggen#84)
</commit_message>
<xml_diff>
--- a/block_0.xlsx
+++ b/block_0.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24916"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A0D56F00-2FF8-4245-9EBC-D59D5B1EA094}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="29" documentId="8_{A0D56F00-2FF8-4245-9EBC-D59D5B1EA094}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{79FE6EF4-014E-4108-8F9D-AAFC4137DCFE}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="149">
   <si>
     <t>block name</t>
     <phoneticPr fontId="1"/>
@@ -444,6 +444,27 @@
     <t>register_9</t>
   </si>
   <si>
+    <t>0x28</t>
+  </si>
+  <si>
+    <t>bit_field_0</t>
+  </si>
+  <si>
+    <t>rwtrg</t>
+  </si>
+  <si>
+    <t>rotrg</t>
+  </si>
+  <si>
+    <t>wotrg</t>
+  </si>
+  <si>
+    <t>rowotrg</t>
+  </si>
+  <si>
+    <t>register_10</t>
+  </si>
+  <si>
     <t>0x30</t>
   </si>
   <si>
@@ -468,7 +489,7 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>register_10</t>
+    <t>register_11</t>
   </si>
   <si>
     <t>0x50</t>
@@ -491,7 +512,7 @@
     <t>8:8:4:16</t>
   </si>
   <si>
-    <t>register_11</t>
+    <t>register_12</t>
   </si>
   <si>
     <t>indirect:
@@ -502,13 +523,13 @@
     <t>1:0</t>
   </si>
   <si>
-    <t>register_12</t>
+    <t>register_13</t>
   </si>
   <si>
     <t>0x54</t>
   </si>
   <si>
-    <t>register_13</t>
+    <t>register_14</t>
   </si>
   <si>
     <t>0x60</t>
@@ -517,7 +538,7 @@
     <t>reserved</t>
   </si>
   <si>
-    <t>register_14</t>
+    <t>register_15</t>
   </si>
   <si>
     <t>0x80</t>
@@ -1383,10 +1404,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:K63"/>
+  <dimension ref="B1:K67"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="F59" sqref="F59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
@@ -2491,24 +2512,22 @@
       <c r="K54" s="42"/>
     </row>
     <row r="55" spans="2:11">
-      <c r="B55" s="30" t="s">
+      <c r="B55" s="28" t="s">
         <v>116</v>
       </c>
-      <c r="C55" s="12" t="s">
+      <c r="C55" s="8" t="s">
         <v>117</v>
       </c>
-      <c r="D55" s="12" t="s">
+      <c r="D55" s="8"/>
+      <c r="E55" s="9"/>
+      <c r="F55" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="E55" s="13"/>
-      <c r="F55" s="2" t="s">
-        <v>12</v>
-      </c>
       <c r="G55" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="H55" s="2" t="s">
         <v>119</v>
-      </c>
-      <c r="H55" s="2" t="s">
-        <v>14</v>
       </c>
       <c r="I55" s="3">
         <v>0</v>
@@ -2522,61 +2541,51 @@
       <c r="D56" s="8"/>
       <c r="E56" s="9"/>
       <c r="F56" s="2" t="s">
-        <v>16</v>
+        <v>107</v>
       </c>
       <c r="G56" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="H56" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="H56" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I56" s="3" t="s">
-        <v>121</v>
-      </c>
+      <c r="I56" s="3"/>
       <c r="J56" s="41"/>
       <c r="K56" s="42"/>
     </row>
     <row r="57" spans="2:11">
-      <c r="B57" s="29"/>
-      <c r="C57" s="10"/>
-      <c r="D57" s="10"/>
-      <c r="E57" s="11"/>
+      <c r="B57" s="28"/>
+      <c r="C57" s="8"/>
+      <c r="D57" s="8"/>
+      <c r="E57" s="9"/>
       <c r="F57" s="2" t="s">
-        <v>17</v>
+        <v>109</v>
       </c>
       <c r="G57" s="2" t="s">
-        <v>122</v>
+        <v>59</v>
       </c>
       <c r="H57" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I57" s="3" t="s">
-        <v>123</v>
+        <v>121</v>
+      </c>
+      <c r="I57" s="3">
+        <v>0</v>
       </c>
       <c r="J57" s="41"/>
       <c r="K57" s="42"/>
     </row>
-    <row r="58" spans="2:11" ht="93.75">
-      <c r="B58" s="30" t="s">
-        <v>124</v>
-      </c>
-      <c r="C58" s="12" t="s">
-        <v>125</v>
-      </c>
-      <c r="D58" s="12" t="s">
-        <v>126</v>
-      </c>
-      <c r="E58" s="14" t="s">
-        <v>127</v>
-      </c>
+    <row r="58" spans="2:11">
+      <c r="B58" s="28"/>
+      <c r="C58" s="8"/>
+      <c r="D58" s="8"/>
+      <c r="E58" s="9"/>
       <c r="F58" s="2" t="s">
-        <v>12</v>
+        <v>111</v>
       </c>
       <c r="G58" s="2" t="s">
-        <v>128</v>
+        <v>61</v>
       </c>
       <c r="H58" s="2" t="s">
-        <v>14</v>
+        <v>122</v>
       </c>
       <c r="I58" s="3">
         <v>0</v>
@@ -2585,15 +2594,21 @@
       <c r="K58" s="42"/>
     </row>
     <row r="59" spans="2:11">
-      <c r="B59" s="29"/>
-      <c r="C59" s="10"/>
-      <c r="D59" s="10"/>
-      <c r="E59" s="11"/>
+      <c r="B59" s="30" t="s">
+        <v>123</v>
+      </c>
+      <c r="C59" s="12" t="s">
+        <v>124</v>
+      </c>
+      <c r="D59" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="E59" s="13"/>
       <c r="F59" s="2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="G59" s="2" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="H59" s="2" t="s">
         <v>14</v>
@@ -2604,95 +2619,183 @@
       <c r="J59" s="41"/>
       <c r="K59" s="42"/>
     </row>
-    <row r="60" spans="2:11" ht="56.25">
-      <c r="B60" s="33" t="s">
-        <v>130</v>
-      </c>
-      <c r="C60" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="D60" s="3"/>
-      <c r="E60" s="15" t="s">
-        <v>131</v>
-      </c>
+    <row r="60" spans="2:11">
+      <c r="B60" s="28"/>
+      <c r="C60" s="8"/>
+      <c r="D60" s="8"/>
+      <c r="E60" s="9"/>
       <c r="F60" s="2" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="G60" s="2" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="H60" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="I60" s="3">
-        <v>0</v>
+      <c r="I60" s="3" t="s">
+        <v>128</v>
       </c>
       <c r="J60" s="41"/>
       <c r="K60" s="42"/>
     </row>
-    <row r="61" spans="2:11" ht="56.25">
-      <c r="B61" s="33" t="s">
-        <v>133</v>
-      </c>
-      <c r="C61" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="D61" s="3"/>
-      <c r="E61" s="15" t="s">
-        <v>131</v>
-      </c>
+    <row r="61" spans="2:11">
+      <c r="B61" s="29"/>
+      <c r="C61" s="10"/>
+      <c r="D61" s="10"/>
+      <c r="E61" s="11"/>
       <c r="F61" s="2" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="G61" s="2" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="H61" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="I61" s="3">
-        <v>0</v>
+      <c r="I61" s="3" t="s">
+        <v>130</v>
       </c>
       <c r="J61" s="41"/>
       <c r="K61" s="42"/>
     </row>
-    <row r="62" spans="2:11">
+    <row r="62" spans="2:11" ht="93.75">
       <c r="B62" s="30" t="s">
+        <v>131</v>
+      </c>
+      <c r="C62" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="D62" s="12" t="s">
+        <v>133</v>
+      </c>
+      <c r="E62" s="14" t="s">
+        <v>134</v>
+      </c>
+      <c r="F62" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G62" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="C62" s="12" t="s">
+      <c r="H62" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I62" s="3">
+        <v>0</v>
+      </c>
+      <c r="J62" s="41"/>
+      <c r="K62" s="42"/>
+    </row>
+    <row r="63" spans="2:11">
+      <c r="B63" s="29"/>
+      <c r="C63" s="10"/>
+      <c r="D63" s="10"/>
+      <c r="E63" s="11"/>
+      <c r="F63" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G63" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="D62" s="12"/>
-      <c r="E62" s="14" t="s">
+      <c r="H63" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I63" s="3">
+        <v>0</v>
+      </c>
+      <c r="J63" s="41"/>
+      <c r="K63" s="42"/>
+    </row>
+    <row r="64" spans="2:11" ht="56.25">
+      <c r="B64" s="33" t="s">
         <v>137</v>
       </c>
-      <c r="F62" s="13"/>
-      <c r="G62" s="13"/>
-      <c r="H62" s="13"/>
-      <c r="I62" s="12"/>
-      <c r="J62" s="48"/>
-      <c r="K62" s="49"/>
-    </row>
-    <row r="63" spans="2:11">
-      <c r="B63" s="34" t="s">
+      <c r="C64" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="D64" s="3"/>
+      <c r="E64" s="15" t="s">
         <v>138</v>
       </c>
-      <c r="C63" s="35" t="s">
+      <c r="F64" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G64" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="D63" s="35" t="s">
+      <c r="H64" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I64" s="3">
+        <v>0</v>
+      </c>
+      <c r="J64" s="41"/>
+      <c r="K64" s="42"/>
+    </row>
+    <row r="65" spans="2:11" ht="56.25">
+      <c r="B65" s="33" t="s">
         <v>140</v>
       </c>
-      <c r="E63" s="36" t="s">
+      <c r="C65" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="F63" s="36"/>
-      <c r="G63" s="36"/>
-      <c r="H63" s="36"/>
-      <c r="I63" s="35"/>
-      <c r="J63" s="46"/>
-      <c r="K63" s="47"/>
+      <c r="D65" s="3"/>
+      <c r="E65" s="15" t="s">
+        <v>138</v>
+      </c>
+      <c r="F65" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G65" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="H65" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I65" s="3">
+        <v>0</v>
+      </c>
+      <c r="J65" s="41"/>
+      <c r="K65" s="42"/>
+    </row>
+    <row r="66" spans="2:11">
+      <c r="B66" s="30" t="s">
+        <v>142</v>
+      </c>
+      <c r="C66" s="12" t="s">
+        <v>143</v>
+      </c>
+      <c r="D66" s="12"/>
+      <c r="E66" s="14" t="s">
+        <v>144</v>
+      </c>
+      <c r="F66" s="13"/>
+      <c r="G66" s="13"/>
+      <c r="H66" s="13"/>
+      <c r="I66" s="12"/>
+      <c r="J66" s="48"/>
+      <c r="K66" s="49"/>
+    </row>
+    <row r="67" spans="2:11">
+      <c r="B67" s="34" t="s">
+        <v>145</v>
+      </c>
+      <c r="C67" s="35" t="s">
+        <v>146</v>
+      </c>
+      <c r="D67" s="35" t="s">
+        <v>147</v>
+      </c>
+      <c r="E67" s="36" t="s">
+        <v>148</v>
+      </c>
+      <c r="F67" s="36"/>
+      <c r="G67" s="36"/>
+      <c r="H67" s="36"/>
+      <c r="I67" s="35"/>
+      <c r="J67" s="46"/>
+      <c r="K67" s="47"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>

</xml_diff>

<commit_message>
update samples because of rggen/rggen#107
</commit_message>
<xml_diff>
--- a/block_0.xlsx
+++ b/block_0.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25425"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="29" documentId="8_{A0D56F00-2FF8-4245-9EBC-D59D5B1EA094}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{79FE6EF4-014E-4108-8F9D-AAFC4137DCFE}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{BC9B0434-2B73-48F8-8004-154DEDB66167}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,6 +22,7 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="148">
   <si>
     <t>block name</t>
     <phoneticPr fontId="1"/>
@@ -517,28 +518,24 @@
   <si>
     <t>indirect:
 register_0.bit_field_2:1</t>
-    <phoneticPr fontId="1"/>
   </si>
   <si>
     <t>1:0</t>
   </si>
   <si>
+    <t>1:32</t>
+  </si>
+  <si>
     <t>register_13</t>
   </si>
   <si>
-    <t>0x54</t>
+    <t>0x60</t>
+  </si>
+  <si>
+    <t>reserved</t>
   </si>
   <si>
     <t>register_14</t>
-  </si>
-  <si>
-    <t>0x60</t>
-  </si>
-  <si>
-    <t>reserved</t>
-  </si>
-  <si>
-    <t>register_15</t>
   </si>
   <si>
     <t>0x80</t>
@@ -581,7 +578,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="35">
+  <borders count="34">
     <border>
       <left/>
       <right/>
@@ -841,21 +838,6 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
@@ -1069,7 +1051,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -1085,9 +1067,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
@@ -1108,22 +1087,24 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
@@ -1406,8 +1387,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:K67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="F59" sqref="F59"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="E65" sqref="B65:E66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
@@ -1440,39 +1421,39 @@
       </c>
     </row>
     <row r="4" spans="2:11">
-      <c r="B4" s="24" t="s">
+      <c r="B4" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="25" t="s">
+      <c r="C4" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="25" t="s">
+      <c r="D4" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="26" t="s">
+      <c r="E4" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="26" t="s">
+      <c r="F4" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="G4" s="26" t="s">
+      <c r="G4" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="H4" s="26" t="s">
+      <c r="H4" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="25" t="s">
+      <c r="I4" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="J4" s="37" t="s">
+      <c r="J4" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="K4" s="38" t="s">
+      <c r="K4" s="36" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="5" spans="2:11">
-      <c r="B5" s="27" t="s">
+      <c r="B5" s="26" t="s">
         <v>11</v>
       </c>
       <c r="C5" s="6"/>
@@ -1490,13 +1471,13 @@
       <c r="I5" s="4">
         <v>0</v>
       </c>
-      <c r="J5" s="39"/>
-      <c r="K5" s="40" t="s">
+      <c r="J5" s="37"/>
+      <c r="K5" s="38" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="6" spans="2:11">
-      <c r="B6" s="28"/>
+      <c r="B6" s="27"/>
       <c r="C6" s="8"/>
       <c r="D6" s="8"/>
       <c r="E6" s="9"/>
@@ -1512,11 +1493,11 @@
       <c r="I6" s="3">
         <v>0</v>
       </c>
-      <c r="J6" s="41"/>
-      <c r="K6" s="42"/>
+      <c r="J6" s="39"/>
+      <c r="K6" s="40"/>
     </row>
     <row r="7" spans="2:11">
-      <c r="B7" s="28"/>
+      <c r="B7" s="27"/>
       <c r="C7" s="8"/>
       <c r="D7" s="8"/>
       <c r="E7" s="9"/>
@@ -1532,11 +1513,11 @@
       <c r="I7" s="3">
         <v>0</v>
       </c>
-      <c r="J7" s="41"/>
-      <c r="K7" s="42"/>
+      <c r="J7" s="39"/>
+      <c r="K7" s="40"/>
     </row>
     <row r="8" spans="2:11">
-      <c r="B8" s="28"/>
+      <c r="B8" s="27"/>
       <c r="C8" s="8"/>
       <c r="D8" s="8"/>
       <c r="E8" s="9"/>
@@ -1552,11 +1533,11 @@
       <c r="I8" s="3">
         <v>0</v>
       </c>
-      <c r="J8" s="41"/>
-      <c r="K8" s="42"/>
+      <c r="J8" s="39"/>
+      <c r="K8" s="40"/>
     </row>
     <row r="9" spans="2:11">
-      <c r="B9" s="28"/>
+      <c r="B9" s="27"/>
       <c r="C9" s="8"/>
       <c r="D9" s="8"/>
       <c r="E9" s="9"/>
@@ -1572,11 +1553,11 @@
       <c r="I9" s="3">
         <v>0</v>
       </c>
-      <c r="J9" s="41"/>
-      <c r="K9" s="42"/>
+      <c r="J9" s="39"/>
+      <c r="K9" s="40"/>
     </row>
     <row r="10" spans="2:11">
-      <c r="B10" s="28"/>
+      <c r="B10" s="27"/>
       <c r="C10" s="8"/>
       <c r="D10" s="8"/>
       <c r="E10" s="9"/>
@@ -1592,11 +1573,11 @@
       <c r="I10" s="3">
         <v>0</v>
       </c>
-      <c r="J10" s="41"/>
-      <c r="K10" s="42"/>
+      <c r="J10" s="39"/>
+      <c r="K10" s="40"/>
     </row>
     <row r="11" spans="2:11">
-      <c r="B11" s="29"/>
+      <c r="B11" s="28"/>
       <c r="C11" s="10"/>
       <c r="D11" s="10"/>
       <c r="E11" s="11"/>
@@ -1612,11 +1593,11 @@
       <c r="I11" s="3">
         <v>0</v>
       </c>
-      <c r="J11" s="41"/>
-      <c r="K11" s="42"/>
+      <c r="J11" s="39"/>
+      <c r="K11" s="40"/>
     </row>
     <row r="12" spans="2:11">
-      <c r="B12" s="30" t="s">
+      <c r="B12" s="29" t="s">
         <v>28</v>
       </c>
       <c r="C12" s="12"/>
@@ -1632,11 +1613,11 @@
       <c r="I12" s="3">
         <v>0</v>
       </c>
-      <c r="J12" s="41"/>
-      <c r="K12" s="42"/>
+      <c r="J12" s="39"/>
+      <c r="K12" s="40"/>
     </row>
     <row r="13" spans="2:11">
-      <c r="B13" s="30" t="s">
+      <c r="B13" s="29" t="s">
         <v>29</v>
       </c>
       <c r="C13" s="12" t="s">
@@ -1654,11 +1635,11 @@
         <v>32</v>
       </c>
       <c r="I13" s="3"/>
-      <c r="J13" s="41"/>
-      <c r="K13" s="42"/>
+      <c r="J13" s="39"/>
+      <c r="K13" s="40"/>
     </row>
     <row r="14" spans="2:11">
-      <c r="B14" s="28"/>
+      <c r="B14" s="27"/>
       <c r="C14" s="8"/>
       <c r="D14" s="8"/>
       <c r="E14" s="9"/>
@@ -1672,11 +1653,11 @@
         <v>32</v>
       </c>
       <c r="I14" s="3"/>
-      <c r="J14" s="41"/>
-      <c r="K14" s="42"/>
+      <c r="J14" s="39"/>
+      <c r="K14" s="40"/>
     </row>
     <row r="15" spans="2:11">
-      <c r="B15" s="28"/>
+      <c r="B15" s="27"/>
       <c r="C15" s="8"/>
       <c r="D15" s="8"/>
       <c r="E15" s="9"/>
@@ -1692,11 +1673,11 @@
       <c r="I15" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="J15" s="41"/>
-      <c r="K15" s="42"/>
+      <c r="J15" s="39"/>
+      <c r="K15" s="40"/>
     </row>
     <row r="16" spans="2:11">
-      <c r="B16" s="29"/>
+      <c r="B16" s="28"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="11"/>
@@ -1710,11 +1691,11 @@
         <v>38</v>
       </c>
       <c r="I16" s="3"/>
-      <c r="J16" s="41"/>
-      <c r="K16" s="42"/>
+      <c r="J16" s="39"/>
+      <c r="K16" s="40"/>
     </row>
     <row r="17" spans="2:11">
-      <c r="B17" s="30" t="s">
+      <c r="B17" s="29" t="s">
         <v>39</v>
       </c>
       <c r="C17" s="12" t="s">
@@ -1734,11 +1715,11 @@
       <c r="I17" s="3">
         <v>0</v>
       </c>
-      <c r="J17" s="41"/>
-      <c r="K17" s="42"/>
+      <c r="J17" s="39"/>
+      <c r="K17" s="40"/>
     </row>
     <row r="18" spans="2:11">
-      <c r="B18" s="28"/>
+      <c r="B18" s="27"/>
       <c r="C18" s="8"/>
       <c r="D18" s="8"/>
       <c r="E18" s="9"/>
@@ -1754,11 +1735,11 @@
       <c r="I18" s="3">
         <v>0</v>
       </c>
-      <c r="J18" s="41"/>
-      <c r="K18" s="42"/>
+      <c r="J18" s="39"/>
+      <c r="K18" s="40"/>
     </row>
     <row r="19" spans="2:11">
-      <c r="B19" s="28"/>
+      <c r="B19" s="27"/>
       <c r="C19" s="8"/>
       <c r="D19" s="8"/>
       <c r="E19" s="9"/>
@@ -1772,11 +1753,11 @@
         <v>43</v>
       </c>
       <c r="I19" s="3"/>
-      <c r="J19" s="41"/>
-      <c r="K19" s="42"/>
+      <c r="J19" s="39"/>
+      <c r="K19" s="40"/>
     </row>
     <row r="20" spans="2:11">
-      <c r="B20" s="28"/>
+      <c r="B20" s="27"/>
       <c r="C20" s="8"/>
       <c r="D20" s="8"/>
       <c r="E20" s="9"/>
@@ -1790,11 +1771,11 @@
         <v>45</v>
       </c>
       <c r="I20" s="3"/>
-      <c r="J20" s="41"/>
-      <c r="K20" s="42"/>
+      <c r="J20" s="39"/>
+      <c r="K20" s="40"/>
     </row>
     <row r="21" spans="2:11">
-      <c r="B21" s="30" t="s">
+      <c r="B21" s="29" t="s">
         <v>46</v>
       </c>
       <c r="C21" s="12" t="s">
@@ -1814,11 +1795,11 @@
       <c r="I21" s="3">
         <v>0</v>
       </c>
-      <c r="J21" s="41"/>
-      <c r="K21" s="42"/>
+      <c r="J21" s="39"/>
+      <c r="K21" s="40"/>
     </row>
     <row r="22" spans="2:11">
-      <c r="B22" s="28"/>
+      <c r="B22" s="27"/>
       <c r="C22" s="8"/>
       <c r="D22" s="8"/>
       <c r="E22" s="9"/>
@@ -1834,13 +1815,13 @@
       <c r="I22" s="3">
         <v>0</v>
       </c>
-      <c r="J22" s="41" t="s">
+      <c r="J22" s="39" t="s">
         <v>49</v>
       </c>
-      <c r="K22" s="42"/>
+      <c r="K22" s="40"/>
     </row>
     <row r="23" spans="2:11">
-      <c r="B23" s="28"/>
+      <c r="B23" s="27"/>
       <c r="C23" s="8"/>
       <c r="D23" s="8"/>
       <c r="E23" s="9"/>
@@ -1854,13 +1835,13 @@
         <v>32</v>
       </c>
       <c r="I23" s="3"/>
-      <c r="J23" s="41" t="s">
+      <c r="J23" s="39" t="s">
         <v>51</v>
       </c>
-      <c r="K23" s="42"/>
+      <c r="K23" s="40"/>
     </row>
     <row r="24" spans="2:11">
-      <c r="B24" s="29"/>
+      <c r="B24" s="28"/>
       <c r="C24" s="10"/>
       <c r="D24" s="10"/>
       <c r="E24" s="11"/>
@@ -1876,11 +1857,11 @@
       <c r="I24" s="3">
         <v>0</v>
       </c>
-      <c r="J24" s="41"/>
-      <c r="K24" s="42"/>
+      <c r="J24" s="39"/>
+      <c r="K24" s="40"/>
     </row>
     <row r="25" spans="2:11">
-      <c r="B25" s="30" t="s">
+      <c r="B25" s="29" t="s">
         <v>53</v>
       </c>
       <c r="C25" s="12" t="s">
@@ -1900,11 +1881,11 @@
       <c r="I25" s="3">
         <v>0</v>
       </c>
-      <c r="J25" s="41"/>
-      <c r="K25" s="42"/>
+      <c r="J25" s="39"/>
+      <c r="K25" s="40"/>
     </row>
     <row r="26" spans="2:11">
-      <c r="B26" s="28"/>
+      <c r="B26" s="27"/>
       <c r="C26" s="8"/>
       <c r="D26" s="8"/>
       <c r="E26" s="9"/>
@@ -1920,13 +1901,13 @@
       <c r="I26" s="3">
         <v>0</v>
       </c>
-      <c r="J26" s="41" t="s">
+      <c r="J26" s="39" t="s">
         <v>58</v>
       </c>
-      <c r="K26" s="42"/>
+      <c r="K26" s="40"/>
     </row>
     <row r="27" spans="2:11">
-      <c r="B27" s="28"/>
+      <c r="B27" s="27"/>
       <c r="C27" s="8"/>
       <c r="D27" s="8"/>
       <c r="E27" s="9"/>
@@ -1942,11 +1923,11 @@
       <c r="I27" s="3">
         <v>0</v>
       </c>
-      <c r="J27" s="41"/>
-      <c r="K27" s="42"/>
+      <c r="J27" s="39"/>
+      <c r="K27" s="40"/>
     </row>
     <row r="28" spans="2:11">
-      <c r="B28" s="28"/>
+      <c r="B28" s="27"/>
       <c r="C28" s="8"/>
       <c r="D28" s="8"/>
       <c r="E28" s="9"/>
@@ -1962,13 +1943,13 @@
       <c r="I28" s="3">
         <v>0</v>
       </c>
-      <c r="J28" s="41" t="s">
+      <c r="J28" s="39" t="s">
         <v>62</v>
       </c>
-      <c r="K28" s="42"/>
+      <c r="K28" s="40"/>
     </row>
     <row r="29" spans="2:11">
-      <c r="B29" s="28"/>
+      <c r="B29" s="27"/>
       <c r="C29" s="8"/>
       <c r="D29" s="8"/>
       <c r="E29" s="9"/>
@@ -1984,11 +1965,11 @@
       <c r="I29" s="3">
         <v>0</v>
       </c>
-      <c r="J29" s="41"/>
-      <c r="K29" s="42"/>
+      <c r="J29" s="39"/>
+      <c r="K29" s="40"/>
     </row>
     <row r="30" spans="2:11">
-      <c r="B30" s="28"/>
+      <c r="B30" s="27"/>
       <c r="C30" s="8"/>
       <c r="D30" s="8"/>
       <c r="E30" s="9"/>
@@ -2004,13 +1985,13 @@
       <c r="I30" s="3">
         <v>0</v>
       </c>
-      <c r="J30" s="41" t="s">
+      <c r="J30" s="39" t="s">
         <v>68</v>
       </c>
-      <c r="K30" s="42"/>
+      <c r="K30" s="40"/>
     </row>
     <row r="31" spans="2:11">
-      <c r="B31" s="28"/>
+      <c r="B31" s="27"/>
       <c r="C31" s="8"/>
       <c r="D31" s="8"/>
       <c r="E31" s="9"/>
@@ -2026,13 +2007,13 @@
       <c r="I31" s="3">
         <v>0</v>
       </c>
-      <c r="J31" s="41" t="s">
+      <c r="J31" s="39" t="s">
         <v>28</v>
       </c>
-      <c r="K31" s="42"/>
+      <c r="K31" s="40"/>
     </row>
     <row r="32" spans="2:11">
-      <c r="B32" s="28"/>
+      <c r="B32" s="27"/>
       <c r="C32" s="8"/>
       <c r="D32" s="8"/>
       <c r="E32" s="9"/>
@@ -2048,11 +2029,11 @@
       <c r="I32" s="3">
         <v>0</v>
       </c>
-      <c r="J32" s="41"/>
-      <c r="K32" s="42"/>
+      <c r="J32" s="39"/>
+      <c r="K32" s="40"/>
     </row>
     <row r="33" spans="2:11">
-      <c r="B33" s="28"/>
+      <c r="B33" s="27"/>
       <c r="C33" s="8"/>
       <c r="D33" s="8"/>
       <c r="E33" s="9"/>
@@ -2068,13 +2049,13 @@
       <c r="I33" s="3">
         <v>0</v>
       </c>
-      <c r="J33" s="41" t="s">
+      <c r="J33" s="39" t="s">
         <v>76</v>
       </c>
-      <c r="K33" s="42"/>
+      <c r="K33" s="40"/>
     </row>
     <row r="34" spans="2:11">
-      <c r="B34" s="29"/>
+      <c r="B34" s="28"/>
       <c r="C34" s="10"/>
       <c r="D34" s="10"/>
       <c r="E34" s="11"/>
@@ -2090,13 +2071,13 @@
       <c r="I34" s="3">
         <v>0</v>
       </c>
-      <c r="J34" s="41" t="s">
+      <c r="J34" s="39" t="s">
         <v>28</v>
       </c>
-      <c r="K34" s="42"/>
+      <c r="K34" s="40"/>
     </row>
     <row r="35" spans="2:11">
-      <c r="B35" s="30" t="s">
+      <c r="B35" s="29" t="s">
         <v>79</v>
       </c>
       <c r="C35" s="12" t="s">
@@ -2116,11 +2097,11 @@
       <c r="I35" s="3">
         <v>0</v>
       </c>
-      <c r="J35" s="41"/>
-      <c r="K35" s="42"/>
+      <c r="J35" s="39"/>
+      <c r="K35" s="40"/>
     </row>
     <row r="36" spans="2:11">
-      <c r="B36" s="28"/>
+      <c r="B36" s="27"/>
       <c r="C36" s="8"/>
       <c r="D36" s="8"/>
       <c r="E36" s="9"/>
@@ -2136,13 +2117,13 @@
       <c r="I36" s="3">
         <v>0</v>
       </c>
-      <c r="J36" s="41" t="s">
+      <c r="J36" s="39" t="s">
         <v>49</v>
       </c>
-      <c r="K36" s="42"/>
+      <c r="K36" s="40"/>
     </row>
     <row r="37" spans="2:11">
-      <c r="B37" s="28"/>
+      <c r="B37" s="27"/>
       <c r="C37" s="8"/>
       <c r="D37" s="8"/>
       <c r="E37" s="9"/>
@@ -2156,13 +2137,13 @@
         <v>32</v>
       </c>
       <c r="I37" s="3"/>
-      <c r="J37" s="41" t="s">
+      <c r="J37" s="39" t="s">
         <v>83</v>
       </c>
-      <c r="K37" s="42"/>
+      <c r="K37" s="40"/>
     </row>
     <row r="38" spans="2:11">
-      <c r="B38" s="28"/>
+      <c r="B38" s="27"/>
       <c r="C38" s="8"/>
       <c r="D38" s="8"/>
       <c r="E38" s="9"/>
@@ -2178,11 +2159,11 @@
       <c r="I38" s="3">
         <v>0</v>
       </c>
-      <c r="J38" s="41"/>
-      <c r="K38" s="42"/>
+      <c r="J38" s="39"/>
+      <c r="K38" s="40"/>
     </row>
     <row r="39" spans="2:11">
-      <c r="B39" s="28"/>
+      <c r="B39" s="27"/>
       <c r="C39" s="8"/>
       <c r="D39" s="8"/>
       <c r="E39" s="9"/>
@@ -2198,13 +2179,13 @@
       <c r="I39" s="3">
         <v>0</v>
       </c>
-      <c r="J39" s="41" t="s">
+      <c r="J39" s="39" t="s">
         <v>49</v>
       </c>
-      <c r="K39" s="42"/>
+      <c r="K39" s="40"/>
     </row>
     <row r="40" spans="2:11">
-      <c r="B40" s="28"/>
+      <c r="B40" s="27"/>
       <c r="C40" s="8"/>
       <c r="D40" s="8"/>
       <c r="E40" s="9"/>
@@ -2218,13 +2199,13 @@
         <v>32</v>
       </c>
       <c r="I40" s="3"/>
-      <c r="J40" s="41" t="s">
+      <c r="J40" s="39" t="s">
         <v>86</v>
       </c>
-      <c r="K40" s="42"/>
+      <c r="K40" s="40"/>
     </row>
     <row r="41" spans="2:11">
-      <c r="B41" s="28"/>
+      <c r="B41" s="27"/>
       <c r="C41" s="8"/>
       <c r="D41" s="8"/>
       <c r="E41" s="9"/>
@@ -2240,11 +2221,11 @@
       <c r="I41" s="3">
         <v>0</v>
       </c>
-      <c r="J41" s="41"/>
-      <c r="K41" s="42"/>
+      <c r="J41" s="39"/>
+      <c r="K41" s="40"/>
     </row>
     <row r="42" spans="2:11">
-      <c r="B42" s="28"/>
+      <c r="B42" s="27"/>
       <c r="C42" s="8"/>
       <c r="D42" s="8"/>
       <c r="E42" s="9"/>
@@ -2260,11 +2241,11 @@
       <c r="I42" s="3">
         <v>0</v>
       </c>
-      <c r="J42" s="41"/>
-      <c r="K42" s="42"/>
+      <c r="J42" s="39"/>
+      <c r="K42" s="40"/>
     </row>
     <row r="43" spans="2:11">
-      <c r="B43" s="28"/>
+      <c r="B43" s="27"/>
       <c r="C43" s="8"/>
       <c r="D43" s="8"/>
       <c r="E43" s="9"/>
@@ -2280,11 +2261,11 @@
       <c r="I43" s="3">
         <v>0</v>
       </c>
-      <c r="J43" s="41"/>
-      <c r="K43" s="42"/>
+      <c r="J43" s="39"/>
+      <c r="K43" s="40"/>
     </row>
     <row r="44" spans="2:11">
-      <c r="B44" s="29"/>
+      <c r="B44" s="28"/>
       <c r="C44" s="10"/>
       <c r="D44" s="10"/>
       <c r="E44" s="11"/>
@@ -2300,11 +2281,11 @@
       <c r="I44" s="3">
         <v>0</v>
       </c>
-      <c r="J44" s="41"/>
-      <c r="K44" s="42"/>
+      <c r="J44" s="39"/>
+      <c r="K44" s="40"/>
     </row>
     <row r="45" spans="2:11">
-      <c r="B45" s="28" t="s">
+      <c r="B45" s="27" t="s">
         <v>98</v>
       </c>
       <c r="C45" s="8" t="s">
@@ -2324,11 +2305,11 @@
       <c r="I45" s="3">
         <v>0</v>
       </c>
-      <c r="J45" s="41"/>
-      <c r="K45" s="42"/>
+      <c r="J45" s="39"/>
+      <c r="K45" s="40"/>
     </row>
     <row r="46" spans="2:11">
-      <c r="B46" s="28"/>
+      <c r="B46" s="27"/>
       <c r="C46" s="8"/>
       <c r="D46" s="8"/>
       <c r="E46" s="9"/>
@@ -2344,11 +2325,11 @@
       <c r="I46" s="3">
         <v>0</v>
       </c>
-      <c r="J46" s="41"/>
-      <c r="K46" s="42"/>
+      <c r="J46" s="39"/>
+      <c r="K46" s="40"/>
     </row>
     <row r="47" spans="2:11">
-      <c r="B47" s="28"/>
+      <c r="B47" s="27"/>
       <c r="C47" s="8"/>
       <c r="D47" s="8"/>
       <c r="E47" s="9"/>
@@ -2364,55 +2345,55 @@
       <c r="I47" s="3">
         <v>0</v>
       </c>
-      <c r="J47" s="41"/>
-      <c r="K47" s="42"/>
+      <c r="J47" s="39"/>
+      <c r="K47" s="40"/>
     </row>
     <row r="48" spans="2:11">
-      <c r="B48" s="31"/>
-      <c r="C48" s="16"/>
-      <c r="D48" s="16"/>
-      <c r="E48" s="17"/>
-      <c r="F48" s="18" t="s">
+      <c r="B48" s="30"/>
+      <c r="C48" s="15"/>
+      <c r="D48" s="15"/>
+      <c r="E48" s="16"/>
+      <c r="F48" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="G48" s="18" t="s">
+      <c r="G48" s="17" t="s">
         <v>87</v>
       </c>
-      <c r="H48" s="18" t="s">
+      <c r="H48" s="17" t="s">
         <v>103</v>
       </c>
-      <c r="I48" s="19">
-        <v>0</v>
-      </c>
-      <c r="J48" s="43"/>
-      <c r="K48" s="42"/>
+      <c r="I48" s="18">
+        <v>0</v>
+      </c>
+      <c r="J48" s="41"/>
+      <c r="K48" s="40"/>
     </row>
     <row r="49" spans="2:11">
-      <c r="B49" s="32" t="s">
+      <c r="B49" s="31" t="s">
         <v>104</v>
       </c>
-      <c r="C49" s="20" t="s">
+      <c r="C49" s="19" t="s">
         <v>105</v>
       </c>
-      <c r="D49" s="20"/>
-      <c r="E49" s="21"/>
-      <c r="F49" s="22" t="s">
+      <c r="D49" s="19"/>
+      <c r="E49" s="20"/>
+      <c r="F49" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="G49" s="22" t="s">
+      <c r="G49" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="H49" s="22" t="s">
+      <c r="H49" s="21" t="s">
         <v>106</v>
       </c>
-      <c r="I49" s="23">
-        <v>0</v>
-      </c>
-      <c r="J49" s="44"/>
-      <c r="K49" s="42"/>
+      <c r="I49" s="22">
+        <v>0</v>
+      </c>
+      <c r="J49" s="42"/>
+      <c r="K49" s="40"/>
     </row>
     <row r="50" spans="2:11">
-      <c r="B50" s="28"/>
+      <c r="B50" s="27"/>
       <c r="C50" s="8"/>
       <c r="D50" s="8"/>
       <c r="E50" s="9"/>
@@ -2428,11 +2409,11 @@
       <c r="I50" s="10">
         <v>0</v>
       </c>
-      <c r="J50" s="45"/>
-      <c r="K50" s="42"/>
+      <c r="J50" s="43"/>
+      <c r="K50" s="40"/>
     </row>
     <row r="51" spans="2:11">
-      <c r="B51" s="28"/>
+      <c r="B51" s="27"/>
       <c r="C51" s="8"/>
       <c r="D51" s="8"/>
       <c r="E51" s="9"/>
@@ -2448,11 +2429,11 @@
       <c r="I51" s="10">
         <v>0</v>
       </c>
-      <c r="J51" s="45"/>
-      <c r="K51" s="42"/>
+      <c r="J51" s="43"/>
+      <c r="K51" s="40"/>
     </row>
     <row r="52" spans="2:11">
-      <c r="B52" s="28"/>
+      <c r="B52" s="27"/>
       <c r="C52" s="8"/>
       <c r="D52" s="8"/>
       <c r="E52" s="9"/>
@@ -2468,11 +2449,11 @@
       <c r="I52" s="3">
         <v>0</v>
       </c>
-      <c r="J52" s="41"/>
-      <c r="K52" s="42"/>
+      <c r="J52" s="39"/>
+      <c r="K52" s="40"/>
     </row>
     <row r="53" spans="2:11">
-      <c r="B53" s="28"/>
+      <c r="B53" s="27"/>
       <c r="C53" s="8"/>
       <c r="D53" s="8"/>
       <c r="E53" s="9"/>
@@ -2488,14 +2469,14 @@
       <c r="I53" s="3">
         <v>0</v>
       </c>
-      <c r="J53" s="41"/>
-      <c r="K53" s="42"/>
+      <c r="J53" s="39"/>
+      <c r="K53" s="40"/>
     </row>
     <row r="54" spans="2:11">
-      <c r="B54" s="28"/>
-      <c r="C54" s="8"/>
-      <c r="D54" s="8"/>
-      <c r="E54" s="9"/>
+      <c r="B54" s="30"/>
+      <c r="C54" s="15"/>
+      <c r="D54" s="15"/>
+      <c r="E54" s="16"/>
       <c r="F54" s="2" t="s">
         <v>24</v>
       </c>
@@ -2508,18 +2489,18 @@
       <c r="I54" s="3">
         <v>0</v>
       </c>
-      <c r="J54" s="41"/>
-      <c r="K54" s="42"/>
+      <c r="J54" s="39"/>
+      <c r="K54" s="40"/>
     </row>
     <row r="55" spans="2:11">
-      <c r="B55" s="28" t="s">
+      <c r="B55" s="31" t="s">
         <v>116</v>
       </c>
-      <c r="C55" s="8" t="s">
+      <c r="C55" s="19" t="s">
         <v>117</v>
       </c>
-      <c r="D55" s="8"/>
-      <c r="E55" s="9"/>
+      <c r="D55" s="19"/>
+      <c r="E55" s="20"/>
       <c r="F55" s="2" t="s">
         <v>118</v>
       </c>
@@ -2532,11 +2513,11 @@
       <c r="I55" s="3">
         <v>0</v>
       </c>
-      <c r="J55" s="41"/>
-      <c r="K55" s="42"/>
+      <c r="J55" s="39"/>
+      <c r="K55" s="40"/>
     </row>
     <row r="56" spans="2:11">
-      <c r="B56" s="28"/>
+      <c r="B56" s="27"/>
       <c r="C56" s="8"/>
       <c r="D56" s="8"/>
       <c r="E56" s="9"/>
@@ -2550,11 +2531,11 @@
         <v>120</v>
       </c>
       <c r="I56" s="3"/>
-      <c r="J56" s="41"/>
-      <c r="K56" s="42"/>
+      <c r="J56" s="39"/>
+      <c r="K56" s="40"/>
     </row>
     <row r="57" spans="2:11">
-      <c r="B57" s="28"/>
+      <c r="B57" s="27"/>
       <c r="C57" s="8"/>
       <c r="D57" s="8"/>
       <c r="E57" s="9"/>
@@ -2570,11 +2551,11 @@
       <c r="I57" s="3">
         <v>0</v>
       </c>
-      <c r="J57" s="41"/>
-      <c r="K57" s="42"/>
+      <c r="J57" s="39"/>
+      <c r="K57" s="40"/>
     </row>
     <row r="58" spans="2:11">
-      <c r="B58" s="28"/>
+      <c r="B58" s="27"/>
       <c r="C58" s="8"/>
       <c r="D58" s="8"/>
       <c r="E58" s="9"/>
@@ -2590,11 +2571,11 @@
       <c r="I58" s="3">
         <v>0</v>
       </c>
-      <c r="J58" s="41"/>
-      <c r="K58" s="42"/>
+      <c r="J58" s="39"/>
+      <c r="K58" s="40"/>
     </row>
     <row r="59" spans="2:11">
-      <c r="B59" s="30" t="s">
+      <c r="B59" s="29" t="s">
         <v>123</v>
       </c>
       <c r="C59" s="12" t="s">
@@ -2616,11 +2597,11 @@
       <c r="I59" s="3">
         <v>0</v>
       </c>
-      <c r="J59" s="41"/>
-      <c r="K59" s="42"/>
+      <c r="J59" s="39"/>
+      <c r="K59" s="40"/>
     </row>
     <row r="60" spans="2:11">
-      <c r="B60" s="28"/>
+      <c r="B60" s="27"/>
       <c r="C60" s="8"/>
       <c r="D60" s="8"/>
       <c r="E60" s="9"/>
@@ -2636,11 +2617,11 @@
       <c r="I60" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="J60" s="41"/>
-      <c r="K60" s="42"/>
+      <c r="J60" s="39"/>
+      <c r="K60" s="40"/>
     </row>
     <row r="61" spans="2:11">
-      <c r="B61" s="29"/>
+      <c r="B61" s="28"/>
       <c r="C61" s="10"/>
       <c r="D61" s="10"/>
       <c r="E61" s="11"/>
@@ -2656,11 +2637,11 @@
       <c r="I61" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="J61" s="41"/>
-      <c r="K61" s="42"/>
+      <c r="J61" s="39"/>
+      <c r="K61" s="40"/>
     </row>
     <row r="62" spans="2:11" ht="93.75">
-      <c r="B62" s="30" t="s">
+      <c r="B62" s="29" t="s">
         <v>131</v>
       </c>
       <c r="C62" s="12" t="s">
@@ -2684,14 +2665,14 @@
       <c r="I62" s="3">
         <v>0</v>
       </c>
-      <c r="J62" s="41"/>
-      <c r="K62" s="42"/>
+      <c r="J62" s="39"/>
+      <c r="K62" s="40"/>
     </row>
     <row r="63" spans="2:11">
-      <c r="B63" s="29"/>
-      <c r="C63" s="10"/>
-      <c r="D63" s="10"/>
-      <c r="E63" s="11"/>
+      <c r="B63" s="30"/>
+      <c r="C63" s="15"/>
+      <c r="D63" s="15"/>
+      <c r="E63" s="16"/>
       <c r="F63" s="2" t="s">
         <v>16</v>
       </c>
@@ -2704,18 +2685,18 @@
       <c r="I63" s="3">
         <v>0</v>
       </c>
-      <c r="J63" s="41"/>
-      <c r="K63" s="42"/>
-    </row>
-    <row r="64" spans="2:11" ht="56.25">
-      <c r="B64" s="33" t="s">
+      <c r="J63" s="39"/>
+      <c r="K63" s="40"/>
+    </row>
+    <row r="64" spans="2:11" ht="67.5">
+      <c r="B64" s="31" t="s">
         <v>137</v>
       </c>
-      <c r="C64" s="3" t="s">
+      <c r="C64" s="19" t="s">
         <v>132</v>
       </c>
-      <c r="D64" s="3"/>
-      <c r="E64" s="15" t="s">
+      <c r="D64" s="19"/>
+      <c r="E64" s="48" t="s">
         <v>138</v>
       </c>
       <c r="F64" s="2" t="s">
@@ -2730,25 +2711,19 @@
       <c r="I64" s="3">
         <v>0</v>
       </c>
-      <c r="J64" s="41"/>
-      <c r="K64" s="42"/>
-    </row>
-    <row r="65" spans="2:11" ht="56.25">
-      <c r="B65" s="33" t="s">
+      <c r="J64" s="39"/>
+      <c r="K64" s="40"/>
+    </row>
+    <row r="65" spans="2:11">
+      <c r="B65" s="30"/>
+      <c r="C65" s="15"/>
+      <c r="D65" s="15"/>
+      <c r="E65" s="16"/>
+      <c r="F65" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="G65" s="2" t="s">
         <v>140</v>
-      </c>
-      <c r="C65" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="D65" s="3"/>
-      <c r="E65" s="15" t="s">
-        <v>138</v>
-      </c>
-      <c r="F65" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G65" s="2" t="s">
-        <v>139</v>
       </c>
       <c r="H65" s="2" t="s">
         <v>14</v>
@@ -2756,46 +2731,46 @@
       <c r="I65" s="3">
         <v>0</v>
       </c>
-      <c r="J65" s="41"/>
-      <c r="K65" s="42"/>
+      <c r="J65" s="39"/>
+      <c r="K65" s="40"/>
     </row>
     <row r="66" spans="2:11">
-      <c r="B66" s="30" t="s">
+      <c r="B66" s="31" t="s">
+        <v>141</v>
+      </c>
+      <c r="C66" s="19" t="s">
         <v>142</v>
       </c>
-      <c r="C66" s="12" t="s">
+      <c r="D66" s="19"/>
+      <c r="E66" s="48" t="s">
         <v>143</v>
-      </c>
-      <c r="D66" s="12"/>
-      <c r="E66" s="14" t="s">
-        <v>144</v>
       </c>
       <c r="F66" s="13"/>
       <c r="G66" s="13"/>
       <c r="H66" s="13"/>
       <c r="I66" s="12"/>
-      <c r="J66" s="48"/>
-      <c r="K66" s="49"/>
+      <c r="J66" s="46"/>
+      <c r="K66" s="47"/>
     </row>
     <row r="67" spans="2:11">
-      <c r="B67" s="34" t="s">
+      <c r="B67" s="32" t="s">
+        <v>144</v>
+      </c>
+      <c r="C67" s="33" t="s">
         <v>145</v>
       </c>
-      <c r="C67" s="35" t="s">
+      <c r="D67" s="33" t="s">
         <v>146</v>
       </c>
-      <c r="D67" s="35" t="s">
+      <c r="E67" s="34" t="s">
         <v>147</v>
       </c>
-      <c r="E67" s="36" t="s">
-        <v>148</v>
-      </c>
-      <c r="F67" s="36"/>
-      <c r="G67" s="36"/>
-      <c r="H67" s="36"/>
-      <c r="I67" s="35"/>
-      <c r="J67" s="46"/>
-      <c r="K67" s="47"/>
+      <c r="F67" s="34"/>
+      <c r="G67" s="34"/>
+      <c r="H67" s="34"/>
+      <c r="I67" s="33"/>
+      <c r="J67" s="44"/>
+      <c r="K67" s="45"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>

</xml_diff>

<commit_message>
update sample register map, SV RTL and UVM RAL model
(refs: rggen/rggen#109)
</commit_message>
<xml_diff>
--- a/block_0.xlsx
+++ b/block_0.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25425"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BC9B0434-2B73-48F8-8004-154DEDB66167}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="91" documentId="8_{A0D56F00-2FF8-4245-9EBC-D59D5B1EA094}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{58C0B580-7FE2-4858-898B-9D5AEDAC4DC6}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="150">
   <si>
     <t>block name</t>
     <phoneticPr fontId="1"/>
@@ -461,6 +461,12 @@
   </si>
   <si>
     <t>rowotrg</t>
+  </si>
+  <si>
+    <t>row0trg</t>
+  </si>
+  <si>
+    <t>row1trg</t>
   </si>
   <si>
     <t>register_10</t>
@@ -1385,10 +1391,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:K67"/>
+  <dimension ref="B1:K69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="E65" sqref="B65:E66"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="I60" sqref="I60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
@@ -2575,28 +2581,20 @@
       <c r="K58" s="40"/>
     </row>
     <row r="59" spans="2:11">
-      <c r="B59" s="29" t="s">
+      <c r="B59" s="27"/>
+      <c r="C59" s="8"/>
+      <c r="D59" s="8"/>
+      <c r="E59" s="9"/>
+      <c r="F59" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G59" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="H59" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="C59" s="12" t="s">
-        <v>124</v>
-      </c>
-      <c r="D59" s="12" t="s">
-        <v>125</v>
-      </c>
-      <c r="E59" s="13"/>
-      <c r="F59" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G59" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="H59" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I59" s="3">
-        <v>0</v>
-      </c>
+      <c r="I59" s="3"/>
       <c r="J59" s="39"/>
       <c r="K59" s="40"/>
     </row>
@@ -2606,104 +2604,102 @@
       <c r="D60" s="8"/>
       <c r="E60" s="9"/>
       <c r="F60" s="2" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="G60" s="2" t="s">
-        <v>127</v>
+        <v>67</v>
       </c>
       <c r="H60" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I60" s="3" t="s">
-        <v>128</v>
-      </c>
+        <v>124</v>
+      </c>
+      <c r="I60" s="3"/>
       <c r="J60" s="39"/>
       <c r="K60" s="40"/>
     </row>
     <row r="61" spans="2:11">
-      <c r="B61" s="28"/>
-      <c r="C61" s="10"/>
-      <c r="D61" s="10"/>
-      <c r="E61" s="11"/>
+      <c r="B61" s="29" t="s">
+        <v>125</v>
+      </c>
+      <c r="C61" s="12" t="s">
+        <v>126</v>
+      </c>
+      <c r="D61" s="12" t="s">
+        <v>127</v>
+      </c>
+      <c r="E61" s="13"/>
       <c r="F61" s="2" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="G61" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="H61" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="I61" s="3" t="s">
-        <v>130</v>
+      <c r="I61" s="3">
+        <v>0</v>
       </c>
       <c r="J61" s="39"/>
       <c r="K61" s="40"/>
     </row>
-    <row r="62" spans="2:11" ht="93.75">
-      <c r="B62" s="29" t="s">
-        <v>131</v>
-      </c>
-      <c r="C62" s="12" t="s">
-        <v>132</v>
-      </c>
-      <c r="D62" s="12" t="s">
-        <v>133</v>
-      </c>
-      <c r="E62" s="14" t="s">
-        <v>134</v>
-      </c>
+    <row r="62" spans="2:11">
+      <c r="B62" s="27"/>
+      <c r="C62" s="8"/>
+      <c r="D62" s="8"/>
+      <c r="E62" s="9"/>
       <c r="F62" s="2" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="G62" s="2" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="H62" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="I62" s="3">
-        <v>0</v>
+      <c r="I62" s="3" t="s">
+        <v>130</v>
       </c>
       <c r="J62" s="39"/>
       <c r="K62" s="40"/>
     </row>
     <row r="63" spans="2:11">
-      <c r="B63" s="30"/>
-      <c r="C63" s="15"/>
-      <c r="D63" s="15"/>
-      <c r="E63" s="16"/>
+      <c r="B63" s="28"/>
+      <c r="C63" s="10"/>
+      <c r="D63" s="10"/>
+      <c r="E63" s="11"/>
       <c r="F63" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G63" s="2" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="H63" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="I63" s="3">
-        <v>0</v>
+      <c r="I63" s="3" t="s">
+        <v>132</v>
       </c>
       <c r="J63" s="39"/>
       <c r="K63" s="40"/>
     </row>
-    <row r="64" spans="2:11" ht="67.5">
-      <c r="B64" s="31" t="s">
-        <v>137</v>
-      </c>
-      <c r="C64" s="19" t="s">
-        <v>132</v>
-      </c>
-      <c r="D64" s="19"/>
-      <c r="E64" s="48" t="s">
-        <v>138</v>
+    <row r="64" spans="2:11" ht="93.75">
+      <c r="B64" s="29" t="s">
+        <v>133</v>
+      </c>
+      <c r="C64" s="12" t="s">
+        <v>134</v>
+      </c>
+      <c r="D64" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="E64" s="14" t="s">
+        <v>136</v>
       </c>
       <c r="F64" s="2" t="s">
         <v>12</v>
       </c>
       <c r="G64" s="2" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="H64" s="2" t="s">
         <v>14</v>
@@ -2720,10 +2716,10 @@
       <c r="D65" s="15"/>
       <c r="E65" s="16"/>
       <c r="F65" s="2" t="s">
-        <v>107</v>
+        <v>16</v>
       </c>
       <c r="G65" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="H65" s="2" t="s">
         <v>14</v>
@@ -2734,43 +2730,89 @@
       <c r="J65" s="39"/>
       <c r="K65" s="40"/>
     </row>
-    <row r="66" spans="2:11">
+    <row r="66" spans="2:11" ht="67.5">
       <c r="B66" s="31" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C66" s="19" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="D66" s="19"/>
       <c r="E66" s="48" t="s">
+        <v>140</v>
+      </c>
+      <c r="F66" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G66" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="H66" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I66" s="3">
+        <v>0</v>
+      </c>
+      <c r="J66" s="39"/>
+      <c r="K66" s="40"/>
+    </row>
+    <row r="67" spans="2:11">
+      <c r="B67" s="30"/>
+      <c r="C67" s="15"/>
+      <c r="D67" s="15"/>
+      <c r="E67" s="16"/>
+      <c r="F67" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="G67" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="H67" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I67" s="3">
+        <v>0</v>
+      </c>
+      <c r="J67" s="39"/>
+      <c r="K67" s="40"/>
+    </row>
+    <row r="68" spans="2:11">
+      <c r="B68" s="31" t="s">
         <v>143</v>
       </c>
-      <c r="F66" s="13"/>
-      <c r="G66" s="13"/>
-      <c r="H66" s="13"/>
-      <c r="I66" s="12"/>
-      <c r="J66" s="46"/>
-      <c r="K66" s="47"/>
-    </row>
-    <row r="67" spans="2:11">
-      <c r="B67" s="32" t="s">
+      <c r="C68" s="19" t="s">
         <v>144</v>
       </c>
-      <c r="C67" s="33" t="s">
+      <c r="D68" s="19"/>
+      <c r="E68" s="48" t="s">
         <v>145</v>
       </c>
-      <c r="D67" s="33" t="s">
+      <c r="F68" s="13"/>
+      <c r="G68" s="13"/>
+      <c r="H68" s="13"/>
+      <c r="I68" s="12"/>
+      <c r="J68" s="46"/>
+      <c r="K68" s="47"/>
+    </row>
+    <row r="69" spans="2:11">
+      <c r="B69" s="32" t="s">
         <v>146</v>
       </c>
-      <c r="E67" s="34" t="s">
+      <c r="C69" s="33" t="s">
         <v>147</v>
       </c>
-      <c r="F67" s="34"/>
-      <c r="G67" s="34"/>
-      <c r="H67" s="34"/>
-      <c r="I67" s="33"/>
-      <c r="J67" s="44"/>
-      <c r="K67" s="45"/>
+      <c r="D69" s="33" t="s">
+        <v>148</v>
+      </c>
+      <c r="E69" s="34" t="s">
+        <v>149</v>
+      </c>
+      <c r="F69" s="34"/>
+      <c r="G69" s="34"/>
+      <c r="H69" s="34"/>
+      <c r="I69" s="33"/>
+      <c r="J69" s="44"/>
+      <c r="K69" s="45"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>

</xml_diff>

<commit_message>
add custom bit field type
(refs: rggen/rggen#119)
</commit_message>
<xml_diff>
--- a/block_0.xlsx
+++ b/block_0.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25721"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="91" documentId="8_{A0D56F00-2FF8-4245-9EBC-D59D5B1EA094}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{58C0B580-7FE2-4858-898B-9D5AEDAC4DC6}"/>
+  <xr:revisionPtr revIDLastSave="146" documentId="8_{A0D56F00-2FF8-4245-9EBC-D59D5B1EA094}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CE63D165-E353-4615-B593-E9A24EEA0883}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,6 +23,7 @@
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="161">
   <si>
     <t>block name</t>
     <phoneticPr fontId="1"/>
@@ -538,10 +539,56 @@
     <t>0x60</t>
   </si>
   <si>
+    <t>custom</t>
+  </si>
+  <si>
+    <t>custom:
+sw_write: none</t>
+  </si>
+  <si>
+    <t>custom:
+sw_write_once: true</t>
+  </si>
+  <si>
+    <t>custom:
+write_trigger: true
+read_trigger: true</t>
+  </si>
+  <si>
+    <t>custom:
+sw_write: set_1
+sw_read: clear</t>
+  </si>
+  <si>
+    <t>custom:
+sw_write: clear_1
+sw_read: set</t>
+  </si>
+  <si>
+    <t>custom:
+sw_write: set_1
+hw_clear: true</t>
+  </si>
+  <si>
+    <t>custom:
+sw_write: clear_1
+hw_set: true</t>
+  </si>
+  <si>
+    <t>custom:
+hw_write: true</t>
+  </si>
+  <si>
+    <t>register_14</t>
+  </si>
+  <si>
+    <t>0x70</t>
+  </si>
+  <si>
     <t>reserved</t>
   </si>
   <si>
-    <t>register_14</t>
+    <t>register_15</t>
   </si>
   <si>
     <t>0x80</t>
@@ -1391,11 +1438,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:K69"/>
+  <dimension ref="B1:K78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="I60" sqref="I60"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
   <cols>
@@ -1404,7 +1449,7 @@
     <col min="5" max="5" width="22" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.5" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9" style="1"/>
+    <col min="8" max="8" width="18.625" style="1" customWidth="1"/>
     <col min="9" max="9" width="11.375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="20.375" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="24.625" customWidth="1"/>
@@ -2777,42 +2822,224 @@
       <c r="K67" s="40"/>
     </row>
     <row r="68" spans="2:11">
-      <c r="B68" s="31" t="s">
+      <c r="B68" s="27" t="s">
         <v>143</v>
       </c>
-      <c r="C68" s="19" t="s">
+      <c r="C68" s="8" t="s">
         <v>144</v>
       </c>
-      <c r="D68" s="19"/>
-      <c r="E68" s="48" t="s">
+      <c r="D68" s="8"/>
+      <c r="E68" s="9"/>
+      <c r="F68" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="G68" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="H68" s="13" t="s">
         <v>145</v>
       </c>
-      <c r="F68" s="13"/>
-      <c r="G68" s="13"/>
-      <c r="H68" s="13"/>
-      <c r="I68" s="12"/>
+      <c r="I68" s="12">
+        <v>0</v>
+      </c>
       <c r="J68" s="46"/>
       <c r="K68" s="47"/>
     </row>
-    <row r="69" spans="2:11">
-      <c r="B69" s="32" t="s">
+    <row r="69" spans="2:11" ht="67.5">
+      <c r="B69" s="27"/>
+      <c r="C69" s="8"/>
+      <c r="D69" s="8"/>
+      <c r="E69" s="9"/>
+      <c r="F69" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="G69" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="H69" s="14" t="s">
         <v>146</v>
       </c>
-      <c r="C69" s="33" t="s">
+      <c r="I69" s="12"/>
+      <c r="J69" s="46"/>
+      <c r="K69" s="47"/>
+    </row>
+    <row r="70" spans="2:11" ht="90">
+      <c r="B70" s="27"/>
+      <c r="C70" s="8"/>
+      <c r="D70" s="8"/>
+      <c r="E70" s="9"/>
+      <c r="F70" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="G70" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="H70" s="14" t="s">
         <v>147</v>
       </c>
-      <c r="D69" s="33" t="s">
+      <c r="I70" s="12">
+        <v>0</v>
+      </c>
+      <c r="J70" s="46"/>
+      <c r="K70" s="47"/>
+    </row>
+    <row r="71" spans="2:11" ht="67.5">
+      <c r="B71" s="27"/>
+      <c r="C71" s="8"/>
+      <c r="D71" s="8"/>
+      <c r="E71" s="9"/>
+      <c r="F71" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="G71" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="H71" s="14" t="s">
         <v>148</v>
       </c>
-      <c r="E69" s="34" t="s">
+      <c r="I71" s="12">
+        <v>0</v>
+      </c>
+      <c r="J71" s="46"/>
+      <c r="K71" s="47"/>
+    </row>
+    <row r="72" spans="2:11" ht="67.5">
+      <c r="B72" s="27"/>
+      <c r="C72" s="8"/>
+      <c r="D72" s="8"/>
+      <c r="E72" s="9"/>
+      <c r="F72" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="G72" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="H72" s="14" t="s">
         <v>149</v>
       </c>
-      <c r="F69" s="34"/>
-      <c r="G69" s="34"/>
-      <c r="H69" s="34"/>
-      <c r="I69" s="33"/>
-      <c r="J69" s="44"/>
-      <c r="K69" s="45"/>
+      <c r="I72" s="12">
+        <v>0</v>
+      </c>
+      <c r="J72" s="46"/>
+      <c r="K72" s="47"/>
+    </row>
+    <row r="73" spans="2:11" ht="67.5">
+      <c r="B73" s="27"/>
+      <c r="C73" s="8"/>
+      <c r="D73" s="8"/>
+      <c r="E73" s="9"/>
+      <c r="F73" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="G73" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="H73" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="I73" s="12">
+        <v>0</v>
+      </c>
+      <c r="J73" s="46"/>
+      <c r="K73" s="47"/>
+    </row>
+    <row r="74" spans="2:11" ht="67.5">
+      <c r="B74" s="27"/>
+      <c r="C74" s="8"/>
+      <c r="D74" s="8"/>
+      <c r="E74" s="9"/>
+      <c r="F74" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="G74" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="H74" s="14" t="s">
+        <v>151</v>
+      </c>
+      <c r="I74" s="12">
+        <v>0</v>
+      </c>
+      <c r="J74" s="46"/>
+      <c r="K74" s="47"/>
+    </row>
+    <row r="75" spans="2:11" ht="67.5">
+      <c r="B75" s="27"/>
+      <c r="C75" s="8"/>
+      <c r="D75" s="8"/>
+      <c r="E75" s="9"/>
+      <c r="F75" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="G75" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="H75" s="14" t="s">
+        <v>152</v>
+      </c>
+      <c r="I75" s="12">
+        <v>0</v>
+      </c>
+      <c r="J75" s="46"/>
+      <c r="K75" s="47"/>
+    </row>
+    <row r="76" spans="2:11" ht="45">
+      <c r="B76" s="27"/>
+      <c r="C76" s="8"/>
+      <c r="D76" s="8"/>
+      <c r="E76" s="9"/>
+      <c r="F76" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="G76" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="H76" s="14" t="s">
+        <v>153</v>
+      </c>
+      <c r="I76" s="12">
+        <v>0</v>
+      </c>
+      <c r="J76" s="46"/>
+      <c r="K76" s="47"/>
+    </row>
+    <row r="77" spans="2:11">
+      <c r="B77" s="31" t="s">
+        <v>154</v>
+      </c>
+      <c r="C77" s="19" t="s">
+        <v>155</v>
+      </c>
+      <c r="D77" s="19"/>
+      <c r="E77" s="48" t="s">
+        <v>156</v>
+      </c>
+      <c r="F77" s="13"/>
+      <c r="G77" s="13"/>
+      <c r="H77" s="13"/>
+      <c r="I77" s="12"/>
+      <c r="J77" s="46"/>
+      <c r="K77" s="47"/>
+    </row>
+    <row r="78" spans="2:11">
+      <c r="B78" s="32" t="s">
+        <v>157</v>
+      </c>
+      <c r="C78" s="33" t="s">
+        <v>158</v>
+      </c>
+      <c r="D78" s="33" t="s">
+        <v>159</v>
+      </c>
+      <c r="E78" s="34" t="s">
+        <v>160</v>
+      </c>
+      <c r="F78" s="34"/>
+      <c r="G78" s="34"/>
+      <c r="H78" s="34"/>
+      <c r="I78" s="33"/>
+      <c r="J78" s="44"/>
+      <c r="K78" s="45"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>

</xml_diff>

<commit_message>
update samples due to adding 'rol' bit field type
(refs: rggen/rggen#120)
</commit_message>
<xml_diff>
--- a/block_0.xlsx
+++ b/block_0.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25721"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25803"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="146" documentId="8_{A0D56F00-2FF8-4245-9EBC-D59D5B1EA094}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CE63D165-E353-4615-B593-E9A24EEA0883}"/>
+  <xr:revisionPtr revIDLastSave="163" documentId="8_{A0D56F00-2FF8-4245-9EBC-D59D5B1EA094}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F4D8A63D-83F7-4872-8050-5C59A83B08C0}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="163">
   <si>
     <t>block name</t>
     <phoneticPr fontId="1"/>
@@ -153,229 +153,239 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
+    <t>8:8</t>
+  </si>
+  <si>
+    <t>rof</t>
+  </si>
+  <si>
+    <t>0xab</t>
+  </si>
+  <si>
+    <t>bit_field_2</t>
+  </si>
+  <si>
+    <t>4:16</t>
+  </si>
+  <si>
+    <t>rol</t>
+  </si>
+  <si>
+    <t>bit_field_3</t>
+  </si>
+  <si>
+    <t>4:20</t>
+  </si>
+  <si>
+    <t>register_3.bit_field_3</t>
+  </si>
+  <si>
+    <t>8:24</t>
+  </si>
+  <si>
+    <t>reserved</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>register_3</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>wo</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>4:4</t>
+  </si>
+  <si>
+    <t>wo1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
     <t>4:8</t>
   </si>
   <si>
-    <t>8:16</t>
-  </si>
-  <si>
-    <t>rof</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>0xab</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>8:24</t>
-  </si>
-  <si>
-    <t>reserved</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>register_3</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>wo</t>
+    <t>w0trg</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>w1trg</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>register_4</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>0x0C</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>rc</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>register_0.bit_field_0</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>4:12</t>
+  </si>
+  <si>
+    <t>register_4.bit_field_1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>rs</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>register_5</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>0x10</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>2:0</t>
+  </si>
+  <si>
+    <t>rwc</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>2:2</t>
+  </si>
+  <si>
+    <t>register_3.bit_field_2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>2:4</t>
+  </si>
+  <si>
+    <t>rws</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>2:6</t>
+  </si>
+  <si>
+    <t>register_3.bit_field_3</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>bit_field_4</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>2:8</t>
+  </si>
+  <si>
+    <t>rwe</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>bit_field_5</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>2:10</t>
+  </si>
+  <si>
+    <t>register_0.bit_field_2</t>
+  </si>
+  <si>
+    <t>bit_field_6</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>2:12</t>
+  </si>
+  <si>
+    <t>bit_field_7</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>2:16</t>
+  </si>
+  <si>
+    <t>rwl</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>bit_field_8</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>2:18</t>
+  </si>
+  <si>
+    <t>register_0.bit_field_2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>bit_field_9</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>2:20</t>
+  </si>
+  <si>
+    <t>register_6</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>0x14</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>w0c</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
     <t>4:4</t>
-  </si>
-  <si>
-    <t>wo1</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>w0trg</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>4:16</t>
-  </si>
-  <si>
-    <t>w1trg</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>register_4</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>0x0C</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>rc</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>register_0.bit_field_0</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>4:12</t>
-  </si>
-  <si>
-    <t>register_4.bit_field_1</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>rs</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>register_5</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>0x10</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>2:0</t>
-  </si>
-  <si>
-    <t>rwc</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>2:2</t>
-  </si>
-  <si>
-    <t>register_3.bit_field_2</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>2:4</t>
-  </si>
-  <si>
-    <t>rws</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>2:6</t>
-  </si>
-  <si>
-    <t>register_3.bit_field_3</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>bit_field_4</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>2:8</t>
-  </si>
-  <si>
-    <t>rwe</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>bit_field_5</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>2:10</t>
-  </si>
-  <si>
-    <t>register_0.bit_field_2</t>
-  </si>
-  <si>
-    <t>bit_field_6</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>2:12</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>register_6.bit_field_1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>w1c</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>register_6.bit_field_4</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>4:24</t>
+  </si>
+  <si>
+    <t>w0s</t>
   </si>
   <si>
     <t>bit_field_7</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>2:16</t>
-  </si>
-  <si>
-    <t>rwl</t>
-    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>4:28</t>
+  </si>
+  <si>
+    <t>w1s</t>
   </si>
   <si>
     <t>bit_field_8</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>2:18</t>
-  </si>
-  <si>
-    <t>register_0.bit_field_2</t>
-    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>4:32</t>
+  </si>
+  <si>
+    <t>w0t</t>
   </si>
   <si>
     <t>bit_field_9</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>2:20</t>
-  </si>
-  <si>
-    <t>register_6</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>0x14</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>w0c</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>4:4</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>register_6.bit_field_1</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>w1c</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>4:20</t>
-  </si>
-  <si>
-    <t>register_6.bit_field_4</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>4:24</t>
-  </si>
-  <si>
-    <t>w0s</t>
-  </si>
-  <si>
-    <t>bit_field_7</t>
-  </si>
-  <si>
-    <t>4:28</t>
-  </si>
-  <si>
-    <t>w1s</t>
-  </si>
-  <si>
-    <t>bit_field_8</t>
-  </si>
-  <si>
-    <t>4:32</t>
-  </si>
-  <si>
-    <t>w0t</t>
-  </si>
-  <si>
-    <t>bit_field_9</t>
   </si>
   <si>
     <t>4:36</t>
@@ -422,13 +432,7 @@
     <t>ws</t>
   </si>
   <si>
-    <t>bit_field_2</t>
-  </si>
-  <si>
     <t>woc</t>
-  </si>
-  <si>
-    <t>bit_field_3</t>
   </si>
   <si>
     <t>wos</t>
@@ -1438,9 +1442,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:K78"/>
+  <dimension ref="B1:K79"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A72" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
   <cols>
@@ -1701,9 +1705,11 @@
         <v>33</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="I14" s="3"/>
+        <v>34</v>
+      </c>
+      <c r="I14" s="3" t="s">
+        <v>35</v>
+      </c>
       <c r="J14" s="39"/>
       <c r="K14" s="40"/>
     </row>
@@ -1713,75 +1719,77 @@
       <c r="D15" s="8"/>
       <c r="E15" s="9"/>
       <c r="F15" s="2" t="s">
-        <v>17</v>
+        <v>36</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="I15" s="3" t="s">
-        <v>36</v>
+        <v>38</v>
+      </c>
+      <c r="I15" s="3">
+        <v>0</v>
       </c>
       <c r="J15" s="39"/>
       <c r="K15" s="40"/>
     </row>
     <row r="16" spans="2:11">
-      <c r="B16" s="28"/>
-      <c r="C16" s="10"/>
-      <c r="D16" s="10"/>
-      <c r="E16" s="11"/>
+      <c r="B16" s="27"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="9"/>
       <c r="F16" s="2" t="s">
-        <v>19</v>
+        <v>39</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="H16" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="I16" s="3"/>
-      <c r="J16" s="39"/>
+      <c r="I16" s="3">
+        <v>0</v>
+      </c>
+      <c r="J16" s="39" t="s">
+        <v>41</v>
+      </c>
       <c r="K16" s="40"/>
     </row>
     <row r="17" spans="2:11">
-      <c r="B17" s="29" t="s">
-        <v>39</v>
-      </c>
-      <c r="C17" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="D17" s="12"/>
-      <c r="E17" s="13"/>
+      <c r="B17" s="28"/>
+      <c r="C17" s="10"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="11"/>
       <c r="F17" s="2" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="I17" s="3">
-        <v>0</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="I17" s="3"/>
       <c r="J17" s="39"/>
       <c r="K17" s="40"/>
     </row>
     <row r="18" spans="2:11">
-      <c r="B18" s="27"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="9"/>
+      <c r="B18" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="C18" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="D18" s="12"/>
+      <c r="E18" s="13"/>
       <c r="F18" s="2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="I18" s="3">
         <v>0</v>
@@ -1795,15 +1803,17 @@
       <c r="D19" s="8"/>
       <c r="E19" s="9"/>
       <c r="F19" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="I19" s="3"/>
+        <v>47</v>
+      </c>
+      <c r="I19" s="3">
+        <v>0</v>
+      </c>
       <c r="J19" s="39"/>
       <c r="K19" s="40"/>
     </row>
@@ -1813,62 +1823,58 @@
       <c r="D20" s="8"/>
       <c r="E20" s="9"/>
       <c r="F20" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="I20" s="3"/>
       <c r="J20" s="39"/>
       <c r="K20" s="40"/>
     </row>
     <row r="21" spans="2:11">
-      <c r="B21" s="29" t="s">
-        <v>46</v>
-      </c>
-      <c r="C21" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="D21" s="12"/>
-      <c r="E21" s="13"/>
+      <c r="B21" s="27"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="8"/>
+      <c r="E21" s="9"/>
       <c r="F21" s="2" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="I21" s="3">
-        <v>0</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="I21" s="3"/>
       <c r="J21" s="39"/>
       <c r="K21" s="40"/>
     </row>
     <row r="22" spans="2:11">
-      <c r="B22" s="27"/>
-      <c r="C22" s="8"/>
-      <c r="D22" s="8"/>
-      <c r="E22" s="9"/>
+      <c r="B22" s="29" t="s">
+        <v>51</v>
+      </c>
+      <c r="C22" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D22" s="12"/>
+      <c r="E22" s="13"/>
       <c r="F22" s="2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="I22" s="3">
         <v>0</v>
       </c>
-      <c r="J22" s="39" t="s">
-        <v>49</v>
-      </c>
+      <c r="J22" s="39"/>
       <c r="K22" s="40"/>
     </row>
     <row r="23" spans="2:11">
@@ -1877,57 +1883,55 @@
       <c r="D23" s="8"/>
       <c r="E23" s="9"/>
       <c r="F23" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="I23" s="3">
+        <v>0</v>
+      </c>
+      <c r="J23" s="39" t="s">
+        <v>54</v>
+      </c>
+      <c r="K23" s="40"/>
+    </row>
+    <row r="24" spans="2:11">
+      <c r="B24" s="27"/>
+      <c r="C24" s="8"/>
+      <c r="D24" s="8"/>
+      <c r="E24" s="9"/>
+      <c r="F24" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="G23" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="H23" s="2" t="s">
+      <c r="G24" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="H24" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="I23" s="3"/>
-      <c r="J23" s="39" t="s">
-        <v>51</v>
-      </c>
-      <c r="K23" s="40"/>
-    </row>
-    <row r="24" spans="2:11">
-      <c r="B24" s="28"/>
-      <c r="C24" s="10"/>
-      <c r="D24" s="10"/>
-      <c r="E24" s="11"/>
-      <c r="F24" s="2" t="s">
+      <c r="I24" s="3"/>
+      <c r="J24" s="39" t="s">
+        <v>56</v>
+      </c>
+      <c r="K24" s="40"/>
+    </row>
+    <row r="25" spans="2:11">
+      <c r="B25" s="28"/>
+      <c r="C25" s="10"/>
+      <c r="D25" s="10"/>
+      <c r="E25" s="11"/>
+      <c r="F25" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G24" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="H24" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="I24" s="3">
-        <v>0</v>
-      </c>
-      <c r="J24" s="39"/>
-      <c r="K24" s="40"/>
-    </row>
-    <row r="25" spans="2:11">
-      <c r="B25" s="29" t="s">
-        <v>53</v>
-      </c>
-      <c r="C25" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="D25" s="12"/>
-      <c r="E25" s="13"/>
-      <c r="F25" s="2" t="s">
-        <v>12</v>
-      </c>
       <c r="G25" s="2" t="s">
-        <v>55</v>
+        <v>37</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="I25" s="3">
         <v>0</v>
@@ -1936,25 +1940,27 @@
       <c r="K25" s="40"/>
     </row>
     <row r="26" spans="2:11">
-      <c r="B26" s="27"/>
-      <c r="C26" s="8"/>
-      <c r="D26" s="8"/>
-      <c r="E26" s="9"/>
+      <c r="B26" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="C26" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="D26" s="12"/>
+      <c r="E26" s="13"/>
       <c r="F26" s="2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="I26" s="3">
         <v>0</v>
       </c>
-      <c r="J26" s="39" t="s">
-        <v>58</v>
-      </c>
+      <c r="J26" s="39"/>
       <c r="K26" s="40"/>
     </row>
     <row r="27" spans="2:11">
@@ -1963,18 +1969,20 @@
       <c r="D27" s="8"/>
       <c r="E27" s="9"/>
       <c r="F27" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="I27" s="3">
         <v>0</v>
       </c>
-      <c r="J27" s="39"/>
+      <c r="J27" s="39" t="s">
+        <v>63</v>
+      </c>
       <c r="K27" s="40"/>
     </row>
     <row r="28" spans="2:11">
@@ -1983,20 +1991,18 @@
       <c r="D28" s="8"/>
       <c r="E28" s="9"/>
       <c r="F28" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="I28" s="3">
         <v>0</v>
       </c>
-      <c r="J28" s="39" t="s">
-        <v>62</v>
-      </c>
+      <c r="J28" s="39"/>
       <c r="K28" s="40"/>
     </row>
     <row r="29" spans="2:11">
@@ -2005,10 +2011,10 @@
       <c r="D29" s="8"/>
       <c r="E29" s="9"/>
       <c r="F29" s="2" t="s">
-        <v>63</v>
+        <v>19</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="H29" s="2" t="s">
         <v>65</v>
@@ -2016,7 +2022,9 @@
       <c r="I29" s="3">
         <v>0</v>
       </c>
-      <c r="J29" s="39"/>
+      <c r="J29" s="39" t="s">
+        <v>67</v>
+      </c>
       <c r="K29" s="40"/>
     </row>
     <row r="30" spans="2:11">
@@ -2025,20 +2033,18 @@
       <c r="D30" s="8"/>
       <c r="E30" s="9"/>
       <c r="F30" s="2" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="I30" s="3">
         <v>0</v>
       </c>
-      <c r="J30" s="39" t="s">
-        <v>68</v>
-      </c>
+      <c r="J30" s="39"/>
       <c r="K30" s="40"/>
     </row>
     <row r="31" spans="2:11">
@@ -2047,19 +2053,19 @@
       <c r="D31" s="8"/>
       <c r="E31" s="9"/>
       <c r="F31" s="2" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="G31" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="H31" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="H31" s="2" t="s">
-        <v>65</v>
-      </c>
       <c r="I31" s="3">
         <v>0</v>
       </c>
       <c r="J31" s="39" t="s">
-        <v>28</v>
+        <v>73</v>
       </c>
       <c r="K31" s="40"/>
     </row>
@@ -2069,18 +2075,20 @@
       <c r="D32" s="8"/>
       <c r="E32" s="9"/>
       <c r="F32" s="2" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="I32" s="3">
         <v>0</v>
       </c>
-      <c r="J32" s="39"/>
+      <c r="J32" s="39" t="s">
+        <v>28</v>
+      </c>
       <c r="K32" s="40"/>
     </row>
     <row r="33" spans="2:11">
@@ -2089,88 +2097,86 @@
       <c r="D33" s="8"/>
       <c r="E33" s="9"/>
       <c r="F33" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="I33" s="3">
         <v>0</v>
       </c>
-      <c r="J33" s="39" t="s">
-        <v>76</v>
-      </c>
+      <c r="J33" s="39"/>
       <c r="K33" s="40"/>
     </row>
     <row r="34" spans="2:11">
-      <c r="B34" s="28"/>
-      <c r="C34" s="10"/>
-      <c r="D34" s="10"/>
-      <c r="E34" s="11"/>
+      <c r="B34" s="27"/>
+      <c r="C34" s="8"/>
+      <c r="D34" s="8"/>
+      <c r="E34" s="9"/>
       <c r="F34" s="2" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="G34" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="H34" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="H34" s="2" t="s">
-        <v>73</v>
-      </c>
       <c r="I34" s="3">
         <v>0</v>
       </c>
       <c r="J34" s="39" t="s">
+        <v>81</v>
+      </c>
+      <c r="K34" s="40"/>
+    </row>
+    <row r="35" spans="2:11">
+      <c r="B35" s="28"/>
+      <c r="C35" s="10"/>
+      <c r="D35" s="10"/>
+      <c r="E35" s="11"/>
+      <c r="F35" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="G35" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="H35" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="I35" s="3">
+        <v>0</v>
+      </c>
+      <c r="J35" s="39" t="s">
         <v>28</v>
       </c>
-      <c r="K34" s="40"/>
-    </row>
-    <row r="35" spans="2:11">
-      <c r="B35" s="29" t="s">
-        <v>79</v>
-      </c>
-      <c r="C35" s="12" t="s">
-        <v>80</v>
-      </c>
-      <c r="D35" s="12"/>
-      <c r="E35" s="13"/>
-      <c r="F35" s="2" t="s">
+      <c r="K35" s="40"/>
+    </row>
+    <row r="36" spans="2:11">
+      <c r="B36" s="29" t="s">
+        <v>84</v>
+      </c>
+      <c r="C36" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="D36" s="12"/>
+      <c r="E36" s="13"/>
+      <c r="F36" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G35" s="2" t="s">
+      <c r="G36" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="H35" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="I35" s="3">
-        <v>0</v>
-      </c>
-      <c r="J35" s="39"/>
-      <c r="K35" s="40"/>
-    </row>
-    <row r="36" spans="2:11">
-      <c r="B36" s="27"/>
-      <c r="C36" s="8"/>
-      <c r="D36" s="8"/>
-      <c r="E36" s="9"/>
-      <c r="F36" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G36" s="2" t="s">
-        <v>82</v>
-      </c>
       <c r="H36" s="2" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="I36" s="3">
         <v>0</v>
       </c>
-      <c r="J36" s="39" t="s">
-        <v>49</v>
-      </c>
+      <c r="J36" s="39"/>
       <c r="K36" s="40"/>
     </row>
     <row r="37" spans="2:11">
@@ -2179,17 +2185,19 @@
       <c r="D37" s="8"/>
       <c r="E37" s="9"/>
       <c r="F37" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>33</v>
+        <v>87</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="I37" s="3"/>
+        <v>86</v>
+      </c>
+      <c r="I37" s="3">
+        <v>0</v>
+      </c>
       <c r="J37" s="39" t="s">
-        <v>83</v>
+        <v>54</v>
       </c>
       <c r="K37" s="40"/>
     </row>
@@ -2199,18 +2207,18 @@
       <c r="D38" s="8"/>
       <c r="E38" s="9"/>
       <c r="F38" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="I38" s="3">
-        <v>0</v>
-      </c>
-      <c r="J38" s="39"/>
+        <v>32</v>
+      </c>
+      <c r="I38" s="3"/>
+      <c r="J38" s="39" t="s">
+        <v>88</v>
+      </c>
       <c r="K38" s="40"/>
     </row>
     <row r="39" spans="2:11">
@@ -2219,20 +2227,18 @@
       <c r="D39" s="8"/>
       <c r="E39" s="9"/>
       <c r="F39" s="2" t="s">
-        <v>63</v>
+        <v>19</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="H39" s="2" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="I39" s="3">
         <v>0</v>
       </c>
-      <c r="J39" s="39" t="s">
-        <v>49</v>
-      </c>
+      <c r="J39" s="39"/>
       <c r="K39" s="40"/>
     </row>
     <row r="40" spans="2:11">
@@ -2241,17 +2247,19 @@
       <c r="D40" s="8"/>
       <c r="E40" s="9"/>
       <c r="F40" s="2" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>85</v>
+        <v>37</v>
       </c>
       <c r="H40" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="I40" s="3"/>
+        <v>89</v>
+      </c>
+      <c r="I40" s="3">
+        <v>0</v>
+      </c>
       <c r="J40" s="39" t="s">
-        <v>86</v>
+        <v>54</v>
       </c>
       <c r="K40" s="40"/>
     </row>
@@ -2261,18 +2269,18 @@
       <c r="D41" s="8"/>
       <c r="E41" s="9"/>
       <c r="F41" s="2" t="s">
-        <v>26</v>
+        <v>71</v>
       </c>
       <c r="G41" s="2" t="s">
-        <v>87</v>
+        <v>40</v>
       </c>
       <c r="H41" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="I41" s="3">
-        <v>0</v>
-      </c>
-      <c r="J41" s="39"/>
+        <v>32</v>
+      </c>
+      <c r="I41" s="3"/>
+      <c r="J41" s="39" t="s">
+        <v>90</v>
+      </c>
       <c r="K41" s="40"/>
     </row>
     <row r="42" spans="2:11">
@@ -2281,13 +2289,13 @@
       <c r="D42" s="8"/>
       <c r="E42" s="9"/>
       <c r="F42" s="2" t="s">
-        <v>89</v>
+        <v>26</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="H42" s="2" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="I42" s="3">
         <v>0</v>
@@ -2301,13 +2309,13 @@
       <c r="D43" s="8"/>
       <c r="E43" s="9"/>
       <c r="F43" s="2" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="G43" s="2" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="H43" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="I43" s="3">
         <v>0</v>
@@ -2316,18 +2324,18 @@
       <c r="K43" s="40"/>
     </row>
     <row r="44" spans="2:11">
-      <c r="B44" s="28"/>
-      <c r="C44" s="10"/>
-      <c r="D44" s="10"/>
-      <c r="E44" s="11"/>
+      <c r="B44" s="27"/>
+      <c r="C44" s="8"/>
+      <c r="D44" s="8"/>
+      <c r="E44" s="9"/>
       <c r="F44" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="G44" s="2" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="H44" s="2" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="I44" s="3">
         <v>0</v>
@@ -2336,22 +2344,18 @@
       <c r="K44" s="40"/>
     </row>
     <row r="45" spans="2:11">
-      <c r="B45" s="27" t="s">
-        <v>98</v>
-      </c>
-      <c r="C45" s="8" t="s">
+      <c r="B45" s="28"/>
+      <c r="C45" s="10"/>
+      <c r="D45" s="10"/>
+      <c r="E45" s="11"/>
+      <c r="F45" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="D45" s="8"/>
-      <c r="E45" s="9"/>
-      <c r="F45" s="2" t="s">
-        <v>12</v>
-      </c>
       <c r="G45" s="2" t="s">
-        <v>31</v>
+        <v>100</v>
       </c>
       <c r="H45" s="2" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="I45" s="3">
         <v>0</v>
@@ -2360,18 +2364,22 @@
       <c r="K45" s="40"/>
     </row>
     <row r="46" spans="2:11">
-      <c r="B46" s="27"/>
-      <c r="C46" s="8"/>
+      <c r="B46" s="27" t="s">
+        <v>102</v>
+      </c>
+      <c r="C46" s="8" t="s">
+        <v>103</v>
+      </c>
       <c r="D46" s="8"/>
       <c r="E46" s="9"/>
       <c r="F46" s="2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="G46" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="H46" s="2" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="I46" s="3">
         <v>0</v>
@@ -2385,13 +2393,13 @@
       <c r="D47" s="8"/>
       <c r="E47" s="9"/>
       <c r="F47" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G47" s="2" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="H47" s="2" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="I47" s="3">
         <v>0</v>
@@ -2400,67 +2408,67 @@
       <c r="K47" s="40"/>
     </row>
     <row r="48" spans="2:11">
-      <c r="B48" s="30"/>
-      <c r="C48" s="15"/>
-      <c r="D48" s="15"/>
-      <c r="E48" s="16"/>
-      <c r="F48" s="17" t="s">
+      <c r="B48" s="27"/>
+      <c r="C48" s="8"/>
+      <c r="D48" s="8"/>
+      <c r="E48" s="9"/>
+      <c r="F48" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G48" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="H48" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="I48" s="3">
+        <v>0</v>
+      </c>
+      <c r="J48" s="39"/>
+      <c r="K48" s="40"/>
+    </row>
+    <row r="49" spans="2:11">
+      <c r="B49" s="30"/>
+      <c r="C49" s="15"/>
+      <c r="D49" s="15"/>
+      <c r="E49" s="16"/>
+      <c r="F49" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="G48" s="17" t="s">
-        <v>87</v>
-      </c>
-      <c r="H48" s="17" t="s">
-        <v>103</v>
-      </c>
-      <c r="I48" s="18">
-        <v>0</v>
-      </c>
-      <c r="J48" s="41"/>
-      <c r="K48" s="40"/>
-    </row>
-    <row r="49" spans="2:11">
-      <c r="B49" s="31" t="s">
-        <v>104</v>
-      </c>
-      <c r="C49" s="19" t="s">
-        <v>105</v>
-      </c>
-      <c r="D49" s="19"/>
-      <c r="E49" s="20"/>
-      <c r="F49" s="21" t="s">
+      <c r="G49" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="H49" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="I49" s="18">
+        <v>0</v>
+      </c>
+      <c r="J49" s="41"/>
+      <c r="K49" s="40"/>
+    </row>
+    <row r="50" spans="2:11">
+      <c r="B50" s="31" t="s">
+        <v>108</v>
+      </c>
+      <c r="C50" s="19" t="s">
+        <v>109</v>
+      </c>
+      <c r="D50" s="19"/>
+      <c r="E50" s="20"/>
+      <c r="F50" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="G49" s="21" t="s">
+      <c r="G50" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="H49" s="21" t="s">
-        <v>106</v>
-      </c>
-      <c r="I49" s="22">
-        <v>0</v>
-      </c>
-      <c r="J49" s="42"/>
-      <c r="K49" s="40"/>
-    </row>
-    <row r="50" spans="2:11">
-      <c r="B50" s="27"/>
-      <c r="C50" s="8"/>
-      <c r="D50" s="8"/>
-      <c r="E50" s="9"/>
-      <c r="F50" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="G50" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="H50" s="11" t="s">
-        <v>108</v>
-      </c>
-      <c r="I50" s="10">
-        <v>0</v>
-      </c>
-      <c r="J50" s="43"/>
+      <c r="H50" s="21" t="s">
+        <v>110</v>
+      </c>
+      <c r="I50" s="22">
+        <v>0</v>
+      </c>
+      <c r="J50" s="42"/>
       <c r="K50" s="40"/>
     </row>
     <row r="51" spans="2:11">
@@ -2469,13 +2477,13 @@
       <c r="D51" s="8"/>
       <c r="E51" s="9"/>
       <c r="F51" s="11" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="G51" s="11" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="H51" s="11" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="I51" s="10">
         <v>0</v>
@@ -2488,19 +2496,19 @@
       <c r="C52" s="8"/>
       <c r="D52" s="8"/>
       <c r="E52" s="9"/>
-      <c r="F52" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="G52" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="H52" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="I52" s="3">
-        <v>0</v>
-      </c>
-      <c r="J52" s="39"/>
+      <c r="F52" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="G52" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="H52" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="I52" s="10">
+        <v>0</v>
+      </c>
+      <c r="J52" s="43"/>
       <c r="K52" s="40"/>
     </row>
     <row r="53" spans="2:11">
@@ -2509,13 +2517,13 @@
       <c r="D53" s="8"/>
       <c r="E53" s="9"/>
       <c r="F53" s="2" t="s">
-        <v>22</v>
+        <v>39</v>
       </c>
       <c r="G53" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="H53" s="2" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="I53" s="3">
         <v>0</v>
@@ -2524,15 +2532,15 @@
       <c r="K53" s="40"/>
     </row>
     <row r="54" spans="2:11">
-      <c r="B54" s="30"/>
-      <c r="C54" s="15"/>
-      <c r="D54" s="15"/>
-      <c r="E54" s="16"/>
+      <c r="B54" s="27"/>
+      <c r="C54" s="8"/>
+      <c r="D54" s="8"/>
+      <c r="E54" s="9"/>
       <c r="F54" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="G54" s="2" t="s">
-        <v>114</v>
+        <v>97</v>
       </c>
       <c r="H54" s="2" t="s">
         <v>115</v>
@@ -2544,22 +2552,18 @@
       <c r="K54" s="40"/>
     </row>
     <row r="55" spans="2:11">
-      <c r="B55" s="31" t="s">
+      <c r="B55" s="30"/>
+      <c r="C55" s="15"/>
+      <c r="D55" s="15"/>
+      <c r="E55" s="16"/>
+      <c r="F55" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G55" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="C55" s="19" t="s">
+      <c r="H55" s="2" t="s">
         <v>117</v>
-      </c>
-      <c r="D55" s="19"/>
-      <c r="E55" s="20"/>
-      <c r="F55" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="G55" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="H55" s="2" t="s">
-        <v>119</v>
       </c>
       <c r="I55" s="3">
         <v>0</v>
@@ -2568,20 +2572,26 @@
       <c r="K55" s="40"/>
     </row>
     <row r="56" spans="2:11">
-      <c r="B56" s="27"/>
-      <c r="C56" s="8"/>
-      <c r="D56" s="8"/>
-      <c r="E56" s="9"/>
+      <c r="B56" s="31" t="s">
+        <v>118</v>
+      </c>
+      <c r="C56" s="19" t="s">
+        <v>119</v>
+      </c>
+      <c r="D56" s="19"/>
+      <c r="E56" s="20"/>
       <c r="F56" s="2" t="s">
-        <v>107</v>
+        <v>120</v>
       </c>
       <c r="G56" s="2" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="H56" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="I56" s="3"/>
+        <v>121</v>
+      </c>
+      <c r="I56" s="3">
+        <v>0</v>
+      </c>
       <c r="J56" s="39"/>
       <c r="K56" s="40"/>
     </row>
@@ -2591,17 +2601,15 @@
       <c r="D57" s="8"/>
       <c r="E57" s="9"/>
       <c r="F57" s="2" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="G57" s="2" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="H57" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="I57" s="3">
-        <v>0</v>
-      </c>
+        <v>122</v>
+      </c>
+      <c r="I57" s="3"/>
       <c r="J57" s="39"/>
       <c r="K57" s="40"/>
     </row>
@@ -2611,13 +2619,13 @@
       <c r="D58" s="8"/>
       <c r="E58" s="9"/>
       <c r="F58" s="2" t="s">
-        <v>111</v>
+        <v>36</v>
       </c>
       <c r="G58" s="2" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="H58" s="2" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="I58" s="3">
         <v>0</v>
@@ -2631,15 +2639,17 @@
       <c r="D59" s="8"/>
       <c r="E59" s="9"/>
       <c r="F59" s="2" t="s">
-        <v>22</v>
+        <v>39</v>
       </c>
       <c r="G59" s="2" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="H59" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="I59" s="3"/>
+        <v>124</v>
+      </c>
+      <c r="I59" s="3">
+        <v>0</v>
+      </c>
       <c r="J59" s="39"/>
       <c r="K59" s="40"/>
     </row>
@@ -2649,71 +2659,69 @@
       <c r="D60" s="8"/>
       <c r="E60" s="9"/>
       <c r="F60" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="G60" s="2" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="H60" s="2" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="I60" s="3"/>
       <c r="J60" s="39"/>
       <c r="K60" s="40"/>
     </row>
     <row r="61" spans="2:11">
-      <c r="B61" s="29" t="s">
-        <v>125</v>
-      </c>
-      <c r="C61" s="12" t="s">
+      <c r="B61" s="27"/>
+      <c r="C61" s="8"/>
+      <c r="D61" s="8"/>
+      <c r="E61" s="9"/>
+      <c r="F61" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G61" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="H61" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="D61" s="12" t="s">
-        <v>127</v>
-      </c>
-      <c r="E61" s="13"/>
-      <c r="F61" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G61" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="H61" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I61" s="3">
-        <v>0</v>
-      </c>
+      <c r="I61" s="3"/>
       <c r="J61" s="39"/>
       <c r="K61" s="40"/>
     </row>
     <row r="62" spans="2:11">
-      <c r="B62" s="27"/>
-      <c r="C62" s="8"/>
-      <c r="D62" s="8"/>
-      <c r="E62" s="9"/>
+      <c r="B62" s="29" t="s">
+        <v>127</v>
+      </c>
+      <c r="C62" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="D62" s="12" t="s">
+        <v>129</v>
+      </c>
+      <c r="E62" s="13"/>
       <c r="F62" s="2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="G62" s="2" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="H62" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="I62" s="3" t="s">
-        <v>130</v>
+      <c r="I62" s="3">
+        <v>0</v>
       </c>
       <c r="J62" s="39"/>
       <c r="K62" s="40"/>
     </row>
     <row r="63" spans="2:11">
-      <c r="B63" s="28"/>
-      <c r="C63" s="10"/>
-      <c r="D63" s="10"/>
-      <c r="E63" s="11"/>
+      <c r="B63" s="27"/>
+      <c r="C63" s="8"/>
+      <c r="D63" s="8"/>
+      <c r="E63" s="9"/>
       <c r="F63" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G63" s="2" t="s">
         <v>131</v>
@@ -2727,44 +2735,44 @@
       <c r="J63" s="39"/>
       <c r="K63" s="40"/>
     </row>
-    <row r="64" spans="2:11" ht="93.75">
-      <c r="B64" s="29" t="s">
+    <row r="64" spans="2:11">
+      <c r="B64" s="28"/>
+      <c r="C64" s="10"/>
+      <c r="D64" s="10"/>
+      <c r="E64" s="11"/>
+      <c r="F64" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G64" s="2" t="s">
         <v>133</v>
-      </c>
-      <c r="C64" s="12" t="s">
-        <v>134</v>
-      </c>
-      <c r="D64" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="E64" s="14" t="s">
-        <v>136</v>
-      </c>
-      <c r="F64" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G64" s="2" t="s">
-        <v>137</v>
       </c>
       <c r="H64" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="I64" s="3">
-        <v>0</v>
+      <c r="I64" s="3" t="s">
+        <v>134</v>
       </c>
       <c r="J64" s="39"/>
       <c r="K64" s="40"/>
     </row>
-    <row r="65" spans="2:11">
-      <c r="B65" s="30"/>
-      <c r="C65" s="15"/>
-      <c r="D65" s="15"/>
-      <c r="E65" s="16"/>
+    <row r="65" spans="2:11" ht="93.75">
+      <c r="B65" s="29" t="s">
+        <v>135</v>
+      </c>
+      <c r="C65" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="D65" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="E65" s="14" t="s">
+        <v>138</v>
+      </c>
       <c r="F65" s="2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="G65" s="2" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="H65" s="2" t="s">
         <v>14</v>
@@ -2775,22 +2783,16 @@
       <c r="J65" s="39"/>
       <c r="K65" s="40"/>
     </row>
-    <row r="66" spans="2:11" ht="67.5">
-      <c r="B66" s="31" t="s">
-        <v>139</v>
-      </c>
-      <c r="C66" s="19" t="s">
-        <v>134</v>
-      </c>
-      <c r="D66" s="19"/>
-      <c r="E66" s="48" t="s">
+    <row r="66" spans="2:11">
+      <c r="B66" s="30"/>
+      <c r="C66" s="15"/>
+      <c r="D66" s="15"/>
+      <c r="E66" s="16"/>
+      <c r="F66" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G66" s="2" t="s">
         <v>140</v>
-      </c>
-      <c r="F66" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G66" s="2" t="s">
-        <v>141</v>
       </c>
       <c r="H66" s="2" t="s">
         <v>14</v>
@@ -2801,16 +2803,22 @@
       <c r="J66" s="39"/>
       <c r="K66" s="40"/>
     </row>
-    <row r="67" spans="2:11">
-      <c r="B67" s="30"/>
-      <c r="C67" s="15"/>
-      <c r="D67" s="15"/>
-      <c r="E67" s="16"/>
+    <row r="67" spans="2:11" ht="67.5">
+      <c r="B67" s="31" t="s">
+        <v>141</v>
+      </c>
+      <c r="C67" s="19" t="s">
+        <v>136</v>
+      </c>
+      <c r="D67" s="19"/>
+      <c r="E67" s="48" t="s">
+        <v>142</v>
+      </c>
       <c r="F67" s="2" t="s">
-        <v>107</v>
+        <v>12</v>
       </c>
       <c r="G67" s="2" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="H67" s="2" t="s">
         <v>14</v>
@@ -2822,80 +2830,80 @@
       <c r="K67" s="40"/>
     </row>
     <row r="68" spans="2:11">
-      <c r="B68" s="27" t="s">
-        <v>143</v>
-      </c>
-      <c r="C68" s="8" t="s">
+      <c r="B68" s="30"/>
+      <c r="C68" s="15"/>
+      <c r="D68" s="15"/>
+      <c r="E68" s="16"/>
+      <c r="F68" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="G68" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="D68" s="8"/>
-      <c r="E68" s="9"/>
-      <c r="F68" s="13" t="s">
-        <v>118</v>
-      </c>
-      <c r="G68" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="H68" s="13" t="s">
+      <c r="H68" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I68" s="3">
+        <v>0</v>
+      </c>
+      <c r="J68" s="39"/>
+      <c r="K68" s="40"/>
+    </row>
+    <row r="69" spans="2:11">
+      <c r="B69" s="27" t="s">
         <v>145</v>
       </c>
-      <c r="I68" s="12">
-        <v>0</v>
-      </c>
-      <c r="J68" s="46"/>
-      <c r="K68" s="47"/>
-    </row>
-    <row r="69" spans="2:11" ht="67.5">
-      <c r="B69" s="27"/>
-      <c r="C69" s="8"/>
+      <c r="C69" s="8" t="s">
+        <v>146</v>
+      </c>
       <c r="D69" s="8"/>
       <c r="E69" s="9"/>
       <c r="F69" s="13" t="s">
-        <v>107</v>
+        <v>120</v>
       </c>
       <c r="G69" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="H69" s="14" t="s">
-        <v>146</v>
-      </c>
-      <c r="I69" s="12"/>
+      <c r="H69" s="13" t="s">
+        <v>147</v>
+      </c>
+      <c r="I69" s="12">
+        <v>0</v>
+      </c>
       <c r="J69" s="46"/>
       <c r="K69" s="47"/>
     </row>
-    <row r="70" spans="2:11" ht="90">
+    <row r="70" spans="2:11" ht="67.5">
       <c r="B70" s="27"/>
       <c r="C70" s="8"/>
       <c r="D70" s="8"/>
       <c r="E70" s="9"/>
       <c r="F70" s="13" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="G70" s="13" t="s">
         <v>20</v>
       </c>
       <c r="H70" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="I70" s="12">
-        <v>0</v>
-      </c>
+        <v>148</v>
+      </c>
+      <c r="I70" s="12"/>
       <c r="J70" s="46"/>
       <c r="K70" s="47"/>
     </row>
-    <row r="71" spans="2:11" ht="67.5">
+    <row r="71" spans="2:11" ht="90">
       <c r="B71" s="27"/>
       <c r="C71" s="8"/>
       <c r="D71" s="8"/>
       <c r="E71" s="9"/>
       <c r="F71" s="13" t="s">
-        <v>111</v>
+        <v>36</v>
       </c>
       <c r="G71" s="13" t="s">
         <v>20</v>
       </c>
       <c r="H71" s="14" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="I71" s="12">
         <v>0</v>
@@ -2909,13 +2917,13 @@
       <c r="D72" s="8"/>
       <c r="E72" s="9"/>
       <c r="F72" s="13" t="s">
-        <v>22</v>
+        <v>39</v>
       </c>
       <c r="G72" s="13" t="s">
         <v>20</v>
       </c>
       <c r="H72" s="14" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="I72" s="12">
         <v>0</v>
@@ -2929,13 +2937,13 @@
       <c r="D73" s="8"/>
       <c r="E73" s="9"/>
       <c r="F73" s="13" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="G73" s="13" t="s">
         <v>20</v>
       </c>
       <c r="H73" s="14" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="I73" s="12">
         <v>0</v>
@@ -2949,13 +2957,13 @@
       <c r="D74" s="8"/>
       <c r="E74" s="9"/>
       <c r="F74" s="13" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="G74" s="13" t="s">
         <v>20</v>
       </c>
       <c r="H74" s="14" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="I74" s="12">
         <v>0</v>
@@ -2969,13 +2977,13 @@
       <c r="D75" s="8"/>
       <c r="E75" s="9"/>
       <c r="F75" s="13" t="s">
-        <v>89</v>
+        <v>26</v>
       </c>
       <c r="G75" s="13" t="s">
         <v>20</v>
       </c>
       <c r="H75" s="14" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="I75" s="12">
         <v>0</v>
@@ -2983,19 +2991,19 @@
       <c r="J75" s="46"/>
       <c r="K75" s="47"/>
     </row>
-    <row r="76" spans="2:11" ht="45">
+    <row r="76" spans="2:11" ht="67.5">
       <c r="B76" s="27"/>
       <c r="C76" s="8"/>
       <c r="D76" s="8"/>
       <c r="E76" s="9"/>
       <c r="F76" s="13" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="G76" s="13" t="s">
         <v>20</v>
       </c>
       <c r="H76" s="14" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="I76" s="12">
         <v>0</v>
@@ -3003,43 +3011,63 @@
       <c r="J76" s="46"/>
       <c r="K76" s="47"/>
     </row>
-    <row r="77" spans="2:11">
-      <c r="B77" s="31" t="s">
-        <v>154</v>
-      </c>
-      <c r="C77" s="19" t="s">
+    <row r="77" spans="2:11" ht="45">
+      <c r="B77" s="27"/>
+      <c r="C77" s="8"/>
+      <c r="D77" s="8"/>
+      <c r="E77" s="9"/>
+      <c r="F77" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="G77" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="H77" s="14" t="s">
         <v>155</v>
       </c>
-      <c r="D77" s="19"/>
-      <c r="E77" s="48" t="s">
-        <v>156</v>
-      </c>
-      <c r="F77" s="13"/>
-      <c r="G77" s="13"/>
-      <c r="H77" s="13"/>
-      <c r="I77" s="12"/>
+      <c r="I77" s="12">
+        <v>0</v>
+      </c>
       <c r="J77" s="46"/>
       <c r="K77" s="47"/>
     </row>
     <row r="78" spans="2:11">
-      <c r="B78" s="32" t="s">
+      <c r="B78" s="31" t="s">
+        <v>156</v>
+      </c>
+      <c r="C78" s="19" t="s">
         <v>157</v>
       </c>
-      <c r="C78" s="33" t="s">
+      <c r="D78" s="19"/>
+      <c r="E78" s="48" t="s">
         <v>158</v>
       </c>
-      <c r="D78" s="33" t="s">
+      <c r="F78" s="13"/>
+      <c r="G78" s="13"/>
+      <c r="H78" s="13"/>
+      <c r="I78" s="12"/>
+      <c r="J78" s="46"/>
+      <c r="K78" s="47"/>
+    </row>
+    <row r="79" spans="2:11">
+      <c r="B79" s="32" t="s">
         <v>159</v>
       </c>
-      <c r="E78" s="34" t="s">
+      <c r="C79" s="33" t="s">
         <v>160</v>
       </c>
-      <c r="F78" s="34"/>
-      <c r="G78" s="34"/>
-      <c r="H78" s="34"/>
-      <c r="I78" s="33"/>
-      <c r="J78" s="44"/>
-      <c r="K78" s="45"/>
+      <c r="D79" s="33" t="s">
+        <v>161</v>
+      </c>
+      <c r="E79" s="34" t="s">
+        <v>162</v>
+      </c>
+      <c r="F79" s="34"/>
+      <c r="G79" s="34"/>
+      <c r="H79" s="34"/>
+      <c r="I79" s="33"/>
+      <c r="J79" s="44"/>
+      <c r="K79" s="45"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>

</xml_diff>

<commit_message>
add an sample for labels bit field property
(refs: rggen/rggen#126)
</commit_message>
<xml_diff>
--- a/block_0.xlsx
+++ b/block_0.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25803"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26012"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="163" documentId="8_{A0D56F00-2FF8-4245-9EBC-D59D5B1EA094}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F4D8A63D-83F7-4872-8050-5C59A83B08C0}"/>
+  <xr:revisionPtr revIDLastSave="186" documentId="8_{A0D56F00-2FF8-4245-9EBC-D59D5B1EA094}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{35F1DE00-9324-445A-9C1B-8EE8982BD35F}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="165">
   <si>
     <t>block name</t>
     <phoneticPr fontId="1"/>
@@ -73,6 +73,9 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
+    <t>labels</t>
+  </si>
+  <si>
     <t>comment</t>
   </si>
   <si>
@@ -136,6 +139,14 @@
   <si>
     <t>register_1</t>
     <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>name: foo
+value: 0
+comment: FOO value
+name: bar
+value: 1
+comment: BAR value</t>
   </si>
   <si>
     <t>register_2</t>
@@ -1108,7 +1119,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -1160,6 +1171,9 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1442,9 +1456,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:K79"/>
+  <dimension ref="B1:L79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A72" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12:XFD12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
   <cols>
@@ -1455,11 +1471,11 @@
     <col min="7" max="7" width="11.625" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="18.625" style="1" customWidth="1"/>
     <col min="9" max="9" width="11.375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="24.625" customWidth="1"/>
+    <col min="10" max="11" width="20.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="24.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11">
+    <row r="1" spans="2:12">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1467,7 +1483,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="2:11">
+    <row r="2" spans="2:12">
       <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
@@ -1475,7 +1491,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="4" spans="2:11">
+    <row r="4" spans="2:12">
       <c r="B4" s="23" t="s">
         <v>3</v>
       </c>
@@ -1503,1571 +1519,1651 @@
       <c r="J4" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="K4" s="36" t="s">
+      <c r="K4" s="35" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="5" spans="2:11">
+      <c r="L4" s="36" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12">
       <c r="B5" s="26" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C5" s="6"/>
       <c r="D5" s="6"/>
       <c r="E5" s="7"/>
       <c r="F5" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I5" s="4">
         <v>0</v>
       </c>
       <c r="J5" s="37"/>
-      <c r="K5" s="38" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="2:11">
+      <c r="K5" s="37"/>
+      <c r="L5" s="38" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12">
       <c r="B6" s="27"/>
       <c r="C6" s="8"/>
       <c r="D6" s="8"/>
       <c r="E6" s="9"/>
       <c r="F6" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I6" s="3">
         <v>0</v>
       </c>
       <c r="J6" s="39"/>
-      <c r="K6" s="40"/>
-    </row>
-    <row r="7" spans="2:11">
+      <c r="K6" s="39"/>
+      <c r="L6" s="40"/>
+    </row>
+    <row r="7" spans="2:12">
       <c r="B7" s="27"/>
       <c r="C7" s="8"/>
       <c r="D7" s="8"/>
       <c r="E7" s="9"/>
       <c r="F7" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I7" s="3">
         <v>0</v>
       </c>
       <c r="J7" s="39"/>
-      <c r="K7" s="40"/>
-    </row>
-    <row r="8" spans="2:11">
+      <c r="K7" s="39"/>
+      <c r="L7" s="40"/>
+    </row>
+    <row r="8" spans="2:12">
       <c r="B8" s="27"/>
       <c r="C8" s="8"/>
       <c r="D8" s="8"/>
       <c r="E8" s="9"/>
       <c r="F8" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I8" s="3">
         <v>0</v>
       </c>
       <c r="J8" s="39"/>
-      <c r="K8" s="40"/>
-    </row>
-    <row r="9" spans="2:11">
+      <c r="K8" s="39"/>
+      <c r="L8" s="40"/>
+    </row>
+    <row r="9" spans="2:12">
       <c r="B9" s="27"/>
       <c r="C9" s="8"/>
       <c r="D9" s="8"/>
       <c r="E9" s="9"/>
       <c r="F9" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I9" s="3">
         <v>0</v>
       </c>
       <c r="J9" s="39"/>
-      <c r="K9" s="40"/>
-    </row>
-    <row r="10" spans="2:11">
+      <c r="K9" s="39"/>
+      <c r="L9" s="40"/>
+    </row>
+    <row r="10" spans="2:12">
       <c r="B10" s="27"/>
       <c r="C10" s="8"/>
       <c r="D10" s="8"/>
       <c r="E10" s="9"/>
       <c r="F10" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I10" s="3">
         <v>0</v>
       </c>
       <c r="J10" s="39"/>
-      <c r="K10" s="40"/>
-    </row>
-    <row r="11" spans="2:11">
+      <c r="K10" s="39"/>
+      <c r="L10" s="40"/>
+    </row>
+    <row r="11" spans="2:12">
       <c r="B11" s="28"/>
       <c r="C11" s="10"/>
       <c r="D11" s="10"/>
       <c r="E11" s="11"/>
       <c r="F11" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="I11" s="3">
         <v>0</v>
       </c>
       <c r="J11" s="39"/>
-      <c r="K11" s="40"/>
-    </row>
-    <row r="12" spans="2:11">
+      <c r="K11" s="39"/>
+      <c r="L11" s="40"/>
+    </row>
+    <row r="12" spans="2:12" ht="202.5">
       <c r="B12" s="29" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C12" s="12"/>
       <c r="D12" s="12"/>
       <c r="E12" s="13"/>
       <c r="F12" s="2"/>
       <c r="G12" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I12" s="3">
         <v>0</v>
       </c>
       <c r="J12" s="39"/>
-      <c r="K12" s="40"/>
-    </row>
-    <row r="13" spans="2:11">
+      <c r="K12" s="49" t="s">
+        <v>30</v>
+      </c>
+      <c r="L12" s="40"/>
+    </row>
+    <row r="13" spans="2:12">
       <c r="B13" s="29" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D13" s="12"/>
       <c r="E13" s="13"/>
       <c r="F13" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="I13" s="3"/>
       <c r="J13" s="39"/>
-      <c r="K13" s="40"/>
-    </row>
-    <row r="14" spans="2:11">
+      <c r="K13" s="39"/>
+      <c r="L13" s="40"/>
+    </row>
+    <row r="14" spans="2:12">
       <c r="B14" s="27"/>
       <c r="C14" s="8"/>
       <c r="D14" s="8"/>
       <c r="E14" s="9"/>
       <c r="F14" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="J14" s="39"/>
-      <c r="K14" s="40"/>
-    </row>
-    <row r="15" spans="2:11">
+      <c r="K14" s="39"/>
+      <c r="L14" s="40"/>
+    </row>
+    <row r="15" spans="2:12">
       <c r="B15" s="27"/>
       <c r="C15" s="8"/>
       <c r="D15" s="8"/>
       <c r="E15" s="9"/>
       <c r="F15" s="2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="I15" s="3">
         <v>0</v>
       </c>
       <c r="J15" s="39"/>
-      <c r="K15" s="40"/>
-    </row>
-    <row r="16" spans="2:11">
+      <c r="K15" s="39"/>
+      <c r="L15" s="40"/>
+    </row>
+    <row r="16" spans="2:12">
       <c r="B16" s="27"/>
       <c r="C16" s="8"/>
       <c r="D16" s="8"/>
       <c r="E16" s="9"/>
       <c r="F16" s="2" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="G16" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="H16" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="H16" s="2" t="s">
-        <v>38</v>
-      </c>
       <c r="I16" s="3">
         <v>0</v>
       </c>
       <c r="J16" s="39" t="s">
-        <v>41</v>
-      </c>
-      <c r="K16" s="40"/>
-    </row>
-    <row r="17" spans="2:11">
+        <v>43</v>
+      </c>
+      <c r="K16" s="39"/>
+      <c r="L16" s="40"/>
+    </row>
+    <row r="17" spans="2:12">
       <c r="B17" s="28"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="11"/>
       <c r="F17" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="I17" s="3"/>
       <c r="J17" s="39"/>
-      <c r="K17" s="40"/>
-    </row>
-    <row r="18" spans="2:11">
+      <c r="K17" s="39"/>
+      <c r="L17" s="40"/>
+    </row>
+    <row r="18" spans="2:12">
       <c r="B18" s="29" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D18" s="12"/>
       <c r="E18" s="13"/>
       <c r="F18" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="I18" s="3">
         <v>0</v>
       </c>
       <c r="J18" s="39"/>
-      <c r="K18" s="40"/>
-    </row>
-    <row r="19" spans="2:11">
+      <c r="K18" s="39"/>
+      <c r="L18" s="40"/>
+    </row>
+    <row r="19" spans="2:12">
       <c r="B19" s="27"/>
       <c r="C19" s="8"/>
       <c r="D19" s="8"/>
       <c r="E19" s="9"/>
       <c r="F19" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="I19" s="3">
         <v>0</v>
       </c>
       <c r="J19" s="39"/>
-      <c r="K19" s="40"/>
-    </row>
-    <row r="20" spans="2:11">
+      <c r="K19" s="39"/>
+      <c r="L19" s="40"/>
+    </row>
+    <row r="20" spans="2:12">
       <c r="B20" s="27"/>
       <c r="C20" s="8"/>
       <c r="D20" s="8"/>
       <c r="E20" s="9"/>
       <c r="F20" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="I20" s="3"/>
       <c r="J20" s="39"/>
-      <c r="K20" s="40"/>
-    </row>
-    <row r="21" spans="2:11">
+      <c r="K20" s="39"/>
+      <c r="L20" s="40"/>
+    </row>
+    <row r="21" spans="2:12">
       <c r="B21" s="27"/>
       <c r="C21" s="8"/>
       <c r="D21" s="8"/>
       <c r="E21" s="9"/>
       <c r="F21" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="I21" s="3"/>
       <c r="J21" s="39"/>
-      <c r="K21" s="40"/>
-    </row>
-    <row r="22" spans="2:11">
+      <c r="K21" s="39"/>
+      <c r="L21" s="40"/>
+    </row>
+    <row r="22" spans="2:12">
       <c r="B22" s="29" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C22" s="12" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D22" s="12"/>
       <c r="E22" s="13"/>
       <c r="F22" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="I22" s="3">
         <v>0</v>
       </c>
       <c r="J22" s="39"/>
-      <c r="K22" s="40"/>
-    </row>
-    <row r="23" spans="2:11">
+      <c r="K22" s="39"/>
+      <c r="L22" s="40"/>
+    </row>
+    <row r="23" spans="2:12">
       <c r="B23" s="27"/>
       <c r="C23" s="8"/>
       <c r="D23" s="8"/>
       <c r="E23" s="9"/>
       <c r="F23" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="I23" s="3">
         <v>0</v>
       </c>
       <c r="J23" s="39" t="s">
-        <v>54</v>
-      </c>
-      <c r="K23" s="40"/>
-    </row>
-    <row r="24" spans="2:11">
+        <v>56</v>
+      </c>
+      <c r="K23" s="39"/>
+      <c r="L23" s="40"/>
+    </row>
+    <row r="24" spans="2:12">
       <c r="B24" s="27"/>
       <c r="C24" s="8"/>
       <c r="D24" s="8"/>
       <c r="E24" s="9"/>
       <c r="F24" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="I24" s="3"/>
       <c r="J24" s="39" t="s">
-        <v>56</v>
-      </c>
-      <c r="K24" s="40"/>
-    </row>
-    <row r="25" spans="2:11">
+        <v>58</v>
+      </c>
+      <c r="K24" s="39"/>
+      <c r="L24" s="40"/>
+    </row>
+    <row r="25" spans="2:12">
       <c r="B25" s="28"/>
       <c r="C25" s="10"/>
       <c r="D25" s="10"/>
       <c r="E25" s="11"/>
       <c r="F25" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="I25" s="3">
         <v>0</v>
       </c>
       <c r="J25" s="39"/>
-      <c r="K25" s="40"/>
-    </row>
-    <row r="26" spans="2:11">
+      <c r="K25" s="39"/>
+      <c r="L25" s="40"/>
+    </row>
+    <row r="26" spans="2:12">
       <c r="B26" s="29" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C26" s="12" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D26" s="12"/>
       <c r="E26" s="13"/>
       <c r="F26" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="I26" s="3">
         <v>0</v>
       </c>
       <c r="J26" s="39"/>
-      <c r="K26" s="40"/>
-    </row>
-    <row r="27" spans="2:11">
+      <c r="K26" s="39"/>
+      <c r="L26" s="40"/>
+    </row>
+    <row r="27" spans="2:12">
       <c r="B27" s="27"/>
       <c r="C27" s="8"/>
       <c r="D27" s="8"/>
       <c r="E27" s="9"/>
       <c r="F27" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="I27" s="3">
         <v>0</v>
       </c>
       <c r="J27" s="39" t="s">
-        <v>63</v>
-      </c>
-      <c r="K27" s="40"/>
-    </row>
-    <row r="28" spans="2:11">
+        <v>65</v>
+      </c>
+      <c r="K27" s="39"/>
+      <c r="L27" s="40"/>
+    </row>
+    <row r="28" spans="2:12">
       <c r="B28" s="27"/>
       <c r="C28" s="8"/>
       <c r="D28" s="8"/>
       <c r="E28" s="9"/>
       <c r="F28" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="I28" s="3">
         <v>0</v>
       </c>
       <c r="J28" s="39"/>
-      <c r="K28" s="40"/>
-    </row>
-    <row r="29" spans="2:11">
+      <c r="K28" s="39"/>
+      <c r="L28" s="40"/>
+    </row>
+    <row r="29" spans="2:12">
       <c r="B29" s="27"/>
       <c r="C29" s="8"/>
       <c r="D29" s="8"/>
       <c r="E29" s="9"/>
       <c r="F29" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="I29" s="3">
         <v>0</v>
       </c>
       <c r="J29" s="39" t="s">
-        <v>67</v>
-      </c>
-      <c r="K29" s="40"/>
-    </row>
-    <row r="30" spans="2:11">
+        <v>69</v>
+      </c>
+      <c r="K29" s="39"/>
+      <c r="L29" s="40"/>
+    </row>
+    <row r="30" spans="2:12">
       <c r="B30" s="27"/>
       <c r="C30" s="8"/>
       <c r="D30" s="8"/>
       <c r="E30" s="9"/>
       <c r="F30" s="2" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="I30" s="3">
         <v>0</v>
       </c>
       <c r="J30" s="39"/>
-      <c r="K30" s="40"/>
-    </row>
-    <row r="31" spans="2:11">
+      <c r="K30" s="39"/>
+      <c r="L30" s="40"/>
+    </row>
+    <row r="31" spans="2:12">
       <c r="B31" s="27"/>
       <c r="C31" s="8"/>
       <c r="D31" s="8"/>
       <c r="E31" s="9"/>
       <c r="F31" s="2" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="G31" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="H31" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="H31" s="2" t="s">
-        <v>70</v>
-      </c>
       <c r="I31" s="3">
         <v>0</v>
       </c>
       <c r="J31" s="39" t="s">
-        <v>73</v>
-      </c>
-      <c r="K31" s="40"/>
-    </row>
-    <row r="32" spans="2:11">
+        <v>75</v>
+      </c>
+      <c r="K31" s="39"/>
+      <c r="L31" s="40"/>
+    </row>
+    <row r="32" spans="2:12">
       <c r="B32" s="27"/>
       <c r="C32" s="8"/>
       <c r="D32" s="8"/>
       <c r="E32" s="9"/>
       <c r="F32" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="I32" s="3">
         <v>0</v>
       </c>
       <c r="J32" s="39" t="s">
-        <v>28</v>
-      </c>
-      <c r="K32" s="40"/>
-    </row>
-    <row r="33" spans="2:11">
+        <v>29</v>
+      </c>
+      <c r="K32" s="39"/>
+      <c r="L32" s="40"/>
+    </row>
+    <row r="33" spans="2:12">
       <c r="B33" s="27"/>
       <c r="C33" s="8"/>
       <c r="D33" s="8"/>
       <c r="E33" s="9"/>
       <c r="F33" s="2" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="I33" s="3">
         <v>0</v>
       </c>
       <c r="J33" s="39"/>
-      <c r="K33" s="40"/>
-    </row>
-    <row r="34" spans="2:11">
+      <c r="K33" s="39"/>
+      <c r="L33" s="40"/>
+    </row>
+    <row r="34" spans="2:12">
       <c r="B34" s="27"/>
       <c r="C34" s="8"/>
       <c r="D34" s="8"/>
       <c r="E34" s="9"/>
       <c r="F34" s="2" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="G34" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="H34" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="H34" s="2" t="s">
-        <v>78</v>
-      </c>
       <c r="I34" s="3">
         <v>0</v>
       </c>
       <c r="J34" s="39" t="s">
-        <v>81</v>
-      </c>
-      <c r="K34" s="40"/>
-    </row>
-    <row r="35" spans="2:11">
+        <v>83</v>
+      </c>
+      <c r="K34" s="39"/>
+      <c r="L34" s="40"/>
+    </row>
+    <row r="35" spans="2:12">
       <c r="B35" s="28"/>
       <c r="C35" s="10"/>
       <c r="D35" s="10"/>
       <c r="E35" s="11"/>
       <c r="F35" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="H35" s="2" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="I35" s="3">
         <v>0</v>
       </c>
       <c r="J35" s="39" t="s">
-        <v>28</v>
-      </c>
-      <c r="K35" s="40"/>
-    </row>
-    <row r="36" spans="2:11">
+        <v>29</v>
+      </c>
+      <c r="K35" s="39"/>
+      <c r="L35" s="40"/>
+    </row>
+    <row r="36" spans="2:12">
       <c r="B36" s="29" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="C36" s="12" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="D36" s="12"/>
       <c r="E36" s="13"/>
       <c r="F36" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="I36" s="3">
         <v>0</v>
       </c>
       <c r="J36" s="39"/>
-      <c r="K36" s="40"/>
-    </row>
-    <row r="37" spans="2:11">
+      <c r="K36" s="39"/>
+      <c r="L36" s="40"/>
+    </row>
+    <row r="37" spans="2:12">
       <c r="B37" s="27"/>
       <c r="C37" s="8"/>
       <c r="D37" s="8"/>
       <c r="E37" s="9"/>
       <c r="F37" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="I37" s="3">
         <v>0</v>
       </c>
       <c r="J37" s="39" t="s">
-        <v>54</v>
-      </c>
-      <c r="K37" s="40"/>
-    </row>
-    <row r="38" spans="2:11">
+        <v>56</v>
+      </c>
+      <c r="K37" s="39"/>
+      <c r="L37" s="40"/>
+    </row>
+    <row r="38" spans="2:12">
       <c r="B38" s="27"/>
       <c r="C38" s="8"/>
       <c r="D38" s="8"/>
       <c r="E38" s="9"/>
       <c r="F38" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="I38" s="3"/>
       <c r="J38" s="39" t="s">
-        <v>88</v>
-      </c>
-      <c r="K38" s="40"/>
-    </row>
-    <row r="39" spans="2:11">
+        <v>90</v>
+      </c>
+      <c r="K38" s="39"/>
+      <c r="L38" s="40"/>
+    </row>
+    <row r="39" spans="2:12">
       <c r="B39" s="27"/>
       <c r="C39" s="8"/>
       <c r="D39" s="8"/>
       <c r="E39" s="9"/>
       <c r="F39" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="H39" s="2" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="I39" s="3">
         <v>0</v>
       </c>
       <c r="J39" s="39"/>
-      <c r="K39" s="40"/>
-    </row>
-    <row r="40" spans="2:11">
+      <c r="K39" s="39"/>
+      <c r="L39" s="40"/>
+    </row>
+    <row r="40" spans="2:12">
       <c r="B40" s="27"/>
       <c r="C40" s="8"/>
       <c r="D40" s="8"/>
       <c r="E40" s="9"/>
       <c r="F40" s="2" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="H40" s="2" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="I40" s="3">
         <v>0</v>
       </c>
       <c r="J40" s="39" t="s">
-        <v>54</v>
-      </c>
-      <c r="K40" s="40"/>
-    </row>
-    <row r="41" spans="2:11">
+        <v>56</v>
+      </c>
+      <c r="K40" s="39"/>
+      <c r="L40" s="40"/>
+    </row>
+    <row r="41" spans="2:12">
       <c r="B41" s="27"/>
       <c r="C41" s="8"/>
       <c r="D41" s="8"/>
       <c r="E41" s="9"/>
       <c r="F41" s="2" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="G41" s="2" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="H41" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="I41" s="3"/>
       <c r="J41" s="39" t="s">
-        <v>90</v>
-      </c>
-      <c r="K41" s="40"/>
-    </row>
-    <row r="42" spans="2:11">
+        <v>92</v>
+      </c>
+      <c r="K41" s="39"/>
+      <c r="L41" s="40"/>
+    </row>
+    <row r="42" spans="2:12">
       <c r="B42" s="27"/>
       <c r="C42" s="8"/>
       <c r="D42" s="8"/>
       <c r="E42" s="9"/>
       <c r="F42" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="H42" s="2" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="I42" s="3">
         <v>0</v>
       </c>
       <c r="J42" s="39"/>
-      <c r="K42" s="40"/>
-    </row>
-    <row r="43" spans="2:11">
+      <c r="K42" s="39"/>
+      <c r="L42" s="40"/>
+    </row>
+    <row r="43" spans="2:12">
       <c r="B43" s="27"/>
       <c r="C43" s="8"/>
       <c r="D43" s="8"/>
       <c r="E43" s="9"/>
       <c r="F43" s="2" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="G43" s="2" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="H43" s="2" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="I43" s="3">
         <v>0</v>
       </c>
       <c r="J43" s="39"/>
-      <c r="K43" s="40"/>
-    </row>
-    <row r="44" spans="2:11">
+      <c r="K43" s="39"/>
+      <c r="L43" s="40"/>
+    </row>
+    <row r="44" spans="2:12">
       <c r="B44" s="27"/>
       <c r="C44" s="8"/>
       <c r="D44" s="8"/>
       <c r="E44" s="9"/>
       <c r="F44" s="2" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="G44" s="2" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="H44" s="2" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="I44" s="3">
         <v>0</v>
       </c>
       <c r="J44" s="39"/>
-      <c r="K44" s="40"/>
-    </row>
-    <row r="45" spans="2:11">
+      <c r="K44" s="39"/>
+      <c r="L44" s="40"/>
+    </row>
+    <row r="45" spans="2:12">
       <c r="B45" s="28"/>
       <c r="C45" s="10"/>
       <c r="D45" s="10"/>
       <c r="E45" s="11"/>
       <c r="F45" s="2" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="G45" s="2" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="H45" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="I45" s="3">
         <v>0</v>
       </c>
       <c r="J45" s="39"/>
-      <c r="K45" s="40"/>
-    </row>
-    <row r="46" spans="2:11">
+      <c r="K45" s="39"/>
+      <c r="L45" s="40"/>
+    </row>
+    <row r="46" spans="2:12">
       <c r="B46" s="27" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="C46" s="8" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="D46" s="8"/>
       <c r="E46" s="9"/>
       <c r="F46" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G46" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="H46" s="2" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="I46" s="3">
         <v>0</v>
       </c>
       <c r="J46" s="39"/>
-      <c r="K46" s="40"/>
-    </row>
-    <row r="47" spans="2:11">
+      <c r="K46" s="39"/>
+      <c r="L46" s="40"/>
+    </row>
+    <row r="47" spans="2:12">
       <c r="B47" s="27"/>
       <c r="C47" s="8"/>
       <c r="D47" s="8"/>
       <c r="E47" s="9"/>
       <c r="F47" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G47" s="2" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="H47" s="2" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="I47" s="3">
         <v>0</v>
       </c>
       <c r="J47" s="39"/>
-      <c r="K47" s="40"/>
-    </row>
-    <row r="48" spans="2:11">
+      <c r="K47" s="39"/>
+      <c r="L47" s="40"/>
+    </row>
+    <row r="48" spans="2:12">
       <c r="B48" s="27"/>
       <c r="C48" s="8"/>
       <c r="D48" s="8"/>
       <c r="E48" s="9"/>
       <c r="F48" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G48" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="H48" s="2" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="I48" s="3">
         <v>0</v>
       </c>
       <c r="J48" s="39"/>
-      <c r="K48" s="40"/>
-    </row>
-    <row r="49" spans="2:11">
+      <c r="K48" s="39"/>
+      <c r="L48" s="40"/>
+    </row>
+    <row r="49" spans="2:12">
       <c r="B49" s="30"/>
       <c r="C49" s="15"/>
       <c r="D49" s="15"/>
       <c r="E49" s="16"/>
       <c r="F49" s="17" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G49" s="17" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="H49" s="17" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="I49" s="18">
         <v>0</v>
       </c>
       <c r="J49" s="41"/>
-      <c r="K49" s="40"/>
-    </row>
-    <row r="50" spans="2:11">
+      <c r="K49" s="41"/>
+      <c r="L49" s="40"/>
+    </row>
+    <row r="50" spans="2:12">
       <c r="B50" s="31" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="C50" s="19" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="D50" s="19"/>
       <c r="E50" s="20"/>
       <c r="F50" s="21" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G50" s="21" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="H50" s="21" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="I50" s="22">
         <v>0</v>
       </c>
       <c r="J50" s="42"/>
-      <c r="K50" s="40"/>
-    </row>
-    <row r="51" spans="2:11">
+      <c r="K50" s="42"/>
+      <c r="L50" s="40"/>
+    </row>
+    <row r="51" spans="2:12">
       <c r="B51" s="27"/>
       <c r="C51" s="8"/>
       <c r="D51" s="8"/>
       <c r="E51" s="9"/>
       <c r="F51" s="11" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="G51" s="11" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="H51" s="11" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="I51" s="10">
         <v>0</v>
       </c>
       <c r="J51" s="43"/>
-      <c r="K51" s="40"/>
-    </row>
-    <row r="52" spans="2:11">
+      <c r="K51" s="43"/>
+      <c r="L51" s="40"/>
+    </row>
+    <row r="52" spans="2:12">
       <c r="B52" s="27"/>
       <c r="C52" s="8"/>
       <c r="D52" s="8"/>
       <c r="E52" s="9"/>
       <c r="F52" s="11" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="G52" s="11" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="H52" s="11" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="I52" s="10">
         <v>0</v>
       </c>
       <c r="J52" s="43"/>
-      <c r="K52" s="40"/>
-    </row>
-    <row r="53" spans="2:11">
+      <c r="K52" s="43"/>
+      <c r="L52" s="40"/>
+    </row>
+    <row r="53" spans="2:12">
       <c r="B53" s="27"/>
       <c r="C53" s="8"/>
       <c r="D53" s="8"/>
       <c r="E53" s="9"/>
       <c r="F53" s="2" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="G53" s="2" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="H53" s="2" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="I53" s="3">
         <v>0</v>
       </c>
       <c r="J53" s="39"/>
-      <c r="K53" s="40"/>
-    </row>
-    <row r="54" spans="2:11">
+      <c r="K53" s="39"/>
+      <c r="L53" s="40"/>
+    </row>
+    <row r="54" spans="2:12">
       <c r="B54" s="27"/>
       <c r="C54" s="8"/>
       <c r="D54" s="8"/>
       <c r="E54" s="9"/>
       <c r="F54" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G54" s="2" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="H54" s="2" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="I54" s="3">
         <v>0</v>
       </c>
       <c r="J54" s="39"/>
-      <c r="K54" s="40"/>
-    </row>
-    <row r="55" spans="2:11">
+      <c r="K54" s="39"/>
+      <c r="L54" s="40"/>
+    </row>
+    <row r="55" spans="2:12">
       <c r="B55" s="30"/>
       <c r="C55" s="15"/>
       <c r="D55" s="15"/>
       <c r="E55" s="16"/>
       <c r="F55" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G55" s="2" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="H55" s="2" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="I55" s="3">
         <v>0</v>
       </c>
       <c r="J55" s="39"/>
-      <c r="K55" s="40"/>
-    </row>
-    <row r="56" spans="2:11">
+      <c r="K55" s="39"/>
+      <c r="L55" s="40"/>
+    </row>
+    <row r="56" spans="2:12">
       <c r="B56" s="31" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="C56" s="19" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="D56" s="19"/>
       <c r="E56" s="20"/>
       <c r="F56" s="2" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="G56" s="2" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="H56" s="2" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="I56" s="3">
         <v>0</v>
       </c>
       <c r="J56" s="39"/>
-      <c r="K56" s="40"/>
-    </row>
-    <row r="57" spans="2:11">
+      <c r="K56" s="39"/>
+      <c r="L56" s="40"/>
+    </row>
+    <row r="57" spans="2:12">
       <c r="B57" s="27"/>
       <c r="C57" s="8"/>
       <c r="D57" s="8"/>
       <c r="E57" s="9"/>
       <c r="F57" s="2" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="G57" s="2" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="H57" s="2" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="I57" s="3"/>
       <c r="J57" s="39"/>
-      <c r="K57" s="40"/>
-    </row>
-    <row r="58" spans="2:11">
+      <c r="K57" s="39"/>
+      <c r="L57" s="40"/>
+    </row>
+    <row r="58" spans="2:12">
       <c r="B58" s="27"/>
       <c r="C58" s="8"/>
       <c r="D58" s="8"/>
       <c r="E58" s="9"/>
       <c r="F58" s="2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="G58" s="2" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="H58" s="2" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="I58" s="3">
         <v>0</v>
       </c>
       <c r="J58" s="39"/>
-      <c r="K58" s="40"/>
-    </row>
-    <row r="59" spans="2:11">
+      <c r="K58" s="39"/>
+      <c r="L58" s="40"/>
+    </row>
+    <row r="59" spans="2:12">
       <c r="B59" s="27"/>
       <c r="C59" s="8"/>
       <c r="D59" s="8"/>
       <c r="E59" s="9"/>
       <c r="F59" s="2" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="G59" s="2" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="H59" s="2" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="I59" s="3">
         <v>0</v>
       </c>
       <c r="J59" s="39"/>
-      <c r="K59" s="40"/>
-    </row>
-    <row r="60" spans="2:11">
+      <c r="K59" s="39"/>
+      <c r="L59" s="40"/>
+    </row>
+    <row r="60" spans="2:12">
       <c r="B60" s="27"/>
       <c r="C60" s="8"/>
       <c r="D60" s="8"/>
       <c r="E60" s="9"/>
       <c r="F60" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G60" s="2" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="H60" s="2" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="I60" s="3"/>
       <c r="J60" s="39"/>
-      <c r="K60" s="40"/>
-    </row>
-    <row r="61" spans="2:11">
+      <c r="K60" s="39"/>
+      <c r="L60" s="40"/>
+    </row>
+    <row r="61" spans="2:12">
       <c r="B61" s="27"/>
       <c r="C61" s="8"/>
       <c r="D61" s="8"/>
       <c r="E61" s="9"/>
       <c r="F61" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G61" s="2" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="H61" s="2" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="I61" s="3"/>
       <c r="J61" s="39"/>
-      <c r="K61" s="40"/>
-    </row>
-    <row r="62" spans="2:11">
+      <c r="K61" s="39"/>
+      <c r="L61" s="40"/>
+    </row>
+    <row r="62" spans="2:12">
       <c r="B62" s="29" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="C62" s="12" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="D62" s="12" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="E62" s="13"/>
       <c r="F62" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G62" s="2" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="H62" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I62" s="3">
         <v>0</v>
       </c>
       <c r="J62" s="39"/>
-      <c r="K62" s="40"/>
-    </row>
-    <row r="63" spans="2:11">
+      <c r="K62" s="39"/>
+      <c r="L62" s="40"/>
+    </row>
+    <row r="63" spans="2:12">
       <c r="B63" s="27"/>
       <c r="C63" s="8"/>
       <c r="D63" s="8"/>
       <c r="E63" s="9"/>
       <c r="F63" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G63" s="2" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="H63" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I63" s="3" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="J63" s="39"/>
-      <c r="K63" s="40"/>
-    </row>
-    <row r="64" spans="2:11">
+      <c r="K63" s="39"/>
+      <c r="L63" s="40"/>
+    </row>
+    <row r="64" spans="2:12">
       <c r="B64" s="28"/>
       <c r="C64" s="10"/>
       <c r="D64" s="10"/>
       <c r="E64" s="11"/>
       <c r="F64" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G64" s="2" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="H64" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I64" s="3" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="J64" s="39"/>
-      <c r="K64" s="40"/>
-    </row>
-    <row r="65" spans="2:11" ht="93.75">
+      <c r="K64" s="39"/>
+      <c r="L64" s="40"/>
+    </row>
+    <row r="65" spans="2:12" ht="112.5">
       <c r="B65" s="29" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="C65" s="12" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="D65" s="12" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="E65" s="14" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="F65" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G65" s="2" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="H65" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I65" s="3">
         <v>0</v>
       </c>
       <c r="J65" s="39"/>
-      <c r="K65" s="40"/>
-    </row>
-    <row r="66" spans="2:11">
+      <c r="K65" s="39"/>
+      <c r="L65" s="40"/>
+    </row>
+    <row r="66" spans="2:12">
       <c r="B66" s="30"/>
       <c r="C66" s="15"/>
       <c r="D66" s="15"/>
       <c r="E66" s="16"/>
       <c r="F66" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G66" s="2" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="H66" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I66" s="3">
         <v>0</v>
       </c>
       <c r="J66" s="39"/>
-      <c r="K66" s="40"/>
-    </row>
-    <row r="67" spans="2:11" ht="67.5">
+      <c r="K66" s="39"/>
+      <c r="L66" s="40"/>
+    </row>
+    <row r="67" spans="2:12" ht="67.5">
       <c r="B67" s="31" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="C67" s="19" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="D67" s="19"/>
       <c r="E67" s="48" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="F67" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G67" s="2" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="H67" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I67" s="3">
         <v>0</v>
       </c>
       <c r="J67" s="39"/>
-      <c r="K67" s="40"/>
-    </row>
-    <row r="68" spans="2:11">
+      <c r="K67" s="39"/>
+      <c r="L67" s="40"/>
+    </row>
+    <row r="68" spans="2:12">
       <c r="B68" s="30"/>
       <c r="C68" s="15"/>
       <c r="D68" s="15"/>
       <c r="E68" s="16"/>
       <c r="F68" s="2" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="G68" s="2" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="H68" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I68" s="3">
         <v>0</v>
       </c>
       <c r="J68" s="39"/>
-      <c r="K68" s="40"/>
-    </row>
-    <row r="69" spans="2:11">
+      <c r="K68" s="39"/>
+      <c r="L68" s="40"/>
+    </row>
+    <row r="69" spans="2:12">
       <c r="B69" s="27" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="C69" s="8" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="D69" s="8"/>
       <c r="E69" s="9"/>
       <c r="F69" s="13" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="G69" s="13" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H69" s="13" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="I69" s="12">
         <v>0</v>
       </c>
       <c r="J69" s="46"/>
-      <c r="K69" s="47"/>
-    </row>
-    <row r="70" spans="2:11" ht="67.5">
+      <c r="K69" s="46"/>
+      <c r="L69" s="47"/>
+    </row>
+    <row r="70" spans="2:12" ht="45">
       <c r="B70" s="27"/>
       <c r="C70" s="8"/>
       <c r="D70" s="8"/>
       <c r="E70" s="9"/>
       <c r="F70" s="13" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="G70" s="13" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H70" s="14" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="I70" s="12"/>
       <c r="J70" s="46"/>
-      <c r="K70" s="47"/>
-    </row>
-    <row r="71" spans="2:11" ht="90">
+      <c r="K70" s="46"/>
+      <c r="L70" s="47"/>
+    </row>
+    <row r="71" spans="2:12" ht="45">
       <c r="B71" s="27"/>
       <c r="C71" s="8"/>
       <c r="D71" s="8"/>
       <c r="E71" s="9"/>
       <c r="F71" s="13" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="G71" s="13" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H71" s="14" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="I71" s="12">
         <v>0</v>
       </c>
       <c r="J71" s="46"/>
-      <c r="K71" s="47"/>
-    </row>
-    <row r="72" spans="2:11" ht="67.5">
+      <c r="K71" s="46"/>
+      <c r="L71" s="47"/>
+    </row>
+    <row r="72" spans="2:12" ht="67.5">
       <c r="B72" s="27"/>
       <c r="C72" s="8"/>
       <c r="D72" s="8"/>
       <c r="E72" s="9"/>
       <c r="F72" s="13" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="G72" s="13" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H72" s="14" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="I72" s="12">
         <v>0</v>
       </c>
       <c r="J72" s="46"/>
-      <c r="K72" s="47"/>
-    </row>
-    <row r="73" spans="2:11" ht="67.5">
+      <c r="K72" s="46"/>
+      <c r="L72" s="47"/>
+    </row>
+    <row r="73" spans="2:12" ht="67.5">
       <c r="B73" s="27"/>
       <c r="C73" s="8"/>
       <c r="D73" s="8"/>
       <c r="E73" s="9"/>
       <c r="F73" s="13" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G73" s="13" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H73" s="14" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="I73" s="12">
         <v>0</v>
       </c>
       <c r="J73" s="46"/>
-      <c r="K73" s="47"/>
-    </row>
-    <row r="74" spans="2:11" ht="67.5">
+      <c r="K73" s="46"/>
+      <c r="L73" s="47"/>
+    </row>
+    <row r="74" spans="2:12" ht="67.5">
       <c r="B74" s="27"/>
       <c r="C74" s="8"/>
       <c r="D74" s="8"/>
       <c r="E74" s="9"/>
       <c r="F74" s="13" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G74" s="13" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H74" s="14" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="I74" s="12">
         <v>0</v>
       </c>
       <c r="J74" s="46"/>
-      <c r="K74" s="47"/>
-    </row>
-    <row r="75" spans="2:11" ht="67.5">
+      <c r="K74" s="46"/>
+      <c r="L74" s="47"/>
+    </row>
+    <row r="75" spans="2:12" ht="67.5">
       <c r="B75" s="27"/>
       <c r="C75" s="8"/>
       <c r="D75" s="8"/>
       <c r="E75" s="9"/>
       <c r="F75" s="13" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G75" s="13" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H75" s="14" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="I75" s="12">
         <v>0</v>
       </c>
       <c r="J75" s="46"/>
-      <c r="K75" s="47"/>
-    </row>
-    <row r="76" spans="2:11" ht="67.5">
+      <c r="K75" s="46"/>
+      <c r="L75" s="47"/>
+    </row>
+    <row r="76" spans="2:12" ht="67.5">
       <c r="B76" s="27"/>
       <c r="C76" s="8"/>
       <c r="D76" s="8"/>
       <c r="E76" s="9"/>
       <c r="F76" s="13" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="G76" s="13" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H76" s="14" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="I76" s="12">
         <v>0</v>
       </c>
       <c r="J76" s="46"/>
-      <c r="K76" s="47"/>
-    </row>
-    <row r="77" spans="2:11" ht="45">
+      <c r="K76" s="46"/>
+      <c r="L76" s="47"/>
+    </row>
+    <row r="77" spans="2:12" ht="45">
       <c r="B77" s="27"/>
       <c r="C77" s="8"/>
       <c r="D77" s="8"/>
       <c r="E77" s="9"/>
       <c r="F77" s="13" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="G77" s="13" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H77" s="14" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="I77" s="12">
         <v>0</v>
       </c>
       <c r="J77" s="46"/>
-      <c r="K77" s="47"/>
-    </row>
-    <row r="78" spans="2:11">
+      <c r="K77" s="46"/>
+      <c r="L77" s="47"/>
+    </row>
+    <row r="78" spans="2:12" ht="22.5">
       <c r="B78" s="31" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="C78" s="19" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="D78" s="19"/>
       <c r="E78" s="48" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="F78" s="13"/>
       <c r="G78" s="13"/>
       <c r="H78" s="13"/>
       <c r="I78" s="12"/>
       <c r="J78" s="46"/>
-      <c r="K78" s="47"/>
-    </row>
-    <row r="79" spans="2:11">
+      <c r="K78" s="46"/>
+      <c r="L78" s="47"/>
+    </row>
+    <row r="79" spans="2:12">
       <c r="B79" s="32" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="C79" s="33" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="D79" s="33" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="E79" s="34" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="F79" s="34"/>
       <c r="G79" s="34"/>
       <c r="H79" s="34"/>
       <c r="I79" s="33"/>
       <c r="J79" s="44"/>
-      <c r="K79" s="45"/>
+      <c r="K79" s="44"/>
+      <c r="L79" s="45"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>

</xml_diff>

<commit_message>
apply 'step' option to 'size' register field
(refs: rggen/rggen#139)
</commit_message>
<xml_diff>
--- a/block_0.xlsx
+++ b/block_0.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26012"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26415"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="186" documentId="8_{A0D56F00-2FF8-4245-9EBC-D59D5B1EA094}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{35F1DE00-9324-445A-9C1B-8EE8982BD35F}"/>
+  <xr:revisionPtr revIDLastSave="194" documentId="8_{A0D56F00-2FF8-4245-9EBC-D59D5B1EA094}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{77D85661-7FEA-424A-855D-B7865FA7AD5B}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="164">
   <si>
     <t>block name</t>
     <phoneticPr fontId="1"/>
@@ -491,21 +491,20 @@
     <t>0x30</t>
   </si>
   <si>
-    <t>[4]</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>4:0:4:16</t>
-  </si>
-  <si>
-    <t>4:4:4:16</t>
+    <t>4: step: 8</t>
+  </si>
+  <si>
+    <t>2:0:4:8</t>
+  </si>
+  <si>
+    <t>2:2:4:8</t>
   </si>
   <si>
     <t>default: 0</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>4:8:4:16</t>
+    <t>2:4:4:8</t>
   </si>
   <si>
     <t>0, 1, 2, 3</t>
@@ -518,8 +517,7 @@
     <t>0x50</t>
   </si>
   <si>
-    <t>[2, 4]</t>
-    <phoneticPr fontId="1"/>
+    <t>2, 4</t>
   </si>
   <si>
     <t>indirect:
@@ -607,10 +605,6 @@
   </si>
   <si>
     <t>0x80</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>[32]</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -1458,8 +1452,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:L79"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:XFD12"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="G65" sqref="G65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
@@ -3151,11 +3145,11 @@
       <c r="C79" s="33" t="s">
         <v>162</v>
       </c>
-      <c r="D79" s="33" t="s">
+      <c r="D79" s="33">
+        <v>32</v>
+      </c>
+      <c r="E79" s="34" t="s">
         <v>163</v>
-      </c>
-      <c r="E79" s="34" t="s">
-        <v>164</v>
       </c>
       <c r="F79" s="34"/>
       <c r="G79" s="34"/>

</xml_diff>

<commit_message>
update samples due to adding rw register type
(refs: rggen/rggen#155)
</commit_message>
<xml_diff>
--- a/block_0.xlsx
+++ b/block_0.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26415"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26903"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="194" documentId="8_{A0D56F00-2FF8-4245-9EBC-D59D5B1EA094}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{77D85661-7FEA-424A-855D-B7865FA7AD5B}"/>
+  <xr:revisionPtr revIDLastSave="221" documentId="8_{A0D56F00-2FF8-4245-9EBC-D59D5B1EA094}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3B6E3F42-067C-42CC-8242-90484E5470DC}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="171">
   <si>
     <t>block name</t>
     <phoneticPr fontId="1"/>
@@ -598,10 +598,31 @@
     <t>0x70</t>
   </si>
   <si>
+    <t>rw</t>
+  </si>
+  <si>
+    <t>ro</t>
+  </si>
+  <si>
+    <t>register_15</t>
+  </si>
+  <si>
+    <t>0x74</t>
+  </si>
+  <si>
+    <t>wo</t>
+  </si>
+  <si>
+    <t>register_16</t>
+  </si>
+  <si>
+    <t>0x78</t>
+  </si>
+  <si>
     <t>reserved</t>
   </si>
   <si>
-    <t>register_15</t>
+    <t>register_17</t>
   </si>
   <si>
     <t>0x80</t>
@@ -1450,10 +1471,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:L79"/>
+  <dimension ref="B1:L81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="G65" sqref="G65"/>
+    <sheetView tabSelected="1" topLeftCell="A74" workbookViewId="0">
+      <selection activeCell="B82" sqref="B82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
@@ -3099,10 +3120,10 @@
       <c r="L76" s="47"/>
     </row>
     <row r="77" spans="2:12" ht="45">
-      <c r="B77" s="27"/>
-      <c r="C77" s="8"/>
-      <c r="D77" s="8"/>
-      <c r="E77" s="9"/>
+      <c r="B77" s="30"/>
+      <c r="C77" s="15"/>
+      <c r="D77" s="15"/>
+      <c r="E77" s="16"/>
       <c r="F77" s="13" t="s">
         <v>98</v>
       </c>
@@ -3127,37 +3148,89 @@
         <v>159</v>
       </c>
       <c r="D78" s="19"/>
-      <c r="E78" s="48" t="s">
+      <c r="E78" s="20" t="s">
         <v>160</v>
       </c>
-      <c r="F78" s="13"/>
-      <c r="G78" s="13"/>
-      <c r="H78" s="13"/>
+      <c r="F78" s="13" t="s">
+        <v>122</v>
+      </c>
+      <c r="G78" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="H78" s="14" t="s">
+        <v>161</v>
+      </c>
       <c r="I78" s="12"/>
       <c r="J78" s="46"/>
       <c r="K78" s="46"/>
       <c r="L78" s="47"/>
     </row>
-    <row r="79" spans="2:12">
-      <c r="B79" s="32" t="s">
-        <v>161</v>
-      </c>
-      <c r="C79" s="33" t="s">
+    <row r="79" spans="2:12" ht="22.5">
+      <c r="B79" s="31" t="s">
         <v>162</v>
       </c>
-      <c r="D79" s="33">
+      <c r="C79" s="19" t="s">
+        <v>163</v>
+      </c>
+      <c r="D79" s="19"/>
+      <c r="E79" s="20" t="s">
+        <v>160</v>
+      </c>
+      <c r="F79" s="13" t="s">
+        <v>122</v>
+      </c>
+      <c r="G79" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="H79" s="14" t="s">
+        <v>164</v>
+      </c>
+      <c r="I79" s="12">
+        <v>0</v>
+      </c>
+      <c r="J79" s="46"/>
+      <c r="K79" s="46"/>
+      <c r="L79" s="47"/>
+    </row>
+    <row r="80" spans="2:12" ht="22.5">
+      <c r="B80" s="31" t="s">
+        <v>165</v>
+      </c>
+      <c r="C80" s="19" t="s">
+        <v>166</v>
+      </c>
+      <c r="D80" s="19"/>
+      <c r="E80" s="48" t="s">
+        <v>167</v>
+      </c>
+      <c r="F80" s="13"/>
+      <c r="G80" s="13"/>
+      <c r="H80" s="13"/>
+      <c r="I80" s="12"/>
+      <c r="J80" s="46"/>
+      <c r="K80" s="46"/>
+      <c r="L80" s="47"/>
+    </row>
+    <row r="81" spans="2:12">
+      <c r="B81" s="32" t="s">
+        <v>168</v>
+      </c>
+      <c r="C81" s="33" t="s">
+        <v>169</v>
+      </c>
+      <c r="D81" s="33">
         <v>32</v>
       </c>
-      <c r="E79" s="34" t="s">
-        <v>163</v>
-      </c>
-      <c r="F79" s="34"/>
-      <c r="G79" s="34"/>
-      <c r="H79" s="34"/>
-      <c r="I79" s="33"/>
-      <c r="J79" s="44"/>
-      <c r="K79" s="44"/>
-      <c r="L79" s="45"/>
+      <c r="E81" s="34" t="s">
+        <v>170</v>
+      </c>
+      <c r="F81" s="34"/>
+      <c r="G81" s="34"/>
+      <c r="H81" s="34"/>
+      <c r="I81" s="33"/>
+      <c r="J81" s="44"/>
+      <c r="K81" s="44"/>
+      <c r="L81" s="45"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>

</xml_diff>

<commit_message>
rename bit field type name
* rol -> rohw
* rws -> rwhw

(refs: rggen/rggen#184)
</commit_message>
<xml_diff>
--- a/block_0.xlsx
+++ b/block_0.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26903"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27316"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="221" documentId="8_{A0D56F00-2FF8-4245-9EBC-D59D5B1EA094}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3B6E3F42-067C-42CC-8242-90484E5470DC}"/>
+  <xr:revisionPtr revIDLastSave="225" documentId="8_{A0D56F00-2FF8-4245-9EBC-D59D5B1EA094}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{60DF440C-2B6A-4F98-8184-3B8D4EB6B5B5}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -179,7 +179,7 @@
     <t>4:16</t>
   </si>
   <si>
-    <t>rol</t>
+    <t>rohw</t>
   </si>
   <si>
     <t>bit_field_3</t>
@@ -276,8 +276,7 @@
     <t>2:4</t>
   </si>
   <si>
-    <t>rws</t>
-    <phoneticPr fontId="1"/>
+    <t>rwhw</t>
   </si>
   <si>
     <t>2:6</t>
@@ -1473,9 +1472,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:L81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A74" workbookViewId="0">
-      <selection activeCell="B82" sqref="B82"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
   <cols>

</xml_diff>

<commit_message>
redefine rws bit field type
(refs: rggen/rggen#184)
</commit_message>
<xml_diff>
--- a/block_0.xlsx
+++ b/block_0.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27316"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="225" documentId="8_{A0D56F00-2FF8-4245-9EBC-D59D5B1EA094}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{60DF440C-2B6A-4F98-8184-3B8D4EB6B5B5}"/>
+  <xr:revisionPtr revIDLastSave="254" documentId="8_{A0D56F00-2FF8-4245-9EBC-D59D5B1EA094}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BCB0E08A-E20A-41CD-A987-B2DEDCF0DABC}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="172">
   <si>
     <t>block name</t>
     <phoneticPr fontId="1"/>
@@ -270,103 +270,110 @@
   </si>
   <si>
     <t>register_3.bit_field_2</t>
-    <phoneticPr fontId="1"/>
   </si>
   <si>
     <t>2:4</t>
   </si>
   <si>
+    <t>rws</t>
+  </si>
+  <si>
+    <t>2:6</t>
+  </si>
+  <si>
+    <t>2:8</t>
+  </si>
+  <si>
     <t>rwhw</t>
   </si>
   <si>
-    <t>2:6</t>
+    <t>2:10</t>
   </si>
   <si>
     <t>register_3.bit_field_3</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
+    <t>2:12</t>
+  </si>
+  <si>
+    <t>rwe</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>bit_field_7</t>
+  </si>
+  <si>
+    <t>2:14</t>
+  </si>
+  <si>
+    <t>register_0.bit_field_2</t>
+  </si>
+  <si>
+    <t>bit_field_8</t>
+  </si>
+  <si>
+    <t>2:16</t>
+  </si>
+  <si>
+    <t>bit_field_9</t>
+  </si>
+  <si>
+    <t>2:20</t>
+  </si>
+  <si>
+    <t>rwl</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>bit_field_10</t>
+  </si>
+  <si>
+    <t>2:22</t>
+  </si>
+  <si>
+    <t>register_0.bit_field_2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>bit_field_11</t>
+  </si>
+  <si>
+    <t>2:24</t>
+  </si>
+  <si>
+    <t>register_6</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>0x14</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>w0c</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>4:4</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>register_6.bit_field_1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>w1c</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
     <t>bit_field_4</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>2:8</t>
-  </si>
-  <si>
-    <t>rwe</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>bit_field_5</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>2:10</t>
-  </si>
-  <si>
-    <t>register_0.bit_field_2</t>
-  </si>
-  <si>
-    <t>bit_field_6</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>2:12</t>
-  </si>
-  <si>
-    <t>bit_field_7</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>2:16</t>
-  </si>
-  <si>
-    <t>rwl</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>bit_field_8</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>2:18</t>
-  </si>
-  <si>
-    <t>register_0.bit_field_2</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>bit_field_9</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>2:20</t>
-  </si>
-  <si>
-    <t>register_6</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>0x14</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>w0c</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>4:4</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>register_6.bit_field_1</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>w1c</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>register_6.bit_field_4</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -377,25 +384,16 @@
     <t>w0s</t>
   </si>
   <si>
-    <t>bit_field_7</t>
-  </si>
-  <si>
     <t>4:28</t>
   </si>
   <si>
     <t>w1s</t>
   </si>
   <si>
-    <t>bit_field_8</t>
-  </si>
-  <si>
     <t>4:32</t>
   </si>
   <si>
     <t>w0t</t>
-  </si>
-  <si>
-    <t>bit_field_9</t>
   </si>
   <si>
     <t>4:36</t>
@@ -1470,7 +1468,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:L81"/>
+  <dimension ref="B1:L83"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -2047,7 +2045,7 @@
       <c r="D28" s="8"/>
       <c r="E28" s="9"/>
       <c r="F28" s="2" t="s">
-        <v>18</v>
+        <v>38</v>
       </c>
       <c r="G28" s="2" t="s">
         <v>66</v>
@@ -2068,7 +2066,7 @@
       <c r="D29" s="8"/>
       <c r="E29" s="9"/>
       <c r="F29" s="2" t="s">
-        <v>20</v>
+        <v>41</v>
       </c>
       <c r="G29" s="2" t="s">
         <v>68</v>
@@ -2080,7 +2078,7 @@
         <v>0</v>
       </c>
       <c r="J29" s="39" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="K29" s="39"/>
       <c r="L29" s="40"/>
@@ -2091,13 +2089,13 @@
       <c r="D30" s="8"/>
       <c r="E30" s="9"/>
       <c r="F30" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="H30" s="2" t="s">
         <v>70</v>
-      </c>
-      <c r="G30" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="H30" s="2" t="s">
-        <v>72</v>
       </c>
       <c r="I30" s="3">
         <v>0</v>
@@ -2112,19 +2110,19 @@
       <c r="D31" s="8"/>
       <c r="E31" s="9"/>
       <c r="F31" s="2" t="s">
-        <v>73</v>
+        <v>25</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="H31" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="I31" s="3">
+        <v>0</v>
+      </c>
+      <c r="J31" s="39" t="s">
         <v>72</v>
-      </c>
-      <c r="I31" s="3">
-        <v>0</v>
-      </c>
-      <c r="J31" s="39" t="s">
-        <v>75</v>
       </c>
       <c r="K31" s="39"/>
       <c r="L31" s="40"/>
@@ -2135,20 +2133,18 @@
       <c r="D32" s="8"/>
       <c r="E32" s="9"/>
       <c r="F32" s="2" t="s">
-        <v>76</v>
+        <v>27</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="I32" s="3">
         <v>0</v>
       </c>
-      <c r="J32" s="39" t="s">
-        <v>29</v>
-      </c>
+      <c r="J32" s="39"/>
       <c r="K32" s="39"/>
       <c r="L32" s="40"/>
     </row>
@@ -2158,18 +2154,20 @@
       <c r="D33" s="8"/>
       <c r="E33" s="9"/>
       <c r="F33" s="2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="I33" s="3">
         <v>0</v>
       </c>
-      <c r="J33" s="39"/>
+      <c r="J33" s="39" t="s">
+        <v>77</v>
+      </c>
       <c r="K33" s="39"/>
       <c r="L33" s="40"/>
     </row>
@@ -2179,112 +2177,112 @@
       <c r="D34" s="8"/>
       <c r="E34" s="9"/>
       <c r="F34" s="2" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="I34" s="3">
         <v>0</v>
       </c>
       <c r="J34" s="39" t="s">
-        <v>83</v>
+        <v>29</v>
       </c>
       <c r="K34" s="39"/>
       <c r="L34" s="40"/>
     </row>
     <row r="35" spans="2:12">
-      <c r="B35" s="28"/>
-      <c r="C35" s="10"/>
-      <c r="D35" s="10"/>
-      <c r="E35" s="11"/>
+      <c r="B35" s="27"/>
+      <c r="C35" s="8"/>
+      <c r="D35" s="8"/>
+      <c r="E35" s="9"/>
       <c r="F35" s="2" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="H35" s="2" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="I35" s="3">
         <v>0</v>
       </c>
-      <c r="J35" s="39" t="s">
-        <v>29</v>
-      </c>
+      <c r="J35" s="39"/>
       <c r="K35" s="39"/>
       <c r="L35" s="40"/>
     </row>
     <row r="36" spans="2:12">
-      <c r="B36" s="29" t="s">
-        <v>86</v>
-      </c>
-      <c r="C36" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="D36" s="12"/>
-      <c r="E36" s="13"/>
+      <c r="B36" s="27"/>
+      <c r="C36" s="8"/>
+      <c r="D36" s="8"/>
+      <c r="E36" s="9"/>
       <c r="F36" s="2" t="s">
-        <v>13</v>
+        <v>83</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>33</v>
+        <v>84</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="I36" s="3">
         <v>0</v>
       </c>
-      <c r="J36" s="39"/>
+      <c r="J36" s="39" t="s">
+        <v>85</v>
+      </c>
       <c r="K36" s="39"/>
       <c r="L36" s="40"/>
     </row>
     <row r="37" spans="2:12">
-      <c r="B37" s="27"/>
-      <c r="C37" s="8"/>
-      <c r="D37" s="8"/>
-      <c r="E37" s="9"/>
+      <c r="B37" s="28"/>
+      <c r="C37" s="10"/>
+      <c r="D37" s="10"/>
+      <c r="E37" s="11"/>
       <c r="F37" s="2" t="s">
-        <v>17</v>
+        <v>86</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="I37" s="3">
         <v>0</v>
       </c>
       <c r="J37" s="39" t="s">
-        <v>56</v>
+        <v>29</v>
       </c>
       <c r="K37" s="39"/>
       <c r="L37" s="40"/>
     </row>
     <row r="38" spans="2:12">
-      <c r="B38" s="27"/>
-      <c r="C38" s="8"/>
-      <c r="D38" s="8"/>
-      <c r="E38" s="9"/>
+      <c r="B38" s="29" t="s">
+        <v>88</v>
+      </c>
+      <c r="C38" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="D38" s="12"/>
+      <c r="E38" s="13"/>
       <c r="F38" s="2" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="I38" s="3"/>
-      <c r="J38" s="39" t="s">
         <v>90</v>
       </c>
+      <c r="I38" s="3">
+        <v>0</v>
+      </c>
+      <c r="J38" s="39"/>
       <c r="K38" s="39"/>
       <c r="L38" s="40"/>
     </row>
@@ -2294,18 +2292,20 @@
       <c r="D39" s="8"/>
       <c r="E39" s="9"/>
       <c r="F39" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>57</v>
+        <v>91</v>
       </c>
       <c r="H39" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="I39" s="3">
         <v>0</v>
       </c>
-      <c r="J39" s="39"/>
+      <c r="J39" s="39" t="s">
+        <v>56</v>
+      </c>
       <c r="K39" s="39"/>
       <c r="L39" s="40"/>
     </row>
@@ -2315,19 +2315,17 @@
       <c r="D40" s="8"/>
       <c r="E40" s="9"/>
       <c r="F40" s="2" t="s">
-        <v>70</v>
+        <v>18</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="H40" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="I40" s="3">
-        <v>0</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="I40" s="3"/>
       <c r="J40" s="39" t="s">
-        <v>56</v>
+        <v>92</v>
       </c>
       <c r="K40" s="39"/>
       <c r="L40" s="40"/>
@@ -2338,18 +2336,18 @@
       <c r="D41" s="8"/>
       <c r="E41" s="9"/>
       <c r="F41" s="2" t="s">
-        <v>73</v>
+        <v>20</v>
       </c>
       <c r="G41" s="2" t="s">
-        <v>42</v>
+        <v>57</v>
       </c>
       <c r="H41" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="I41" s="3"/>
-      <c r="J41" s="39" t="s">
-        <v>92</v>
-      </c>
+        <v>93</v>
+      </c>
+      <c r="I41" s="3">
+        <v>0</v>
+      </c>
+      <c r="J41" s="39"/>
       <c r="K41" s="39"/>
       <c r="L41" s="40"/>
     </row>
@@ -2359,18 +2357,20 @@
       <c r="D42" s="8"/>
       <c r="E42" s="9"/>
       <c r="F42" s="2" t="s">
-        <v>27</v>
+        <v>94</v>
       </c>
       <c r="G42" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="H42" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="H42" s="2" t="s">
-        <v>94</v>
-      </c>
       <c r="I42" s="3">
         <v>0</v>
       </c>
-      <c r="J42" s="39"/>
+      <c r="J42" s="39" t="s">
+        <v>56</v>
+      </c>
       <c r="K42" s="39"/>
       <c r="L42" s="40"/>
     </row>
@@ -2383,15 +2383,15 @@
         <v>95</v>
       </c>
       <c r="G43" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="H43" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="I43" s="3"/>
+      <c r="J43" s="39" t="s">
         <v>96</v>
       </c>
-      <c r="H43" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="I43" s="3">
-        <v>0</v>
-      </c>
-      <c r="J43" s="39"/>
       <c r="K43" s="39"/>
       <c r="L43" s="40"/>
     </row>
@@ -2401,13 +2401,13 @@
       <c r="D44" s="8"/>
       <c r="E44" s="9"/>
       <c r="F44" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G44" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="H44" s="2" t="s">
         <v>98</v>
-      </c>
-      <c r="G44" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="H44" s="2" t="s">
-        <v>100</v>
       </c>
       <c r="I44" s="3">
         <v>0</v>
@@ -2417,18 +2417,18 @@
       <c r="L44" s="40"/>
     </row>
     <row r="45" spans="2:12">
-      <c r="B45" s="28"/>
-      <c r="C45" s="10"/>
-      <c r="D45" s="10"/>
-      <c r="E45" s="11"/>
+      <c r="B45" s="27"/>
+      <c r="C45" s="8"/>
+      <c r="D45" s="8"/>
+      <c r="E45" s="9"/>
       <c r="F45" s="2" t="s">
-        <v>101</v>
+        <v>75</v>
       </c>
       <c r="G45" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="H45" s="2" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="I45" s="3">
         <v>0</v>
@@ -2438,22 +2438,18 @@
       <c r="L45" s="40"/>
     </row>
     <row r="46" spans="2:12">
-      <c r="B46" s="27" t="s">
-        <v>104</v>
-      </c>
-      <c r="C46" s="8" t="s">
-        <v>105</v>
-      </c>
+      <c r="B46" s="27"/>
+      <c r="C46" s="8"/>
       <c r="D46" s="8"/>
       <c r="E46" s="9"/>
       <c r="F46" s="2" t="s">
-        <v>13</v>
+        <v>78</v>
       </c>
       <c r="G46" s="2" t="s">
-        <v>33</v>
+        <v>101</v>
       </c>
       <c r="H46" s="2" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="I46" s="3">
         <v>0</v>
@@ -2463,18 +2459,18 @@
       <c r="L46" s="40"/>
     </row>
     <row r="47" spans="2:12">
-      <c r="B47" s="27"/>
-      <c r="C47" s="8"/>
-      <c r="D47" s="8"/>
-      <c r="E47" s="9"/>
+      <c r="B47" s="28"/>
+      <c r="C47" s="10"/>
+      <c r="D47" s="10"/>
+      <c r="E47" s="11"/>
       <c r="F47" s="2" t="s">
-        <v>17</v>
+        <v>80</v>
       </c>
       <c r="G47" s="2" t="s">
-        <v>50</v>
+        <v>103</v>
       </c>
       <c r="H47" s="2" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="I47" s="3">
         <v>0</v>
@@ -2484,18 +2480,22 @@
       <c r="L47" s="40"/>
     </row>
     <row r="48" spans="2:12">
-      <c r="B48" s="27"/>
-      <c r="C48" s="8"/>
+      <c r="B48" s="27" t="s">
+        <v>105</v>
+      </c>
+      <c r="C48" s="8" t="s">
+        <v>106</v>
+      </c>
       <c r="D48" s="8"/>
       <c r="E48" s="9"/>
       <c r="F48" s="2" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="G48" s="2" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="H48" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I48" s="3">
         <v>0</v>
@@ -2505,91 +2505,91 @@
       <c r="L48" s="40"/>
     </row>
     <row r="49" spans="2:12">
-      <c r="B49" s="30"/>
-      <c r="C49" s="15"/>
-      <c r="D49" s="15"/>
-      <c r="E49" s="16"/>
-      <c r="F49" s="17" t="s">
+      <c r="B49" s="27"/>
+      <c r="C49" s="8"/>
+      <c r="D49" s="8"/>
+      <c r="E49" s="9"/>
+      <c r="F49" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G49" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="H49" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="I49" s="3">
+        <v>0</v>
+      </c>
+      <c r="J49" s="39"/>
+      <c r="K49" s="39"/>
+      <c r="L49" s="40"/>
+    </row>
+    <row r="50" spans="2:12">
+      <c r="B50" s="27"/>
+      <c r="C50" s="8"/>
+      <c r="D50" s="8"/>
+      <c r="E50" s="9"/>
+      <c r="F50" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G50" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="H50" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="I50" s="3">
+        <v>0</v>
+      </c>
+      <c r="J50" s="39"/>
+      <c r="K50" s="39"/>
+      <c r="L50" s="40"/>
+    </row>
+    <row r="51" spans="2:12">
+      <c r="B51" s="30"/>
+      <c r="C51" s="15"/>
+      <c r="D51" s="15"/>
+      <c r="E51" s="16"/>
+      <c r="F51" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="G49" s="17" t="s">
-        <v>93</v>
-      </c>
-      <c r="H49" s="17" t="s">
-        <v>109</v>
-      </c>
-      <c r="I49" s="18">
-        <v>0</v>
-      </c>
-      <c r="J49" s="41"/>
-      <c r="K49" s="41"/>
-      <c r="L49" s="40"/>
-    </row>
-    <row r="50" spans="2:12">
-      <c r="B50" s="31" t="s">
+      <c r="G51" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="H51" s="17" t="s">
         <v>110</v>
       </c>
-      <c r="C50" s="19" t="s">
+      <c r="I51" s="18">
+        <v>0</v>
+      </c>
+      <c r="J51" s="41"/>
+      <c r="K51" s="41"/>
+      <c r="L51" s="40"/>
+    </row>
+    <row r="52" spans="2:12">
+      <c r="B52" s="31" t="s">
         <v>111</v>
       </c>
-      <c r="D50" s="19"/>
-      <c r="E50" s="20"/>
-      <c r="F50" s="21" t="s">
+      <c r="C52" s="19" t="s">
+        <v>112</v>
+      </c>
+      <c r="D52" s="19"/>
+      <c r="E52" s="20"/>
+      <c r="F52" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="G50" s="21" t="s">
+      <c r="G52" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="H50" s="21" t="s">
-        <v>112</v>
-      </c>
-      <c r="I50" s="22">
-        <v>0</v>
-      </c>
-      <c r="J50" s="42"/>
-      <c r="K50" s="42"/>
-      <c r="L50" s="40"/>
-    </row>
-    <row r="51" spans="2:12">
-      <c r="B51" s="27"/>
-      <c r="C51" s="8"/>
-      <c r="D51" s="8"/>
-      <c r="E51" s="9"/>
-      <c r="F51" s="11" t="s">
+      <c r="H52" s="21" t="s">
         <v>113</v>
       </c>
-      <c r="G51" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="H51" s="11" t="s">
-        <v>114</v>
-      </c>
-      <c r="I51" s="10">
-        <v>0</v>
-      </c>
-      <c r="J51" s="43"/>
-      <c r="K51" s="43"/>
-      <c r="L51" s="40"/>
-    </row>
-    <row r="52" spans="2:12">
-      <c r="B52" s="27"/>
-      <c r="C52" s="8"/>
-      <c r="D52" s="8"/>
-      <c r="E52" s="9"/>
-      <c r="F52" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="G52" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="H52" s="11" t="s">
-        <v>115</v>
-      </c>
-      <c r="I52" s="10">
-        <v>0</v>
-      </c>
-      <c r="J52" s="43"/>
-      <c r="K52" s="43"/>
+      <c r="I52" s="22">
+        <v>0</v>
+      </c>
+      <c r="J52" s="42"/>
+      <c r="K52" s="42"/>
       <c r="L52" s="40"/>
     </row>
     <row r="53" spans="2:12">
@@ -2597,20 +2597,20 @@
       <c r="C53" s="8"/>
       <c r="D53" s="8"/>
       <c r="E53" s="9"/>
-      <c r="F53" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="G53" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="H53" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="I53" s="3">
-        <v>0</v>
-      </c>
-      <c r="J53" s="39"/>
-      <c r="K53" s="39"/>
+      <c r="F53" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="G53" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="H53" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="I53" s="10">
+        <v>0</v>
+      </c>
+      <c r="J53" s="43"/>
+      <c r="K53" s="43"/>
       <c r="L53" s="40"/>
     </row>
     <row r="54" spans="2:12">
@@ -2618,35 +2618,35 @@
       <c r="C54" s="8"/>
       <c r="D54" s="8"/>
       <c r="E54" s="9"/>
-      <c r="F54" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="G54" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="H54" s="2" t="s">
+      <c r="F54" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="G54" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="H54" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="I54" s="10">
+        <v>0</v>
+      </c>
+      <c r="J54" s="43"/>
+      <c r="K54" s="43"/>
+      <c r="L54" s="40"/>
+    </row>
+    <row r="55" spans="2:12">
+      <c r="B55" s="27"/>
+      <c r="C55" s="8"/>
+      <c r="D55" s="8"/>
+      <c r="E55" s="9"/>
+      <c r="F55" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="G55" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="H55" s="2" t="s">
         <v>117</v>
-      </c>
-      <c r="I54" s="3">
-        <v>0</v>
-      </c>
-      <c r="J54" s="39"/>
-      <c r="K54" s="39"/>
-      <c r="L54" s="40"/>
-    </row>
-    <row r="55" spans="2:12">
-      <c r="B55" s="30"/>
-      <c r="C55" s="15"/>
-      <c r="D55" s="15"/>
-      <c r="E55" s="16"/>
-      <c r="F55" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="G55" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="H55" s="2" t="s">
-        <v>119</v>
       </c>
       <c r="I55" s="3">
         <v>0</v>
@@ -2656,22 +2656,18 @@
       <c r="L55" s="40"/>
     </row>
     <row r="56" spans="2:12">
-      <c r="B56" s="31" t="s">
-        <v>120</v>
-      </c>
-      <c r="C56" s="19" t="s">
-        <v>121</v>
-      </c>
-      <c r="D56" s="19"/>
-      <c r="E56" s="20"/>
+      <c r="B56" s="27"/>
+      <c r="C56" s="8"/>
+      <c r="D56" s="8"/>
+      <c r="E56" s="9"/>
       <c r="F56" s="2" t="s">
-        <v>122</v>
+        <v>23</v>
       </c>
       <c r="G56" s="2" t="s">
-        <v>62</v>
+        <v>101</v>
       </c>
       <c r="H56" s="2" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="I56" s="3">
         <v>0</v>
@@ -2681,37 +2677,43 @@
       <c r="L56" s="40"/>
     </row>
     <row r="57" spans="2:12">
-      <c r="B57" s="27"/>
-      <c r="C57" s="8"/>
-      <c r="D57" s="8"/>
-      <c r="E57" s="9"/>
+      <c r="B57" s="30"/>
+      <c r="C57" s="15"/>
+      <c r="D57" s="15"/>
+      <c r="E57" s="16"/>
       <c r="F57" s="2" t="s">
-        <v>113</v>
+        <v>25</v>
       </c>
       <c r="G57" s="2" t="s">
-        <v>64</v>
+        <v>119</v>
       </c>
       <c r="H57" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="I57" s="3"/>
+        <v>120</v>
+      </c>
+      <c r="I57" s="3">
+        <v>0</v>
+      </c>
       <c r="J57" s="39"/>
       <c r="K57" s="39"/>
       <c r="L57" s="40"/>
     </row>
     <row r="58" spans="2:12">
-      <c r="B58" s="27"/>
-      <c r="C58" s="8"/>
-      <c r="D58" s="8"/>
-      <c r="E58" s="9"/>
+      <c r="B58" s="31" t="s">
+        <v>121</v>
+      </c>
+      <c r="C58" s="19" t="s">
+        <v>122</v>
+      </c>
+      <c r="D58" s="19"/>
+      <c r="E58" s="20"/>
       <c r="F58" s="2" t="s">
-        <v>38</v>
+        <v>123</v>
       </c>
       <c r="G58" s="2" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="H58" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="I58" s="3">
         <v>0</v>
@@ -2726,17 +2728,15 @@
       <c r="D59" s="8"/>
       <c r="E59" s="9"/>
       <c r="F59" s="2" t="s">
-        <v>41</v>
+        <v>114</v>
       </c>
       <c r="G59" s="2" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="H59" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="I59" s="3">
-        <v>0</v>
-      </c>
+        <v>125</v>
+      </c>
+      <c r="I59" s="3"/>
       <c r="J59" s="39"/>
       <c r="K59" s="39"/>
       <c r="L59" s="40"/>
@@ -2747,15 +2747,17 @@
       <c r="D60" s="8"/>
       <c r="E60" s="9"/>
       <c r="F60" s="2" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="G60" s="2" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="H60" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="I60" s="3"/>
+        <v>126</v>
+      </c>
+      <c r="I60" s="3">
+        <v>0</v>
+      </c>
       <c r="J60" s="39"/>
       <c r="K60" s="39"/>
       <c r="L60" s="40"/>
@@ -2766,42 +2768,36 @@
       <c r="D61" s="8"/>
       <c r="E61" s="9"/>
       <c r="F61" s="2" t="s">
-        <v>25</v>
+        <v>41</v>
       </c>
       <c r="G61" s="2" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="H61" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="I61" s="3"/>
+        <v>127</v>
+      </c>
+      <c r="I61" s="3">
+        <v>0</v>
+      </c>
       <c r="J61" s="39"/>
       <c r="K61" s="39"/>
       <c r="L61" s="40"/>
     </row>
     <row r="62" spans="2:12">
-      <c r="B62" s="29" t="s">
-        <v>129</v>
-      </c>
-      <c r="C62" s="12" t="s">
-        <v>130</v>
-      </c>
-      <c r="D62" s="12" t="s">
-        <v>131</v>
-      </c>
-      <c r="E62" s="13"/>
+      <c r="B62" s="27"/>
+      <c r="C62" s="8"/>
+      <c r="D62" s="8"/>
+      <c r="E62" s="9"/>
       <c r="F62" s="2" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="G62" s="2" t="s">
-        <v>132</v>
+        <v>69</v>
       </c>
       <c r="H62" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="I62" s="3">
-        <v>0</v>
-      </c>
+        <v>128</v>
+      </c>
+      <c r="I62" s="3"/>
       <c r="J62" s="39"/>
       <c r="K62" s="39"/>
       <c r="L62" s="40"/>
@@ -2812,108 +2808,106 @@
       <c r="D63" s="8"/>
       <c r="E63" s="9"/>
       <c r="F63" s="2" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="G63" s="2" t="s">
-        <v>133</v>
+        <v>71</v>
       </c>
       <c r="H63" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="I63" s="3" t="s">
-        <v>134</v>
-      </c>
+        <v>129</v>
+      </c>
+      <c r="I63" s="3"/>
       <c r="J63" s="39"/>
       <c r="K63" s="39"/>
       <c r="L63" s="40"/>
     </row>
     <row r="64" spans="2:12">
-      <c r="B64" s="28"/>
-      <c r="C64" s="10"/>
-      <c r="D64" s="10"/>
-      <c r="E64" s="11"/>
+      <c r="B64" s="29" t="s">
+        <v>130</v>
+      </c>
+      <c r="C64" s="12" t="s">
+        <v>131</v>
+      </c>
+      <c r="D64" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="E64" s="13"/>
       <c r="F64" s="2" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="G64" s="2" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="H64" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="I64" s="3" t="s">
-        <v>136</v>
+      <c r="I64" s="3">
+        <v>0</v>
       </c>
       <c r="J64" s="39"/>
       <c r="K64" s="39"/>
       <c r="L64" s="40"/>
     </row>
-    <row r="65" spans="2:12" ht="112.5">
-      <c r="B65" s="29" t="s">
-        <v>137</v>
-      </c>
-      <c r="C65" s="12" t="s">
-        <v>138</v>
-      </c>
-      <c r="D65" s="12" t="s">
-        <v>139</v>
-      </c>
-      <c r="E65" s="14" t="s">
-        <v>140</v>
-      </c>
+    <row r="65" spans="2:12">
+      <c r="B65" s="27"/>
+      <c r="C65" s="8"/>
+      <c r="D65" s="8"/>
+      <c r="E65" s="9"/>
       <c r="F65" s="2" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="G65" s="2" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="H65" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="I65" s="3">
-        <v>0</v>
+      <c r="I65" s="3" t="s">
+        <v>135</v>
       </c>
       <c r="J65" s="39"/>
       <c r="K65" s="39"/>
       <c r="L65" s="40"/>
     </row>
     <row r="66" spans="2:12">
-      <c r="B66" s="30"/>
-      <c r="C66" s="15"/>
-      <c r="D66" s="15"/>
-      <c r="E66" s="16"/>
+      <c r="B66" s="28"/>
+      <c r="C66" s="10"/>
+      <c r="D66" s="10"/>
+      <c r="E66" s="11"/>
       <c r="F66" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G66" s="2" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="H66" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="I66" s="3">
-        <v>0</v>
+      <c r="I66" s="3" t="s">
+        <v>137</v>
       </c>
       <c r="J66" s="39"/>
       <c r="K66" s="39"/>
       <c r="L66" s="40"/>
     </row>
-    <row r="67" spans="2:12" ht="67.5">
-      <c r="B67" s="31" t="s">
-        <v>143</v>
-      </c>
-      <c r="C67" s="19" t="s">
+    <row r="67" spans="2:12" ht="112.5">
+      <c r="B67" s="29" t="s">
         <v>138</v>
       </c>
-      <c r="D67" s="19"/>
-      <c r="E67" s="48" t="s">
-        <v>144</v>
+      <c r="C67" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="D67" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="E67" s="14" t="s">
+        <v>141</v>
       </c>
       <c r="F67" s="2" t="s">
         <v>13</v>
       </c>
       <c r="G67" s="2" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="H67" s="2" t="s">
         <v>15</v>
@@ -2931,10 +2925,10 @@
       <c r="D68" s="15"/>
       <c r="E68" s="16"/>
       <c r="F68" s="2" t="s">
-        <v>113</v>
+        <v>17</v>
       </c>
       <c r="G68" s="2" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="H68" s="2" t="s">
         <v>15</v>
@@ -2946,63 +2940,71 @@
       <c r="K68" s="39"/>
       <c r="L68" s="40"/>
     </row>
-    <row r="69" spans="2:12">
-      <c r="B69" s="27" t="s">
+    <row r="69" spans="2:12" ht="67.5">
+      <c r="B69" s="31" t="s">
+        <v>144</v>
+      </c>
+      <c r="C69" s="19" t="s">
+        <v>139</v>
+      </c>
+      <c r="D69" s="19"/>
+      <c r="E69" s="48" t="s">
+        <v>145</v>
+      </c>
+      <c r="F69" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G69" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="H69" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I69" s="3">
+        <v>0</v>
+      </c>
+      <c r="J69" s="39"/>
+      <c r="K69" s="39"/>
+      <c r="L69" s="40"/>
+    </row>
+    <row r="70" spans="2:12">
+      <c r="B70" s="30"/>
+      <c r="C70" s="15"/>
+      <c r="D70" s="15"/>
+      <c r="E70" s="16"/>
+      <c r="F70" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="G70" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="C69" s="8" t="s">
+      <c r="H70" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I70" s="3">
+        <v>0</v>
+      </c>
+      <c r="J70" s="39"/>
+      <c r="K70" s="39"/>
+      <c r="L70" s="40"/>
+    </row>
+    <row r="71" spans="2:12">
+      <c r="B71" s="27" t="s">
         <v>148</v>
       </c>
-      <c r="D69" s="8"/>
-      <c r="E69" s="9"/>
-      <c r="F69" s="13" t="s">
-        <v>122</v>
-      </c>
-      <c r="G69" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="H69" s="13" t="s">
+      <c r="C71" s="8" t="s">
         <v>149</v>
       </c>
-      <c r="I69" s="12">
-        <v>0</v>
-      </c>
-      <c r="J69" s="46"/>
-      <c r="K69" s="46"/>
-      <c r="L69" s="47"/>
-    </row>
-    <row r="70" spans="2:12" ht="45">
-      <c r="B70" s="27"/>
-      <c r="C70" s="8"/>
-      <c r="D70" s="8"/>
-      <c r="E70" s="9"/>
-      <c r="F70" s="13" t="s">
-        <v>113</v>
-      </c>
-      <c r="G70" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="H70" s="14" t="s">
-        <v>150</v>
-      </c>
-      <c r="I70" s="12"/>
-      <c r="J70" s="46"/>
-      <c r="K70" s="46"/>
-      <c r="L70" s="47"/>
-    </row>
-    <row r="71" spans="2:12" ht="45">
-      <c r="B71" s="27"/>
-      <c r="C71" s="8"/>
       <c r="D71" s="8"/>
       <c r="E71" s="9"/>
       <c r="F71" s="13" t="s">
-        <v>38</v>
+        <v>123</v>
       </c>
       <c r="G71" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="H71" s="14" t="s">
-        <v>151</v>
+      <c r="H71" s="13" t="s">
+        <v>150</v>
       </c>
       <c r="I71" s="12">
         <v>0</v>
@@ -3011,40 +3013,38 @@
       <c r="K71" s="46"/>
       <c r="L71" s="47"/>
     </row>
-    <row r="72" spans="2:12" ht="67.5">
+    <row r="72" spans="2:12" ht="45">
       <c r="B72" s="27"/>
       <c r="C72" s="8"/>
       <c r="D72" s="8"/>
       <c r="E72" s="9"/>
       <c r="F72" s="13" t="s">
-        <v>41</v>
+        <v>114</v>
       </c>
       <c r="G72" s="13" t="s">
         <v>21</v>
       </c>
       <c r="H72" s="14" t="s">
-        <v>152</v>
-      </c>
-      <c r="I72" s="12">
-        <v>0</v>
-      </c>
+        <v>151</v>
+      </c>
+      <c r="I72" s="12"/>
       <c r="J72" s="46"/>
       <c r="K72" s="46"/>
       <c r="L72" s="47"/>
     </row>
-    <row r="73" spans="2:12" ht="67.5">
+    <row r="73" spans="2:12" ht="45">
       <c r="B73" s="27"/>
       <c r="C73" s="8"/>
       <c r="D73" s="8"/>
       <c r="E73" s="9"/>
       <c r="F73" s="13" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="G73" s="13" t="s">
         <v>21</v>
       </c>
       <c r="H73" s="14" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="I73" s="12">
         <v>0</v>
@@ -3059,13 +3059,13 @@
       <c r="D74" s="8"/>
       <c r="E74" s="9"/>
       <c r="F74" s="13" t="s">
-        <v>25</v>
+        <v>41</v>
       </c>
       <c r="G74" s="13" t="s">
         <v>21</v>
       </c>
       <c r="H74" s="14" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="I74" s="12">
         <v>0</v>
@@ -3080,13 +3080,13 @@
       <c r="D75" s="8"/>
       <c r="E75" s="9"/>
       <c r="F75" s="13" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="G75" s="13" t="s">
         <v>21</v>
       </c>
       <c r="H75" s="14" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I75" s="12">
         <v>0</v>
@@ -3101,13 +3101,13 @@
       <c r="D76" s="8"/>
       <c r="E76" s="9"/>
       <c r="F76" s="13" t="s">
-        <v>95</v>
+        <v>25</v>
       </c>
       <c r="G76" s="13" t="s">
         <v>21</v>
       </c>
       <c r="H76" s="14" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I76" s="12">
         <v>0</v>
@@ -3116,19 +3116,19 @@
       <c r="K76" s="46"/>
       <c r="L76" s="47"/>
     </row>
-    <row r="77" spans="2:12" ht="45">
-      <c r="B77" s="30"/>
-      <c r="C77" s="15"/>
-      <c r="D77" s="15"/>
-      <c r="E77" s="16"/>
+    <row r="77" spans="2:12" ht="67.5">
+      <c r="B77" s="27"/>
+      <c r="C77" s="8"/>
+      <c r="D77" s="8"/>
+      <c r="E77" s="9"/>
       <c r="F77" s="13" t="s">
-        <v>98</v>
+        <v>27</v>
       </c>
       <c r="G77" s="13" t="s">
         <v>21</v>
       </c>
       <c r="H77" s="14" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="I77" s="12">
         <v>0</v>
@@ -3137,50 +3137,40 @@
       <c r="K77" s="46"/>
       <c r="L77" s="47"/>
     </row>
-    <row r="78" spans="2:12" ht="22.5">
-      <c r="B78" s="31" t="s">
-        <v>158</v>
-      </c>
-      <c r="C78" s="19" t="s">
-        <v>159</v>
-      </c>
-      <c r="D78" s="19"/>
-      <c r="E78" s="20" t="s">
-        <v>160</v>
-      </c>
+    <row r="78" spans="2:12" ht="67.5">
+      <c r="B78" s="27"/>
+      <c r="C78" s="8"/>
+      <c r="D78" s="8"/>
+      <c r="E78" s="9"/>
       <c r="F78" s="13" t="s">
-        <v>122</v>
+        <v>75</v>
       </c>
       <c r="G78" s="13" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="H78" s="14" t="s">
-        <v>161</v>
-      </c>
-      <c r="I78" s="12"/>
+        <v>157</v>
+      </c>
+      <c r="I78" s="12">
+        <v>0</v>
+      </c>
       <c r="J78" s="46"/>
       <c r="K78" s="46"/>
       <c r="L78" s="47"/>
     </row>
-    <row r="79" spans="2:12" ht="22.5">
-      <c r="B79" s="31" t="s">
-        <v>162</v>
-      </c>
-      <c r="C79" s="19" t="s">
-        <v>163</v>
-      </c>
-      <c r="D79" s="19"/>
-      <c r="E79" s="20" t="s">
-        <v>160</v>
-      </c>
+    <row r="79" spans="2:12" ht="45">
+      <c r="B79" s="30"/>
+      <c r="C79" s="15"/>
+      <c r="D79" s="15"/>
+      <c r="E79" s="16"/>
       <c r="F79" s="13" t="s">
-        <v>122</v>
+        <v>78</v>
       </c>
       <c r="G79" s="13" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="H79" s="14" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="I79" s="12">
         <v>0</v>
@@ -3191,43 +3181,95 @@
     </row>
     <row r="80" spans="2:12" ht="22.5">
       <c r="B80" s="31" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="C80" s="19" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="D80" s="19"/>
-      <c r="E80" s="48" t="s">
-        <v>167</v>
-      </c>
-      <c r="F80" s="13"/>
-      <c r="G80" s="13"/>
-      <c r="H80" s="13"/>
+      <c r="E80" s="20" t="s">
+        <v>161</v>
+      </c>
+      <c r="F80" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="G80" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="H80" s="14" t="s">
+        <v>162</v>
+      </c>
       <c r="I80" s="12"/>
       <c r="J80" s="46"/>
       <c r="K80" s="46"/>
       <c r="L80" s="47"/>
     </row>
-    <row r="81" spans="2:12">
-      <c r="B81" s="32" t="s">
+    <row r="81" spans="2:12" ht="22.5">
+      <c r="B81" s="31" t="s">
+        <v>163</v>
+      </c>
+      <c r="C81" s="19" t="s">
+        <v>164</v>
+      </c>
+      <c r="D81" s="19"/>
+      <c r="E81" s="20" t="s">
+        <v>161</v>
+      </c>
+      <c r="F81" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="G81" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="H81" s="14" t="s">
+        <v>165</v>
+      </c>
+      <c r="I81" s="12">
+        <v>0</v>
+      </c>
+      <c r="J81" s="46"/>
+      <c r="K81" s="46"/>
+      <c r="L81" s="47"/>
+    </row>
+    <row r="82" spans="2:12" ht="22.5">
+      <c r="B82" s="31" t="s">
+        <v>166</v>
+      </c>
+      <c r="C82" s="19" t="s">
+        <v>167</v>
+      </c>
+      <c r="D82" s="19"/>
+      <c r="E82" s="48" t="s">
         <v>168</v>
       </c>
-      <c r="C81" s="33" t="s">
+      <c r="F82" s="13"/>
+      <c r="G82" s="13"/>
+      <c r="H82" s="13"/>
+      <c r="I82" s="12"/>
+      <c r="J82" s="46"/>
+      <c r="K82" s="46"/>
+      <c r="L82" s="47"/>
+    </row>
+    <row r="83" spans="2:12">
+      <c r="B83" s="32" t="s">
         <v>169</v>
       </c>
-      <c r="D81" s="33">
+      <c r="C83" s="33" t="s">
+        <v>170</v>
+      </c>
+      <c r="D83" s="33">
         <v>32</v>
       </c>
-      <c r="E81" s="34" t="s">
-        <v>170</v>
-      </c>
-      <c r="F81" s="34"/>
-      <c r="G81" s="34"/>
-      <c r="H81" s="34"/>
-      <c r="I81" s="33"/>
-      <c r="J81" s="44"/>
-      <c r="K81" s="44"/>
-      <c r="L81" s="45"/>
+      <c r="E83" s="34" t="s">
+        <v>171</v>
+      </c>
+      <c r="F83" s="34"/>
+      <c r="G83" s="34"/>
+      <c r="H83" s="34"/>
+      <c r="I83" s="33"/>
+      <c r="J83" s="44"/>
+      <c r="K83" s="44"/>
+      <c r="L83" s="45"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>

</xml_diff>

<commit_message>
add `bus_width` and `protocol` to spredsheet samples
(refs: rggen/rggen#221)
</commit_message>
<xml_diff>
--- a/block_0.xlsx
+++ b/block_0.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27316"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28512"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="254" documentId="8_{A0D56F00-2FF8-4245-9EBC-D59D5B1EA094}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BCB0E08A-E20A-41CD-A987-B2DEDCF0DABC}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B7053C41-96B5-4FDA-BFF1-696E0C16680A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="175">
   <si>
     <t>block name</t>
     <phoneticPr fontId="1"/>
@@ -43,6 +43,15 @@
   <si>
     <t>byte size</t>
     <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>bus width</t>
+  </si>
+  <si>
+    <t>protocol</t>
+  </si>
+  <si>
+    <t>apb</t>
   </si>
   <si>
     <t>name</t>
@@ -1468,9 +1477,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:L83"/>
+  <dimension ref="B1:L85"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
   <cols>
@@ -1501,107 +1512,81 @@
         <v>256</v>
       </c>
     </row>
+    <row r="3" spans="2:12">
+      <c r="B3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3">
+        <v>32</v>
+      </c>
+    </row>
     <row r="4" spans="2:12">
-      <c r="B4" s="23" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="24" t="s">
+      <c r="B4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="24" t="s">
+      <c r="C4" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="25" t="s">
+    </row>
+    <row r="6" spans="2:12">
+      <c r="B6" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="25" t="s">
-        <v>3</v>
-      </c>
-      <c r="G4" s="25" t="s">
+      <c r="C6" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="H4" s="25" t="s">
+      <c r="D6" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="24" t="s">
-        <v>8</v>
-      </c>
-      <c r="J4" s="35" t="s">
+      <c r="G6" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="H6" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="K4" s="35" t="s">
-        <v>10</v>
-      </c>
-      <c r="L4" s="36" t="s">
+      <c r="I6" s="24" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="5" spans="2:12">
-      <c r="B5" s="26" t="s">
+      <c r="J6" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="5" t="s">
+      <c r="K6" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="L6" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="H5" s="5" t="s">
+    </row>
+    <row r="7" spans="2:12">
+      <c r="B7" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="I5" s="4">
-        <v>0</v>
-      </c>
-      <c r="J5" s="37"/>
-      <c r="K5" s="37"/>
-      <c r="L5" s="38" t="s">
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="5" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="6" spans="2:12">
-      <c r="B6" s="27"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="2" t="s">
+      <c r="G7" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="G6" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="I6" s="3">
-        <v>0</v>
-      </c>
-      <c r="J6" s="39"/>
-      <c r="K6" s="39"/>
-      <c r="L6" s="40"/>
-    </row>
-    <row r="7" spans="2:12">
-      <c r="B7" s="27"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="2" t="s">
+      <c r="H7" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="I7" s="4">
+        <v>0</v>
+      </c>
+      <c r="J7" s="37"/>
+      <c r="K7" s="37"/>
+      <c r="L7" s="38" t="s">
         <v>19</v>
       </c>
-      <c r="H7" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="I7" s="3">
-        <v>0</v>
-      </c>
-      <c r="J7" s="39"/>
-      <c r="K7" s="39"/>
-      <c r="L7" s="40"/>
     </row>
     <row r="8" spans="2:12">
       <c r="B8" s="27"/>
@@ -1612,10 +1597,10 @@
         <v>20</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="I8" s="3">
         <v>0</v>
@@ -1630,13 +1615,13 @@
       <c r="D9" s="8"/>
       <c r="E9" s="9"/>
       <c r="F9" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="I9" s="3">
         <v>0</v>
@@ -1651,13 +1636,13 @@
       <c r="D10" s="8"/>
       <c r="E10" s="9"/>
       <c r="F10" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H10" s="2" t="s">
         <v>25</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>26</v>
       </c>
       <c r="I10" s="3">
         <v>0</v>
@@ -1667,18 +1652,18 @@
       <c r="L10" s="40"/>
     </row>
     <row r="11" spans="2:12">
-      <c r="B11" s="28"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="11"/>
+      <c r="B11" s="27"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="9"/>
       <c r="F11" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H11" s="2" t="s">
         <v>27</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>28</v>
       </c>
       <c r="I11" s="3">
         <v>0</v>
@@ -1687,90 +1672,90 @@
       <c r="K11" s="39"/>
       <c r="L11" s="40"/>
     </row>
-    <row r="12" spans="2:12" ht="202.5">
-      <c r="B12" s="29" t="s">
+    <row r="12" spans="2:12">
+      <c r="B12" s="27"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H12" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C12" s="12"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>15</v>
-      </c>
       <c r="I12" s="3">
         <v>0</v>
       </c>
       <c r="J12" s="39"/>
-      <c r="K12" s="49" t="s">
+      <c r="K12" s="39"/>
+      <c r="L12" s="40"/>
+    </row>
+    <row r="13" spans="2:12">
+      <c r="B13" s="28"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="L12" s="40"/>
-    </row>
-    <row r="13" spans="2:12">
-      <c r="B13" s="29" t="s">
+      <c r="G13" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H13" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C13" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="D13" s="12"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="H13" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="I13" s="3"/>
+      <c r="I13" s="3">
+        <v>0</v>
+      </c>
       <c r="J13" s="39"/>
       <c r="K13" s="39"/>
       <c r="L13" s="40"/>
     </row>
-    <row r="14" spans="2:12">
-      <c r="B14" s="27"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="9"/>
-      <c r="F14" s="2" t="s">
-        <v>17</v>
-      </c>
+    <row r="14" spans="2:12" ht="202.5">
+      <c r="B14" s="29" t="s">
+        <v>32</v>
+      </c>
+      <c r="C14" s="12"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="2"/>
       <c r="G14" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I14" s="3">
+        <v>0</v>
+      </c>
+      <c r="J14" s="39"/>
+      <c r="K14" s="49" t="s">
+        <v>33</v>
+      </c>
+      <c r="L14" s="40"/>
+    </row>
+    <row r="15" spans="2:12">
+      <c r="B15" s="29" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="H14" s="2" t="s">
+      <c r="D15" s="12"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G15" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="I14" s="3" t="s">
+      <c r="H15" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="J14" s="39"/>
-      <c r="K14" s="39"/>
-      <c r="L14" s="40"/>
-    </row>
-    <row r="15" spans="2:12">
-      <c r="B15" s="27"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="9"/>
-      <c r="F15" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="H15" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="I15" s="3">
-        <v>0</v>
-      </c>
+      <c r="I15" s="3"/>
       <c r="J15" s="39"/>
       <c r="K15" s="39"/>
       <c r="L15" s="40"/>
@@ -1781,103 +1766,105 @@
       <c r="D16" s="8"/>
       <c r="E16" s="9"/>
       <c r="F16" s="2" t="s">
-        <v>41</v>
+        <v>20</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="H16" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="I16" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="I16" s="3">
-        <v>0</v>
-      </c>
-      <c r="J16" s="39" t="s">
-        <v>43</v>
-      </c>
+      <c r="J16" s="39"/>
       <c r="K16" s="39"/>
       <c r="L16" s="40"/>
     </row>
     <row r="17" spans="2:12">
-      <c r="B17" s="28"/>
-      <c r="C17" s="10"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="11"/>
+      <c r="B17" s="27"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="9"/>
       <c r="F17" s="2" t="s">
-        <v>23</v>
+        <v>41</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="I17" s="3"/>
+        <v>43</v>
+      </c>
+      <c r="I17" s="3">
+        <v>0</v>
+      </c>
       <c r="J17" s="39"/>
       <c r="K17" s="39"/>
       <c r="L17" s="40"/>
     </row>
     <row r="18" spans="2:12">
-      <c r="B18" s="29" t="s">
+      <c r="B18" s="27"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="I18" s="3">
+        <v>0</v>
+      </c>
+      <c r="J18" s="39" t="s">
         <v>46</v>
       </c>
-      <c r="C18" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="D18" s="12"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G18" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="H18" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="I18" s="3">
-        <v>0</v>
-      </c>
-      <c r="J18" s="39"/>
       <c r="K18" s="39"/>
       <c r="L18" s="40"/>
     </row>
     <row r="19" spans="2:12">
-      <c r="B19" s="27"/>
-      <c r="C19" s="8"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="9"/>
+      <c r="B19" s="28"/>
+      <c r="C19" s="10"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="11"/>
       <c r="F19" s="2" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="G19" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="H19" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="H19" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="I19" s="3">
-        <v>0</v>
-      </c>
+      <c r="I19" s="3"/>
       <c r="J19" s="39"/>
       <c r="K19" s="39"/>
       <c r="L19" s="40"/>
     </row>
     <row r="20" spans="2:12">
-      <c r="B20" s="27"/>
-      <c r="C20" s="8"/>
-      <c r="D20" s="8"/>
-      <c r="E20" s="9"/>
+      <c r="B20" s="29" t="s">
+        <v>49</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="D20" s="12"/>
+      <c r="E20" s="13"/>
       <c r="F20" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="G20" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="H20" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="H20" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="I20" s="3"/>
+      <c r="I20" s="3">
+        <v>0</v>
+      </c>
       <c r="J20" s="39"/>
       <c r="K20" s="39"/>
       <c r="L20" s="40"/>
@@ -1891,37 +1878,33 @@
         <v>20</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="H21" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="I21" s="3"/>
+      <c r="I21" s="3">
+        <v>0</v>
+      </c>
       <c r="J21" s="39"/>
       <c r="K21" s="39"/>
       <c r="L21" s="40"/>
     </row>
     <row r="22" spans="2:12">
-      <c r="B22" s="29" t="s">
+      <c r="B22" s="27"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="9"/>
+      <c r="F22" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G22" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C22" s="12" t="s">
+      <c r="H22" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D22" s="12"/>
-      <c r="E22" s="13"/>
-      <c r="F22" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G22" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="H22" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="I22" s="3">
-        <v>0</v>
-      </c>
+      <c r="I22" s="3"/>
       <c r="J22" s="39"/>
       <c r="K22" s="39"/>
       <c r="L22" s="40"/>
@@ -1932,126 +1915,126 @@
       <c r="D23" s="8"/>
       <c r="E23" s="9"/>
       <c r="F23" s="2" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="H23" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="I23" s="3">
-        <v>0</v>
-      </c>
-      <c r="J23" s="39" t="s">
-        <v>56</v>
-      </c>
+      <c r="I23" s="3"/>
+      <c r="J23" s="39"/>
       <c r="K23" s="39"/>
       <c r="L23" s="40"/>
     </row>
     <row r="24" spans="2:12">
-      <c r="B24" s="27"/>
-      <c r="C24" s="8"/>
-      <c r="D24" s="8"/>
-      <c r="E24" s="9"/>
+      <c r="B24" s="29" t="s">
+        <v>56</v>
+      </c>
+      <c r="C24" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="D24" s="12"/>
+      <c r="E24" s="13"/>
       <c r="F24" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>57</v>
+        <v>36</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="I24" s="3"/>
-      <c r="J24" s="39" t="s">
         <v>58</v>
       </c>
+      <c r="I24" s="3">
+        <v>0</v>
+      </c>
+      <c r="J24" s="39"/>
       <c r="K24" s="39"/>
       <c r="L24" s="40"/>
     </row>
     <row r="25" spans="2:12">
-      <c r="B25" s="28"/>
-      <c r="C25" s="10"/>
-      <c r="D25" s="10"/>
-      <c r="E25" s="11"/>
+      <c r="B25" s="27"/>
+      <c r="C25" s="8"/>
+      <c r="D25" s="8"/>
+      <c r="E25" s="9"/>
       <c r="F25" s="2" t="s">
         <v>20</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>39</v>
+        <v>53</v>
       </c>
       <c r="H25" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="I25" s="3">
+        <v>0</v>
+      </c>
+      <c r="J25" s="39" t="s">
         <v>59</v>
       </c>
-      <c r="I25" s="3">
-        <v>0</v>
-      </c>
-      <c r="J25" s="39"/>
       <c r="K25" s="39"/>
       <c r="L25" s="40"/>
     </row>
     <row r="26" spans="2:12">
-      <c r="B26" s="29" t="s">
+      <c r="B26" s="27"/>
+      <c r="C26" s="8"/>
+      <c r="D26" s="8"/>
+      <c r="E26" s="9"/>
+      <c r="F26" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G26" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="C26" s="12" t="s">
+      <c r="H26" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="I26" s="3"/>
+      <c r="J26" s="39" t="s">
         <v>61</v>
       </c>
-      <c r="D26" s="12"/>
-      <c r="E26" s="13"/>
-      <c r="F26" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G26" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="H26" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="I26" s="3">
-        <v>0</v>
-      </c>
-      <c r="J26" s="39"/>
       <c r="K26" s="39"/>
       <c r="L26" s="40"/>
     </row>
     <row r="27" spans="2:12">
-      <c r="B27" s="27"/>
-      <c r="C27" s="8"/>
-      <c r="D27" s="8"/>
-      <c r="E27" s="9"/>
+      <c r="B27" s="28"/>
+      <c r="C27" s="10"/>
+      <c r="D27" s="10"/>
+      <c r="E27" s="11"/>
       <c r="F27" s="2" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>64</v>
+        <v>42</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I27" s="3">
         <v>0</v>
       </c>
-      <c r="J27" s="39" t="s">
-        <v>65</v>
-      </c>
+      <c r="J27" s="39"/>
       <c r="K27" s="39"/>
       <c r="L27" s="40"/>
     </row>
     <row r="28" spans="2:12">
-      <c r="B28" s="27"/>
-      <c r="C28" s="8"/>
-      <c r="D28" s="8"/>
-      <c r="E28" s="9"/>
+      <c r="B28" s="29" t="s">
+        <v>63</v>
+      </c>
+      <c r="C28" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="D28" s="12"/>
+      <c r="E28" s="13"/>
       <c r="F28" s="2" t="s">
-        <v>38</v>
+        <v>16</v>
       </c>
       <c r="G28" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="H28" s="2" t="s">
         <v>66</v>
-      </c>
-      <c r="H28" s="2" t="s">
-        <v>67</v>
       </c>
       <c r="I28" s="3">
         <v>0</v>
@@ -2066,19 +2049,19 @@
       <c r="D29" s="8"/>
       <c r="E29" s="9"/>
       <c r="F29" s="2" t="s">
-        <v>41</v>
+        <v>20</v>
       </c>
       <c r="G29" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="H29" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="I29" s="3">
+        <v>0</v>
+      </c>
+      <c r="J29" s="39" t="s">
         <v>68</v>
-      </c>
-      <c r="H29" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="I29" s="3">
-        <v>0</v>
-      </c>
-      <c r="J29" s="39" t="s">
-        <v>65</v>
       </c>
       <c r="K29" s="39"/>
       <c r="L29" s="40"/>
@@ -2089,7 +2072,7 @@
       <c r="D30" s="8"/>
       <c r="E30" s="9"/>
       <c r="F30" s="2" t="s">
-        <v>23</v>
+        <v>41</v>
       </c>
       <c r="G30" s="2" t="s">
         <v>69</v>
@@ -2110,7 +2093,7 @@
       <c r="D31" s="8"/>
       <c r="E31" s="9"/>
       <c r="F31" s="2" t="s">
-        <v>25</v>
+        <v>44</v>
       </c>
       <c r="G31" s="2" t="s">
         <v>71</v>
@@ -2122,7 +2105,7 @@
         <v>0</v>
       </c>
       <c r="J31" s="39" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="K31" s="39"/>
       <c r="L31" s="40"/>
@@ -2133,13 +2116,13 @@
       <c r="D32" s="8"/>
       <c r="E32" s="9"/>
       <c r="F32" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G32" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="H32" s="2" t="s">
         <v>73</v>
-      </c>
-      <c r="H32" s="2" t="s">
-        <v>74</v>
       </c>
       <c r="I32" s="3">
         <v>0</v>
@@ -2154,19 +2137,19 @@
       <c r="D33" s="8"/>
       <c r="E33" s="9"/>
       <c r="F33" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="H33" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="I33" s="3">
+        <v>0</v>
+      </c>
+      <c r="J33" s="39" t="s">
         <v>75</v>
-      </c>
-      <c r="G33" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="H33" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="I33" s="3">
-        <v>0</v>
-      </c>
-      <c r="J33" s="39" t="s">
-        <v>77</v>
       </c>
       <c r="K33" s="39"/>
       <c r="L33" s="40"/>
@@ -2177,20 +2160,18 @@
       <c r="D34" s="8"/>
       <c r="E34" s="9"/>
       <c r="F34" s="2" t="s">
-        <v>78</v>
+        <v>30</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="I34" s="3">
         <v>0</v>
       </c>
-      <c r="J34" s="39" t="s">
-        <v>29</v>
-      </c>
+      <c r="J34" s="39"/>
       <c r="K34" s="39"/>
       <c r="L34" s="40"/>
     </row>
@@ -2200,18 +2181,20 @@
       <c r="D35" s="8"/>
       <c r="E35" s="9"/>
       <c r="F35" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="G35" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="H35" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="I35" s="3">
+        <v>0</v>
+      </c>
+      <c r="J35" s="39" t="s">
         <v>80</v>
       </c>
-      <c r="G35" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="H35" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="I35" s="3">
-        <v>0</v>
-      </c>
-      <c r="J35" s="39"/>
       <c r="K35" s="39"/>
       <c r="L35" s="40"/>
     </row>
@@ -2221,112 +2204,112 @@
       <c r="D36" s="8"/>
       <c r="E36" s="9"/>
       <c r="F36" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="I36" s="3">
         <v>0</v>
       </c>
       <c r="J36" s="39" t="s">
-        <v>85</v>
+        <v>32</v>
       </c>
       <c r="K36" s="39"/>
       <c r="L36" s="40"/>
     </row>
     <row r="37" spans="2:12">
-      <c r="B37" s="28"/>
-      <c r="C37" s="10"/>
-      <c r="D37" s="10"/>
-      <c r="E37" s="11"/>
+      <c r="B37" s="27"/>
+      <c r="C37" s="8"/>
+      <c r="D37" s="8"/>
+      <c r="E37" s="9"/>
       <c r="F37" s="2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="I37" s="3">
         <v>0</v>
       </c>
-      <c r="J37" s="39" t="s">
-        <v>29</v>
-      </c>
+      <c r="J37" s="39"/>
       <c r="K37" s="39"/>
       <c r="L37" s="40"/>
     </row>
     <row r="38" spans="2:12">
-      <c r="B38" s="29" t="s">
+      <c r="B38" s="27"/>
+      <c r="C38" s="8"/>
+      <c r="D38" s="8"/>
+      <c r="E38" s="9"/>
+      <c r="F38" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="G38" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="H38" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="I38" s="3">
+        <v>0</v>
+      </c>
+      <c r="J38" s="39" t="s">
         <v>88</v>
       </c>
-      <c r="C38" s="12" t="s">
-        <v>89</v>
-      </c>
-      <c r="D38" s="12"/>
-      <c r="E38" s="13"/>
-      <c r="F38" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G38" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="H38" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="I38" s="3">
-        <v>0</v>
-      </c>
-      <c r="J38" s="39"/>
       <c r="K38" s="39"/>
       <c r="L38" s="40"/>
     </row>
     <row r="39" spans="2:12">
-      <c r="B39" s="27"/>
-      <c r="C39" s="8"/>
-      <c r="D39" s="8"/>
-      <c r="E39" s="9"/>
+      <c r="B39" s="28"/>
+      <c r="C39" s="10"/>
+      <c r="D39" s="10"/>
+      <c r="E39" s="11"/>
       <c r="F39" s="2" t="s">
-        <v>17</v>
+        <v>89</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H39" s="2" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="I39" s="3">
         <v>0</v>
       </c>
       <c r="J39" s="39" t="s">
-        <v>56</v>
+        <v>32</v>
       </c>
       <c r="K39" s="39"/>
       <c r="L39" s="40"/>
     </row>
     <row r="40" spans="2:12">
-      <c r="B40" s="27"/>
-      <c r="C40" s="8"/>
-      <c r="D40" s="8"/>
-      <c r="E40" s="9"/>
+      <c r="B40" s="29" t="s">
+        <v>91</v>
+      </c>
+      <c r="C40" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="D40" s="12"/>
+      <c r="E40" s="13"/>
       <c r="F40" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="H40" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="I40" s="3"/>
-      <c r="J40" s="39" t="s">
-        <v>92</v>
-      </c>
+        <v>93</v>
+      </c>
+      <c r="I40" s="3">
+        <v>0</v>
+      </c>
+      <c r="J40" s="39"/>
       <c r="K40" s="39"/>
       <c r="L40" s="40"/>
     </row>
@@ -2339,7 +2322,7 @@
         <v>20</v>
       </c>
       <c r="G41" s="2" t="s">
-        <v>57</v>
+        <v>94</v>
       </c>
       <c r="H41" s="2" t="s">
         <v>93</v>
@@ -2347,7 +2330,9 @@
       <c r="I41" s="3">
         <v>0</v>
       </c>
-      <c r="J41" s="39"/>
+      <c r="J41" s="39" t="s">
+        <v>59</v>
+      </c>
       <c r="K41" s="39"/>
       <c r="L41" s="40"/>
     </row>
@@ -2357,19 +2342,17 @@
       <c r="D42" s="8"/>
       <c r="E42" s="9"/>
       <c r="F42" s="2" t="s">
-        <v>94</v>
+        <v>21</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>39</v>
+        <v>53</v>
       </c>
       <c r="H42" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="I42" s="3">
-        <v>0</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="I42" s="3"/>
       <c r="J42" s="39" t="s">
-        <v>56</v>
+        <v>95</v>
       </c>
       <c r="K42" s="39"/>
       <c r="L42" s="40"/>
@@ -2380,18 +2363,18 @@
       <c r="D43" s="8"/>
       <c r="E43" s="9"/>
       <c r="F43" s="2" t="s">
-        <v>95</v>
+        <v>23</v>
       </c>
       <c r="G43" s="2" t="s">
-        <v>42</v>
+        <v>60</v>
       </c>
       <c r="H43" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="I43" s="3"/>
-      <c r="J43" s="39" t="s">
         <v>96</v>
       </c>
+      <c r="I43" s="3">
+        <v>0</v>
+      </c>
+      <c r="J43" s="39"/>
       <c r="K43" s="39"/>
       <c r="L43" s="40"/>
     </row>
@@ -2401,18 +2384,20 @@
       <c r="D44" s="8"/>
       <c r="E44" s="9"/>
       <c r="F44" s="2" t="s">
-        <v>27</v>
+        <v>97</v>
       </c>
       <c r="G44" s="2" t="s">
-        <v>97</v>
+        <v>42</v>
       </c>
       <c r="H44" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="I44" s="3">
         <v>0</v>
       </c>
-      <c r="J44" s="39"/>
+      <c r="J44" s="39" t="s">
+        <v>59</v>
+      </c>
       <c r="K44" s="39"/>
       <c r="L44" s="40"/>
     </row>
@@ -2422,18 +2407,18 @@
       <c r="D45" s="8"/>
       <c r="E45" s="9"/>
       <c r="F45" s="2" t="s">
-        <v>75</v>
+        <v>98</v>
       </c>
       <c r="G45" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="H45" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="I45" s="3"/>
+      <c r="J45" s="39" t="s">
         <v>99</v>
       </c>
-      <c r="H45" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="I45" s="3">
-        <v>0</v>
-      </c>
-      <c r="J45" s="39"/>
       <c r="K45" s="39"/>
       <c r="L45" s="40"/>
     </row>
@@ -2443,13 +2428,13 @@
       <c r="D46" s="8"/>
       <c r="E46" s="9"/>
       <c r="F46" s="2" t="s">
-        <v>78</v>
+        <v>30</v>
       </c>
       <c r="G46" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="H46" s="2" t="s">
         <v>101</v>
-      </c>
-      <c r="H46" s="2" t="s">
-        <v>102</v>
       </c>
       <c r="I46" s="3">
         <v>0</v>
@@ -2459,18 +2444,18 @@
       <c r="L46" s="40"/>
     </row>
     <row r="47" spans="2:12">
-      <c r="B47" s="28"/>
-      <c r="C47" s="10"/>
-      <c r="D47" s="10"/>
-      <c r="E47" s="11"/>
+      <c r="B47" s="27"/>
+      <c r="C47" s="8"/>
+      <c r="D47" s="8"/>
+      <c r="E47" s="9"/>
       <c r="F47" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G47" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="H47" s="2" t="s">
         <v>103</v>
-      </c>
-      <c r="H47" s="2" t="s">
-        <v>104</v>
       </c>
       <c r="I47" s="3">
         <v>0</v>
@@ -2480,22 +2465,18 @@
       <c r="L47" s="40"/>
     </row>
     <row r="48" spans="2:12">
-      <c r="B48" s="27" t="s">
-        <v>105</v>
-      </c>
-      <c r="C48" s="8" t="s">
-        <v>106</v>
-      </c>
+      <c r="B48" s="27"/>
+      <c r="C48" s="8"/>
       <c r="D48" s="8"/>
       <c r="E48" s="9"/>
       <c r="F48" s="2" t="s">
-        <v>13</v>
+        <v>81</v>
       </c>
       <c r="G48" s="2" t="s">
-        <v>33</v>
+        <v>104</v>
       </c>
       <c r="H48" s="2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="I48" s="3">
         <v>0</v>
@@ -2505,18 +2486,18 @@
       <c r="L48" s="40"/>
     </row>
     <row r="49" spans="2:12">
-      <c r="B49" s="27"/>
-      <c r="C49" s="8"/>
-      <c r="D49" s="8"/>
-      <c r="E49" s="9"/>
+      <c r="B49" s="28"/>
+      <c r="C49" s="10"/>
+      <c r="D49" s="10"/>
+      <c r="E49" s="11"/>
       <c r="F49" s="2" t="s">
-        <v>17</v>
+        <v>83</v>
       </c>
       <c r="G49" s="2" t="s">
-        <v>50</v>
+        <v>106</v>
       </c>
       <c r="H49" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I49" s="3">
         <v>0</v>
@@ -2526,18 +2507,22 @@
       <c r="L49" s="40"/>
     </row>
     <row r="50" spans="2:12">
-      <c r="B50" s="27"/>
-      <c r="C50" s="8"/>
+      <c r="B50" s="27" t="s">
+        <v>108</v>
+      </c>
+      <c r="C50" s="8" t="s">
+        <v>109</v>
+      </c>
       <c r="D50" s="8"/>
       <c r="E50" s="9"/>
       <c r="F50" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="G50" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="H50" s="2" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="I50" s="3">
         <v>0</v>
@@ -2547,91 +2532,91 @@
       <c r="L50" s="40"/>
     </row>
     <row r="51" spans="2:12">
-      <c r="B51" s="30"/>
-      <c r="C51" s="15"/>
-      <c r="D51" s="15"/>
-      <c r="E51" s="16"/>
-      <c r="F51" s="17" t="s">
+      <c r="B51" s="27"/>
+      <c r="C51" s="8"/>
+      <c r="D51" s="8"/>
+      <c r="E51" s="9"/>
+      <c r="F51" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="G51" s="17" t="s">
-        <v>97</v>
-      </c>
-      <c r="H51" s="17" t="s">
-        <v>110</v>
-      </c>
-      <c r="I51" s="18">
-        <v>0</v>
-      </c>
-      <c r="J51" s="41"/>
-      <c r="K51" s="41"/>
+      <c r="G51" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="H51" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="I51" s="3">
+        <v>0</v>
+      </c>
+      <c r="J51" s="39"/>
+      <c r="K51" s="39"/>
       <c r="L51" s="40"/>
     </row>
     <row r="52" spans="2:12">
-      <c r="B52" s="31" t="s">
-        <v>111</v>
-      </c>
-      <c r="C52" s="19" t="s">
+      <c r="B52" s="27"/>
+      <c r="C52" s="8"/>
+      <c r="D52" s="8"/>
+      <c r="E52" s="9"/>
+      <c r="F52" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G52" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="H52" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="D52" s="19"/>
-      <c r="E52" s="20"/>
-      <c r="F52" s="21" t="s">
-        <v>13</v>
-      </c>
-      <c r="G52" s="21" t="s">
-        <v>33</v>
-      </c>
-      <c r="H52" s="21" t="s">
+      <c r="I52" s="3">
+        <v>0</v>
+      </c>
+      <c r="J52" s="39"/>
+      <c r="K52" s="39"/>
+      <c r="L52" s="40"/>
+    </row>
+    <row r="53" spans="2:12">
+      <c r="B53" s="30"/>
+      <c r="C53" s="15"/>
+      <c r="D53" s="15"/>
+      <c r="E53" s="16"/>
+      <c r="F53" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="G53" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="H53" s="17" t="s">
         <v>113</v>
       </c>
-      <c r="I52" s="22">
-        <v>0</v>
-      </c>
-      <c r="J52" s="42"/>
-      <c r="K52" s="42"/>
-      <c r="L52" s="40"/>
-    </row>
-    <row r="53" spans="2:12">
-      <c r="B53" s="27"/>
-      <c r="C53" s="8"/>
-      <c r="D53" s="8"/>
-      <c r="E53" s="9"/>
-      <c r="F53" s="11" t="s">
+      <c r="I53" s="18">
+        <v>0</v>
+      </c>
+      <c r="J53" s="41"/>
+      <c r="K53" s="41"/>
+      <c r="L53" s="40"/>
+    </row>
+    <row r="54" spans="2:12">
+      <c r="B54" s="31" t="s">
         <v>114</v>
       </c>
-      <c r="G53" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="H53" s="11" t="s">
+      <c r="C54" s="19" t="s">
         <v>115</v>
       </c>
-      <c r="I53" s="10">
-        <v>0</v>
-      </c>
-      <c r="J53" s="43"/>
-      <c r="K53" s="43"/>
-      <c r="L53" s="40"/>
-    </row>
-    <row r="54" spans="2:12">
-      <c r="B54" s="27"/>
-      <c r="C54" s="8"/>
-      <c r="D54" s="8"/>
-      <c r="E54" s="9"/>
-      <c r="F54" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="G54" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="H54" s="11" t="s">
+      <c r="D54" s="19"/>
+      <c r="E54" s="20"/>
+      <c r="F54" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="G54" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="H54" s="21" t="s">
         <v>116</v>
       </c>
-      <c r="I54" s="10">
-        <v>0</v>
-      </c>
-      <c r="J54" s="43"/>
-      <c r="K54" s="43"/>
+      <c r="I54" s="22">
+        <v>0</v>
+      </c>
+      <c r="J54" s="42"/>
+      <c r="K54" s="42"/>
       <c r="L54" s="40"/>
     </row>
     <row r="55" spans="2:12">
@@ -2639,20 +2624,20 @@
       <c r="C55" s="8"/>
       <c r="D55" s="8"/>
       <c r="E55" s="9"/>
-      <c r="F55" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="G55" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="H55" s="2" t="s">
+      <c r="F55" s="11" t="s">
         <v>117</v>
       </c>
-      <c r="I55" s="3">
-        <v>0</v>
-      </c>
-      <c r="J55" s="39"/>
-      <c r="K55" s="39"/>
+      <c r="G55" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="H55" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="I55" s="10">
+        <v>0</v>
+      </c>
+      <c r="J55" s="43"/>
+      <c r="K55" s="43"/>
       <c r="L55" s="40"/>
     </row>
     <row r="56" spans="2:12">
@@ -2660,32 +2645,32 @@
       <c r="C56" s="8"/>
       <c r="D56" s="8"/>
       <c r="E56" s="9"/>
-      <c r="F56" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="G56" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="H56" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="I56" s="3">
-        <v>0</v>
-      </c>
-      <c r="J56" s="39"/>
-      <c r="K56" s="39"/>
+      <c r="F56" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="G56" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="H56" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="I56" s="10">
+        <v>0</v>
+      </c>
+      <c r="J56" s="43"/>
+      <c r="K56" s="43"/>
       <c r="L56" s="40"/>
     </row>
     <row r="57" spans="2:12">
-      <c r="B57" s="30"/>
-      <c r="C57" s="15"/>
-      <c r="D57" s="15"/>
-      <c r="E57" s="16"/>
+      <c r="B57" s="27"/>
+      <c r="C57" s="8"/>
+      <c r="D57" s="8"/>
+      <c r="E57" s="9"/>
       <c r="F57" s="2" t="s">
-        <v>25</v>
+        <v>44</v>
       </c>
       <c r="G57" s="2" t="s">
-        <v>119</v>
+        <v>100</v>
       </c>
       <c r="H57" s="2" t="s">
         <v>120</v>
@@ -2698,22 +2683,18 @@
       <c r="L57" s="40"/>
     </row>
     <row r="58" spans="2:12">
-      <c r="B58" s="31" t="s">
+      <c r="B58" s="27"/>
+      <c r="C58" s="8"/>
+      <c r="D58" s="8"/>
+      <c r="E58" s="9"/>
+      <c r="F58" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G58" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="H58" s="2" t="s">
         <v>121</v>
-      </c>
-      <c r="C58" s="19" t="s">
-        <v>122</v>
-      </c>
-      <c r="D58" s="19"/>
-      <c r="E58" s="20"/>
-      <c r="F58" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="G58" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="H58" s="2" t="s">
-        <v>124</v>
       </c>
       <c r="I58" s="3">
         <v>0</v>
@@ -2723,37 +2704,43 @@
       <c r="L58" s="40"/>
     </row>
     <row r="59" spans="2:12">
-      <c r="B59" s="27"/>
-      <c r="C59" s="8"/>
-      <c r="D59" s="8"/>
-      <c r="E59" s="9"/>
+      <c r="B59" s="30"/>
+      <c r="C59" s="15"/>
+      <c r="D59" s="15"/>
+      <c r="E59" s="16"/>
       <c r="F59" s="2" t="s">
-        <v>114</v>
+        <v>28</v>
       </c>
       <c r="G59" s="2" t="s">
-        <v>64</v>
+        <v>122</v>
       </c>
       <c r="H59" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="I59" s="3"/>
+        <v>123</v>
+      </c>
+      <c r="I59" s="3">
+        <v>0</v>
+      </c>
       <c r="J59" s="39"/>
       <c r="K59" s="39"/>
       <c r="L59" s="40"/>
     </row>
     <row r="60" spans="2:12">
-      <c r="B60" s="27"/>
-      <c r="C60" s="8"/>
-      <c r="D60" s="8"/>
-      <c r="E60" s="9"/>
+      <c r="B60" s="31" t="s">
+        <v>124</v>
+      </c>
+      <c r="C60" s="19" t="s">
+        <v>125</v>
+      </c>
+      <c r="D60" s="19"/>
+      <c r="E60" s="20"/>
       <c r="F60" s="2" t="s">
-        <v>38</v>
+        <v>126</v>
       </c>
       <c r="G60" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H60" s="2" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="I60" s="3">
         <v>0</v>
@@ -2768,17 +2755,15 @@
       <c r="D61" s="8"/>
       <c r="E61" s="9"/>
       <c r="F61" s="2" t="s">
-        <v>41</v>
+        <v>117</v>
       </c>
       <c r="G61" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H61" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="I61" s="3">
-        <v>0</v>
-      </c>
+        <v>128</v>
+      </c>
+      <c r="I61" s="3"/>
       <c r="J61" s="39"/>
       <c r="K61" s="39"/>
       <c r="L61" s="40"/>
@@ -2789,15 +2774,17 @@
       <c r="D62" s="8"/>
       <c r="E62" s="9"/>
       <c r="F62" s="2" t="s">
-        <v>23</v>
+        <v>41</v>
       </c>
       <c r="G62" s="2" t="s">
         <v>69</v>
       </c>
       <c r="H62" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="I62" s="3"/>
+        <v>129</v>
+      </c>
+      <c r="I62" s="3">
+        <v>0</v>
+      </c>
       <c r="J62" s="39"/>
       <c r="K62" s="39"/>
       <c r="L62" s="40"/>
@@ -2808,42 +2795,36 @@
       <c r="D63" s="8"/>
       <c r="E63" s="9"/>
       <c r="F63" s="2" t="s">
-        <v>25</v>
+        <v>44</v>
       </c>
       <c r="G63" s="2" t="s">
         <v>71</v>
       </c>
       <c r="H63" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="I63" s="3"/>
+        <v>130</v>
+      </c>
+      <c r="I63" s="3">
+        <v>0</v>
+      </c>
       <c r="J63" s="39"/>
       <c r="K63" s="39"/>
       <c r="L63" s="40"/>
     </row>
     <row r="64" spans="2:12">
-      <c r="B64" s="29" t="s">
-        <v>130</v>
-      </c>
-      <c r="C64" s="12" t="s">
+      <c r="B64" s="27"/>
+      <c r="C64" s="8"/>
+      <c r="D64" s="8"/>
+      <c r="E64" s="9"/>
+      <c r="F64" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G64" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="H64" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="D64" s="12" t="s">
-        <v>132</v>
-      </c>
-      <c r="E64" s="13"/>
-      <c r="F64" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G64" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="H64" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="I64" s="3">
-        <v>0</v>
-      </c>
+      <c r="I64" s="3"/>
       <c r="J64" s="39"/>
       <c r="K64" s="39"/>
       <c r="L64" s="40"/>
@@ -2854,111 +2835,109 @@
       <c r="D65" s="8"/>
       <c r="E65" s="9"/>
       <c r="F65" s="2" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="G65" s="2" t="s">
-        <v>134</v>
+        <v>74</v>
       </c>
       <c r="H65" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="I65" s="3" t="s">
-        <v>135</v>
-      </c>
+        <v>132</v>
+      </c>
+      <c r="I65" s="3"/>
       <c r="J65" s="39"/>
       <c r="K65" s="39"/>
       <c r="L65" s="40"/>
     </row>
     <row r="66" spans="2:12">
-      <c r="B66" s="28"/>
-      <c r="C66" s="10"/>
-      <c r="D66" s="10"/>
-      <c r="E66" s="11"/>
+      <c r="B66" s="29" t="s">
+        <v>133</v>
+      </c>
+      <c r="C66" s="12" t="s">
+        <v>134</v>
+      </c>
+      <c r="D66" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="E66" s="13"/>
       <c r="F66" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="G66" s="2" t="s">
         <v>136</v>
       </c>
       <c r="H66" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="I66" s="3" t="s">
-        <v>137</v>
+        <v>18</v>
+      </c>
+      <c r="I66" s="3">
+        <v>0</v>
       </c>
       <c r="J66" s="39"/>
       <c r="K66" s="39"/>
       <c r="L66" s="40"/>
     </row>
-    <row r="67" spans="2:12" ht="112.5">
-      <c r="B67" s="29" t="s">
+    <row r="67" spans="2:12">
+      <c r="B67" s="27"/>
+      <c r="C67" s="8"/>
+      <c r="D67" s="8"/>
+      <c r="E67" s="9"/>
+      <c r="F67" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G67" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="H67" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I67" s="3" t="s">
         <v>138</v>
-      </c>
-      <c r="C67" s="12" t="s">
-        <v>139</v>
-      </c>
-      <c r="D67" s="12" t="s">
-        <v>140</v>
-      </c>
-      <c r="E67" s="14" t="s">
-        <v>141</v>
-      </c>
-      <c r="F67" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G67" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="H67" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="I67" s="3">
-        <v>0</v>
       </c>
       <c r="J67" s="39"/>
       <c r="K67" s="39"/>
       <c r="L67" s="40"/>
     </row>
     <row r="68" spans="2:12">
-      <c r="B68" s="30"/>
-      <c r="C68" s="15"/>
-      <c r="D68" s="15"/>
-      <c r="E68" s="16"/>
+      <c r="B68" s="28"/>
+      <c r="C68" s="10"/>
+      <c r="D68" s="10"/>
+      <c r="E68" s="11"/>
       <c r="F68" s="2" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="G68" s="2" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="H68" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="I68" s="3">
-        <v>0</v>
+        <v>18</v>
+      </c>
+      <c r="I68" s="3" t="s">
+        <v>140</v>
       </c>
       <c r="J68" s="39"/>
       <c r="K68" s="39"/>
       <c r="L68" s="40"/>
     </row>
-    <row r="69" spans="2:12" ht="67.5">
-      <c r="B69" s="31" t="s">
+    <row r="69" spans="2:12" ht="112.5">
+      <c r="B69" s="29" t="s">
+        <v>141</v>
+      </c>
+      <c r="C69" s="12" t="s">
+        <v>142</v>
+      </c>
+      <c r="D69" s="12" t="s">
+        <v>143</v>
+      </c>
+      <c r="E69" s="14" t="s">
         <v>144</v>
       </c>
-      <c r="C69" s="19" t="s">
-        <v>139</v>
-      </c>
-      <c r="D69" s="19"/>
-      <c r="E69" s="48" t="s">
+      <c r="F69" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G69" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="F69" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G69" s="2" t="s">
-        <v>146</v>
-      </c>
       <c r="H69" s="2" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="I69" s="3">
         <v>0</v>
@@ -2973,13 +2952,13 @@
       <c r="D70" s="15"/>
       <c r="E70" s="16"/>
       <c r="F70" s="2" t="s">
-        <v>114</v>
+        <v>20</v>
       </c>
       <c r="G70" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H70" s="2" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="I70" s="3">
         <v>0</v>
@@ -2988,63 +2967,71 @@
       <c r="K70" s="39"/>
       <c r="L70" s="40"/>
     </row>
-    <row r="71" spans="2:12">
-      <c r="B71" s="27" t="s">
+    <row r="71" spans="2:12" ht="67.5">
+      <c r="B71" s="31" t="s">
+        <v>147</v>
+      </c>
+      <c r="C71" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="D71" s="19"/>
+      <c r="E71" s="48" t="s">
         <v>148</v>
       </c>
-      <c r="C71" s="8" t="s">
+      <c r="F71" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G71" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="D71" s="8"/>
-      <c r="E71" s="9"/>
-      <c r="F71" s="13" t="s">
-        <v>123</v>
-      </c>
-      <c r="G71" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="H71" s="13" t="s">
+      <c r="H71" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I71" s="3">
+        <v>0</v>
+      </c>
+      <c r="J71" s="39"/>
+      <c r="K71" s="39"/>
+      <c r="L71" s="40"/>
+    </row>
+    <row r="72" spans="2:12">
+      <c r="B72" s="30"/>
+      <c r="C72" s="15"/>
+      <c r="D72" s="15"/>
+      <c r="E72" s="16"/>
+      <c r="F72" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="G72" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="I71" s="12">
-        <v>0</v>
-      </c>
-      <c r="J71" s="46"/>
-      <c r="K71" s="46"/>
-      <c r="L71" s="47"/>
-    </row>
-    <row r="72" spans="2:12" ht="45">
-      <c r="B72" s="27"/>
-      <c r="C72" s="8"/>
-      <c r="D72" s="8"/>
-      <c r="E72" s="9"/>
-      <c r="F72" s="13" t="s">
-        <v>114</v>
-      </c>
-      <c r="G72" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="H72" s="14" t="s">
+      <c r="H72" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I72" s="3">
+        <v>0</v>
+      </c>
+      <c r="J72" s="39"/>
+      <c r="K72" s="39"/>
+      <c r="L72" s="40"/>
+    </row>
+    <row r="73" spans="2:12">
+      <c r="B73" s="27" t="s">
         <v>151</v>
       </c>
-      <c r="I72" s="12"/>
-      <c r="J72" s="46"/>
-      <c r="K72" s="46"/>
-      <c r="L72" s="47"/>
-    </row>
-    <row r="73" spans="2:12" ht="45">
-      <c r="B73" s="27"/>
-      <c r="C73" s="8"/>
+      <c r="C73" s="8" t="s">
+        <v>152</v>
+      </c>
       <c r="D73" s="8"/>
       <c r="E73" s="9"/>
       <c r="F73" s="13" t="s">
-        <v>38</v>
+        <v>126</v>
       </c>
       <c r="G73" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="H73" s="14" t="s">
-        <v>152</v>
+        <v>24</v>
+      </c>
+      <c r="H73" s="13" t="s">
+        <v>153</v>
       </c>
       <c r="I73" s="12">
         <v>0</v>
@@ -3053,40 +3040,38 @@
       <c r="K73" s="46"/>
       <c r="L73" s="47"/>
     </row>
-    <row r="74" spans="2:12" ht="67.5">
+    <row r="74" spans="2:12" ht="45">
       <c r="B74" s="27"/>
       <c r="C74" s="8"/>
       <c r="D74" s="8"/>
       <c r="E74" s="9"/>
       <c r="F74" s="13" t="s">
-        <v>41</v>
+        <v>117</v>
       </c>
       <c r="G74" s="13" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="H74" s="14" t="s">
-        <v>153</v>
-      </c>
-      <c r="I74" s="12">
-        <v>0</v>
-      </c>
+        <v>154</v>
+      </c>
+      <c r="I74" s="12"/>
       <c r="J74" s="46"/>
       <c r="K74" s="46"/>
       <c r="L74" s="47"/>
     </row>
-    <row r="75" spans="2:12" ht="67.5">
+    <row r="75" spans="2:12" ht="45">
       <c r="B75" s="27"/>
       <c r="C75" s="8"/>
       <c r="D75" s="8"/>
       <c r="E75" s="9"/>
       <c r="F75" s="13" t="s">
-        <v>23</v>
+        <v>41</v>
       </c>
       <c r="G75" s="13" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="H75" s="14" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="I75" s="12">
         <v>0</v>
@@ -3101,13 +3086,13 @@
       <c r="D76" s="8"/>
       <c r="E76" s="9"/>
       <c r="F76" s="13" t="s">
-        <v>25</v>
+        <v>44</v>
       </c>
       <c r="G76" s="13" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="H76" s="14" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="I76" s="12">
         <v>0</v>
@@ -3122,13 +3107,13 @@
       <c r="D77" s="8"/>
       <c r="E77" s="9"/>
       <c r="F77" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G77" s="13" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="H77" s="14" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="I77" s="12">
         <v>0</v>
@@ -3143,13 +3128,13 @@
       <c r="D78" s="8"/>
       <c r="E78" s="9"/>
       <c r="F78" s="13" t="s">
-        <v>75</v>
+        <v>28</v>
       </c>
       <c r="G78" s="13" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="H78" s="14" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="I78" s="12">
         <v>0</v>
@@ -3158,19 +3143,19 @@
       <c r="K78" s="46"/>
       <c r="L78" s="47"/>
     </row>
-    <row r="79" spans="2:12" ht="45">
-      <c r="B79" s="30"/>
-      <c r="C79" s="15"/>
-      <c r="D79" s="15"/>
-      <c r="E79" s="16"/>
+    <row r="79" spans="2:12" ht="67.5">
+      <c r="B79" s="27"/>
+      <c r="C79" s="8"/>
+      <c r="D79" s="8"/>
+      <c r="E79" s="9"/>
       <c r="F79" s="13" t="s">
-        <v>78</v>
+        <v>30</v>
       </c>
       <c r="G79" s="13" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="H79" s="14" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="I79" s="12">
         <v>0</v>
@@ -3179,50 +3164,40 @@
       <c r="K79" s="46"/>
       <c r="L79" s="47"/>
     </row>
-    <row r="80" spans="2:12" ht="22.5">
-      <c r="B80" s="31" t="s">
-        <v>159</v>
-      </c>
-      <c r="C80" s="19" t="s">
+    <row r="80" spans="2:12" ht="67.5">
+      <c r="B80" s="27"/>
+      <c r="C80" s="8"/>
+      <c r="D80" s="8"/>
+      <c r="E80" s="9"/>
+      <c r="F80" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="G80" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="H80" s="14" t="s">
         <v>160</v>
       </c>
-      <c r="D80" s="19"/>
-      <c r="E80" s="20" t="s">
-        <v>161</v>
-      </c>
-      <c r="F80" s="13" t="s">
-        <v>123</v>
-      </c>
-      <c r="G80" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="H80" s="14" t="s">
-        <v>162</v>
-      </c>
-      <c r="I80" s="12"/>
+      <c r="I80" s="12">
+        <v>0</v>
+      </c>
       <c r="J80" s="46"/>
       <c r="K80" s="46"/>
       <c r="L80" s="47"/>
     </row>
-    <row r="81" spans="2:12" ht="22.5">
-      <c r="B81" s="31" t="s">
-        <v>163</v>
-      </c>
-      <c r="C81" s="19" t="s">
-        <v>164</v>
-      </c>
-      <c r="D81" s="19"/>
-      <c r="E81" s="20" t="s">
+    <row r="81" spans="2:12" ht="45">
+      <c r="B81" s="30"/>
+      <c r="C81" s="15"/>
+      <c r="D81" s="15"/>
+      <c r="E81" s="16"/>
+      <c r="F81" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="G81" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="H81" s="14" t="s">
         <v>161</v>
-      </c>
-      <c r="F81" s="13" t="s">
-        <v>123</v>
-      </c>
-      <c r="G81" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="H81" s="14" t="s">
-        <v>165</v>
       </c>
       <c r="I81" s="12">
         <v>0</v>
@@ -3233,43 +3208,95 @@
     </row>
     <row r="82" spans="2:12" ht="22.5">
       <c r="B82" s="31" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="C82" s="19" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="D82" s="19"/>
-      <c r="E82" s="48" t="s">
-        <v>168</v>
-      </c>
-      <c r="F82" s="13"/>
-      <c r="G82" s="13"/>
-      <c r="H82" s="13"/>
+      <c r="E82" s="20" t="s">
+        <v>164</v>
+      </c>
+      <c r="F82" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="G82" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="H82" s="14" t="s">
+        <v>165</v>
+      </c>
       <c r="I82" s="12"/>
       <c r="J82" s="46"/>
       <c r="K82" s="46"/>
       <c r="L82" s="47"/>
     </row>
-    <row r="83" spans="2:12">
-      <c r="B83" s="32" t="s">
+    <row r="83" spans="2:12" ht="22.5">
+      <c r="B83" s="31" t="s">
+        <v>166</v>
+      </c>
+      <c r="C83" s="19" t="s">
+        <v>167</v>
+      </c>
+      <c r="D83" s="19"/>
+      <c r="E83" s="20" t="s">
+        <v>164</v>
+      </c>
+      <c r="F83" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="G83" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="H83" s="14" t="s">
+        <v>168</v>
+      </c>
+      <c r="I83" s="12">
+        <v>0</v>
+      </c>
+      <c r="J83" s="46"/>
+      <c r="K83" s="46"/>
+      <c r="L83" s="47"/>
+    </row>
+    <row r="84" spans="2:12" ht="22.5">
+      <c r="B84" s="31" t="s">
         <v>169</v>
       </c>
-      <c r="C83" s="33" t="s">
+      <c r="C84" s="19" t="s">
         <v>170</v>
       </c>
-      <c r="D83" s="33">
+      <c r="D84" s="19"/>
+      <c r="E84" s="48" t="s">
+        <v>171</v>
+      </c>
+      <c r="F84" s="13"/>
+      <c r="G84" s="13"/>
+      <c r="H84" s="13"/>
+      <c r="I84" s="12"/>
+      <c r="J84" s="46"/>
+      <c r="K84" s="46"/>
+      <c r="L84" s="47"/>
+    </row>
+    <row r="85" spans="2:12">
+      <c r="B85" s="32" t="s">
+        <v>172</v>
+      </c>
+      <c r="C85" s="33" t="s">
+        <v>173</v>
+      </c>
+      <c r="D85" s="33">
         <v>32</v>
       </c>
-      <c r="E83" s="34" t="s">
-        <v>171</v>
-      </c>
-      <c r="F83" s="34"/>
-      <c r="G83" s="34"/>
-      <c r="H83" s="34"/>
-      <c r="I83" s="33"/>
-      <c r="J83" s="44"/>
-      <c r="K83" s="44"/>
-      <c r="L83" s="45"/>
+      <c r="E85" s="34" t="s">
+        <v>174</v>
+      </c>
+      <c r="F85" s="34"/>
+      <c r="G85" s="34"/>
+      <c r="H85" s="34"/>
+      <c r="I85" s="33"/>
+      <c r="J85" s="44"/>
+      <c r="K85" s="44"/>
+      <c r="L85" s="45"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>

</xml_diff>

<commit_message>
add template comment sample
(refs: rggen/rggen#219)
</commit_message>
<xml_diff>
--- a/block_0.xlsx
+++ b/block_0.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28512"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B7053C41-96B5-4FDA-BFF1-696E0C16680A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{477346D9-788D-496D-8950-CBE58FB18A11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -103,7 +103,7 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>this is register_0.bit_field_0</t>
+    <t>this is &lt;%= bit_field.full_name %&gt;</t>
   </si>
   <si>
     <t>bit_field_1</t>
@@ -1480,7 +1480,7 @@
   <dimension ref="B1:L85"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
@@ -1493,7 +1493,7 @@
     <col min="8" max="8" width="18.625" style="1" customWidth="1"/>
     <col min="9" max="9" width="11.375" bestFit="1" customWidth="1"/>
     <col min="10" max="11" width="20.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="24.625" customWidth="1"/>
+    <col min="12" max="12" width="33.625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:12">
@@ -1563,7 +1563,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="2:12">
+    <row r="7" spans="2:12" ht="15.75">
       <c r="B7" s="26" t="s">
         <v>15</v>
       </c>

</xml_diff>

<commit_message>
update samples due to `initial_valeu` update
(refs: rggen/rggen#241)
</commit_message>
<xml_diff>
--- a/block_0.xlsx
+++ b/block_0.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28609"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{477346D9-788D-496D-8950-CBE58FB18A11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="277" documentId="8_{A0D56F00-2FF8-4245-9EBC-D59D5B1EA094}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A5392AF5-A4DE-4A24-9D68-AEEA8892980C}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -513,8 +513,10 @@
     <t>2:4:4:8</t>
   </si>
   <si>
-    <t>0, 1, 2, 3</t>
-    <phoneticPr fontId="1"/>
+    <t>0, 1, 2, 3
+1, 2, 3, 0
+2, 3, 0, 1
+3, 0, 1, 2</t>
   </si>
   <si>
     <t>register_11</t>
@@ -1140,7 +1142,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -1195,6 +1197,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1479,8 +1484,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:L85"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
+      <selection activeCell="I68" sqref="I68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
@@ -2896,7 +2901,7 @@
       <c r="K67" s="39"/>
       <c r="L67" s="40"/>
     </row>
-    <row r="68" spans="2:12">
+    <row r="68" spans="2:12" ht="76.5" customHeight="1">
       <c r="B68" s="28"/>
       <c r="C68" s="10"/>
       <c r="D68" s="10"/>
@@ -2910,7 +2915,7 @@
       <c r="H68" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="I68" s="3" t="s">
+      <c r="I68" s="50" t="s">
         <v>140</v>
       </c>
       <c r="J68" s="39"/>

</xml_diff>

<commit_message>
add `maskable` register type
(refs: rggen/rggen#262)
</commit_message>
<xml_diff>
--- a/block_0.xlsx
+++ b/block_0.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29609"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="277" documentId="8_{A0D56F00-2FF8-4245-9EBC-D59D5B1EA094}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A5392AF5-A4DE-4A24-9D68-AEEA8892980C}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D5032DF8-6DE2-4D98-A45E-7709AFC68906}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="179">
   <si>
     <t>block name</t>
     <phoneticPr fontId="1"/>
@@ -627,10 +627,22 @@
     <t>0x78</t>
   </si>
   <si>
+    <t>maskable</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>register_17</t>
+  </si>
+  <si>
+    <t>0x7C</t>
+  </si>
+  <si>
     <t>reserved</t>
   </si>
   <si>
-    <t>register_17</t>
+    <t>register_18</t>
   </si>
   <si>
     <t>0x80</t>
@@ -1482,10 +1494,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:L85"/>
+  <dimension ref="B1:L86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
-      <selection activeCell="I68" sqref="I68"/>
+    <sheetView tabSelected="1" topLeftCell="A80" workbookViewId="0">
+      <selection activeCell="I83" sqref="I83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
@@ -3263,7 +3275,7 @@
       <c r="K83" s="46"/>
       <c r="L83" s="47"/>
     </row>
-    <row r="84" spans="2:12" ht="22.5">
+    <row r="84" spans="2:12" ht="15.75">
       <c r="B84" s="31" t="s">
         <v>169</v>
       </c>
@@ -3271,37 +3283,64 @@
         <v>170</v>
       </c>
       <c r="D84" s="19"/>
-      <c r="E84" s="48" t="s">
+      <c r="E84" s="20" t="s">
         <v>171</v>
       </c>
-      <c r="F84" s="13"/>
-      <c r="G84" s="13"/>
-      <c r="H84" s="13"/>
-      <c r="I84" s="12"/>
+      <c r="F84" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="G84" s="13" t="s">
+        <v>172</v>
+      </c>
+      <c r="H84" s="14" t="s">
+        <v>164</v>
+      </c>
+      <c r="I84" s="12">
+        <v>0</v>
+      </c>
       <c r="J84" s="46"/>
       <c r="K84" s="46"/>
       <c r="L84" s="47"/>
     </row>
-    <row r="85" spans="2:12">
-      <c r="B85" s="32" t="s">
-        <v>172</v>
-      </c>
-      <c r="C85" s="33" t="s">
+    <row r="85" spans="2:12" ht="22.5">
+      <c r="B85" s="31" t="s">
         <v>173</v>
       </c>
-      <c r="D85" s="33">
+      <c r="C85" s="19" t="s">
+        <v>174</v>
+      </c>
+      <c r="D85" s="19"/>
+      <c r="E85" s="48" t="s">
+        <v>175</v>
+      </c>
+      <c r="F85" s="13"/>
+      <c r="G85" s="13"/>
+      <c r="H85" s="13"/>
+      <c r="I85" s="12"/>
+      <c r="J85" s="46"/>
+      <c r="K85" s="46"/>
+      <c r="L85" s="47"/>
+    </row>
+    <row r="86" spans="2:12">
+      <c r="B86" s="32" t="s">
+        <v>176</v>
+      </c>
+      <c r="C86" s="33" t="s">
+        <v>177</v>
+      </c>
+      <c r="D86" s="33">
         <v>32</v>
       </c>
-      <c r="E85" s="34" t="s">
-        <v>174</v>
-      </c>
-      <c r="F85" s="34"/>
-      <c r="G85" s="34"/>
-      <c r="H85" s="34"/>
-      <c r="I85" s="33"/>
-      <c r="J85" s="44"/>
-      <c r="K85" s="44"/>
-      <c r="L85" s="45"/>
+      <c r="E86" s="34" t="s">
+        <v>178</v>
+      </c>
+      <c r="F86" s="34"/>
+      <c r="G86" s="34"/>
+      <c r="H86" s="34"/>
+      <c r="I86" s="33"/>
+      <c r="J86" s="44"/>
+      <c r="K86" s="44"/>
+      <c r="L86" s="45"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>

</xml_diff>

<commit_message>
add `coutner` bit feild type
(refs: rggen/rggen#266)
</commit_message>
<xml_diff>
--- a/block_0.xlsx
+++ b/block_0.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29609"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D5032DF8-6DE2-4D98-A45E-7709AFC68906}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{13D5861D-718C-4293-8F87-38F330358390}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="183">
   <si>
     <t>block name</t>
     <phoneticPr fontId="1"/>
@@ -603,6 +603,18 @@
     <t>register_14</t>
   </si>
   <si>
+    <t>0x64</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>counter</t>
+  </si>
+  <si>
+    <t>register_15</t>
+  </si>
+  <si>
     <t>0x70</t>
   </si>
   <si>
@@ -612,7 +624,7 @@
     <t>ro</t>
   </si>
   <si>
-    <t>register_15</t>
+    <t>register_16</t>
   </si>
   <si>
     <t>0x74</t>
@@ -621,7 +633,7 @@
     <t>wo</t>
   </si>
   <si>
-    <t>register_16</t>
+    <t>register_17</t>
   </si>
   <si>
     <t>0x78</t>
@@ -633,7 +645,7 @@
     <t>16</t>
   </si>
   <si>
-    <t>register_17</t>
+    <t>register_18</t>
   </si>
   <si>
     <t>0x7C</t>
@@ -642,7 +654,7 @@
     <t>reserved</t>
   </si>
   <si>
-    <t>register_18</t>
+    <t>register_19</t>
   </si>
   <si>
     <t>0x80</t>
@@ -1494,10 +1506,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:L86"/>
+  <dimension ref="B1:L88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A80" workbookViewId="0">
-      <selection activeCell="I83" sqref="I83"/>
+    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="C83" sqref="C83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
@@ -3223,124 +3235,172 @@
       <c r="K81" s="46"/>
       <c r="L81" s="47"/>
     </row>
-    <row r="82" spans="2:12" ht="22.5">
-      <c r="B82" s="31" t="s">
+    <row r="82" spans="2:12" ht="15.75">
+      <c r="B82" s="27" t="s">
         <v>162</v>
       </c>
-      <c r="C82" s="19" t="s">
+      <c r="C82" s="8" t="s">
         <v>163</v>
       </c>
-      <c r="D82" s="19"/>
-      <c r="E82" s="20" t="s">
-        <v>164</v>
-      </c>
+      <c r="D82" s="8"/>
+      <c r="E82" s="9"/>
       <c r="F82" s="13" t="s">
         <v>126</v>
       </c>
       <c r="G82" s="13" t="s">
-        <v>22</v>
+        <v>164</v>
       </c>
       <c r="H82" s="14" t="s">
         <v>165</v>
       </c>
-      <c r="I82" s="12"/>
+      <c r="I82" s="12">
+        <v>0</v>
+      </c>
       <c r="J82" s="46"/>
       <c r="K82" s="46"/>
       <c r="L82" s="47"/>
     </row>
-    <row r="83" spans="2:12" ht="22.5">
-      <c r="B83" s="31" t="s">
-        <v>166</v>
-      </c>
-      <c r="C83" s="19" t="s">
-        <v>167</v>
-      </c>
-      <c r="D83" s="19"/>
-      <c r="E83" s="20" t="s">
+    <row r="83" spans="2:12" ht="15.75">
+      <c r="B83" s="27"/>
+      <c r="C83" s="8"/>
+      <c r="D83" s="8"/>
+      <c r="E83" s="9"/>
+      <c r="F83" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="G83" s="13" t="s">
         <v>164</v>
       </c>
-      <c r="F83" s="13" t="s">
-        <v>126</v>
-      </c>
-      <c r="G83" s="13" t="s">
-        <v>22</v>
-      </c>
       <c r="H83" s="14" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="I83" s="12">
         <v>0</v>
       </c>
-      <c r="J83" s="46"/>
+      <c r="J83" s="46" t="s">
+        <v>46</v>
+      </c>
       <c r="K83" s="46"/>
       <c r="L83" s="47"/>
     </row>
-    <row r="84" spans="2:12" ht="15.75">
+    <row r="84" spans="2:12" ht="22.5">
       <c r="B84" s="31" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="C84" s="19" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="D84" s="19"/>
       <c r="E84" s="20" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="F84" s="13" t="s">
         <v>126</v>
       </c>
       <c r="G84" s="13" t="s">
-        <v>172</v>
+        <v>22</v>
       </c>
       <c r="H84" s="14" t="s">
-        <v>164</v>
-      </c>
-      <c r="I84" s="12">
-        <v>0</v>
-      </c>
+        <v>169</v>
+      </c>
+      <c r="I84" s="12"/>
       <c r="J84" s="46"/>
       <c r="K84" s="46"/>
       <c r="L84" s="47"/>
     </row>
     <row r="85" spans="2:12" ht="22.5">
       <c r="B85" s="31" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="C85" s="19" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="D85" s="19"/>
-      <c r="E85" s="48" t="s">
-        <v>175</v>
-      </c>
-      <c r="F85" s="13"/>
-      <c r="G85" s="13"/>
-      <c r="H85" s="13"/>
-      <c r="I85" s="12"/>
+      <c r="E85" s="20" t="s">
+        <v>168</v>
+      </c>
+      <c r="F85" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="G85" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="H85" s="14" t="s">
+        <v>172</v>
+      </c>
+      <c r="I85" s="12">
+        <v>0</v>
+      </c>
       <c r="J85" s="46"/>
       <c r="K85" s="46"/>
       <c r="L85" s="47"/>
     </row>
-    <row r="86" spans="2:12">
-      <c r="B86" s="32" t="s">
+    <row r="86" spans="2:12" ht="15.75">
+      <c r="B86" s="31" t="s">
+        <v>173</v>
+      </c>
+      <c r="C86" s="19" t="s">
+        <v>174</v>
+      </c>
+      <c r="D86" s="19"/>
+      <c r="E86" s="20" t="s">
+        <v>175</v>
+      </c>
+      <c r="F86" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="G86" s="13" t="s">
         <v>176</v>
       </c>
-      <c r="C86" s="33" t="s">
+      <c r="H86" s="14" t="s">
+        <v>168</v>
+      </c>
+      <c r="I86" s="12">
+        <v>0</v>
+      </c>
+      <c r="J86" s="46"/>
+      <c r="K86" s="46"/>
+      <c r="L86" s="47"/>
+    </row>
+    <row r="87" spans="2:12" ht="22.5">
+      <c r="B87" s="31" t="s">
         <v>177</v>
       </c>
-      <c r="D86" s="33">
+      <c r="C87" s="19" t="s">
+        <v>178</v>
+      </c>
+      <c r="D87" s="19"/>
+      <c r="E87" s="48" t="s">
+        <v>179</v>
+      </c>
+      <c r="F87" s="13"/>
+      <c r="G87" s="13"/>
+      <c r="H87" s="13"/>
+      <c r="I87" s="12"/>
+      <c r="J87" s="46"/>
+      <c r="K87" s="46"/>
+      <c r="L87" s="47"/>
+    </row>
+    <row r="88" spans="2:12">
+      <c r="B88" s="32" t="s">
+        <v>180</v>
+      </c>
+      <c r="C88" s="33" t="s">
+        <v>181</v>
+      </c>
+      <c r="D88" s="33">
         <v>32</v>
       </c>
-      <c r="E86" s="34" t="s">
-        <v>178</v>
-      </c>
-      <c r="F86" s="34"/>
-      <c r="G86" s="34"/>
-      <c r="H86" s="34"/>
-      <c r="I86" s="33"/>
-      <c r="J86" s="44"/>
-      <c r="K86" s="44"/>
-      <c r="L86" s="45"/>
+      <c r="E88" s="34" t="s">
+        <v>182</v>
+      </c>
+      <c r="F88" s="34"/>
+      <c r="G88" s="34"/>
+      <c r="H88" s="34"/>
+      <c r="I88" s="33"/>
+      <c r="J88" s="44"/>
+      <c r="K88" s="44"/>
+      <c r="L88" s="45"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>

</xml_diff>